<commit_message>
Issue #374: Namespace - add "clipper" - Upd2
Add the namespace "clipper" to the Namespace Registry and the config.properties file. Now uploading the Namespace Registry document.

Resolves #374
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\AAANameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77360AA-4D0D-475D-94C6-24FDAE736705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3DF3A8B-61B4-4020-BE47-41A1F1736400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5213" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="531">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1521,9 +1521,6 @@
     <t>http://pds.nasa.gov/pds4/clementine/v1</t>
   </si>
   <si>
-    <t>PDS4_clementine</t>
-  </si>
-  <si>
     <t>The Clementine mission dictionary contains a class with attributes specific to the Deep Space Program Science Experiment, including the Clementine orbiter and its instruments. This dictionary was created for the migration of Clementine data products from PDS3 to PDS4 by Million Concepts (contact M. St. Clair).</t>
   </si>
   <si>
@@ -1606,6 +1603,21 @@
   </si>
   <si>
     <t>Y. Yamamoto</t>
+  </si>
+  <si>
+    <t>clipper</t>
+  </si>
+  <si>
+    <t>The Europa Clipper mission dictionary contains classes that describe aspects of the Clipper mission and related instruments.</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/clipper/v1</t>
+  </si>
+  <si>
+    <t>PDS4_CLIPPER</t>
+  </si>
+  <si>
+    <t>PDS4_CLEMENTINE</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1839,6 +1851,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2157,10 +2172,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U94"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2376,7 +2391,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>35</v>
@@ -2887,28 +2902,28 @@
     </row>
     <row r="14" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>500</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="D14" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>502</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>501</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>503</v>
-      </c>
       <c r="F14" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>38</v>
@@ -2917,7 +2932,7 @@
         <v>25</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L14" s="16" t="s">
         <v>97</v>
@@ -3202,28 +3217,28 @@
     </row>
     <row r="19" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>505</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>513</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>512</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>506</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>514</v>
-      </c>
       <c r="F19" s="32" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I19" s="30" t="s">
         <v>38</v>
@@ -3232,7 +3247,7 @@
         <v>25</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L19" s="30" t="s">
         <v>109</v>
@@ -3241,10 +3256,10 @@
         <v>110</v>
       </c>
       <c r="N19" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="O19" s="19" t="s">
         <v>509</v>
-      </c>
-      <c r="O19" s="19" t="s">
-        <v>510</v>
       </c>
       <c r="P19" s="30" t="s">
         <v>44</v>
@@ -3253,7 +3268,7 @@
         <v>44333</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="S19" s="30" t="s">
         <v>33</v>
@@ -4235,7 +4250,7 @@
         <v>496</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>495</v>
@@ -4250,7 +4265,7 @@
         <v>23</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>498</v>
+        <v>530</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>216</v>
@@ -4290,150 +4305,152 @@
       </c>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="M37" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q37" s="6">
+        <v>44385</v>
+      </c>
+      <c r="R37" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U37" s="7"/>
+    </row>
+    <row r="38" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30" t="s">
+      <c r="B38" s="30"/>
+      <c r="C38" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D38" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E38" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="L38" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="N38" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O38" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="P38" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q38" s="33">
+        <v>44193</v>
+      </c>
+      <c r="R38" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="F37" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="I37" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="J37" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K37" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="L37" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M37" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="N37" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O37" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="P37" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q37" s="33">
-        <v>44193</v>
-      </c>
-      <c r="R37" s="19" t="s">
-        <v>526</v>
-      </c>
-      <c r="S37" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T37" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U37" s="34"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N38" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O38" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>42119</v>
-      </c>
-      <c r="R38" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S38" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T38" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U38" s="7"/>
+      <c r="S38" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T38" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U38" s="34"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>237</v>
+      <c r="H39" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>216</v>
@@ -4442,28 +4459,28 @@
         <v>25</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>102</v>
+        <v>193</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q39" s="6">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R39" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="S39" s="5" t="s">
         <v>33</v>
@@ -4479,13 +4496,13 @@
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F40" s="24" t="s">
         <v>234</v>
@@ -4534,152 +4551,152 @@
       </c>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U41" s="7"/>
+    </row>
+    <row r="42" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D42" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="E42" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>514</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="C41" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="D41" s="35" t="s">
-        <v>516</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="I42" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="F41" s="36" t="s">
-        <v>515</v>
-      </c>
-      <c r="G41" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I41" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="J41" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>518</v>
-      </c>
-      <c r="L41" s="19" t="s">
+      <c r="L42" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M41" s="30" t="s">
+      <c r="M42" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N41" s="30" t="s">
+      <c r="N42" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O41" s="30" t="s">
+      <c r="O42" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P41" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q41" s="33">
+      <c r="P42" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="33">
         <v>44333</v>
       </c>
-      <c r="R41" s="30" t="s">
+      <c r="R42" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U41" s="34"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>522</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R42" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="7"/>
+      <c r="S42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="34"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>216</v>
@@ -4688,28 +4705,28 @@
         <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q43" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>33</v>
@@ -4721,26 +4738,26 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>216</v>
@@ -4749,7 +4766,7 @@
         <v>25</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>109</v>
@@ -4767,10 +4784,10 @@
         <v>44</v>
       </c>
       <c r="Q44" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R44" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S44" s="5" t="s">
         <v>33</v>
@@ -4782,26 +4799,26 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>262</v>
+      <c r="H45" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>216</v>
@@ -4810,28 +4827,28 @@
         <v>25</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P45" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q45" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R45" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S45" s="5" t="s">
         <v>33</v>
@@ -4847,13 +4864,13 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>259</v>
@@ -4904,26 +4921,26 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>216</v>
@@ -4932,28 +4949,28 @@
         <v>25</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q47" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S47" s="5" t="s">
         <v>33</v>
@@ -4963,87 +4980,89 @@
       </c>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U48" s="7"/>
     </row>
     <row r="49" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D49" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E49" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5064,7 +5083,7 @@
         <v>278</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
@@ -5073,10 +5092,10 @@
         <v>43788</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S49" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T49" s="5" t="s">
         <v>281</v>
@@ -5085,24 +5104,24 @@
     </row>
     <row r="50" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5110,9 +5129,15 @@
       <c r="J50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
+      <c r="K50" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N50" s="5" t="s">
         <v>278</v>
       </c>
@@ -5129,7 +5154,7 @@
         <v>288</v>
       </c>
       <c r="S50" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T50" s="5" t="s">
         <v>281</v>
@@ -5138,24 +5163,24 @@
     </row>
     <row r="51" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>216</v>
@@ -5182,7 +5207,7 @@
         <v>288</v>
       </c>
       <c r="S51" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T51" s="5" t="s">
         <v>281</v>
@@ -5191,24 +5216,24 @@
     </row>
     <row r="52" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
@@ -5244,24 +5269,24 @@
     </row>
     <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
@@ -5297,24 +5322,24 @@
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5350,24 +5375,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5403,24 +5428,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5456,24 +5481,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5509,24 +5534,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5562,24 +5587,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5615,24 +5640,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5668,24 +5693,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5721,137 +5746,135 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J62" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O62" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P62" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q62" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R62" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S62" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T62" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U62" s="7"/>
+    </row>
+    <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K63" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L62" s="5" t="s">
+      <c r="L63" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M62" s="5" t="s">
+      <c r="M63" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N62" s="5" t="s">
+      <c r="N63" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O62" s="5" t="s">
+      <c r="O63" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q62" s="6">
+      <c r="P63" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q63" s="6">
         <v>44111</v>
       </c>
-      <c r="R62" s="5" t="s">
+      <c r="R63" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S62" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T62" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U62" s="7"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P63" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q63" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R63" s="5"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="5"/>
+      <c r="S63" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T63" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U63" s="7"/>
     </row>
-    <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" s="5"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D64" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K64" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L64" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M64" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N64" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
       <c r="O64" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>44</v>
@@ -5859,37 +5882,33 @@
       <c r="Q64" s="6">
         <v>43788</v>
       </c>
-      <c r="R64" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S64" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T64" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
       <c r="U64" s="7"/>
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D65" s="21"/>
+        <v>360</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>356</v>
+      </c>
       <c r="E65" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -5910,7 +5929,7 @@
         <v>359</v>
       </c>
       <c r="O65" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P65" s="5" t="s">
         <v>44</v>
@@ -5919,7 +5938,7 @@
         <v>43788</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S65" s="5" t="s">
         <v>33</v>
@@ -5931,24 +5950,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -5969,7 +5988,7 @@
         <v>359</v>
       </c>
       <c r="O66" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>44</v>
@@ -5978,7 +5997,7 @@
         <v>43788</v>
       </c>
       <c r="R66" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S66" s="5" t="s">
         <v>33</v>
@@ -5990,24 +6009,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6049,24 +6068,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6087,7 +6106,7 @@
         <v>359</v>
       </c>
       <c r="O68" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>44</v>
@@ -6096,7 +6115,7 @@
         <v>43788</v>
       </c>
       <c r="R68" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S68" s="5" t="s">
         <v>33</v>
@@ -6106,23 +6125,47 @@
       </c>
       <c r="U68" s="7"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
+    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D69" s="21"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
+      <c r="E69" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L69" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O69" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6130,52 +6173,32 @@
       <c r="Q69" s="6">
         <v>43788</v>
       </c>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
+      <c r="R69" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U69" s="7"/>
     </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D70" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L70" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
       <c r="O70" s="5" t="s">
         <v>65</v>
       </c>
@@ -6185,37 +6208,33 @@
       <c r="Q70" s="6">
         <v>43788</v>
       </c>
-      <c r="R70" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S70" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
       <c r="U70" s="7"/>
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D71" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E71" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6248,7 +6267,7 @@
         <v>361</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T71" s="5" t="s">
         <v>281</v>
@@ -6257,24 +6276,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6307,7 +6326,7 @@
         <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T72" s="5" t="s">
         <v>281</v>
@@ -6316,24 +6335,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6375,24 +6394,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6434,24 +6453,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6493,24 +6512,24 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6552,24 +6571,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6611,24 +6630,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6670,24 +6689,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6729,24 +6748,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6788,24 +6807,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6847,24 +6866,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -6905,102 +6924,104 @@
       <c r="U82" s="7"/>
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D83" s="21"/>
+      <c r="E83" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L83" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M83" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O83" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P83" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q83" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R83" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S83" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T83" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U83" s="7"/>
+    </row>
+    <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B83" s="15"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="10"/>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10"/>
-      <c r="O83" s="10"/>
-      <c r="P83" s="10"/>
-      <c r="Q83" s="10"/>
-      <c r="R83" s="10"/>
-      <c r="S83" s="10"/>
-      <c r="T83" s="10"/>
-      <c r="U83" s="10"/>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D84" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F84" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K84" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L84" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M84" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N84" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O84" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P84" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q84" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R84" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S84" s="5"/>
-      <c r="T84" s="5"/>
-      <c r="U84" s="7"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
+      <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>23</v>
@@ -7015,28 +7036,28 @@
         <v>25</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L85" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N85" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O85" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P85" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q85" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R85" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
@@ -7044,20 +7065,20 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>23</v>
@@ -7072,19 +7093,19 @@
         <v>25</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L86" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N86" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O86" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>44</v>
@@ -7101,20 +7122,20 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>23</v>
@@ -7129,19 +7150,19 @@
         <v>25</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L87" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O87" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>44</v>
@@ -7157,54 +7178,88 @@
       <c r="U87" s="7"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88" s="28"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="L88"/>
-      <c r="M88"/>
-      <c r="N88"/>
-      <c r="O88"/>
-      <c r="P88"/>
-      <c r="Q88"/>
-      <c r="R88"/>
-      <c r="S88"/>
-      <c r="T88"/>
-      <c r="U88"/>
+      <c r="A88" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R88" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S88" s="5"/>
+      <c r="T88" s="5"/>
+      <c r="U88" s="7"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B89" s="9"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-      <c r="I89" s="10"/>
-      <c r="K89" s="9"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="10"/>
-      <c r="Q89" s="12"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="10"/>
-      <c r="T89" s="10"/>
-      <c r="U89" s="10"/>
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89" s="28"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+      <c r="P89"/>
+      <c r="Q89"/>
+      <c r="R89"/>
+      <c r="S89"/>
+      <c r="T89"/>
+      <c r="U89"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
@@ -7226,17 +7281,17 @@
       <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B91" s="10"/>
+      <c r="A91" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
       <c r="H91" s="10"/>
       <c r="I91" s="10"/>
-      <c r="K91" s="10"/>
+      <c r="K91" s="9"/>
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
@@ -7250,7 +7305,7 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -7272,30 +7327,53 @@
       <c r="U92" s="10"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="13" t="s">
+      <c r="A93" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+      <c r="O93" s="10"/>
+      <c r="P93" s="10"/>
+      <c r="Q93" s="12"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10"/>
+      <c r="U93" s="10"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
-      <c r="M93" s="13"/>
-      <c r="N93" s="13"/>
-      <c r="O93" s="13"/>
-      <c r="P93" s="13"/>
-      <c r="R93" s="13"/>
-      <c r="S93" s="13"/>
-      <c r="T93" s="13"/>
-      <c r="U93" s="13"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="11" t="s">
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="13"/>
+      <c r="K94" s="13"/>
+      <c r="L94" s="13"/>
+      <c r="M94" s="13"/>
+      <c r="N94" s="13"/>
+      <c r="O94" s="13"/>
+      <c r="P94" s="13"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="13"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A95" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #374: Namespace - add "clipper" - Upd2 (#382)
Add the namespace "clipper" to the Namespace Registry and the config.properties file. Now uploading the Namespace Registry document.

Resolves #374
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\AAANameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77360AA-4D0D-475D-94C6-24FDAE736705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3DF3A8B-61B4-4020-BE47-41A1F1736400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5213" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="531">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1521,9 +1521,6 @@
     <t>http://pds.nasa.gov/pds4/clementine/v1</t>
   </si>
   <si>
-    <t>PDS4_clementine</t>
-  </si>
-  <si>
     <t>The Clementine mission dictionary contains a class with attributes specific to the Deep Space Program Science Experiment, including the Clementine orbiter and its instruments. This dictionary was created for the migration of Clementine data products from PDS3 to PDS4 by Million Concepts (contact M. St. Clair).</t>
   </si>
   <si>
@@ -1606,6 +1603,21 @@
   </si>
   <si>
     <t>Y. Yamamoto</t>
+  </si>
+  <si>
+    <t>clipper</t>
+  </si>
+  <si>
+    <t>The Europa Clipper mission dictionary contains classes that describe aspects of the Clipper mission and related instruments.</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/clipper/v1</t>
+  </si>
+  <si>
+    <t>PDS4_CLIPPER</t>
+  </si>
+  <si>
+    <t>PDS4_CLEMENTINE</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1839,6 +1851,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2157,10 +2172,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U94"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2376,7 +2391,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>35</v>
@@ -2887,28 +2902,28 @@
     </row>
     <row r="14" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>500</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="D14" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>502</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>501</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>503</v>
-      </c>
       <c r="F14" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>38</v>
@@ -2917,7 +2932,7 @@
         <v>25</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L14" s="16" t="s">
         <v>97</v>
@@ -3202,28 +3217,28 @@
     </row>
     <row r="19" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>505</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>513</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>512</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>506</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>514</v>
-      </c>
       <c r="F19" s="32" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I19" s="30" t="s">
         <v>38</v>
@@ -3232,7 +3247,7 @@
         <v>25</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L19" s="30" t="s">
         <v>109</v>
@@ -3241,10 +3256,10 @@
         <v>110</v>
       </c>
       <c r="N19" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="O19" s="19" t="s">
         <v>509</v>
-      </c>
-      <c r="O19" s="19" t="s">
-        <v>510</v>
       </c>
       <c r="P19" s="30" t="s">
         <v>44</v>
@@ -3253,7 +3268,7 @@
         <v>44333</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="S19" s="30" t="s">
         <v>33</v>
@@ -4235,7 +4250,7 @@
         <v>496</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>495</v>
@@ -4250,7 +4265,7 @@
         <v>23</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>498</v>
+        <v>530</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>216</v>
@@ -4290,150 +4305,152 @@
       </c>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="M37" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q37" s="6">
+        <v>44385</v>
+      </c>
+      <c r="R37" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U37" s="7"/>
+    </row>
+    <row r="38" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30" t="s">
+      <c r="B38" s="30"/>
+      <c r="C38" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D38" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E38" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="L38" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="N38" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O38" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="P38" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q38" s="33">
+        <v>44193</v>
+      </c>
+      <c r="R38" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="F37" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="I37" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="J37" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K37" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="L37" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M37" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="N37" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O37" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="P37" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q37" s="33">
-        <v>44193</v>
-      </c>
-      <c r="R37" s="19" t="s">
-        <v>526</v>
-      </c>
-      <c r="S37" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T37" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U37" s="34"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N38" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O38" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>42119</v>
-      </c>
-      <c r="R38" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S38" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T38" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U38" s="7"/>
+      <c r="S38" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T38" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U38" s="34"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>237</v>
+      <c r="H39" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>216</v>
@@ -4442,28 +4459,28 @@
         <v>25</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>102</v>
+        <v>193</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q39" s="6">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R39" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="S39" s="5" t="s">
         <v>33</v>
@@ -4479,13 +4496,13 @@
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F40" s="24" t="s">
         <v>234</v>
@@ -4534,152 +4551,152 @@
       </c>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U41" s="7"/>
+    </row>
+    <row r="42" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D42" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="E42" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>514</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="C41" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="D41" s="35" t="s">
-        <v>516</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="I42" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="F41" s="36" t="s">
-        <v>515</v>
-      </c>
-      <c r="G41" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I41" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="J41" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>518</v>
-      </c>
-      <c r="L41" s="19" t="s">
+      <c r="L42" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M41" s="30" t="s">
+      <c r="M42" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N41" s="30" t="s">
+      <c r="N42" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O41" s="30" t="s">
+      <c r="O42" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P41" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q41" s="33">
+      <c r="P42" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="33">
         <v>44333</v>
       </c>
-      <c r="R41" s="30" t="s">
+      <c r="R42" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U41" s="34"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>522</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R42" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="7"/>
+      <c r="S42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="34"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>216</v>
@@ -4688,28 +4705,28 @@
         <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q43" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>33</v>
@@ -4721,26 +4738,26 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>216</v>
@@ -4749,7 +4766,7 @@
         <v>25</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>109</v>
@@ -4767,10 +4784,10 @@
         <v>44</v>
       </c>
       <c r="Q44" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R44" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S44" s="5" t="s">
         <v>33</v>
@@ -4782,26 +4799,26 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>262</v>
+      <c r="H45" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>216</v>
@@ -4810,28 +4827,28 @@
         <v>25</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P45" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q45" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R45" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S45" s="5" t="s">
         <v>33</v>
@@ -4847,13 +4864,13 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>259</v>
@@ -4904,26 +4921,26 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>216</v>
@@ -4932,28 +4949,28 @@
         <v>25</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q47" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S47" s="5" t="s">
         <v>33</v>
@@ -4963,87 +4980,89 @@
       </c>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U48" s="7"/>
     </row>
     <row r="49" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D49" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E49" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5064,7 +5083,7 @@
         <v>278</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
@@ -5073,10 +5092,10 @@
         <v>43788</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S49" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T49" s="5" t="s">
         <v>281</v>
@@ -5085,24 +5104,24 @@
     </row>
     <row r="50" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5110,9 +5129,15 @@
       <c r="J50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
+      <c r="K50" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N50" s="5" t="s">
         <v>278</v>
       </c>
@@ -5129,7 +5154,7 @@
         <v>288</v>
       </c>
       <c r="S50" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T50" s="5" t="s">
         <v>281</v>
@@ -5138,24 +5163,24 @@
     </row>
     <row r="51" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>216</v>
@@ -5182,7 +5207,7 @@
         <v>288</v>
       </c>
       <c r="S51" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T51" s="5" t="s">
         <v>281</v>
@@ -5191,24 +5216,24 @@
     </row>
     <row r="52" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
@@ -5244,24 +5269,24 @@
     </row>
     <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
@@ -5297,24 +5322,24 @@
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5350,24 +5375,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5403,24 +5428,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5456,24 +5481,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5509,24 +5534,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5562,24 +5587,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5615,24 +5640,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5668,24 +5693,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5721,137 +5746,135 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J62" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O62" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P62" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q62" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R62" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S62" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T62" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U62" s="7"/>
+    </row>
+    <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K63" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L62" s="5" t="s">
+      <c r="L63" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M62" s="5" t="s">
+      <c r="M63" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N62" s="5" t="s">
+      <c r="N63" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O62" s="5" t="s">
+      <c r="O63" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q62" s="6">
+      <c r="P63" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q63" s="6">
         <v>44111</v>
       </c>
-      <c r="R62" s="5" t="s">
+      <c r="R63" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S62" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T62" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U62" s="7"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P63" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q63" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R63" s="5"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="5"/>
+      <c r="S63" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T63" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U63" s="7"/>
     </row>
-    <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" s="5"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D64" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K64" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L64" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M64" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N64" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
       <c r="O64" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>44</v>
@@ -5859,37 +5882,33 @@
       <c r="Q64" s="6">
         <v>43788</v>
       </c>
-      <c r="R64" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S64" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T64" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
       <c r="U64" s="7"/>
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D65" s="21"/>
+        <v>360</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>356</v>
+      </c>
       <c r="E65" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -5910,7 +5929,7 @@
         <v>359</v>
       </c>
       <c r="O65" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P65" s="5" t="s">
         <v>44</v>
@@ -5919,7 +5938,7 @@
         <v>43788</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S65" s="5" t="s">
         <v>33</v>
@@ -5931,24 +5950,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -5969,7 +5988,7 @@
         <v>359</v>
       </c>
       <c r="O66" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>44</v>
@@ -5978,7 +5997,7 @@
         <v>43788</v>
       </c>
       <c r="R66" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S66" s="5" t="s">
         <v>33</v>
@@ -5990,24 +6009,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6049,24 +6068,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6087,7 +6106,7 @@
         <v>359</v>
       </c>
       <c r="O68" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>44</v>
@@ -6096,7 +6115,7 @@
         <v>43788</v>
       </c>
       <c r="R68" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S68" s="5" t="s">
         <v>33</v>
@@ -6106,23 +6125,47 @@
       </c>
       <c r="U68" s="7"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
+    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D69" s="21"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
+      <c r="E69" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L69" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O69" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6130,52 +6173,32 @@
       <c r="Q69" s="6">
         <v>43788</v>
       </c>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
+      <c r="R69" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U69" s="7"/>
     </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D70" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L70" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
       <c r="O70" s="5" t="s">
         <v>65</v>
       </c>
@@ -6185,37 +6208,33 @@
       <c r="Q70" s="6">
         <v>43788</v>
       </c>
-      <c r="R70" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S70" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
       <c r="U70" s="7"/>
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D71" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E71" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6248,7 +6267,7 @@
         <v>361</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T71" s="5" t="s">
         <v>281</v>
@@ -6257,24 +6276,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6307,7 +6326,7 @@
         <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T72" s="5" t="s">
         <v>281</v>
@@ -6316,24 +6335,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6375,24 +6394,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6434,24 +6453,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6493,24 +6512,24 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6552,24 +6571,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6611,24 +6630,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6670,24 +6689,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6729,24 +6748,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6788,24 +6807,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6847,24 +6866,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -6905,102 +6924,104 @@
       <c r="U82" s="7"/>
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D83" s="21"/>
+      <c r="E83" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L83" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M83" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O83" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P83" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q83" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R83" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S83" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T83" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U83" s="7"/>
+    </row>
+    <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B83" s="15"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="10"/>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10"/>
-      <c r="O83" s="10"/>
-      <c r="P83" s="10"/>
-      <c r="Q83" s="10"/>
-      <c r="R83" s="10"/>
-      <c r="S83" s="10"/>
-      <c r="T83" s="10"/>
-      <c r="U83" s="10"/>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D84" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F84" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K84" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L84" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M84" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N84" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O84" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P84" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q84" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R84" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S84" s="5"/>
-      <c r="T84" s="5"/>
-      <c r="U84" s="7"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
+      <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>23</v>
@@ -7015,28 +7036,28 @@
         <v>25</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L85" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N85" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O85" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P85" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q85" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R85" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
@@ -7044,20 +7065,20 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>23</v>
@@ -7072,19 +7093,19 @@
         <v>25</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L86" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N86" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O86" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>44</v>
@@ -7101,20 +7122,20 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>23</v>
@@ -7129,19 +7150,19 @@
         <v>25</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L87" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O87" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>44</v>
@@ -7157,54 +7178,88 @@
       <c r="U87" s="7"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88" s="28"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="L88"/>
-      <c r="M88"/>
-      <c r="N88"/>
-      <c r="O88"/>
-      <c r="P88"/>
-      <c r="Q88"/>
-      <c r="R88"/>
-      <c r="S88"/>
-      <c r="T88"/>
-      <c r="U88"/>
+      <c r="A88" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R88" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S88" s="5"/>
+      <c r="T88" s="5"/>
+      <c r="U88" s="7"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B89" s="9"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-      <c r="I89" s="10"/>
-      <c r="K89" s="9"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="10"/>
-      <c r="Q89" s="12"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="10"/>
-      <c r="T89" s="10"/>
-      <c r="U89" s="10"/>
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89" s="28"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+      <c r="P89"/>
+      <c r="Q89"/>
+      <c r="R89"/>
+      <c r="S89"/>
+      <c r="T89"/>
+      <c r="U89"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
@@ -7226,17 +7281,17 @@
       <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B91" s="10"/>
+      <c r="A91" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
       <c r="H91" s="10"/>
       <c r="I91" s="10"/>
-      <c r="K91" s="10"/>
+      <c r="K91" s="9"/>
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
@@ -7250,7 +7305,7 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -7272,30 +7327,53 @@
       <c r="U92" s="10"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="13" t="s">
+      <c r="A93" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+      <c r="O93" s="10"/>
+      <c r="P93" s="10"/>
+      <c r="Q93" s="12"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10"/>
+      <c r="U93" s="10"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
-      <c r="M93" s="13"/>
-      <c r="N93" s="13"/>
-      <c r="O93" s="13"/>
-      <c r="P93" s="13"/>
-      <c r="R93" s="13"/>
-      <c r="S93" s="13"/>
-      <c r="T93" s="13"/>
-      <c r="U93" s="13"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="11" t="s">
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="13"/>
+      <c r="K94" s="13"/>
+      <c r="L94" s="13"/>
+      <c r="M94" s="13"/>
+      <c r="N94" s="13"/>
+      <c r="O94" s="13"/>
+      <c r="P94" s="13"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="13"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A95" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #386 - Namespace - ebt
Add the namespace "ebt" to the Namespace Registry and the config.properties file.

Resolves #386
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\AAANameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3DF3A8B-61B4-4020-BE47-41A1F1736400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473BE556-DD81-4437-AA35-EB425EFC01A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="539">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1618,6 +1618,30 @@
   </si>
   <si>
     <t>PDS4_CLEMENTINE</t>
+  </si>
+  <si>
+    <t>ebt</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/ebt/v1</t>
+  </si>
+  <si>
+    <t>PDS4_EBT</t>
+  </si>
+  <si>
+    <t>B. Hirsch</t>
+  </si>
+  <si>
+    <t>Ben Hirsch</t>
+  </si>
+  <si>
+    <t>bhirsch1 at umd.edu</t>
+  </si>
+  <si>
+    <t>This namespace will provide observing parameters, provenance, and geometry relevant to ground-based telescopes on Earth and for Earth-orbiting (or Lagrange point) telescopes</t>
+  </si>
+  <si>
+    <t>Earth-Based Telescope</t>
   </si>
 </sst>
 </file>
@@ -2172,10 +2196,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U95"/>
+  <dimension ref="A1:U96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="E16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3026,93 +3050,93 @@
       </c>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="5" t="s">
+    <row r="16" spans="1:21" s="17" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>531</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>532</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>531</v>
+      </c>
+      <c r="G16" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="H16" s="19" t="s">
+        <v>533</v>
+      </c>
+      <c r="I16" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>42124</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U16" s="7"/>
+      <c r="K16" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>536</v>
+      </c>
+      <c r="P16" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q16" s="33">
+        <v>44398</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="S16" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T16" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U16" s="34"/>
     </row>
     <row r="17" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>38</v>
@@ -3120,29 +3144,29 @@
       <c r="J17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>132</v>
+      <c r="K17" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q17" s="6">
-        <v>41002</v>
+        <v>42124</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>33</v>
@@ -3154,28 +3178,28 @@
     </row>
     <row r="18" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>484</v>
+        <v>132</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>38</v>
@@ -3183,11 +3207,11 @@
       <c r="J18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>138</v>
+      <c r="K18" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>110</v>
@@ -3202,169 +3226,169 @@
         <v>44</v>
       </c>
       <c r="Q18" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q19" s="6">
         <v>43734</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R19" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="S18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U18" s="7"/>
-    </row>
-    <row r="19" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="S19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="19" t="s">
         <v>512</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D20" s="35" t="s">
         <v>505</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E20" s="18" t="s">
         <v>513</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F20" s="32" t="s">
         <v>505</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G20" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="I19" s="30" t="s">
+      <c r="I20" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J19" s="30" t="s">
+      <c r="J20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K20" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="L19" s="30" t="s">
+      <c r="L20" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="M20" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="N19" s="19" t="s">
+      <c r="N20" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="O20" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="P19" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q19" s="33">
+      <c r="P20" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q20" s="33">
         <v>44333</v>
       </c>
-      <c r="R19" s="19" t="s">
+      <c r="R20" s="19" t="s">
         <v>510</v>
       </c>
-      <c r="S19" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T19" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U19" s="34"/>
-    </row>
-    <row r="20" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="S20" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T20" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U20" s="34"/>
+    </row>
+    <row r="21" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D21" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F21" s="24" t="s">
         <v>211</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>42650</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U20" s="7"/>
-    </row>
-    <row r="21" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>141</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>38</v>
@@ -3373,10 +3397,10 @@
         <v>25</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>110</v>
@@ -3391,10 +3415,10 @@
         <v>44</v>
       </c>
       <c r="Q21" s="6">
-        <v>43734</v>
+        <v>42650</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>140</v>
+        <v>32</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>33</v>
@@ -3404,30 +3428,30 @@
       </c>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="78" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>209</v>
+        <v>145</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>207</v>
+        <v>141</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>38</v>
@@ -3436,28 +3460,28 @@
         <v>25</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q22" s="6">
-        <v>44257</v>
+        <v>43734</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="S22" s="5" t="s">
         <v>33</v>
@@ -3467,30 +3491,30 @@
       </c>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="78" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>152</v>
+        <v>209</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>147</v>
+        <v>206</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>207</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>38</v>
@@ -3499,28 +3523,28 @@
         <v>25</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q23" s="6">
-        <v>44110</v>
+        <v>44257</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="S23" s="5" t="s">
         <v>33</v>
@@ -3532,28 +3556,28 @@
     </row>
     <row r="24" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>147</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>38</v>
@@ -3562,28 +3586,28 @@
         <v>25</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q24" s="6">
-        <v>42118</v>
+        <v>44110</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="S24" s="5" t="s">
         <v>33</v>
@@ -3593,30 +3617,30 @@
       </c>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>38</v>
@@ -3625,28 +3649,28 @@
         <v>25</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>157</v>
+        <v>90</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q25" s="6">
-        <v>41002</v>
+        <v>42118</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="S25" s="5" t="s">
         <v>33</v>
@@ -3656,28 +3680,30 @@
       </c>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>489</v>
+      </c>
       <c r="C26" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>161</v>
+        <v>24</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>38</v>
@@ -3686,19 +3712,19 @@
         <v>25</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>44</v>
@@ -3717,30 +3743,28 @@
       </c>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>490</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>38</v>
@@ -3749,28 +3773,28 @@
         <v>25</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="P27" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q27" s="6">
-        <v>43734</v>
+        <v>41002</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>140</v>
+        <v>32</v>
       </c>
       <c r="S27" s="5" t="s">
         <v>33</v>
@@ -3782,28 +3806,28 @@
     </row>
     <row r="28" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>38</v>
@@ -3812,60 +3836,62 @@
         <v>25</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L28" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>43734</v>
+      </c>
+      <c r="R28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="S28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="M28" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>41002</v>
-      </c>
-      <c r="R28" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="S28" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T28" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U28" s="7"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="B29" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="I29" s="5" t="s">
         <v>38</v>
       </c>
@@ -3873,19 +3899,19 @@
         <v>25</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>44</v>
@@ -3894,7 +3920,7 @@
         <v>41002</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="S29" s="5" t="s">
         <v>33</v>
@@ -3904,39 +3930,37 @@
       </c>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>186</v>
+        <v>493</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>185</v>
-      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>186</v>
+      <c r="K30" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>176</v>
@@ -3954,10 +3978,10 @@
         <v>44</v>
       </c>
       <c r="Q30" s="6">
-        <v>41589</v>
+        <v>41002</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="S30" s="5" t="s">
         <v>33</v>
@@ -3969,28 +3993,28 @@
     </row>
     <row r="31" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>38</v>
@@ -3999,28 +4023,28 @@
         <v>25</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q31" s="6">
-        <v>42870</v>
+        <v>41589</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="S31" s="5" t="s">
         <v>33</v>
@@ -4032,28 +4056,28 @@
     </row>
     <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>198</v>
+        <v>189</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>38</v>
@@ -4062,28 +4086,28 @@
         <v>25</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>151</v>
+        <v>193</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q32" s="6">
-        <v>44110</v>
+        <v>42870</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="S32" s="5" t="s">
         <v>33</v>
@@ -4095,28 +4119,28 @@
     </row>
     <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>492</v>
+        <v>200</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>198</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>38</v>
@@ -4125,177 +4149,177 @@
         <v>25</v>
       </c>
       <c r="K33" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>44110</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U33" s="7"/>
+    </row>
+    <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="N33" s="5" t="s">
+      <c r="N34" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="O33" s="5" t="s">
+      <c r="O34" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="P33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q33" s="6">
+      <c r="P34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q34" s="6">
         <v>42118</v>
       </c>
-      <c r="R33" s="5" t="s">
+      <c r="R34" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U33" s="7"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="S34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U34" s="7"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D36" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F36" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q35" s="6">
-        <v>42089</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>498</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="F36" s="25" t="s">
-        <v>495</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="16" t="s">
-        <v>530</v>
-      </c>
-      <c r="I36" s="16" t="s">
+      <c r="H36" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I36" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K36" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L36" s="16" t="s">
-        <v>109</v>
+      <c r="K36" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>111</v>
+        <v>179</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="P36" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q36" s="6">
-        <v>44329</v>
-      </c>
-      <c r="R36" s="16" t="s">
-        <v>111</v>
+        <v>42089</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="S36" s="5" t="s">
         <v>33</v>
@@ -4305,30 +4329,30 @@
       </c>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>526</v>
+        <v>495</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>526</v>
+        <v>496</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E37" s="37" t="s">
-        <v>528</v>
+        <v>495</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>497</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>526</v>
+        <v>495</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>216</v>
@@ -4355,7 +4379,7 @@
         <v>44</v>
       </c>
       <c r="Q37" s="6">
-        <v>44385</v>
+        <v>44329</v>
       </c>
       <c r="R37" s="16" t="s">
         <v>111</v>
@@ -4368,150 +4392,152 @@
       </c>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q38" s="6">
+        <v>44385</v>
+      </c>
+      <c r="R38" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="S38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U38" s="7"/>
+    </row>
+    <row r="39" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D39" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E39" s="18" t="s">
         <v>524</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F39" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G39" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H39" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="I38" s="30" t="s">
+      <c r="I39" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J39" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K38" s="30" t="s">
+      <c r="K39" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L39" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M38" s="30" t="s">
+      <c r="M39" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="N38" s="19" t="s">
+      <c r="N39" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O38" s="30" t="s">
+      <c r="O39" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="P38" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q38" s="33">
+      <c r="P39" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q39" s="33">
         <v>44193</v>
       </c>
-      <c r="R38" s="19" t="s">
+      <c r="R39" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="S38" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T38" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U38" s="34"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>42119</v>
-      </c>
-      <c r="R39" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U39" s="7"/>
+      <c r="S39" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T39" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U39" s="34"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>237</v>
+      <c r="H40" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>216</v>
@@ -4520,28 +4546,28 @@
         <v>25</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>102</v>
+        <v>193</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q40" s="6">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R40" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="S40" s="5" t="s">
         <v>33</v>
@@ -4557,13 +4583,13 @@
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>234</v>
@@ -4612,152 +4638,152 @@
       </c>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="7"/>
+    </row>
+    <row r="43" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B43" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C43" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D43" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E43" s="18" t="s">
         <v>516</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F43" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G43" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="H43" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="I42" s="30" t="s">
+      <c r="I43" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="30" t="s">
+      <c r="J43" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K42" s="19" t="s">
+      <c r="K43" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="L42" s="19" t="s">
+      <c r="L43" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M42" s="30" t="s">
+      <c r="M43" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N42" s="30" t="s">
+      <c r="N43" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O42" s="30" t="s">
+      <c r="O43" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P42" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="33">
+      <c r="P43" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="33">
         <v>44333</v>
       </c>
-      <c r="R42" s="30" t="s">
+      <c r="R43" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S42" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="34"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R43" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U43" s="7"/>
+      <c r="S43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" s="34"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>216</v>
@@ -4766,28 +4792,28 @@
         <v>25</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q44" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R44" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S44" s="5" t="s">
         <v>33</v>
@@ -4799,26 +4825,26 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>216</v>
@@ -4827,7 +4853,7 @@
         <v>25</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>109</v>
@@ -4845,10 +4871,10 @@
         <v>44</v>
       </c>
       <c r="Q45" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R45" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S45" s="5" t="s">
         <v>33</v>
@@ -4860,26 +4886,26 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H46" s="5" t="s">
-        <v>262</v>
+      <c r="H46" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>216</v>
@@ -4888,28 +4914,28 @@
         <v>25</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q46" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S46" s="5" t="s">
         <v>33</v>
@@ -4925,13 +4951,13 @@
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F47" s="24" t="s">
         <v>259</v>
@@ -4982,26 +5008,26 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5010,28 +5036,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5041,87 +5067,89 @@
       </c>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U49" s="7"/>
     </row>
     <row r="50" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D50" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E50" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5142,7 +5170,7 @@
         <v>278</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
@@ -5151,10 +5179,10 @@
         <v>43788</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S50" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T50" s="5" t="s">
         <v>281</v>
@@ -5163,24 +5191,24 @@
     </row>
     <row r="51" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>216</v>
@@ -5188,9 +5216,15 @@
       <c r="J51" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
+      <c r="K51" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N51" s="5" t="s">
         <v>278</v>
       </c>
@@ -5207,7 +5241,7 @@
         <v>288</v>
       </c>
       <c r="S51" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T51" s="5" t="s">
         <v>281</v>
@@ -5216,24 +5250,24 @@
     </row>
     <row r="52" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
@@ -5260,7 +5294,7 @@
         <v>288</v>
       </c>
       <c r="S52" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T52" s="5" t="s">
         <v>281</v>
@@ -5269,24 +5303,24 @@
     </row>
     <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
@@ -5322,24 +5356,24 @@
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5375,24 +5409,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5428,24 +5462,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5481,24 +5515,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5534,24 +5568,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5587,24 +5621,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5640,24 +5674,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5693,24 +5727,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5746,24 +5780,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5799,137 +5833,135 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E63" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J63" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O63" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P63" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q63" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R63" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S63" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T63" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U63" s="7"/>
+    </row>
+    <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J64" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K64" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L63" s="5" t="s">
+      <c r="L64" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M63" s="5" t="s">
+      <c r="M64" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N63" s="5" t="s">
+      <c r="N64" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O63" s="5" t="s">
+      <c r="O64" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P63" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q63" s="6">
+      <c r="P64" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q64" s="6">
         <v>44111</v>
       </c>
-      <c r="R63" s="5" t="s">
+      <c r="R64" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S63" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T63" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U63" s="7"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P64" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q64" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
+      <c r="S64" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T64" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U64" s="7"/>
     </row>
-    <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D65" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K65" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L65" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M65" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N65" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
       <c r="O65" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P65" s="5" t="s">
         <v>44</v>
@@ -5937,37 +5969,33 @@
       <c r="Q65" s="6">
         <v>43788</v>
       </c>
-      <c r="R65" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S65" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T65" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+      <c r="T65" s="5"/>
       <c r="U65" s="7"/>
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D66" s="21"/>
+        <v>360</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>356</v>
+      </c>
       <c r="E66" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -5988,7 +6016,7 @@
         <v>359</v>
       </c>
       <c r="O66" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>44</v>
@@ -5997,7 +6025,7 @@
         <v>43788</v>
       </c>
       <c r="R66" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S66" s="5" t="s">
         <v>33</v>
@@ -6009,24 +6037,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6047,7 +6075,7 @@
         <v>359</v>
       </c>
       <c r="O67" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P67" s="5" t="s">
         <v>44</v>
@@ -6056,7 +6084,7 @@
         <v>43788</v>
       </c>
       <c r="R67" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S67" s="5" t="s">
         <v>33</v>
@@ -6068,24 +6096,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6127,24 +6155,24 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D69" s="21"/>
       <c r="E69" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
@@ -6165,7 +6193,7 @@
         <v>359</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6174,7 +6202,7 @@
         <v>43788</v>
       </c>
       <c r="R69" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S69" s="5" t="s">
         <v>33</v>
@@ -6184,23 +6212,47 @@
       </c>
       <c r="U69" s="7"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
+    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D70" s="21"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
+      <c r="E70" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L70" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M70" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N70" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O70" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6208,52 +6260,32 @@
       <c r="Q70" s="6">
         <v>43788</v>
       </c>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
+      <c r="R70" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T70" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U70" s="7"/>
     </row>
-    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D71" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L71" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M71" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
       <c r="O71" s="5" t="s">
         <v>65</v>
       </c>
@@ -6263,37 +6295,33 @@
       <c r="Q71" s="6">
         <v>43788</v>
       </c>
-      <c r="R71" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S71" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T71" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
       <c r="U71" s="7"/>
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D72" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E72" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6326,7 +6354,7 @@
         <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T72" s="5" t="s">
         <v>281</v>
@@ -6335,24 +6363,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6385,7 +6413,7 @@
         <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T73" s="5" t="s">
         <v>281</v>
@@ -6394,24 +6422,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6453,24 +6481,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6512,24 +6540,24 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6571,24 +6599,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6630,24 +6658,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6689,24 +6717,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6748,24 +6776,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6807,24 +6835,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6866,24 +6894,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -6925,24 +6953,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -6983,102 +7011,104 @@
       <c r="U83" s="7"/>
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D84" s="21"/>
+      <c r="E84" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L84" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M84" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N84" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O84" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P84" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q84" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R84" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S84" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T84" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U84" s="7"/>
+    </row>
+    <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B84" s="15"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
-      <c r="H84" s="10"/>
-      <c r="I84" s="10"/>
-      <c r="J84" s="10"/>
-      <c r="K84" s="10"/>
-      <c r="L84" s="10"/>
-      <c r="M84" s="10"/>
-      <c r="N84" s="10"/>
-      <c r="O84" s="10"/>
-      <c r="P84" s="10"/>
-      <c r="Q84" s="10"/>
-      <c r="R84" s="10"/>
-      <c r="S84" s="10"/>
-      <c r="T84" s="10"/>
-      <c r="U84" s="10"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D85" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F85" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H85" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K85" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L85" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M85" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N85" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O85" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P85" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q85" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R85" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S85" s="5"/>
-      <c r="T85" s="5"/>
-      <c r="U85" s="7"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+      <c r="M85" s="10"/>
+      <c r="N85" s="10"/>
+      <c r="O85" s="10"/>
+      <c r="P85" s="10"/>
+      <c r="Q85" s="10"/>
+      <c r="R85" s="10"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10"/>
+      <c r="U85" s="10"/>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>23</v>
@@ -7093,28 +7123,28 @@
         <v>25</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L86" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N86" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O86" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q86" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R86" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S86" s="5"/>
       <c r="T86" s="5"/>
@@ -7122,20 +7152,20 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>23</v>
@@ -7150,19 +7180,19 @@
         <v>25</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L87" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O87" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>44</v>
@@ -7179,20 +7209,20 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>23</v>
@@ -7207,19 +7237,19 @@
         <v>25</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L88" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M88" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N88" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O88" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>44</v>
@@ -7235,54 +7265,88 @@
       <c r="U88" s="7"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89" s="28"/>
-      <c r="F89"/>
-      <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
-      <c r="J89"/>
-      <c r="K89"/>
-      <c r="L89"/>
-      <c r="M89"/>
-      <c r="N89"/>
-      <c r="O89"/>
-      <c r="P89"/>
-      <c r="Q89"/>
-      <c r="R89"/>
-      <c r="S89"/>
-      <c r="T89"/>
-      <c r="U89"/>
+      <c r="A89" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N89" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O89" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P89" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q89" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R89" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S89" s="5"/>
+      <c r="T89" s="5"/>
+      <c r="U89" s="7"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-      <c r="I90" s="10"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10"/>
-      <c r="O90" s="10"/>
-      <c r="P90" s="10"/>
-      <c r="Q90" s="12"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="10"/>
-      <c r="T90" s="10"/>
-      <c r="U90" s="10"/>
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90" s="28"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
+      <c r="P90"/>
+      <c r="Q90"/>
+      <c r="R90"/>
+      <c r="S90"/>
+      <c r="T90"/>
+      <c r="U90"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
@@ -7304,17 +7368,17 @@
       <c r="U91" s="10"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B92" s="10"/>
+      <c r="A92" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B92" s="9"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
       <c r="H92" s="10"/>
       <c r="I92" s="10"/>
-      <c r="K92" s="10"/>
+      <c r="K92" s="9"/>
       <c r="L92" s="10"/>
       <c r="M92" s="10"/>
       <c r="N92" s="10"/>
@@ -7328,7 +7392,7 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
@@ -7350,35 +7414,58 @@
       <c r="U93" s="10"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="13" t="s">
+      <c r="A94" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="12"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
+      <c r="U94" s="10"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A95" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13"/>
-      <c r="N94" s="13"/>
-      <c r="O94" s="13"/>
-      <c r="P94" s="13"/>
-      <c r="R94" s="13"/>
-      <c r="S94" s="13"/>
-      <c r="T94" s="13"/>
-      <c r="U94" s="13"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="11" t="s">
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="13"/>
+      <c r="M95" s="13"/>
+      <c r="N95" s="13"/>
+      <c r="O95" s="13"/>
+      <c r="P95" s="13"/>
+      <c r="R95" s="13"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="13"/>
+      <c r="U95" s="13"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A96" s="11" t="s">
         <v>480</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="19" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="25" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #406 : [namespace-registry] add new namespace "kplo" #406
Add the namespaces "kplo" to the Namespace Registry and the config.properties file.
kplo - Namespace for the Korea Pathfinder Lunar Orbiter(KPLO)

@c-suh  [namespace-registry] add new namespace "kplo" #406

Resolves #406
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\AAANameSpaceRegistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\From Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8196AB-BE6B-44B7-BD44-69BB9B6974F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0248E4D2-C73D-40E1-8979-9DB917B6735E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="565">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1690,6 +1690,36 @@
   </si>
   <si>
     <t>KARI</t>
+  </si>
+  <si>
+    <t>kplo</t>
+  </si>
+  <si>
+    <t>mission/kplo</t>
+  </si>
+  <si>
+    <t>urn:kari:kpds:</t>
+  </si>
+  <si>
+    <t>PDS4_KARI_KPDS_KPLO</t>
+  </si>
+  <si>
+    <t>eunhyeuk@kari.re.kr</t>
+  </si>
+  <si>
+    <t>Eunhyeuk Kim (KARI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eunhyeuk Kim (KARI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eunhyeuk Kim</t>
+  </si>
+  <si>
+    <t>Korea Pathfinder Lunar Orbiter (KPLO)</t>
+  </si>
+  <si>
+    <t>Namespace for the Korea Pathfinder Lunar Orbiter (KPLO).</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1729,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1718,6 +1748,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1813,10 +1851,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1927,8 +1966,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2244,12 +2290,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U98"/>
+  <dimension ref="A1:U99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="L41" sqref="L41"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4687,7 +4733,7 @@
       <c r="U41" s="34"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="16" t="s">
         <v>228</v>
       </c>
       <c r="B42" s="5"/>
@@ -4747,66 +4793,68 @@
       </c>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="I43" s="5" t="s">
+    <row r="43" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>556</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>555</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="I43" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>41837</v>
-      </c>
-      <c r="R43" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="S43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U43" s="7"/>
+      <c r="J43" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="L43" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="M43" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="O43" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="P43" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="33">
+        <v>44448</v>
+      </c>
+      <c r="R43" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="S43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" s="34"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
@@ -4814,13 +4862,13 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>234</v>
@@ -4869,152 +4917,152 @@
       </c>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="7"/>
+    </row>
+    <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D46" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E46" s="18" t="s">
         <v>516</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F46" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G46" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H46" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="I45" s="30" t="s">
+      <c r="I46" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J45" s="30" t="s">
+      <c r="J46" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="19" t="s">
+      <c r="K46" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="L45" s="19" t="s">
+      <c r="L46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M45" s="30" t="s">
+      <c r="M46" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N45" s="30" t="s">
+      <c r="N46" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O45" s="30" t="s">
+      <c r="O46" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P45" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q45" s="33">
+      <c r="P46" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="33">
         <v>44333</v>
       </c>
-      <c r="R45" s="30" t="s">
+      <c r="R46" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S45" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="34"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O46" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R46" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="7"/>
+      <c r="S46" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="34"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>216</v>
@@ -5023,28 +5071,28 @@
         <v>25</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q47" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S47" s="5" t="s">
         <v>33</v>
@@ -5056,26 +5104,26 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5084,7 +5132,7 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>109</v>
@@ -5102,10 +5150,10 @@
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5117,26 +5165,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>262</v>
+      <c r="H49" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5145,28 +5193,28 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5182,13 +5230,13 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F50" s="24" t="s">
         <v>259</v>
@@ -5239,26 +5287,26 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>216</v>
@@ -5267,28 +5315,28 @@
         <v>25</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q51" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R51" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S51" s="5" t="s">
         <v>33</v>
@@ -5298,87 +5346,89 @@
       </c>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q52" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R52" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S52" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T52" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U52" s="7"/>
     </row>
     <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D53" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E53" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
@@ -5399,7 +5449,7 @@
         <v>278</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>44</v>
@@ -5408,10 +5458,10 @@
         <v>43788</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S53" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T53" s="5" t="s">
         <v>281</v>
@@ -5420,24 +5470,24 @@
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5445,9 +5495,15 @@
       <c r="J54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
+      <c r="K54" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N54" s="5" t="s">
         <v>278</v>
       </c>
@@ -5464,7 +5520,7 @@
         <v>288</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T54" s="5" t="s">
         <v>281</v>
@@ -5473,24 +5529,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5517,7 +5573,7 @@
         <v>288</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5526,24 +5582,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5579,24 +5635,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5632,24 +5688,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5685,24 +5741,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5738,24 +5794,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5791,24 +5847,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5844,24 +5900,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5897,24 +5953,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -5950,24 +6006,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6003,24 +6059,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H65" s="5" t="s">
-        <v>347</v>
+      <c r="H65" s="16" t="s">
+        <v>342</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6056,137 +6112,135 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J66" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O66" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q66" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R66" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S66" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T66" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U66" s="7"/>
+    </row>
+    <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J67" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K66" s="5" t="s">
+      <c r="K67" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L66" s="5" t="s">
+      <c r="L67" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M66" s="5" t="s">
+      <c r="M67" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N66" s="5" t="s">
+      <c r="N67" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O66" s="5" t="s">
+      <c r="O67" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P66" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q66" s="6">
+      <c r="P67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q67" s="6">
         <v>44111</v>
       </c>
-      <c r="R66" s="5" t="s">
+      <c r="R67" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S66" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T66" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U66" s="7"/>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q67" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
-      <c r="T67" s="5"/>
+      <c r="S67" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U67" s="7"/>
     </row>
-    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D68" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K68" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L68" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N68" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
       <c r="O68" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>44</v>
@@ -6194,37 +6248,33 @@
       <c r="Q68" s="6">
         <v>43788</v>
       </c>
-      <c r="R68" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T68" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
       <c r="U68" s="7"/>
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D69" s="21"/>
-      <c r="E69" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>357</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
@@ -6245,7 +6295,7 @@
         <v>359</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6254,7 +6304,7 @@
         <v>43788</v>
       </c>
       <c r="R69" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S69" s="5" t="s">
         <v>33</v>
@@ -6266,24 +6316,24 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>216</v>
@@ -6304,7 +6354,7 @@
         <v>359</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6313,7 +6363,7 @@
         <v>43788</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>33</v>
@@ -6325,24 +6375,24 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6384,24 +6434,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6422,7 +6472,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6431,7 +6481,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6441,23 +6491,47 @@
       </c>
       <c r="U72" s="7"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A73" s="5"/>
+    <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D73" s="21"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
+      <c r="E73" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L73" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N73" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O73" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6465,52 +6539,32 @@
       <c r="Q73" s="6">
         <v>43788</v>
       </c>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
+      <c r="R73" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S73" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T73" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A74" s="5"/>
       <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D74" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K74" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L74" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M74" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N74" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
       <c r="O74" s="5" t="s">
         <v>65</v>
       </c>
@@ -6520,37 +6574,33 @@
       <c r="Q74" s="6">
         <v>43788</v>
       </c>
-      <c r="R74" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S74" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T74" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
       <c r="U74" s="7"/>
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D75" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E75" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6583,7 +6633,7 @@
         <v>361</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T75" s="5" t="s">
         <v>281</v>
@@ -6592,24 +6642,24 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6642,7 +6692,7 @@
         <v>361</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>281</v>
@@ -6651,24 +6701,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6710,24 +6760,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6769,24 +6819,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6828,24 +6878,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6887,24 +6937,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6946,24 +6996,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7005,24 +7055,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7064,24 +7114,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7123,24 +7173,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7182,24 +7232,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7240,102 +7290,104 @@
       <c r="U86" s="7"/>
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D87" s="21"/>
+      <c r="E87" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L87" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M87" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N87" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O87" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P87" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q87" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R87" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S87" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T87" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U87" s="7"/>
+    </row>
+    <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B87" s="15"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
-      <c r="H87" s="10"/>
-      <c r="I87" s="10"/>
-      <c r="J87" s="10"/>
-      <c r="K87" s="10"/>
-      <c r="L87" s="10"/>
-      <c r="M87" s="10"/>
-      <c r="N87" s="10"/>
-      <c r="O87" s="10"/>
-      <c r="P87" s="10"/>
-      <c r="Q87" s="10"/>
-      <c r="R87" s="10"/>
-      <c r="S87" s="10"/>
-      <c r="T87" s="10"/>
-      <c r="U87" s="10"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F88" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L88" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N88" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P88" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q88" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R88" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="7"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="10"/>
+      <c r="T88" s="10"/>
+      <c r="U88" s="10"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F89" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>23</v>
@@ -7350,28 +7402,28 @@
         <v>25</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L89" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M89" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N89" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O89" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P89" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q89" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R89" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
@@ -7379,20 +7431,20 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>23</v>
@@ -7407,19 +7459,19 @@
         <v>25</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>44</v>
@@ -7436,20 +7488,20 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7464,19 +7516,19 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
@@ -7492,54 +7544,88 @@
       <c r="U91" s="7"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92" s="28"/>
-      <c r="F92"/>
-      <c r="G92"/>
-      <c r="H92"/>
-      <c r="I92"/>
-      <c r="J92"/>
-      <c r="K92"/>
-      <c r="L92"/>
-      <c r="M92"/>
-      <c r="N92"/>
-      <c r="O92"/>
-      <c r="P92"/>
-      <c r="Q92"/>
-      <c r="R92"/>
-      <c r="S92"/>
-      <c r="T92"/>
-      <c r="U92"/>
+      <c r="A92" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K92" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L92" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M92" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O92" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P92" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q92" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R92" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="7"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
-      <c r="I93" s="10"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="10"/>
-      <c r="M93" s="10"/>
-      <c r="N93" s="10"/>
-      <c r="O93" s="10"/>
-      <c r="P93" s="10"/>
-      <c r="Q93" s="12"/>
-      <c r="R93" s="10"/>
-      <c r="S93" s="10"/>
-      <c r="T93" s="10"/>
-      <c r="U93" s="10"/>
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93" s="28"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+      <c r="P93"/>
+      <c r="Q93"/>
+      <c r="R93"/>
+      <c r="S93"/>
+      <c r="T93"/>
+      <c r="U93"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
@@ -7561,17 +7647,17 @@
       <c r="U94" s="10"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B95" s="10"/>
+      <c r="A95" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
-      <c r="K95" s="10"/>
+      <c r="K95" s="9"/>
       <c r="L95" s="10"/>
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
@@ -7585,7 +7671,7 @@
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -7607,35 +7693,61 @@
       <c r="U96" s="10"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="10"/>
+      <c r="N97" s="10"/>
+      <c r="O97" s="10"/>
+      <c r="P97" s="10"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="10"/>
+      <c r="S97" s="10"/>
+      <c r="T97" s="10"/>
+      <c r="U97" s="10"/>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A98" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
-      <c r="N97" s="13"/>
-      <c r="O97" s="13"/>
-      <c r="P97" s="13"/>
-      <c r="R97" s="13"/>
-      <c r="S97" s="13"/>
-      <c r="T97" s="13"/>
-      <c r="U97" s="13"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="11" t="s">
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+      <c r="M98" s="13"/>
+      <c r="N98" s="13"/>
+      <c r="O98" s="13"/>
+      <c r="P98" s="13"/>
+      <c r="R98" s="13"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="13"/>
+      <c r="U98" s="13"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A99" s="11" t="s">
         <v>480</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E69" r:id="rId1" xr:uid="{0EA114DD-6E08-431E-ACB9-AC955FE74158}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="19" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="25" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #406 : [namespace-registry] add new namespace "kplo" #406 (#407)
Add the namespaces "kplo" to the Namespace Registry and the config.properties file.
kplo - Namespace for the Korea Pathfinder Lunar Orbiter(KPLO)

@c-suh  [namespace-registry] add new namespace "kplo" #406

Resolves #406

Co-authored-by: John Hughes <John.S.Hughes@jpl.nasa.gov>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\AAANameSpaceRegistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\From Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8196AB-BE6B-44B7-BD44-69BB9B6974F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0248E4D2-C73D-40E1-8979-9DB917B6735E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="565">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1690,6 +1690,36 @@
   </si>
   <si>
     <t>KARI</t>
+  </si>
+  <si>
+    <t>kplo</t>
+  </si>
+  <si>
+    <t>mission/kplo</t>
+  </si>
+  <si>
+    <t>urn:kari:kpds:</t>
+  </si>
+  <si>
+    <t>PDS4_KARI_KPDS_KPLO</t>
+  </si>
+  <si>
+    <t>eunhyeuk@kari.re.kr</t>
+  </si>
+  <si>
+    <t>Eunhyeuk Kim (KARI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eunhyeuk Kim (KARI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eunhyeuk Kim</t>
+  </si>
+  <si>
+    <t>Korea Pathfinder Lunar Orbiter (KPLO)</t>
+  </si>
+  <si>
+    <t>Namespace for the Korea Pathfinder Lunar Orbiter (KPLO).</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1729,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1718,6 +1748,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1813,10 +1851,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1927,8 +1966,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2244,12 +2290,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U98"/>
+  <dimension ref="A1:U99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="L41" sqref="L41"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4687,7 +4733,7 @@
       <c r="U41" s="34"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="16" t="s">
         <v>228</v>
       </c>
       <c r="B42" s="5"/>
@@ -4747,66 +4793,68 @@
       </c>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="I43" s="5" t="s">
+    <row r="43" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>556</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>555</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="I43" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>41837</v>
-      </c>
-      <c r="R43" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="S43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U43" s="7"/>
+      <c r="J43" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="L43" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="M43" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="O43" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="P43" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="33">
+        <v>44448</v>
+      </c>
+      <c r="R43" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="S43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" s="34"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
@@ -4814,13 +4862,13 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>234</v>
@@ -4869,152 +4917,152 @@
       </c>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="7"/>
+    </row>
+    <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D46" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E46" s="18" t="s">
         <v>516</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F46" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G46" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H46" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="I45" s="30" t="s">
+      <c r="I46" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J45" s="30" t="s">
+      <c r="J46" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="19" t="s">
+      <c r="K46" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="L45" s="19" t="s">
+      <c r="L46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M45" s="30" t="s">
+      <c r="M46" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N45" s="30" t="s">
+      <c r="N46" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O45" s="30" t="s">
+      <c r="O46" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P45" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q45" s="33">
+      <c r="P46" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="33">
         <v>44333</v>
       </c>
-      <c r="R45" s="30" t="s">
+      <c r="R46" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S45" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="34"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O46" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R46" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="7"/>
+      <c r="S46" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="34"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>216</v>
@@ -5023,28 +5071,28 @@
         <v>25</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q47" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S47" s="5" t="s">
         <v>33</v>
@@ -5056,26 +5104,26 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5084,7 +5132,7 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>109</v>
@@ -5102,10 +5150,10 @@
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5117,26 +5165,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>262</v>
+      <c r="H49" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5145,28 +5193,28 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5182,13 +5230,13 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F50" s="24" t="s">
         <v>259</v>
@@ -5239,26 +5287,26 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>216</v>
@@ -5267,28 +5315,28 @@
         <v>25</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q51" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R51" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S51" s="5" t="s">
         <v>33</v>
@@ -5298,87 +5346,89 @@
       </c>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q52" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R52" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S52" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T52" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U52" s="7"/>
     </row>
     <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D53" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E53" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
@@ -5399,7 +5449,7 @@
         <v>278</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>44</v>
@@ -5408,10 +5458,10 @@
         <v>43788</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S53" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T53" s="5" t="s">
         <v>281</v>
@@ -5420,24 +5470,24 @@
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5445,9 +5495,15 @@
       <c r="J54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
+      <c r="K54" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N54" s="5" t="s">
         <v>278</v>
       </c>
@@ -5464,7 +5520,7 @@
         <v>288</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T54" s="5" t="s">
         <v>281</v>
@@ -5473,24 +5529,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5517,7 +5573,7 @@
         <v>288</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5526,24 +5582,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5579,24 +5635,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5632,24 +5688,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5685,24 +5741,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5738,24 +5794,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5791,24 +5847,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5844,24 +5900,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5897,24 +5953,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -5950,24 +6006,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6003,24 +6059,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H65" s="5" t="s">
-        <v>347</v>
+      <c r="H65" s="16" t="s">
+        <v>342</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6056,137 +6112,135 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J66" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O66" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q66" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R66" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S66" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T66" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U66" s="7"/>
+    </row>
+    <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J67" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K66" s="5" t="s">
+      <c r="K67" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L66" s="5" t="s">
+      <c r="L67" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M66" s="5" t="s">
+      <c r="M67" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N66" s="5" t="s">
+      <c r="N67" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O66" s="5" t="s">
+      <c r="O67" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P66" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q66" s="6">
+      <c r="P67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q67" s="6">
         <v>44111</v>
       </c>
-      <c r="R66" s="5" t="s">
+      <c r="R67" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S66" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T66" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U66" s="7"/>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q67" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
-      <c r="T67" s="5"/>
+      <c r="S67" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U67" s="7"/>
     </row>
-    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D68" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K68" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L68" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N68" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
       <c r="O68" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>44</v>
@@ -6194,37 +6248,33 @@
       <c r="Q68" s="6">
         <v>43788</v>
       </c>
-      <c r="R68" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T68" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
       <c r="U68" s="7"/>
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D69" s="21"/>
-      <c r="E69" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>357</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
@@ -6245,7 +6295,7 @@
         <v>359</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6254,7 +6304,7 @@
         <v>43788</v>
       </c>
       <c r="R69" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S69" s="5" t="s">
         <v>33</v>
@@ -6266,24 +6316,24 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>216</v>
@@ -6304,7 +6354,7 @@
         <v>359</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6313,7 +6363,7 @@
         <v>43788</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>33</v>
@@ -6325,24 +6375,24 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6384,24 +6434,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6422,7 +6472,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6431,7 +6481,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6441,23 +6491,47 @@
       </c>
       <c r="U72" s="7"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A73" s="5"/>
+    <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D73" s="21"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
+      <c r="E73" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L73" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N73" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O73" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6465,52 +6539,32 @@
       <c r="Q73" s="6">
         <v>43788</v>
       </c>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
+      <c r="R73" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S73" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T73" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A74" s="5"/>
       <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D74" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K74" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L74" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M74" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N74" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
       <c r="O74" s="5" t="s">
         <v>65</v>
       </c>
@@ -6520,37 +6574,33 @@
       <c r="Q74" s="6">
         <v>43788</v>
       </c>
-      <c r="R74" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S74" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T74" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
       <c r="U74" s="7"/>
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D75" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E75" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6583,7 +6633,7 @@
         <v>361</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T75" s="5" t="s">
         <v>281</v>
@@ -6592,24 +6642,24 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6642,7 +6692,7 @@
         <v>361</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>281</v>
@@ -6651,24 +6701,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6710,24 +6760,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6769,24 +6819,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6828,24 +6878,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6887,24 +6937,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6946,24 +6996,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7005,24 +7055,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7064,24 +7114,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7123,24 +7173,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7182,24 +7232,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7240,102 +7290,104 @@
       <c r="U86" s="7"/>
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D87" s="21"/>
+      <c r="E87" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L87" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M87" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N87" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O87" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P87" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q87" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R87" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S87" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T87" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U87" s="7"/>
+    </row>
+    <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B87" s="15"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
-      <c r="H87" s="10"/>
-      <c r="I87" s="10"/>
-      <c r="J87" s="10"/>
-      <c r="K87" s="10"/>
-      <c r="L87" s="10"/>
-      <c r="M87" s="10"/>
-      <c r="N87" s="10"/>
-      <c r="O87" s="10"/>
-      <c r="P87" s="10"/>
-      <c r="Q87" s="10"/>
-      <c r="R87" s="10"/>
-      <c r="S87" s="10"/>
-      <c r="T87" s="10"/>
-      <c r="U87" s="10"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F88" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L88" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N88" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P88" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q88" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R88" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="7"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="10"/>
+      <c r="T88" s="10"/>
+      <c r="U88" s="10"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F89" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>23</v>
@@ -7350,28 +7402,28 @@
         <v>25</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L89" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M89" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N89" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O89" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P89" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q89" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R89" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
@@ -7379,20 +7431,20 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>23</v>
@@ -7407,19 +7459,19 @@
         <v>25</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>44</v>
@@ -7436,20 +7488,20 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7464,19 +7516,19 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
@@ -7492,54 +7544,88 @@
       <c r="U91" s="7"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92" s="28"/>
-      <c r="F92"/>
-      <c r="G92"/>
-      <c r="H92"/>
-      <c r="I92"/>
-      <c r="J92"/>
-      <c r="K92"/>
-      <c r="L92"/>
-      <c r="M92"/>
-      <c r="N92"/>
-      <c r="O92"/>
-      <c r="P92"/>
-      <c r="Q92"/>
-      <c r="R92"/>
-      <c r="S92"/>
-      <c r="T92"/>
-      <c r="U92"/>
+      <c r="A92" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K92" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L92" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M92" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O92" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P92" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q92" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R92" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="7"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
-      <c r="I93" s="10"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="10"/>
-      <c r="M93" s="10"/>
-      <c r="N93" s="10"/>
-      <c r="O93" s="10"/>
-      <c r="P93" s="10"/>
-      <c r="Q93" s="12"/>
-      <c r="R93" s="10"/>
-      <c r="S93" s="10"/>
-      <c r="T93" s="10"/>
-      <c r="U93" s="10"/>
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93" s="28"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+      <c r="P93"/>
+      <c r="Q93"/>
+      <c r="R93"/>
+      <c r="S93"/>
+      <c r="T93"/>
+      <c r="U93"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
@@ -7561,17 +7647,17 @@
       <c r="U94" s="10"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B95" s="10"/>
+      <c r="A95" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
-      <c r="K95" s="10"/>
+      <c r="K95" s="9"/>
       <c r="L95" s="10"/>
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
@@ -7585,7 +7671,7 @@
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -7607,35 +7693,61 @@
       <c r="U96" s="10"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="10"/>
+      <c r="N97" s="10"/>
+      <c r="O97" s="10"/>
+      <c r="P97" s="10"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="10"/>
+      <c r="S97" s="10"/>
+      <c r="T97" s="10"/>
+      <c r="U97" s="10"/>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A98" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
-      <c r="N97" s="13"/>
-      <c r="O97" s="13"/>
-      <c r="P97" s="13"/>
-      <c r="R97" s="13"/>
-      <c r="S97" s="13"/>
-      <c r="T97" s="13"/>
-      <c r="U97" s="13"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="11" t="s">
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+      <c r="M98" s="13"/>
+      <c r="N98" s="13"/>
+      <c r="O98" s="13"/>
+      <c r="P98" s="13"/>
+      <c r="R98" s="13"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="13"/>
+      <c r="U98" s="13"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A99" s="11" t="s">
         <v>480</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E69" r:id="rId1" xr:uid="{0EA114DD-6E08-431E-ACB9-AC955FE74158}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="19" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="25" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #409 :  [namespace-registry] add new namespace "radar"
Add the namespaces "radar" to the Namespace Registry and the config.properties file.

This LDD is necessary to archive radar data from Arecibo, Goldstone, and similar installations. There is currently no similar dictionary that covers classes and attributes specific to RADAR observations.

@c-suh  [namespace-registry] add new namespace "radar" #409

Resolves #409
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\From Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\00_RepositoryUpdates\211020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0248E4D2-C73D-40E1-8979-9DB917B6735E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F721658B-2FFB-4472-8140-687D81B27CC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="573">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1720,6 +1720,30 @@
   </si>
   <si>
     <t>Namespace for the Korea Pathfinder Lunar Orbiter (KPLO).</t>
+  </si>
+  <si>
+    <t>radar</t>
+  </si>
+  <si>
+    <t>Radar</t>
+  </si>
+  <si>
+    <t>The Radar Dictionary describes the circumstances surrounding radar observations.</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/radar/v1</t>
+  </si>
+  <si>
+    <t>PDS4_RADAR</t>
+  </si>
+  <si>
+    <t>PDS Small Bodies Node</t>
+  </si>
+  <si>
+    <t>Beatrice Mueller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mueller at psi.edu</t>
   </si>
 </sst>
 </file>
@@ -2290,12 +2314,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U99"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4020,30 +4044,30 @@
       </c>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>491</v>
+        <v>566</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>175</v>
+        <v>567</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>169</v>
+        <v>568</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>170</v>
+        <v>569</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>38</v>
@@ -4052,80 +4076,82 @@
         <v>25</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>171</v>
+        <v>570</v>
       </c>
       <c r="L30" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>44489</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="M30" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>41002</v>
-      </c>
-      <c r="R30" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U30" s="7"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="B31" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="I31" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K31" s="16" t="s">
-        <v>178</v>
+      <c r="K31" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>44</v>
@@ -4134,7 +4160,7 @@
         <v>41002</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="S31" s="5" t="s">
         <v>33</v>
@@ -4144,39 +4170,37 @@
       </c>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>186</v>
+        <v>493</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>185</v>
-      </c>
+      <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>186</v>
+      <c r="K32" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>176</v>
@@ -4194,10 +4218,10 @@
         <v>44</v>
       </c>
       <c r="Q32" s="6">
-        <v>41589</v>
+        <v>41002</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="S32" s="5" t="s">
         <v>33</v>
@@ -4209,28 +4233,28 @@
     </row>
     <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>38</v>
@@ -4239,28 +4263,28 @@
         <v>25</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q33" s="6">
-        <v>42870</v>
+        <v>41589</v>
       </c>
       <c r="R33" s="5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="S33" s="5" t="s">
         <v>33</v>
@@ -4272,28 +4296,28 @@
     </row>
     <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>198</v>
+        <v>189</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>38</v>
@@ -4302,28 +4326,28 @@
         <v>25</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="O34" s="10" t="s">
-        <v>151</v>
+        <v>193</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q34" s="6">
-        <v>44110</v>
+        <v>42870</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="S34" s="5" t="s">
         <v>33</v>
@@ -4335,28 +4359,28 @@
     </row>
     <row r="35" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>492</v>
+        <v>200</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>198</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>38</v>
@@ -4365,177 +4389,177 @@
         <v>25</v>
       </c>
       <c r="K35" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>44110</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U35" s="7"/>
+    </row>
+    <row r="36" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="N35" s="5" t="s">
+      <c r="N36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="O35" s="5" t="s">
+      <c r="O36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="P35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q35" s="6">
+      <c r="P36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q36" s="6">
         <v>42118</v>
       </c>
-      <c r="R35" s="5" t="s">
+      <c r="R36" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="S36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="B37" s="15"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D38" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F38" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M37" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="P37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q37" s="6">
-        <v>42089</v>
-      </c>
-      <c r="R37" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="S37" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T37" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U37" s="7"/>
-    </row>
-    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>498</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>495</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="16" t="s">
-        <v>530</v>
-      </c>
-      <c r="I38" s="16" t="s">
+      <c r="H38" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I38" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L38" s="16" t="s">
-        <v>109</v>
+      <c r="K38" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N38" s="16" t="s">
-        <v>111</v>
+        <v>179</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q38" s="6">
-        <v>44329</v>
+        <v>42089</v>
       </c>
       <c r="R38" s="16" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="S38" s="5" t="s">
         <v>33</v>
@@ -4545,30 +4569,30 @@
       </c>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>526</v>
+        <v>495</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>526</v>
+        <v>496</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E39" s="37" t="s">
-        <v>528</v>
+        <v>495</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>497</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>526</v>
+        <v>495</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="I39" s="16" t="s">
         <v>216</v>
@@ -4595,7 +4619,7 @@
         <v>44</v>
       </c>
       <c r="Q39" s="6">
-        <v>44385</v>
+        <v>44329</v>
       </c>
       <c r="R39" s="16" t="s">
         <v>111</v>
@@ -4608,314 +4632,316 @@
       </c>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
+    <row r="40" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>44385</v>
+      </c>
+      <c r="R40" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="S40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U40" s="7"/>
+    </row>
+    <row r="41" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
         <v>539</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B41" s="19" t="s">
         <v>539</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C41" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D41" s="35" t="s">
         <v>539</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E41" s="18" t="s">
         <v>540</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F41" s="36" t="s">
         <v>539</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G41" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H41" s="19" t="s">
         <v>541</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I41" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="J40" s="30" t="s">
+      <c r="J41" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="K41" s="19" t="s">
         <v>542</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="L41" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="M40" s="19" t="s">
+      <c r="M41" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="N40" s="19" t="s">
+      <c r="N41" s="19" t="s">
         <v>535</v>
       </c>
-      <c r="O40" s="19" t="s">
+      <c r="O41" s="19" t="s">
         <v>536</v>
       </c>
-      <c r="P40" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q40" s="33">
+      <c r="P41" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q41" s="33">
         <v>44426</v>
       </c>
-      <c r="R40" s="19" t="s">
+      <c r="R41" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="S40" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T40" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U40" s="34"/>
-    </row>
-    <row r="41" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="30" t="s">
+      <c r="S41" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T41" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U41" s="34"/>
+    </row>
+    <row r="42" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D42" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>524</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F42" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G42" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="H42" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="I41" s="30" t="s">
+      <c r="I42" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K41" s="30" t="s">
+      <c r="K42" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="L41" s="19" t="s">
+      <c r="L42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M41" s="30" t="s">
+      <c r="M42" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="N41" s="19" t="s">
+      <c r="N42" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O41" s="30" t="s">
+      <c r="O42" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="P41" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q41" s="33">
+      <c r="P42" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="33">
         <v>44193</v>
       </c>
-      <c r="R41" s="19" t="s">
+      <c r="R42" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="S41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U41" s="34"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="S42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="34"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D43" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="F42" s="24" t="s">
+      <c r="F43" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H43" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I43" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J43" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K43" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L43" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="M43" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N43" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O43" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="6">
+      <c r="P43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="6">
         <v>42119</v>
       </c>
-      <c r="R42" s="5" t="s">
+      <c r="R43" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="7"/>
-    </row>
-    <row r="43" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
+      <c r="S43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B44" s="19" t="s">
         <v>563</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C44" s="19" t="s">
         <v>564</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D44" s="35" t="s">
         <v>556</v>
       </c>
-      <c r="E43" s="39" t="s">
+      <c r="E44" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F44" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G44" s="19" t="s">
         <v>557</v>
       </c>
-      <c r="H43" s="19" t="s">
+      <c r="H44" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="I43" s="30" t="s">
+      <c r="I44" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="J44" s="19" t="s">
         <v>552</v>
       </c>
-      <c r="K43" s="19" t="s">
+      <c r="K44" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="L43" s="19" t="s">
+      <c r="L44" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="M43" s="19" t="s">
+      <c r="M44" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="N43" s="19" t="s">
+      <c r="N44" s="19" t="s">
         <v>561</v>
       </c>
-      <c r="O43" s="19" t="s">
+      <c r="O44" s="19" t="s">
         <v>559</v>
       </c>
-      <c r="P43" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q43" s="33">
+      <c r="P44" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="33">
         <v>44448</v>
       </c>
-      <c r="R43" s="19" t="s">
+      <c r="R44" s="19" t="s">
         <v>562</v>
       </c>
-      <c r="S43" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U43" s="34"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M44" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N44" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O44" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q44" s="6">
-        <v>41837</v>
-      </c>
-      <c r="R44" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="S44" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T44" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U44" s="7"/>
+      <c r="S44" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T44" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U44" s="34"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
@@ -4923,13 +4949,13 @@
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F45" s="24" t="s">
         <v>234</v>
@@ -4978,152 +5004,152 @@
       </c>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P46" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R46" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S46" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="7"/>
+    </row>
+    <row r="47" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B47" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C47" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D47" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E47" s="18" t="s">
         <v>516</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F47" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G47" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H46" s="19" t="s">
+      <c r="H47" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="I46" s="30" t="s">
+      <c r="I47" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J46" s="30" t="s">
+      <c r="J47" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K46" s="19" t="s">
+      <c r="K47" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="L46" s="19" t="s">
+      <c r="L47" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M46" s="30" t="s">
+      <c r="M47" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N46" s="30" t="s">
+      <c r="N47" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O46" s="30" t="s">
+      <c r="O47" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P46" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="33">
+      <c r="P47" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="33">
         <v>44333</v>
       </c>
-      <c r="R46" s="30" t="s">
+      <c r="R47" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S46" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="34"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F47" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N47" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O47" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R47" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="7"/>
+      <c r="S47" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="34"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5132,28 +5158,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5165,26 +5191,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5193,7 +5219,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>109</v>
@@ -5211,10 +5237,10 @@
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5226,26 +5252,26 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>262</v>
+      <c r="H50" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5254,28 +5280,28 @@
         <v>25</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q50" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S50" s="5" t="s">
         <v>33</v>
@@ -5291,13 +5317,13 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>259</v>
@@ -5348,26 +5374,26 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
@@ -5376,28 +5402,28 @@
         <v>25</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q52" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R52" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S52" s="5" t="s">
         <v>33</v>
@@ -5407,87 +5433,89 @@
       </c>
       <c r="U52" s="7"/>
     </row>
-    <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q53" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S53" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U53" s="7"/>
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D54" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5508,7 +5536,7 @@
         <v>278</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>44</v>
@@ -5517,10 +5545,10 @@
         <v>43788</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T54" s="5" t="s">
         <v>281</v>
@@ -5529,24 +5557,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5554,9 +5582,15 @@
       <c r="J55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N55" s="5" t="s">
         <v>278</v>
       </c>
@@ -5573,7 +5607,7 @@
         <v>288</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5582,24 +5616,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5626,7 +5660,7 @@
         <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5635,24 +5669,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5688,24 +5722,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5741,24 +5775,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5794,24 +5828,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5847,24 +5881,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5900,24 +5934,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5953,24 +5987,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6006,24 +6040,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6059,24 +6093,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H65" s="16" t="s">
-        <v>342</v>
+      <c r="H65" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6112,24 +6146,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H66" s="5" t="s">
-        <v>347</v>
+      <c r="H66" s="16" t="s">
+        <v>342</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6165,137 +6199,135 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D67" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J67" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R67" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U67" s="7"/>
+    </row>
+    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K67" s="5" t="s">
+      <c r="K68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L67" s="5" t="s">
+      <c r="L68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M67" s="5" t="s">
+      <c r="M68" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N67" s="5" t="s">
+      <c r="N68" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O67" s="5" t="s">
+      <c r="O68" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q67" s="6">
+      <c r="P68" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q68" s="6">
         <v>44111</v>
       </c>
-      <c r="R67" s="5" t="s">
+      <c r="R68" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U67" s="7"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
+      <c r="S68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T68" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U68" s="7"/>
     </row>
-    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D69" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E69" s="38" t="s">
-        <v>357</v>
-      </c>
-      <c r="F69" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
       <c r="O69" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6303,37 +6335,33 @@
       <c r="Q69" s="6">
         <v>43788</v>
       </c>
-      <c r="R69" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
       <c r="U69" s="7"/>
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D70" s="21"/>
-      <c r="E70" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>357</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>216</v>
@@ -6354,7 +6382,7 @@
         <v>359</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6363,7 +6391,7 @@
         <v>43788</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>33</v>
@@ -6375,24 +6403,24 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6413,7 +6441,7 @@
         <v>359</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6422,7 +6450,7 @@
         <v>43788</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>33</v>
@@ -6434,24 +6462,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6493,24 +6521,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6531,7 +6559,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6540,7 +6568,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6550,23 +6578,47 @@
       </c>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D74" s="21"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
+      <c r="E74" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O74" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>44</v>
@@ -6574,52 +6626,32 @@
       <c r="Q74" s="6">
         <v>43788</v>
       </c>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
+      <c r="R74" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S74" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T74" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D75" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N75" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
       <c r="O75" s="5" t="s">
         <v>65</v>
       </c>
@@ -6629,37 +6661,33 @@
       <c r="Q75" s="6">
         <v>43788</v>
       </c>
-      <c r="R75" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S75" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T75" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
       <c r="U75" s="7"/>
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D76" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D76" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E76" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6692,7 +6720,7 @@
         <v>361</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>281</v>
@@ -6701,24 +6729,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6751,7 +6779,7 @@
         <v>361</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>281</v>
@@ -6760,24 +6788,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6819,24 +6847,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6878,24 +6906,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6937,24 +6965,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6996,24 +7024,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7055,24 +7083,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7114,24 +7142,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7173,24 +7201,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7232,24 +7260,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7291,24 +7319,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7349,102 +7377,104 @@
       <c r="U87" s="7"/>
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D88" s="21"/>
+      <c r="E88" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R88" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U88" s="7"/>
+    </row>
+    <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B88" s="15"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10"/>
-      <c r="J88" s="10"/>
-      <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10"/>
-      <c r="O88" s="10"/>
-      <c r="P88" s="10"/>
-      <c r="Q88" s="10"/>
-      <c r="R88" s="10"/>
-      <c r="S88" s="10"/>
-      <c r="T88" s="10"/>
-      <c r="U88" s="10"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F89" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K89" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L89" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q89" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R89" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="7"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>23</v>
@@ -7459,28 +7489,28 @@
         <v>25</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q90" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R90" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
@@ -7488,20 +7518,20 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7516,19 +7546,19 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
@@ -7545,20 +7575,20 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F92" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7573,19 +7603,19 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
@@ -7601,54 +7631,88 @@
       <c r="U92" s="7"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93" s="28"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
-      <c r="N93"/>
-      <c r="O93"/>
-      <c r="P93"/>
-      <c r="Q93"/>
-      <c r="R93"/>
-      <c r="S93"/>
-      <c r="T93"/>
-      <c r="U93"/>
+      <c r="A93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q93" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R93" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="7"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-      <c r="I94" s="10"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="10"/>
-      <c r="M94" s="10"/>
-      <c r="N94" s="10"/>
-      <c r="O94" s="10"/>
-      <c r="P94" s="10"/>
-      <c r="Q94" s="12"/>
-      <c r="R94" s="10"/>
-      <c r="S94" s="10"/>
-      <c r="T94" s="10"/>
-      <c r="U94" s="10"/>
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94" s="28"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
+      <c r="R94"/>
+      <c r="S94"/>
+      <c r="T94"/>
+      <c r="U94"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
@@ -7670,17 +7734,17 @@
       <c r="U95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B96" s="10"/>
+      <c r="A96" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
       <c r="I96" s="10"/>
-      <c r="K96" s="10"/>
+      <c r="K96" s="9"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
@@ -7694,7 +7758,7 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -7716,36 +7780,59 @@
       <c r="U97" s="10"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+      <c r="O98" s="10"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10"/>
+      <c r="U98" s="10"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="13"/>
-      <c r="P98" s="13"/>
-      <c r="R98" s="13"/>
-      <c r="S98" s="13"/>
-      <c r="T98" s="13"/>
-      <c r="U98" s="13"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="11" t="s">
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+      <c r="O99" s="13"/>
+      <c r="P99" s="13"/>
+      <c r="R99" s="13"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="13"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A100" s="11" t="s">
         <v>480</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E69" r:id="rId1" xr:uid="{0EA114DD-6E08-431E-ACB9-AC955FE74158}"/>
+    <hyperlink ref="E70" r:id="rId1" xr:uid="{0EA114DD-6E08-431E-ACB9-AC955FE74158}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Issue #409 :  [namespace-registry] add new namespace "radar" (#411)
Add the namespaces "radar" to the Namespace Registry and the config.properties file.

This LDD is necessary to archive radar data from Arecibo, Goldstone, and similar installations. There is currently no similar dictionary that covers classes and attributes specific to RADAR observations.

@c-suh  [namespace-registry] add new namespace "radar" #409

Resolves #409

Co-authored-by: John Hughes <John.S.Hughes@jpl.nasa.gov>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\From Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\00_RepositoryUpdates\211020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0248E4D2-C73D-40E1-8979-9DB917B6735E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F721658B-2FFB-4472-8140-687D81B27CC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="573">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1720,6 +1720,30 @@
   </si>
   <si>
     <t>Namespace for the Korea Pathfinder Lunar Orbiter (KPLO).</t>
+  </si>
+  <si>
+    <t>radar</t>
+  </si>
+  <si>
+    <t>Radar</t>
+  </si>
+  <si>
+    <t>The Radar Dictionary describes the circumstances surrounding radar observations.</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/radar/v1</t>
+  </si>
+  <si>
+    <t>PDS4_RADAR</t>
+  </si>
+  <si>
+    <t>PDS Small Bodies Node</t>
+  </si>
+  <si>
+    <t>Beatrice Mueller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mueller at psi.edu</t>
   </si>
 </sst>
 </file>
@@ -2290,12 +2314,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U99"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4020,30 +4044,30 @@
       </c>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>491</v>
+        <v>566</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>175</v>
+        <v>567</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>169</v>
+        <v>568</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>170</v>
+        <v>569</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>38</v>
@@ -4052,80 +4076,82 @@
         <v>25</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>171</v>
+        <v>570</v>
       </c>
       <c r="L30" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>44489</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="M30" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>41002</v>
-      </c>
-      <c r="R30" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U30" s="7"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="B31" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="I31" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K31" s="16" t="s">
-        <v>178</v>
+      <c r="K31" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>44</v>
@@ -4134,7 +4160,7 @@
         <v>41002</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="S31" s="5" t="s">
         <v>33</v>
@@ -4144,39 +4170,37 @@
       </c>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>186</v>
+        <v>493</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>185</v>
-      </c>
+      <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>186</v>
+      <c r="K32" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>176</v>
@@ -4194,10 +4218,10 @@
         <v>44</v>
       </c>
       <c r="Q32" s="6">
-        <v>41589</v>
+        <v>41002</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="S32" s="5" t="s">
         <v>33</v>
@@ -4209,28 +4233,28 @@
     </row>
     <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>38</v>
@@ -4239,28 +4263,28 @@
         <v>25</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q33" s="6">
-        <v>42870</v>
+        <v>41589</v>
       </c>
       <c r="R33" s="5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="S33" s="5" t="s">
         <v>33</v>
@@ -4272,28 +4296,28 @@
     </row>
     <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>198</v>
+        <v>189</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>38</v>
@@ -4302,28 +4326,28 @@
         <v>25</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="O34" s="10" t="s">
-        <v>151</v>
+        <v>193</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q34" s="6">
-        <v>44110</v>
+        <v>42870</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="S34" s="5" t="s">
         <v>33</v>
@@ -4335,28 +4359,28 @@
     </row>
     <row r="35" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>492</v>
+        <v>200</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>198</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>38</v>
@@ -4365,177 +4389,177 @@
         <v>25</v>
       </c>
       <c r="K35" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>44110</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U35" s="7"/>
+    </row>
+    <row r="36" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="N35" s="5" t="s">
+      <c r="N36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="O35" s="5" t="s">
+      <c r="O36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="P35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q35" s="6">
+      <c r="P36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q36" s="6">
         <v>42118</v>
       </c>
-      <c r="R35" s="5" t="s">
+      <c r="R36" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="S36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="B37" s="15"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D38" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F38" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M37" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="P37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q37" s="6">
-        <v>42089</v>
-      </c>
-      <c r="R37" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="S37" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T37" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U37" s="7"/>
-    </row>
-    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>498</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>495</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="16" t="s">
-        <v>530</v>
-      </c>
-      <c r="I38" s="16" t="s">
+      <c r="H38" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I38" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L38" s="16" t="s">
-        <v>109</v>
+      <c r="K38" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N38" s="16" t="s">
-        <v>111</v>
+        <v>179</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q38" s="6">
-        <v>44329</v>
+        <v>42089</v>
       </c>
       <c r="R38" s="16" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="S38" s="5" t="s">
         <v>33</v>
@@ -4545,30 +4569,30 @@
       </c>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>526</v>
+        <v>495</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>526</v>
+        <v>496</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E39" s="37" t="s">
-        <v>528</v>
+        <v>495</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>497</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>526</v>
+        <v>495</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="I39" s="16" t="s">
         <v>216</v>
@@ -4595,7 +4619,7 @@
         <v>44</v>
       </c>
       <c r="Q39" s="6">
-        <v>44385</v>
+        <v>44329</v>
       </c>
       <c r="R39" s="16" t="s">
         <v>111</v>
@@ -4608,314 +4632,316 @@
       </c>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
+    <row r="40" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>44385</v>
+      </c>
+      <c r="R40" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="S40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U40" s="7"/>
+    </row>
+    <row r="41" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
         <v>539</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B41" s="19" t="s">
         <v>539</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C41" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D41" s="35" t="s">
         <v>539</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E41" s="18" t="s">
         <v>540</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F41" s="36" t="s">
         <v>539</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G41" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H41" s="19" t="s">
         <v>541</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I41" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="J40" s="30" t="s">
+      <c r="J41" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="K41" s="19" t="s">
         <v>542</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="L41" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="M40" s="19" t="s">
+      <c r="M41" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="N40" s="19" t="s">
+      <c r="N41" s="19" t="s">
         <v>535</v>
       </c>
-      <c r="O40" s="19" t="s">
+      <c r="O41" s="19" t="s">
         <v>536</v>
       </c>
-      <c r="P40" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q40" s="33">
+      <c r="P41" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q41" s="33">
         <v>44426</v>
       </c>
-      <c r="R40" s="19" t="s">
+      <c r="R41" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="S40" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T40" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U40" s="34"/>
-    </row>
-    <row r="41" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="30" t="s">
+      <c r="S41" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T41" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U41" s="34"/>
+    </row>
+    <row r="42" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D42" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>524</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F42" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G42" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="H42" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="I41" s="30" t="s">
+      <c r="I42" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K41" s="30" t="s">
+      <c r="K42" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="L41" s="19" t="s">
+      <c r="L42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M41" s="30" t="s">
+      <c r="M42" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="N41" s="19" t="s">
+      <c r="N42" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O41" s="30" t="s">
+      <c r="O42" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="P41" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q41" s="33">
+      <c r="P42" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="33">
         <v>44193</v>
       </c>
-      <c r="R41" s="19" t="s">
+      <c r="R42" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="S41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T41" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U41" s="34"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="S42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="34"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D43" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="F42" s="24" t="s">
+      <c r="F43" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H43" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I43" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J43" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K43" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L43" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="M43" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N43" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O43" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="6">
+      <c r="P43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="6">
         <v>42119</v>
       </c>
-      <c r="R42" s="5" t="s">
+      <c r="R43" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="7"/>
-    </row>
-    <row r="43" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
+      <c r="S43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B44" s="19" t="s">
         <v>563</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C44" s="19" t="s">
         <v>564</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D44" s="35" t="s">
         <v>556</v>
       </c>
-      <c r="E43" s="39" t="s">
+      <c r="E44" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F44" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G44" s="19" t="s">
         <v>557</v>
       </c>
-      <c r="H43" s="19" t="s">
+      <c r="H44" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="I43" s="30" t="s">
+      <c r="I44" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="J44" s="19" t="s">
         <v>552</v>
       </c>
-      <c r="K43" s="19" t="s">
+      <c r="K44" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="L43" s="19" t="s">
+      <c r="L44" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="M43" s="19" t="s">
+      <c r="M44" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="N43" s="19" t="s">
+      <c r="N44" s="19" t="s">
         <v>561</v>
       </c>
-      <c r="O43" s="19" t="s">
+      <c r="O44" s="19" t="s">
         <v>559</v>
       </c>
-      <c r="P43" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q43" s="33">
+      <c r="P44" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="33">
         <v>44448</v>
       </c>
-      <c r="R43" s="19" t="s">
+      <c r="R44" s="19" t="s">
         <v>562</v>
       </c>
-      <c r="S43" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U43" s="34"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M44" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N44" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O44" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q44" s="6">
-        <v>41837</v>
-      </c>
-      <c r="R44" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="S44" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T44" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U44" s="7"/>
+      <c r="S44" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T44" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U44" s="34"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
@@ -4923,13 +4949,13 @@
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F45" s="24" t="s">
         <v>234</v>
@@ -4978,152 +5004,152 @@
       </c>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P46" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R46" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S46" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="7"/>
+    </row>
+    <row r="47" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B47" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C47" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D47" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E47" s="18" t="s">
         <v>516</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F47" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G47" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H46" s="19" t="s">
+      <c r="H47" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="I46" s="30" t="s">
+      <c r="I47" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="J46" s="30" t="s">
+      <c r="J47" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K46" s="19" t="s">
+      <c r="K47" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="L46" s="19" t="s">
+      <c r="L47" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M46" s="30" t="s">
+      <c r="M47" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N46" s="30" t="s">
+      <c r="N47" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="O46" s="30" t="s">
+      <c r="O47" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="P46" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="33">
+      <c r="P47" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="33">
         <v>44333</v>
       </c>
-      <c r="R46" s="30" t="s">
+      <c r="R47" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="S46" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="34"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="F47" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N47" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O47" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R47" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="7"/>
+      <c r="S47" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="34"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5132,28 +5158,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5165,26 +5191,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5193,7 +5219,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>109</v>
@@ -5211,10 +5237,10 @@
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5226,26 +5252,26 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>262</v>
+      <c r="H50" s="19" t="s">
+        <v>523</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5254,28 +5280,28 @@
         <v>25</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q50" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S50" s="5" t="s">
         <v>33</v>
@@ -5291,13 +5317,13 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>259</v>
@@ -5348,26 +5374,26 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>216</v>
@@ -5376,28 +5402,28 @@
         <v>25</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q52" s="6">
-        <v>41771</v>
+        <v>42158</v>
       </c>
       <c r="R52" s="5" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="S52" s="5" t="s">
         <v>33</v>
@@ -5407,87 +5433,89 @@
       </c>
       <c r="U52" s="7"/>
     </row>
-    <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q53" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S53" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U53" s="7"/>
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D54" s="21"/>
+        <v>280</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>274</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5508,7 +5536,7 @@
         <v>278</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>44</v>
@@ -5517,10 +5545,10 @@
         <v>43788</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T54" s="5" t="s">
         <v>281</v>
@@ -5529,24 +5557,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5554,9 +5582,15 @@
       <c r="J55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N55" s="5" t="s">
         <v>278</v>
       </c>
@@ -5573,7 +5607,7 @@
         <v>288</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5582,24 +5616,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5626,7 +5660,7 @@
         <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5635,24 +5669,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5688,24 +5722,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5741,24 +5775,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5794,24 +5828,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5847,24 +5881,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5900,24 +5934,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5953,24 +5987,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6006,24 +6040,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6059,24 +6093,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H65" s="16" t="s">
-        <v>342</v>
+      <c r="H65" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6112,24 +6146,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H66" s="5" t="s">
-        <v>347</v>
+      <c r="H66" s="16" t="s">
+        <v>342</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6165,137 +6199,135 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D67" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="8" t="s">
+        <v>345</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J67" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R67" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U67" s="7"/>
+    </row>
+    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K67" s="5" t="s">
+      <c r="K68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L67" s="5" t="s">
+      <c r="L68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M67" s="5" t="s">
+      <c r="M68" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N67" s="5" t="s">
+      <c r="N68" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O67" s="5" t="s">
+      <c r="O68" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q67" s="6">
+      <c r="P68" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q68" s="6">
         <v>44111</v>
       </c>
-      <c r="R67" s="5" t="s">
+      <c r="R68" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U67" s="7"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
+      <c r="S68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T68" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U68" s="7"/>
     </row>
-    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D69" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="E69" s="38" t="s">
-        <v>357</v>
-      </c>
-      <c r="F69" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
       <c r="O69" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6303,37 +6335,33 @@
       <c r="Q69" s="6">
         <v>43788</v>
       </c>
-      <c r="R69" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
       <c r="U69" s="7"/>
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D70" s="21"/>
-      <c r="E70" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>357</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>216</v>
@@ -6354,7 +6382,7 @@
         <v>359</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6363,7 +6391,7 @@
         <v>43788</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>33</v>
@@ -6375,24 +6403,24 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6413,7 +6441,7 @@
         <v>359</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6422,7 +6450,7 @@
         <v>43788</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>33</v>
@@ -6434,24 +6462,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6493,24 +6521,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6531,7 +6559,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6540,7 +6568,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6550,23 +6578,47 @@
       </c>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D74" s="21"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
+      <c r="E74" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O74" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>44</v>
@@ -6574,52 +6626,32 @@
       <c r="Q74" s="6">
         <v>43788</v>
       </c>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
+      <c r="R74" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S74" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T74" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D75" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N75" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
       <c r="O75" s="5" t="s">
         <v>65</v>
       </c>
@@ -6629,37 +6661,33 @@
       <c r="Q75" s="6">
         <v>43788</v>
       </c>
-      <c r="R75" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S75" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T75" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
       <c r="U75" s="7"/>
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D76" s="21"/>
+        <v>388</v>
+      </c>
+      <c r="D76" s="21" t="s">
+        <v>384</v>
+      </c>
       <c r="E76" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6692,7 +6720,7 @@
         <v>361</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>281</v>
@@ -6701,24 +6729,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6751,7 +6779,7 @@
         <v>361</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>281</v>
@@ -6760,24 +6788,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6819,24 +6847,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6878,24 +6906,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6937,24 +6965,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6996,24 +7024,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7055,24 +7083,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7114,24 +7142,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7173,24 +7201,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7232,24 +7260,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7291,24 +7319,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7349,102 +7377,104 @@
       <c r="U87" s="7"/>
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D88" s="21"/>
+      <c r="E88" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R88" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U88" s="7"/>
+    </row>
+    <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B88" s="15"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10"/>
-      <c r="J88" s="10"/>
-      <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10"/>
-      <c r="O88" s="10"/>
-      <c r="P88" s="10"/>
-      <c r="Q88" s="10"/>
-      <c r="R88" s="10"/>
-      <c r="S88" s="10"/>
-      <c r="T88" s="10"/>
-      <c r="U88" s="10"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F89" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K89" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L89" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q89" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R89" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="7"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>23</v>
@@ -7459,28 +7489,28 @@
         <v>25</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q90" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R90" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
@@ -7488,20 +7518,20 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7516,19 +7546,19 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
@@ -7545,20 +7575,20 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F92" s="24" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7573,19 +7603,19 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
@@ -7601,54 +7631,88 @@
       <c r="U92" s="7"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93" s="28"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
-      <c r="N93"/>
-      <c r="O93"/>
-      <c r="P93"/>
-      <c r="Q93"/>
-      <c r="R93"/>
-      <c r="S93"/>
-      <c r="T93"/>
-      <c r="U93"/>
+      <c r="A93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q93" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R93" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="7"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-      <c r="I94" s="10"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="10"/>
-      <c r="M94" s="10"/>
-      <c r="N94" s="10"/>
-      <c r="O94" s="10"/>
-      <c r="P94" s="10"/>
-      <c r="Q94" s="12"/>
-      <c r="R94" s="10"/>
-      <c r="S94" s="10"/>
-      <c r="T94" s="10"/>
-      <c r="U94" s="10"/>
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94" s="28"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
+      <c r="R94"/>
+      <c r="S94"/>
+      <c r="T94"/>
+      <c r="U94"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
@@ -7670,17 +7734,17 @@
       <c r="U95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B96" s="10"/>
+      <c r="A96" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
       <c r="I96" s="10"/>
-      <c r="K96" s="10"/>
+      <c r="K96" s="9"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
@@ -7694,7 +7758,7 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -7716,36 +7780,59 @@
       <c r="U97" s="10"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+      <c r="O98" s="10"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10"/>
+      <c r="U98" s="10"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="13"/>
-      <c r="P98" s="13"/>
-      <c r="R98" s="13"/>
-      <c r="S98" s="13"/>
-      <c r="T98" s="13"/>
-      <c r="U98" s="13"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="11" t="s">
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+      <c r="O99" s="13"/>
+      <c r="P99" s="13"/>
+      <c r="R99" s="13"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="13"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A100" s="11" t="s">
         <v>480</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E69" r:id="rId1" xr:uid="{0EA114DD-6E08-431E-ACB9-AC955FE74158}"/>
+    <hyperlink ref="E70" r:id="rId1" xr:uid="{0EA114DD-6E08-431E-ACB9-AC955FE74158}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Issue #236 : Namespace - add "lt"
Issue #236 : [ldd-request] Create new LDD "lt"
Add the namespaces "lt" to the Namespace Registry and the config.properties file.
lt - Lunar Trailblazer LDD

@c-suh  [namespace-registry] add new namespace "neas" #236

Resolves #236
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88D37B9-F07D-4565-93B6-C3CF80B6768C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FD927-2CA6-428A-8782-0292BF271A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5360" uniqueCount="568">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1584,9 +1584,6 @@
     <t>Namespace for the Mars2020 Mission Local Data Dictionary</t>
   </si>
   <si>
-    <t xml:space="preserve">Mars2020 Mission </t>
-  </si>
-  <si>
     <t>PDS4_MARS2020</t>
   </si>
   <si>
@@ -1714,6 +1711,24 @@
   </si>
   <si>
     <t>Near Earth Asteroid Scout</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mars 2020 Mission </t>
+  </si>
+  <si>
+    <t>Lunar Trailblazer</t>
+  </si>
+  <si>
+    <t>Namespace for the Geo Node's Lunar Trailblazer dictionary.</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/lt/v1</t>
+  </si>
+  <si>
+    <t>LT</t>
   </si>
 </sst>
 </file>
@@ -2254,12 +2269,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U99"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2475,7 +2490,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>35</v>
@@ -2587,47 +2602,47 @@
     </row>
     <row r="7" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="19" t="s">
+        <v>548</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>549</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="F7" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>550</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>544</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>550</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>545</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="19" t="s">
+        <v>551</v>
+      </c>
+      <c r="K7" s="19" t="s">
         <v>552</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="L7" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>553</v>
       </c>
-      <c r="L7" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>554</v>
-      </c>
       <c r="N7" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="O7" s="19" t="s">
         <v>546</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>547</v>
       </c>
       <c r="P7" s="27" t="s">
         <v>44</v>
@@ -2636,7 +2651,7 @@
         <v>44426</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S7" s="27"/>
       <c r="T7" s="27"/>
@@ -3169,28 +3184,28 @@
     </row>
     <row r="17" spans="1:21" s="17" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>536</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>537</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>531</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>532</v>
-      </c>
       <c r="F17" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>38</v>
@@ -3208,10 +3223,10 @@
         <v>179</v>
       </c>
       <c r="N17" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="O17" s="30" t="s">
         <v>535</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>536</v>
       </c>
       <c r="P17" s="27" t="s">
         <v>44</v>
@@ -3220,7 +3235,7 @@
         <v>44398</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="S17" s="27" t="s">
         <v>33</v>
@@ -4469,7 +4484,7 @@
         <v>23</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>216</v>
@@ -4511,28 +4526,28 @@
     </row>
     <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="C39" s="16" t="s">
+      <c r="D39" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>527</v>
       </c>
-      <c r="D39" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>528</v>
-      </c>
       <c r="F39" s="16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I39" s="16" t="s">
         <v>216</v>
@@ -4574,28 +4589,28 @@
     </row>
     <row r="40" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>539</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>539</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>543</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>539</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>540</v>
-      </c>
       <c r="F40" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G40" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I40" s="19" t="s">
         <v>216</v>
@@ -4604,7 +4619,7 @@
         <v>25</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L40" s="19" t="s">
         <v>221</v>
@@ -4613,10 +4628,10 @@
         <v>179</v>
       </c>
       <c r="N40" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="O40" s="19" t="s">
         <v>535</v>
-      </c>
-      <c r="O40" s="19" t="s">
-        <v>536</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>44</v>
@@ -4647,7 +4662,7 @@
         <v>224</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>223</v>
@@ -4686,7 +4701,7 @@
         <v>44193</v>
       </c>
       <c r="R41" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S41" s="27" t="s">
         <v>33</v>
@@ -4734,10 +4749,10 @@
       <c r="M42" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N42" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O42" s="16" t="s">
         <v>194</v>
       </c>
       <c r="P42" s="5" t="s">
@@ -4881,28 +4896,28 @@
     </row>
     <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>519</v>
+        <v>564</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>518</v>
+        <v>565</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>516</v>
+        <v>562</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>566</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="G45" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>520</v>
+        <v>567</v>
       </c>
       <c r="I45" s="27" t="s">
         <v>216</v>
@@ -4911,120 +4926,122 @@
         <v>25</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>517</v>
+        <v>567</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M45" s="27" t="s">
+      <c r="M45" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N45" s="27" t="s">
+      <c r="N45" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="O45" s="27" t="s">
+      <c r="O45" s="19" t="s">
         <v>194</v>
       </c>
       <c r="P45" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q45" s="28">
+        <v>44608</v>
+      </c>
+      <c r="R45" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="S45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="29"/>
+    </row>
+    <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="L46" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="M46" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="N46" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="O46" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="P46" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="28">
         <v>44333</v>
       </c>
-      <c r="R45" s="27" t="s">
+      <c r="R46" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="S45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="29"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O46" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R46" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="7"/>
+      <c r="S46" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="29"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>244</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>216</v>
@@ -5033,28 +5050,28 @@
         <v>25</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q47" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S47" s="5" t="s">
         <v>33</v>
@@ -5066,26 +5083,26 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5094,7 +5111,7 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>109</v>
@@ -5112,10 +5129,10 @@
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5127,26 +5144,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>262</v>
+      <c r="H49" s="19" t="s">
+        <v>522</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5155,28 +5172,28 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5192,13 +5209,13 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>259</v>
@@ -5247,211 +5264,213 @@
       </c>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="19" t="s">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>42158</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U51" s="7"/>
+    </row>
+    <row r="52" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="C51" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="E52" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="F52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="I52" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J52" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="L52" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="N52" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="O52" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="P52" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="28">
+        <v>43871</v>
+      </c>
+      <c r="R52" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>555</v>
-      </c>
-      <c r="G51" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>560</v>
-      </c>
-      <c r="I51" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J51" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K51" s="19" t="s">
-        <v>561</v>
-      </c>
-      <c r="L51" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M51" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="N51" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="O51" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="P51" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q51" s="28">
-        <v>43871</v>
-      </c>
-      <c r="R51" s="19" t="s">
-        <v>559</v>
-      </c>
-      <c r="S51" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T51" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U51" s="29"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="S52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U52" s="29"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N52" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="O52" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q52" s="6">
-        <v>41771</v>
-      </c>
-      <c r="R52" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U52" s="7"/>
-    </row>
-    <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q53" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S53" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U53" s="7"/>
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D54" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5472,7 +5491,7 @@
         <v>278</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>44</v>
@@ -5481,10 +5500,10 @@
         <v>43788</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T54" s="5" t="s">
         <v>281</v>
@@ -5493,24 +5512,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5518,9 +5537,15 @@
       <c r="J55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N55" s="5" t="s">
         <v>278</v>
       </c>
@@ -5537,7 +5562,7 @@
         <v>288</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5546,24 +5571,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5590,7 +5615,7 @@
         <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5599,24 +5624,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5652,24 +5677,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5705,24 +5730,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5758,24 +5783,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5811,24 +5836,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5864,24 +5889,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5917,24 +5942,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -5970,24 +5995,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6023,24 +6048,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6076,24 +6101,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6129,137 +6154,135 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J67" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R67" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U67" s="7"/>
+    </row>
+    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K67" s="5" t="s">
+      <c r="K68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L67" s="5" t="s">
+      <c r="L68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M67" s="5" t="s">
+      <c r="M68" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N67" s="5" t="s">
+      <c r="N68" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O67" s="5" t="s">
+      <c r="O68" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q67" s="6">
+      <c r="P68" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q68" s="6">
         <v>44111</v>
       </c>
-      <c r="R67" s="5" t="s">
+      <c r="R68" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U67" s="7"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
+      <c r="S68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T68" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U68" s="7"/>
     </row>
-    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
       <c r="O69" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6267,37 +6290,33 @@
       <c r="Q69" s="6">
         <v>43788</v>
       </c>
-      <c r="R69" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
       <c r="U69" s="7"/>
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D70" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E70" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>216</v>
@@ -6318,7 +6337,7 @@
         <v>359</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6327,7 +6346,7 @@
         <v>43788</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>33</v>
@@ -6339,24 +6358,24 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6377,7 +6396,7 @@
         <v>359</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6386,7 +6405,7 @@
         <v>43788</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>33</v>
@@ -6398,24 +6417,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6457,24 +6476,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6495,7 +6514,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6504,7 +6523,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6514,23 +6533,47 @@
       </c>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
+      <c r="E74" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O74" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>44</v>
@@ -6538,52 +6581,32 @@
       <c r="Q74" s="6">
         <v>43788</v>
       </c>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
+      <c r="R74" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S74" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T74" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N75" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
       <c r="O75" s="5" t="s">
         <v>65</v>
       </c>
@@ -6593,37 +6616,33 @@
       <c r="Q75" s="6">
         <v>43788</v>
       </c>
-      <c r="R75" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S75" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T75" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
       <c r="U75" s="7"/>
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D76" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E76" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6656,7 +6675,7 @@
         <v>361</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>281</v>
@@ -6665,24 +6684,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6715,7 +6734,7 @@
         <v>361</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>281</v>
@@ -6724,24 +6743,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6783,24 +6802,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6842,24 +6861,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6901,24 +6920,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6960,24 +6979,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7019,24 +7038,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7078,24 +7097,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7137,24 +7156,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7196,24 +7215,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7255,24 +7274,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7313,102 +7332,104 @@
       <c r="U87" s="7"/>
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R88" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U88" s="7"/>
+    </row>
+    <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B88" s="15"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10"/>
-      <c r="J88" s="10"/>
-      <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10"/>
-      <c r="O88" s="10"/>
-      <c r="P88" s="10"/>
-      <c r="Q88" s="10"/>
-      <c r="R88" s="10"/>
-      <c r="S88" s="10"/>
-      <c r="T88" s="10"/>
-      <c r="U88" s="10"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F89" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K89" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L89" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q89" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R89" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="7"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F90" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>23</v>
@@ -7423,28 +7444,28 @@
         <v>25</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q90" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R90" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
@@ -7452,20 +7473,20 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7480,19 +7501,19 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
@@ -7509,20 +7530,20 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7537,19 +7558,19 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
@@ -7565,54 +7586,88 @@
       <c r="U92" s="7"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93" s="25"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
-      <c r="N93"/>
-      <c r="O93"/>
-      <c r="P93"/>
-      <c r="Q93"/>
-      <c r="R93"/>
-      <c r="S93"/>
-      <c r="T93"/>
-      <c r="U93"/>
+      <c r="A93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F93" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q93" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R93" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="7"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-      <c r="I94" s="10"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="10"/>
-      <c r="M94" s="10"/>
-      <c r="N94" s="10"/>
-      <c r="O94" s="10"/>
-      <c r="P94" s="10"/>
-      <c r="Q94" s="12"/>
-      <c r="R94" s="10"/>
-      <c r="S94" s="10"/>
-      <c r="T94" s="10"/>
-      <c r="U94" s="10"/>
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94" s="25"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
+      <c r="R94"/>
+      <c r="S94"/>
+      <c r="T94"/>
+      <c r="U94"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
@@ -7634,17 +7689,17 @@
       <c r="U95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B96" s="10"/>
+      <c r="A96" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
       <c r="I96" s="10"/>
-      <c r="K96" s="10"/>
+      <c r="K96" s="9"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
@@ -7658,7 +7713,7 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -7680,30 +7735,53 @@
       <c r="U97" s="10"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+      <c r="O98" s="10"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10"/>
+      <c r="U98" s="10"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="13"/>
-      <c r="P98" s="13"/>
-      <c r="R98" s="13"/>
-      <c r="S98" s="13"/>
-      <c r="T98" s="13"/>
-      <c r="U98" s="13"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="11" t="s">
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+      <c r="O99" s="13"/>
+      <c r="P99" s="13"/>
+      <c r="R99" s="13"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="13"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A100" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #236 : Namespace - add "lt" (#438)
Issue #236 : [ldd-request] Create new LDD "lt"
Add the namespaces "lt" to the Namespace Registry and the config.properties file.
lt - Lunar Trailblazer LDD

@c-suh  [namespace-registry] add new namespace "neas" #236

Resolves #236

Co-authored-by: John Hughes <John.S.Hughes@jpl.nasa.gov>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88D37B9-F07D-4565-93B6-C3CF80B6768C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FD927-2CA6-428A-8782-0292BF271A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5360" uniqueCount="568">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1584,9 +1584,6 @@
     <t>Namespace for the Mars2020 Mission Local Data Dictionary</t>
   </si>
   <si>
-    <t xml:space="preserve">Mars2020 Mission </t>
-  </si>
-  <si>
     <t>PDS4_MARS2020</t>
   </si>
   <si>
@@ -1714,6 +1711,24 @@
   </si>
   <si>
     <t>Near Earth Asteroid Scout</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mars 2020 Mission </t>
+  </si>
+  <si>
+    <t>Lunar Trailblazer</t>
+  </si>
+  <si>
+    <t>Namespace for the Geo Node's Lunar Trailblazer dictionary.</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/lt/v1</t>
+  </si>
+  <si>
+    <t>LT</t>
   </si>
 </sst>
 </file>
@@ -2254,12 +2269,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U99"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2475,7 +2490,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>35</v>
@@ -2587,47 +2602,47 @@
     </row>
     <row r="7" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="19" t="s">
+        <v>548</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>549</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="F7" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>550</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>544</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>550</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>545</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="19" t="s">
+        <v>551</v>
+      </c>
+      <c r="K7" s="19" t="s">
         <v>552</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="L7" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>553</v>
       </c>
-      <c r="L7" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>554</v>
-      </c>
       <c r="N7" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="O7" s="19" t="s">
         <v>546</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>547</v>
       </c>
       <c r="P7" s="27" t="s">
         <v>44</v>
@@ -2636,7 +2651,7 @@
         <v>44426</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S7" s="27"/>
       <c r="T7" s="27"/>
@@ -3169,28 +3184,28 @@
     </row>
     <row r="17" spans="1:21" s="17" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>536</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>537</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>531</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>532</v>
-      </c>
       <c r="F17" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>38</v>
@@ -3208,10 +3223,10 @@
         <v>179</v>
       </c>
       <c r="N17" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="O17" s="30" t="s">
         <v>535</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>536</v>
       </c>
       <c r="P17" s="27" t="s">
         <v>44</v>
@@ -3220,7 +3235,7 @@
         <v>44398</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="S17" s="27" t="s">
         <v>33</v>
@@ -4469,7 +4484,7 @@
         <v>23</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>216</v>
@@ -4511,28 +4526,28 @@
     </row>
     <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="C39" s="16" t="s">
+      <c r="D39" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>527</v>
       </c>
-      <c r="D39" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>528</v>
-      </c>
       <c r="F39" s="16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I39" s="16" t="s">
         <v>216</v>
@@ -4574,28 +4589,28 @@
     </row>
     <row r="40" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>539</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>539</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>543</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>539</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>540</v>
-      </c>
       <c r="F40" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G40" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I40" s="19" t="s">
         <v>216</v>
@@ -4604,7 +4619,7 @@
         <v>25</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L40" s="19" t="s">
         <v>221</v>
@@ -4613,10 +4628,10 @@
         <v>179</v>
       </c>
       <c r="N40" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="O40" s="19" t="s">
         <v>535</v>
-      </c>
-      <c r="O40" s="19" t="s">
-        <v>536</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>44</v>
@@ -4647,7 +4662,7 @@
         <v>224</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>223</v>
@@ -4686,7 +4701,7 @@
         <v>44193</v>
       </c>
       <c r="R41" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S41" s="27" t="s">
         <v>33</v>
@@ -4734,10 +4749,10 @@
       <c r="M42" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N42" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O42" s="16" t="s">
         <v>194</v>
       </c>
       <c r="P42" s="5" t="s">
@@ -4881,28 +4896,28 @@
     </row>
     <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>519</v>
+        <v>564</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>518</v>
+        <v>565</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>516</v>
+        <v>562</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>566</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="G45" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>520</v>
+        <v>567</v>
       </c>
       <c r="I45" s="27" t="s">
         <v>216</v>
@@ -4911,120 +4926,122 @@
         <v>25</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>517</v>
+        <v>567</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M45" s="27" t="s">
+      <c r="M45" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N45" s="27" t="s">
+      <c r="N45" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="O45" s="27" t="s">
+      <c r="O45" s="19" t="s">
         <v>194</v>
       </c>
       <c r="P45" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q45" s="28">
+        <v>44608</v>
+      </c>
+      <c r="R45" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="S45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="29"/>
+    </row>
+    <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="L46" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="M46" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="N46" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="O46" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="P46" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="28">
         <v>44333</v>
       </c>
-      <c r="R45" s="27" t="s">
+      <c r="R46" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="S45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="29"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O46" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R46" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="7"/>
+      <c r="S46" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="29"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>244</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>216</v>
@@ -5033,28 +5050,28 @@
         <v>25</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q47" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S47" s="5" t="s">
         <v>33</v>
@@ -5066,26 +5083,26 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5094,7 +5111,7 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>109</v>
@@ -5112,10 +5129,10 @@
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5127,26 +5144,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>262</v>
+      <c r="H49" s="19" t="s">
+        <v>522</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5155,28 +5172,28 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5192,13 +5209,13 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>259</v>
@@ -5247,211 +5264,213 @@
       </c>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="19" t="s">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>42158</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U51" s="7"/>
+    </row>
+    <row r="52" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="C51" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="E52" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="F52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="I52" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J52" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="L52" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="N52" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="O52" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="P52" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="28">
+        <v>43871</v>
+      </c>
+      <c r="R52" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>555</v>
-      </c>
-      <c r="G51" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>560</v>
-      </c>
-      <c r="I51" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J51" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K51" s="19" t="s">
-        <v>561</v>
-      </c>
-      <c r="L51" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M51" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="N51" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="O51" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="P51" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q51" s="28">
-        <v>43871</v>
-      </c>
-      <c r="R51" s="19" t="s">
-        <v>559</v>
-      </c>
-      <c r="S51" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T51" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U51" s="29"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="S52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U52" s="29"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N52" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="O52" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q52" s="6">
-        <v>41771</v>
-      </c>
-      <c r="R52" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U52" s="7"/>
-    </row>
-    <row r="53" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q53" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S53" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U53" s="7"/>
     </row>
     <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D54" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
@@ -5472,7 +5491,7 @@
         <v>278</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>44</v>
@@ -5481,10 +5500,10 @@
         <v>43788</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T54" s="5" t="s">
         <v>281</v>
@@ -5493,24 +5512,24 @@
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5518,9 +5537,15 @@
       <c r="J55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N55" s="5" t="s">
         <v>278</v>
       </c>
@@ -5537,7 +5562,7 @@
         <v>288</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5546,24 +5571,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5590,7 +5615,7 @@
         <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5599,24 +5624,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5652,24 +5677,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5705,24 +5730,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5758,24 +5783,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5811,24 +5836,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5864,24 +5889,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5917,24 +5942,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -5970,24 +5995,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6023,24 +6048,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6076,24 +6101,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6129,137 +6154,135 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J67" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R67" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U67" s="7"/>
+    </row>
+    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K67" s="5" t="s">
+      <c r="K68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L67" s="5" t="s">
+      <c r="L68" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M67" s="5" t="s">
+      <c r="M68" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N67" s="5" t="s">
+      <c r="N68" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O67" s="5" t="s">
+      <c r="O68" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q67" s="6">
+      <c r="P68" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q68" s="6">
         <v>44111</v>
       </c>
-      <c r="R67" s="5" t="s">
+      <c r="R68" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U67" s="7"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
+      <c r="S68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T68" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U68" s="7"/>
     </row>
-    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
       <c r="O69" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>44</v>
@@ -6267,37 +6290,33 @@
       <c r="Q69" s="6">
         <v>43788</v>
       </c>
-      <c r="R69" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
       <c r="U69" s="7"/>
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D70" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E70" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>216</v>
@@ -6318,7 +6337,7 @@
         <v>359</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6327,7 +6346,7 @@
         <v>43788</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>33</v>
@@ -6339,24 +6358,24 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6377,7 +6396,7 @@
         <v>359</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6386,7 +6405,7 @@
         <v>43788</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>33</v>
@@ -6398,24 +6417,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6457,24 +6476,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6495,7 +6514,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6504,7 +6523,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6514,23 +6533,47 @@
       </c>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
+      <c r="E74" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O74" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>44</v>
@@ -6538,52 +6581,32 @@
       <c r="Q74" s="6">
         <v>43788</v>
       </c>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
+      <c r="R74" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S74" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T74" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M75" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N75" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
       <c r="O75" s="5" t="s">
         <v>65</v>
       </c>
@@ -6593,37 +6616,33 @@
       <c r="Q75" s="6">
         <v>43788</v>
       </c>
-      <c r="R75" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S75" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T75" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
       <c r="U75" s="7"/>
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D76" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E76" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>216</v>
@@ -6656,7 +6675,7 @@
         <v>361</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>281</v>
@@ -6665,24 +6684,24 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6715,7 +6734,7 @@
         <v>361</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>281</v>
@@ -6724,24 +6743,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6783,24 +6802,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6842,24 +6861,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6901,24 +6920,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6960,24 +6979,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7019,24 +7038,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7078,24 +7097,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7137,24 +7156,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7196,24 +7215,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7255,24 +7274,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7313,102 +7332,104 @@
       <c r="U87" s="7"/>
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R88" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T88" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U88" s="7"/>
+    </row>
+    <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B88" s="15"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10"/>
-      <c r="J88" s="10"/>
-      <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10"/>
-      <c r="O88" s="10"/>
-      <c r="P88" s="10"/>
-      <c r="Q88" s="10"/>
-      <c r="R88" s="10"/>
-      <c r="S88" s="10"/>
-      <c r="T88" s="10"/>
-      <c r="U88" s="10"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F89" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K89" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L89" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q89" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R89" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="7"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F90" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>23</v>
@@ -7423,28 +7444,28 @@
         <v>25</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q90" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R90" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
@@ -7452,20 +7473,20 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7480,19 +7501,19 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
@@ -7509,20 +7530,20 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7537,19 +7558,19 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
@@ -7565,54 +7586,88 @@
       <c r="U92" s="7"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93" s="25"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
-      <c r="N93"/>
-      <c r="O93"/>
-      <c r="P93"/>
-      <c r="Q93"/>
-      <c r="R93"/>
-      <c r="S93"/>
-      <c r="T93"/>
-      <c r="U93"/>
+      <c r="A93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F93" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L93" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P93" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q93" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R93" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="7"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-      <c r="I94" s="10"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="10"/>
-      <c r="M94" s="10"/>
-      <c r="N94" s="10"/>
-      <c r="O94" s="10"/>
-      <c r="P94" s="10"/>
-      <c r="Q94" s="12"/>
-      <c r="R94" s="10"/>
-      <c r="S94" s="10"/>
-      <c r="T94" s="10"/>
-      <c r="U94" s="10"/>
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94" s="25"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
+      <c r="R94"/>
+      <c r="S94"/>
+      <c r="T94"/>
+      <c r="U94"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
@@ -7634,17 +7689,17 @@
       <c r="U95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B96" s="10"/>
+      <c r="A96" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
       <c r="I96" s="10"/>
-      <c r="K96" s="10"/>
+      <c r="K96" s="9"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
@@ -7658,7 +7713,7 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -7680,30 +7735,53 @@
       <c r="U97" s="10"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+      <c r="O98" s="10"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10"/>
+      <c r="U98" s="10"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="13"/>
-      <c r="P98" s="13"/>
-      <c r="R98" s="13"/>
-      <c r="S98" s="13"/>
-      <c r="T98" s="13"/>
-      <c r="U98" s="13"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="11" t="s">
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+      <c r="O99" s="13"/>
+      <c r="P99" s="13"/>
+      <c r="R99" s="13"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="13"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A100" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #444 - Source Files in XML Schema file header
Issue #444 - XML Schema files generated by LDDTool should not write the source file names in the header

Remove the following from future XSD file outputs generated by LDDTool

 <!--   file:/path/to/ingest_ldd --> Example: <!--   file:PDS4_DISP_IngestLDD.xml

This type of information is not exactly "archival" :-), and actually a very minor potential IT security concern it could show the absolute path of an online server

Note: This issue was originally associated with Issue #440 - "remaining code cleanup / refactoring" but was fixed separately during some general cleanup.

@c-suh An update to the namespace registry documents (doc) is included. This is a fix for Issue #406 - add new namespace "kplo"

Resolves #444
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FD927-2CA6-428A-8782-0292BF271A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949DBC8B-BE6B-4554-A596-0FB41550860D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5360" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="574">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1729,6 +1729,24 @@
   </si>
   <si>
     <t>LT</t>
+  </si>
+  <si>
+    <t>kplo</t>
+  </si>
+  <si>
+    <t>Namespace for the Korea Pathfinder Lunar Orbiter(KPLO).</t>
+  </si>
+  <si>
+    <t>Korea Pathfinder Lunar Orbiter</t>
+  </si>
+  <si>
+    <t>mission/kplo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eunhyeuk Kim </t>
+  </si>
+  <si>
+    <t>eunhyeuk at kari.re.kr</t>
   </si>
 </sst>
 </file>
@@ -2269,12 +2287,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:U101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD45"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4711,89 +4729,91 @@
       </c>
       <c r="U41" s="29"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="I42" s="5" t="s">
+    <row r="42" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>550</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="I42" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N42" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>42119</v>
-      </c>
-      <c r="R42" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="7"/>
+      <c r="J42" s="19" t="s">
+        <v>551</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="L42" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>553</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="O42" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="P42" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="28">
+        <v>44426</v>
+      </c>
+      <c r="R42" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="S42" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="29"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="5" t="s">
-        <v>237</v>
+      <c r="H43" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>216</v>
@@ -4802,28 +4822,28 @@
         <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>103</v>
+        <v>126</v>
+      </c>
+      <c r="N43" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="O43" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q43" s="6">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>33</v>
@@ -4839,13 +4859,13 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>234</v>
@@ -4894,93 +4914,91 @@
       </c>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>564</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>565</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>566</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="G45" s="27" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>567</v>
-      </c>
-      <c r="I45" s="27" t="s">
+      <c r="H45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="19" t="s">
-        <v>567</v>
-      </c>
-      <c r="L45" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="M45" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="N45" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="O45" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="P45" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q45" s="28">
-        <v>44608</v>
-      </c>
-      <c r="R45" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="S45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="29"/>
+      <c r="K45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="7"/>
     </row>
     <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>518</v>
+        <v>565</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>516</v>
+        <v>562</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>566</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G46" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="G46" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>519</v>
+        <v>567</v>
       </c>
       <c r="I46" s="27" t="s">
         <v>216</v>
@@ -4989,7 +5007,7 @@
         <v>25</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>517</v>
+        <v>567</v>
       </c>
       <c r="L46" s="19" t="s">
         <v>125</v>
@@ -4997,17 +5015,17 @@
       <c r="M46" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N46" s="27" t="s">
+      <c r="N46" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="O46" s="27" t="s">
+      <c r="O46" s="19" t="s">
         <v>194</v>
       </c>
       <c r="P46" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q46" s="28">
-        <v>44333</v>
+        <v>44608</v>
       </c>
       <c r="R46" s="19" t="s">
         <v>196</v>
@@ -5020,89 +5038,91 @@
       </c>
       <c r="U46" s="29"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G47" s="5" t="s">
+    <row r="47" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="G47" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>520</v>
-      </c>
-      <c r="I47" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="I47" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J47" s="5" t="s">
+      <c r="J47" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K47" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L47" s="5" t="s">
+      <c r="K47" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="L47" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="M47" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N47" s="5" t="s">
+      <c r="N47" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="O47" s="5" t="s">
+      <c r="O47" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="P47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R47" s="5" t="s">
+      <c r="P47" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="28">
+        <v>44333</v>
+      </c>
+      <c r="R47" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="S47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="7"/>
+      <c r="S47" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="29"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>244</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5111,28 +5131,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5144,26 +5164,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5172,7 +5192,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>109</v>
@@ -5190,10 +5210,10 @@
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5205,26 +5225,26 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>262</v>
+      <c r="H50" s="19" t="s">
+        <v>522</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5233,28 +5253,28 @@
         <v>25</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q50" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S50" s="5" t="s">
         <v>33</v>
@@ -5270,13 +5290,13 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>259</v>
@@ -5325,211 +5345,213 @@
       </c>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>42158</v>
+      </c>
+      <c r="R52" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U52" s="7"/>
+    </row>
+    <row r="53" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="19" t="s">
         <v>554</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B53" s="19" t="s">
         <v>561</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D53" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E53" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F53" s="19" t="s">
         <v>554</v>
       </c>
-      <c r="G52" s="27" t="s">
+      <c r="G53" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="19" t="s">
+      <c r="H53" s="19" t="s">
         <v>559</v>
       </c>
-      <c r="I52" s="27" t="s">
+      <c r="I53" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J52" s="27" t="s">
+      <c r="J53" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K52" s="19" t="s">
+      <c r="K53" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="L52" s="27" t="s">
+      <c r="L53" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="M52" s="27" t="s">
+      <c r="M53" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="N52" s="27" t="s">
+      <c r="N53" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="O52" s="27" t="s">
+      <c r="O53" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="P52" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q52" s="28">
+      <c r="P53" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q53" s="28">
         <v>43871</v>
       </c>
-      <c r="R52" s="19" t="s">
+      <c r="R53" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="S52" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T52" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U52" s="29"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+      <c r="S53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" s="29"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L53" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N53" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="O53" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="P53" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q53" s="6">
-        <v>41771</v>
-      </c>
-      <c r="R53" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U53" s="7"/>
-    </row>
-    <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q54" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S54" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U54" s="7"/>
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D55" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E55" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5550,7 +5572,7 @@
         <v>278</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
@@ -5559,10 +5581,10 @@
         <v>43788</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5571,24 +5593,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5596,9 +5618,15 @@
       <c r="J56" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
+      <c r="K56" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N56" s="5" t="s">
         <v>278</v>
       </c>
@@ -5615,7 +5643,7 @@
         <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5624,24 +5652,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5668,7 +5696,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5677,24 +5705,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5730,24 +5758,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5783,24 +5811,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5836,24 +5864,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5889,24 +5917,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5942,24 +5970,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -5995,24 +6023,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6048,24 +6076,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6101,24 +6129,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6154,24 +6182,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6207,137 +6235,135 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J68" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O68" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P68" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q68" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R68" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S68" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T68" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U68" s="7"/>
+    </row>
+    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K68" s="5" t="s">
+      <c r="K69" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L68" s="5" t="s">
+      <c r="L69" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M68" s="5" t="s">
+      <c r="M69" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N68" s="5" t="s">
+      <c r="N69" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O68" s="5" t="s">
+      <c r="O69" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q68" s="6">
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
         <v>44111</v>
       </c>
-      <c r="R68" s="5" t="s">
+      <c r="R69" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U68" s="7"/>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
+      <c r="S69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U69" s="7"/>
     </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
       <c r="O70" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6345,37 +6371,33 @@
       <c r="Q70" s="6">
         <v>43788</v>
       </c>
-      <c r="R70" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
       <c r="U70" s="7"/>
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D71" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E71" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6396,7 +6418,7 @@
         <v>359</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6405,7 +6427,7 @@
         <v>43788</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>33</v>
@@ -6417,24 +6439,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6455,7 +6477,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6464,7 +6486,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6476,24 +6498,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6535,24 +6557,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6573,7 +6595,7 @@
         <v>359</v>
       </c>
       <c r="O74" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>44</v>
@@ -6582,7 +6604,7 @@
         <v>43788</v>
       </c>
       <c r="R74" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S74" s="5" t="s">
         <v>33</v>
@@ -6592,23 +6614,47 @@
       </c>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
+    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
+      <c r="E75" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L75" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M75" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N75" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O75" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6616,52 +6662,32 @@
       <c r="Q75" s="6">
         <v>43788</v>
       </c>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
+      <c r="R75" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S75" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T75" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
       <c r="O76" s="5" t="s">
         <v>65</v>
       </c>
@@ -6671,37 +6697,33 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S76" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T76" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
       <c r="U76" s="7"/>
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D77" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E77" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6734,7 +6756,7 @@
         <v>361</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>281</v>
@@ -6743,24 +6765,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6793,7 +6815,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6802,24 +6824,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6861,24 +6883,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6920,24 +6942,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6979,24 +7001,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7038,24 +7060,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7097,24 +7119,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7156,24 +7178,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7215,24 +7237,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7274,24 +7296,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7333,24 +7355,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7391,102 +7413,104 @@
       <c r="U88" s="7"/>
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N89" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O89" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P89" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q89" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R89" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S89" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T89" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U89" s="7"/>
+    </row>
+    <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B89" s="15"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-      <c r="I89" s="10"/>
-      <c r="J89" s="10"/>
-      <c r="K89" s="10"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="10"/>
-      <c r="Q89" s="10"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="10"/>
-      <c r="T89" s="10"/>
-      <c r="U89" s="10"/>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F90" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P90" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q90" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R90" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S90" s="5"/>
-      <c r="T90" s="5"/>
-      <c r="U90" s="7"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7501,28 +7525,28 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q91" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R91" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
@@ -7530,20 +7554,20 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7558,19 +7582,19 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
@@ -7587,20 +7611,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7615,19 +7639,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7643,54 +7667,88 @@
       <c r="U93" s="7"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94"/>
-      <c r="E94" s="25"/>
-      <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94"/>
-      <c r="I94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94"/>
-      <c r="M94"/>
-      <c r="N94"/>
-      <c r="O94"/>
-      <c r="P94"/>
-      <c r="Q94"/>
-      <c r="R94"/>
-      <c r="S94"/>
-      <c r="T94"/>
-      <c r="U94"/>
+      <c r="A94" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F94" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L94" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M94" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N94" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O94" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q94" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R94" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="7"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
-      <c r="H95" s="10"/>
-      <c r="I95" s="10"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="10"/>
-      <c r="M95" s="10"/>
-      <c r="N95" s="10"/>
-      <c r="O95" s="10"/>
-      <c r="P95" s="10"/>
-      <c r="Q95" s="12"/>
-      <c r="R95" s="10"/>
-      <c r="S95" s="10"/>
-      <c r="T95" s="10"/>
-      <c r="U95" s="10"/>
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95" s="25"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+      <c r="N95"/>
+      <c r="O95"/>
+      <c r="P95"/>
+      <c r="Q95"/>
+      <c r="R95"/>
+      <c r="S95"/>
+      <c r="T95"/>
+      <c r="U95"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
@@ -7712,17 +7770,17 @@
       <c r="U96" s="10"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B97" s="10"/>
+      <c r="A97" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
       <c r="H97" s="10"/>
       <c r="I97" s="10"/>
-      <c r="K97" s="10"/>
+      <c r="K97" s="9"/>
       <c r="L97" s="10"/>
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
@@ -7736,7 +7794,7 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -7758,30 +7816,53 @@
       <c r="U98" s="10"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="13" t="s">
+      <c r="A99" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
+      <c r="M99" s="10"/>
+      <c r="N99" s="10"/>
+      <c r="O99" s="10"/>
+      <c r="P99" s="10"/>
+      <c r="Q99" s="12"/>
+      <c r="R99" s="10"/>
+      <c r="S99" s="10"/>
+      <c r="T99" s="10"/>
+      <c r="U99" s="10"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13"/>
-      <c r="K99" s="13"/>
-      <c r="L99" s="13"/>
-      <c r="M99" s="13"/>
-      <c r="N99" s="13"/>
-      <c r="O99" s="13"/>
-      <c r="P99" s="13"/>
-      <c r="R99" s="13"/>
-      <c r="S99" s="13"/>
-      <c r="T99" s="13"/>
-      <c r="U99" s="13"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100" s="11" t="s">
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="13"/>
+      <c r="N100" s="13"/>
+      <c r="O100" s="13"/>
+      <c r="P100" s="13"/>
+      <c r="R100" s="13"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="13"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A101" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #444 - Source Files in XML Schema file header (#445)
Issue #444 - XML Schema files generated by LDDTool should not write the source file names in the header

Remove the following from future XSD file outputs generated by LDDTool

 <!--   file:/path/to/ingest_ldd --> Example: <!--   file:PDS4_DISP_IngestLDD.xml

This type of information is not exactly "archival" :-), and actually a very minor potential IT security concern it could show the absolute path of an online server

Note: This issue was originally associated with Issue #440 - "remaining code cleanup / refactoring" but was fixed separately during some general cleanup.

@c-suh An update to the namespace registry documents (doc) is included. This is a fix for Issue #406 - add new namespace "kplo"

Resolves #444

Co-authored-by: John Hughes <John.S.Hughes@jpl.nasa.gov>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FD927-2CA6-428A-8782-0292BF271A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949DBC8B-BE6B-4554-A596-0FB41550860D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5360" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="574">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1729,6 +1729,24 @@
   </si>
   <si>
     <t>LT</t>
+  </si>
+  <si>
+    <t>kplo</t>
+  </si>
+  <si>
+    <t>Namespace for the Korea Pathfinder Lunar Orbiter(KPLO).</t>
+  </si>
+  <si>
+    <t>Korea Pathfinder Lunar Orbiter</t>
+  </si>
+  <si>
+    <t>mission/kplo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eunhyeuk Kim </t>
+  </si>
+  <si>
+    <t>eunhyeuk at kari.re.kr</t>
   </si>
 </sst>
 </file>
@@ -2269,12 +2287,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:U101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD45"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4711,89 +4729,91 @@
       </c>
       <c r="U41" s="29"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="I42" s="5" t="s">
+    <row r="42" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>550</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="I42" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N42" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>42119</v>
-      </c>
-      <c r="R42" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="7"/>
+      <c r="J42" s="19" t="s">
+        <v>551</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="L42" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>553</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="O42" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="P42" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="28">
+        <v>44426</v>
+      </c>
+      <c r="R42" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="S42" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="29"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="5" t="s">
-        <v>237</v>
+      <c r="H43" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>216</v>
@@ -4802,28 +4822,28 @@
         <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>103</v>
+        <v>126</v>
+      </c>
+      <c r="N43" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="O43" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q43" s="6">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>33</v>
@@ -4839,13 +4859,13 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>234</v>
@@ -4894,93 +4914,91 @@
       </c>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>564</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>565</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>566</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="G45" s="27" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>567</v>
-      </c>
-      <c r="I45" s="27" t="s">
+      <c r="H45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="19" t="s">
-        <v>567</v>
-      </c>
-      <c r="L45" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="M45" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="N45" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="O45" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="P45" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q45" s="28">
-        <v>44608</v>
-      </c>
-      <c r="R45" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="S45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="29"/>
+      <c r="K45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>41837</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="7"/>
     </row>
     <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>518</v>
+        <v>565</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>516</v>
+        <v>562</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>566</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G46" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="G46" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>519</v>
+        <v>567</v>
       </c>
       <c r="I46" s="27" t="s">
         <v>216</v>
@@ -4989,7 +5007,7 @@
         <v>25</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>517</v>
+        <v>567</v>
       </c>
       <c r="L46" s="19" t="s">
         <v>125</v>
@@ -4997,17 +5015,17 @@
       <c r="M46" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N46" s="27" t="s">
+      <c r="N46" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="O46" s="27" t="s">
+      <c r="O46" s="19" t="s">
         <v>194</v>
       </c>
       <c r="P46" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q46" s="28">
-        <v>44333</v>
+        <v>44608</v>
       </c>
       <c r="R46" s="19" t="s">
         <v>196</v>
@@ -5020,89 +5038,91 @@
       </c>
       <c r="U46" s="29"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G47" s="5" t="s">
+    <row r="47" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="G47" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>520</v>
-      </c>
-      <c r="I47" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="I47" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J47" s="5" t="s">
+      <c r="J47" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K47" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="L47" s="5" t="s">
+      <c r="K47" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="L47" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="M47" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N47" s="5" t="s">
+      <c r="N47" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="O47" s="5" t="s">
+      <c r="O47" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="P47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>43935</v>
-      </c>
-      <c r="R47" s="5" t="s">
+      <c r="P47" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="28">
+        <v>44333</v>
+      </c>
+      <c r="R47" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="S47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="7"/>
+      <c r="S47" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="29"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>244</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5111,28 +5131,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5144,26 +5164,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5172,7 +5192,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>109</v>
@@ -5190,10 +5210,10 @@
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5205,26 +5225,26 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>262</v>
+      <c r="H50" s="19" t="s">
+        <v>522</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5233,28 +5253,28 @@
         <v>25</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q50" s="6">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="S50" s="5" t="s">
         <v>33</v>
@@ -5270,13 +5290,13 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>259</v>
@@ -5325,211 +5345,213 @@
       </c>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>42158</v>
+      </c>
+      <c r="R52" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U52" s="7"/>
+    </row>
+    <row r="53" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="19" t="s">
         <v>554</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B53" s="19" t="s">
         <v>561</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D53" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E53" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F53" s="19" t="s">
         <v>554</v>
       </c>
-      <c r="G52" s="27" t="s">
+      <c r="G53" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="19" t="s">
+      <c r="H53" s="19" t="s">
         <v>559</v>
       </c>
-      <c r="I52" s="27" t="s">
+      <c r="I53" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J52" s="27" t="s">
+      <c r="J53" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K52" s="19" t="s">
+      <c r="K53" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="L52" s="27" t="s">
+      <c r="L53" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="M52" s="27" t="s">
+      <c r="M53" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="N52" s="27" t="s">
+      <c r="N53" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="O52" s="27" t="s">
+      <c r="O53" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="P52" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q52" s="28">
+      <c r="P53" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q53" s="28">
         <v>43871</v>
       </c>
-      <c r="R52" s="19" t="s">
+      <c r="R53" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="S52" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T52" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U52" s="29"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+      <c r="S53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" s="29"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L53" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N53" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="O53" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="P53" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q53" s="6">
-        <v>41771</v>
-      </c>
-      <c r="R53" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U53" s="7"/>
-    </row>
-    <row r="54" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q54" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S54" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U54" s="7"/>
     </row>
     <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D55" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E55" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
@@ -5550,7 +5572,7 @@
         <v>278</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
@@ -5559,10 +5581,10 @@
         <v>43788</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
         <v>281</v>
@@ -5571,24 +5593,24 @@
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5596,9 +5618,15 @@
       <c r="J56" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
+      <c r="K56" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N56" s="5" t="s">
         <v>278</v>
       </c>
@@ -5615,7 +5643,7 @@
         <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5624,24 +5652,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5668,7 +5696,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5677,24 +5705,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5730,24 +5758,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5783,24 +5811,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5836,24 +5864,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5889,24 +5917,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5942,24 +5970,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -5995,24 +6023,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6048,24 +6076,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6101,24 +6129,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6154,24 +6182,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6207,137 +6235,135 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J68" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O68" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P68" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q68" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R68" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S68" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T68" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U68" s="7"/>
+    </row>
+    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K68" s="5" t="s">
+      <c r="K69" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L68" s="5" t="s">
+      <c r="L69" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M68" s="5" t="s">
+      <c r="M69" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N68" s="5" t="s">
+      <c r="N69" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O68" s="5" t="s">
+      <c r="O69" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P68" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q68" s="6">
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
         <v>44111</v>
       </c>
-      <c r="R68" s="5" t="s">
+      <c r="R69" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U68" s="7"/>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
+      <c r="S69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U69" s="7"/>
     </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
       <c r="O70" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>44</v>
@@ -6345,37 +6371,33 @@
       <c r="Q70" s="6">
         <v>43788</v>
       </c>
-      <c r="R70" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
       <c r="U70" s="7"/>
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D71" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E71" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>216</v>
@@ -6396,7 +6418,7 @@
         <v>359</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6405,7 +6427,7 @@
         <v>43788</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>33</v>
@@ -6417,24 +6439,24 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6455,7 +6477,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6464,7 +6486,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6476,24 +6498,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6535,24 +6557,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6573,7 +6595,7 @@
         <v>359</v>
       </c>
       <c r="O74" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P74" s="5" t="s">
         <v>44</v>
@@ -6582,7 +6604,7 @@
         <v>43788</v>
       </c>
       <c r="R74" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S74" s="5" t="s">
         <v>33</v>
@@ -6592,23 +6614,47 @@
       </c>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
+    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
+      <c r="E75" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L75" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M75" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N75" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O75" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6616,52 +6662,32 @@
       <c r="Q75" s="6">
         <v>43788</v>
       </c>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
+      <c r="R75" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S75" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T75" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
       <c r="O76" s="5" t="s">
         <v>65</v>
       </c>
@@ -6671,37 +6697,33 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S76" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T76" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
       <c r="U76" s="7"/>
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D77" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E77" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>216</v>
@@ -6734,7 +6756,7 @@
         <v>361</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>281</v>
@@ -6743,24 +6765,24 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6793,7 +6815,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6802,24 +6824,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6861,24 +6883,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6920,24 +6942,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -6979,24 +7001,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7038,24 +7060,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7097,24 +7119,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7156,24 +7178,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7215,24 +7237,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7274,24 +7296,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7333,24 +7355,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7391,102 +7413,104 @@
       <c r="U88" s="7"/>
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N89" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O89" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P89" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q89" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R89" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S89" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T89" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U89" s="7"/>
+    </row>
+    <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B89" s="15"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-      <c r="I89" s="10"/>
-      <c r="J89" s="10"/>
-      <c r="K89" s="10"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="10"/>
-      <c r="Q89" s="10"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="10"/>
-      <c r="T89" s="10"/>
-      <c r="U89" s="10"/>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F90" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P90" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q90" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R90" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S90" s="5"/>
-      <c r="T90" s="5"/>
-      <c r="U90" s="7"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>23</v>
@@ -7501,28 +7525,28 @@
         <v>25</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q91" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R91" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
@@ -7530,20 +7554,20 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7558,19 +7582,19 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
@@ -7587,20 +7611,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7615,19 +7639,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7643,54 +7667,88 @@
       <c r="U93" s="7"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94"/>
-      <c r="E94" s="25"/>
-      <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94"/>
-      <c r="I94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94"/>
-      <c r="M94"/>
-      <c r="N94"/>
-      <c r="O94"/>
-      <c r="P94"/>
-      <c r="Q94"/>
-      <c r="R94"/>
-      <c r="S94"/>
-      <c r="T94"/>
-      <c r="U94"/>
+      <c r="A94" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F94" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L94" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M94" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N94" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O94" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q94" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R94" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="7"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
-      <c r="H95" s="10"/>
-      <c r="I95" s="10"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="10"/>
-      <c r="M95" s="10"/>
-      <c r="N95" s="10"/>
-      <c r="O95" s="10"/>
-      <c r="P95" s="10"/>
-      <c r="Q95" s="12"/>
-      <c r="R95" s="10"/>
-      <c r="S95" s="10"/>
-      <c r="T95" s="10"/>
-      <c r="U95" s="10"/>
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95" s="25"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+      <c r="N95"/>
+      <c r="O95"/>
+      <c r="P95"/>
+      <c r="Q95"/>
+      <c r="R95"/>
+      <c r="S95"/>
+      <c r="T95"/>
+      <c r="U95"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
@@ -7712,17 +7770,17 @@
       <c r="U96" s="10"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B97" s="10"/>
+      <c r="A97" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
       <c r="H97" s="10"/>
       <c r="I97" s="10"/>
-      <c r="K97" s="10"/>
+      <c r="K97" s="9"/>
       <c r="L97" s="10"/>
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
@@ -7736,7 +7794,7 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -7758,30 +7816,53 @@
       <c r="U98" s="10"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="13" t="s">
+      <c r="A99" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
+      <c r="M99" s="10"/>
+      <c r="N99" s="10"/>
+      <c r="O99" s="10"/>
+      <c r="P99" s="10"/>
+      <c r="Q99" s="12"/>
+      <c r="R99" s="10"/>
+      <c r="S99" s="10"/>
+      <c r="T99" s="10"/>
+      <c r="U99" s="10"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13"/>
-      <c r="K99" s="13"/>
-      <c r="L99" s="13"/>
-      <c r="M99" s="13"/>
-      <c r="N99" s="13"/>
-      <c r="O99" s="13"/>
-      <c r="P99" s="13"/>
-      <c r="R99" s="13"/>
-      <c r="S99" s="13"/>
-      <c r="T99" s="13"/>
-      <c r="U99" s="13"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100" s="11" t="s">
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="13"/>
+      <c r="N100" s="13"/>
+      <c r="O100" s="13"/>
+      <c r="P100" s="13"/>
+      <c r="R100" s="13"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="13"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A101" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #240 : Namespace - add "nh"
Add the namespaces "nh" to the Namespace Registry and the config.properties file.
nh - New Horizons Primary and Extended Missions

@c-suh  [namespace-registry] add new namespace "nh" #240

Resolves #240
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949DBC8B-BE6B-4554-A596-0FB41550860D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F984C-4CFF-451B-90D9-549AD784B9E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="583">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1747,6 +1747,33 @@
   </si>
   <si>
     <t>eunhyeuk at kari.re.kr</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>mission/nh</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/nh/v1</t>
+  </si>
+  <si>
+    <t>Adeline Gicquel</t>
+  </si>
+  <si>
+    <t>agicquel at umd.edu</t>
+  </si>
+  <si>
+    <t>PDS4_NH</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>Namespace for the New Horizons Primary and Extended Missions dictionary.</t>
+  </si>
+  <si>
+    <t>New Horizons Primary and Extended Missions</t>
   </si>
 </sst>
 </file>
@@ -2287,12 +2314,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5469,148 +5496,152 @@
       </c>
       <c r="U53" s="29"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>575</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>576</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="I54" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J54" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="19" t="s">
+        <v>580</v>
+      </c>
+      <c r="L54" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M54" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="N54" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="O54" s="19" t="s">
+        <v>578</v>
+      </c>
+      <c r="P54" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q54" s="28">
+        <v>44643</v>
+      </c>
+      <c r="R54" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U54" s="29"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N54" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="O54" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="P54" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q54" s="6">
-        <v>41771</v>
-      </c>
-      <c r="R54" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U54" s="7"/>
-    </row>
-    <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q55" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S55" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U55" s="7"/>
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D56" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E56" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5631,7 +5662,7 @@
         <v>278</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>44</v>
@@ -5640,10 +5671,10 @@
         <v>43788</v>
       </c>
       <c r="R56" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5652,24 +5683,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5677,9 +5708,15 @@
       <c r="J57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
+      <c r="K57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N57" s="5" t="s">
         <v>278</v>
       </c>
@@ -5696,7 +5733,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5705,24 +5742,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5749,7 +5786,7 @@
         <v>288</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T58" s="5" t="s">
         <v>281</v>
@@ -5758,24 +5795,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5811,24 +5848,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5864,24 +5901,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5917,24 +5954,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5970,24 +6007,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6023,24 +6060,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6076,24 +6113,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6129,24 +6166,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6182,24 +6219,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6235,24 +6272,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6288,137 +6325,135 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D69" s="5"/>
       <c r="E69" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J69" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R69" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U69" s="7"/>
+    </row>
+    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J70" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="K70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L69" s="5" t="s">
+      <c r="L70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M69" s="5" t="s">
+      <c r="M70" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N69" s="5" t="s">
+      <c r="N70" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O69" s="5" t="s">
+      <c r="O70" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
+      <c r="P70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q70" s="6">
         <v>44111</v>
       </c>
-      <c r="R69" s="5" t="s">
+      <c r="R70" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U69" s="7"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
+      <c r="S70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T70" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U70" s="7"/>
     </row>
-    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6426,37 +6461,33 @@
       <c r="Q71" s="6">
         <v>43788</v>
       </c>
-      <c r="R71" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S71" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T71" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
       <c r="U71" s="7"/>
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D72" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E72" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6477,7 +6508,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6486,7 +6517,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6498,24 +6529,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6536,7 +6567,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6545,7 +6576,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6557,24 +6588,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6616,24 +6647,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6654,7 +6685,7 @@
         <v>359</v>
       </c>
       <c r="O75" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6663,7 +6694,7 @@
         <v>43788</v>
       </c>
       <c r="R75" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S75" s="5" t="s">
         <v>33</v>
@@ -6673,23 +6704,47 @@
       </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
+    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
+      <c r="E76" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O76" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>44</v>
@@ -6697,52 +6752,32 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
+      <c r="R76" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T76" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U76" s="7"/>
     </row>
-    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A77" s="5"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N77" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
       <c r="O77" s="5" t="s">
         <v>65</v>
       </c>
@@ -6752,37 +6787,33 @@
       <c r="Q77" s="6">
         <v>43788</v>
       </c>
-      <c r="R77" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S77" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T77" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
       <c r="U77" s="7"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D78" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E78" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6815,7 +6846,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6824,24 +6855,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6874,7 +6905,7 @@
         <v>361</v>
       </c>
       <c r="S79" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>281</v>
@@ -6883,24 +6914,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6942,24 +6973,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -7001,24 +7032,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7060,24 +7091,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7119,24 +7150,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7178,24 +7209,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7237,24 +7268,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7296,24 +7327,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7355,24 +7386,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7414,24 +7445,24 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>216</v>
@@ -7472,102 +7503,104 @@
       <c r="U89" s="7"/>
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O90" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P90" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q90" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R90" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U90" s="7"/>
+    </row>
+    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-      <c r="I90" s="10"/>
-      <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10"/>
-      <c r="O90" s="10"/>
-      <c r="P90" s="10"/>
-      <c r="Q90" s="10"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="10"/>
-      <c r="T90" s="10"/>
-      <c r="U90" s="10"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F91" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L91" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N91" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P91" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q91" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R91" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S91" s="5"/>
-      <c r="T91" s="5"/>
-      <c r="U91" s="7"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
+      <c r="U91" s="10"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7582,28 +7615,28 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q92" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R92" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
@@ -7611,20 +7644,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7639,19 +7672,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7668,20 +7701,20 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>23</v>
@@ -7696,19 +7729,19 @@
         <v>25</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O94" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>44</v>
@@ -7724,54 +7757,88 @@
       <c r="U94" s="7"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="D95"/>
-      <c r="E95" s="25"/>
-      <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95"/>
-      <c r="I95"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95"/>
-      <c r="M95"/>
-      <c r="N95"/>
-      <c r="O95"/>
-      <c r="P95"/>
-      <c r="Q95"/>
-      <c r="R95"/>
-      <c r="S95"/>
-      <c r="T95"/>
-      <c r="U95"/>
+      <c r="A95" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F95" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N95" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O95" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P95" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q95" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R95" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="7"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B96" s="9"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
-      <c r="H96" s="10"/>
-      <c r="I96" s="10"/>
-      <c r="K96" s="9"/>
-      <c r="L96" s="10"/>
-      <c r="M96" s="10"/>
-      <c r="N96" s="10"/>
-      <c r="O96" s="10"/>
-      <c r="P96" s="10"/>
-      <c r="Q96" s="12"/>
-      <c r="R96" s="10"/>
-      <c r="S96" s="10"/>
-      <c r="T96" s="10"/>
-      <c r="U96" s="10"/>
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96" s="25"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
+      <c r="N96"/>
+      <c r="O96"/>
+      <c r="P96"/>
+      <c r="Q96"/>
+      <c r="R96"/>
+      <c r="S96"/>
+      <c r="T96"/>
+      <c r="U96"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
@@ -7793,17 +7860,17 @@
       <c r="U97" s="10"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B98" s="10"/>
+      <c r="A98" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
       <c r="I98" s="10"/>
-      <c r="K98" s="10"/>
+      <c r="K98" s="9"/>
       <c r="L98" s="10"/>
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
@@ -7817,7 +7884,7 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -7839,30 +7906,53 @@
       <c r="U99" s="10"/>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="K100" s="10"/>
+      <c r="L100" s="10"/>
+      <c r="M100" s="10"/>
+      <c r="N100" s="10"/>
+      <c r="O100" s="10"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="12"/>
+      <c r="R100" s="10"/>
+      <c r="S100" s="10"/>
+      <c r="T100" s="10"/>
+      <c r="U100" s="10"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A101" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-      <c r="K100" s="13"/>
-      <c r="L100" s="13"/>
-      <c r="M100" s="13"/>
-      <c r="N100" s="13"/>
-      <c r="O100" s="13"/>
-      <c r="P100" s="13"/>
-      <c r="R100" s="13"/>
-      <c r="S100" s="13"/>
-      <c r="T100" s="13"/>
-      <c r="U100" s="13"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="11" t="s">
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="13"/>
+      <c r="M101" s="13"/>
+      <c r="N101" s="13"/>
+      <c r="O101" s="13"/>
+      <c r="P101" s="13"/>
+      <c r="R101" s="13"/>
+      <c r="S101" s="13"/>
+      <c r="T101" s="13"/>
+      <c r="U101" s="13"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A102" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #240 : Namespace - add "nh" (#456)
Add the namespaces "nh" to the Namespace Registry and the config.properties file.
nh - New Horizons Primary and Extended Missions

@c-suh  [namespace-registry] add new namespace "nh" #240

Resolves #240

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949DBC8B-BE6B-4554-A596-0FB41550860D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F984C-4CFF-451B-90D9-549AD784B9E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="583">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1747,6 +1747,33 @@
   </si>
   <si>
     <t>eunhyeuk at kari.re.kr</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>mission/nh</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/nh/v1</t>
+  </si>
+  <si>
+    <t>Adeline Gicquel</t>
+  </si>
+  <si>
+    <t>agicquel at umd.edu</t>
+  </si>
+  <si>
+    <t>PDS4_NH</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>Namespace for the New Horizons Primary and Extended Missions dictionary.</t>
+  </si>
+  <si>
+    <t>New Horizons Primary and Extended Missions</t>
   </si>
 </sst>
 </file>
@@ -2287,12 +2314,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5469,148 +5496,152 @@
       </c>
       <c r="U53" s="29"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>575</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>576</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="I54" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J54" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="19" t="s">
+        <v>580</v>
+      </c>
+      <c r="L54" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M54" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="N54" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="O54" s="19" t="s">
+        <v>578</v>
+      </c>
+      <c r="P54" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q54" s="28">
+        <v>44643</v>
+      </c>
+      <c r="R54" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U54" s="29"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N54" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="O54" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="P54" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q54" s="6">
-        <v>41771</v>
-      </c>
-      <c r="R54" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="S54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U54" s="7"/>
-    </row>
-    <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q55" s="6">
-        <v>43788</v>
+        <v>41771</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="S55" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U55" s="7"/>
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D56" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E56" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5631,7 +5662,7 @@
         <v>278</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>44</v>
@@ -5640,10 +5671,10 @@
         <v>43788</v>
       </c>
       <c r="R56" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5652,24 +5683,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5677,9 +5708,15 @@
       <c r="J57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
+      <c r="K57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N57" s="5" t="s">
         <v>278</v>
       </c>
@@ -5696,7 +5733,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5705,24 +5742,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5749,7 +5786,7 @@
         <v>288</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T58" s="5" t="s">
         <v>281</v>
@@ -5758,24 +5795,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5811,24 +5848,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5864,24 +5901,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5917,24 +5954,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5970,24 +6007,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6023,24 +6060,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6076,24 +6113,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6129,24 +6166,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6182,24 +6219,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6235,24 +6272,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6288,137 +6325,135 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D69" s="5"/>
       <c r="E69" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J69" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R69" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U69" s="7"/>
+    </row>
+    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J70" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="K70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L69" s="5" t="s">
+      <c r="L70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M69" s="5" t="s">
+      <c r="M70" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N69" s="5" t="s">
+      <c r="N70" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O69" s="5" t="s">
+      <c r="O70" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
+      <c r="P70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q70" s="6">
         <v>44111</v>
       </c>
-      <c r="R69" s="5" t="s">
+      <c r="R70" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U69" s="7"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
+      <c r="S70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T70" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U70" s="7"/>
     </row>
-    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6426,37 +6461,33 @@
       <c r="Q71" s="6">
         <v>43788</v>
       </c>
-      <c r="R71" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S71" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T71" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
       <c r="U71" s="7"/>
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D72" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E72" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6477,7 +6508,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6486,7 +6517,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6498,24 +6529,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6536,7 +6567,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6545,7 +6576,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6557,24 +6588,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6616,24 +6647,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6654,7 +6685,7 @@
         <v>359</v>
       </c>
       <c r="O75" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6663,7 +6694,7 @@
         <v>43788</v>
       </c>
       <c r="R75" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S75" s="5" t="s">
         <v>33</v>
@@ -6673,23 +6704,47 @@
       </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
+    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
+      <c r="E76" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O76" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>44</v>
@@ -6697,52 +6752,32 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
+      <c r="R76" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T76" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U76" s="7"/>
     </row>
-    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A77" s="5"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N77" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
       <c r="O77" s="5" t="s">
         <v>65</v>
       </c>
@@ -6752,37 +6787,33 @@
       <c r="Q77" s="6">
         <v>43788</v>
       </c>
-      <c r="R77" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S77" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T77" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
       <c r="U77" s="7"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D78" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E78" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6815,7 +6846,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6824,24 +6855,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6874,7 +6905,7 @@
         <v>361</v>
       </c>
       <c r="S79" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>281</v>
@@ -6883,24 +6914,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6942,24 +6973,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -7001,24 +7032,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7060,24 +7091,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7119,24 +7150,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7178,24 +7209,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7237,24 +7268,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7296,24 +7327,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7355,24 +7386,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7414,24 +7445,24 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>216</v>
@@ -7472,102 +7503,104 @@
       <c r="U89" s="7"/>
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O90" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P90" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q90" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R90" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U90" s="7"/>
+    </row>
+    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-      <c r="I90" s="10"/>
-      <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10"/>
-      <c r="O90" s="10"/>
-      <c r="P90" s="10"/>
-      <c r="Q90" s="10"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="10"/>
-      <c r="T90" s="10"/>
-      <c r="U90" s="10"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F91" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L91" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N91" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P91" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q91" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R91" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S91" s="5"/>
-      <c r="T91" s="5"/>
-      <c r="U91" s="7"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
+      <c r="U91" s="10"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7582,28 +7615,28 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q92" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R92" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
@@ -7611,20 +7644,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7639,19 +7672,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7668,20 +7701,20 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>23</v>
@@ -7696,19 +7729,19 @@
         <v>25</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O94" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>44</v>
@@ -7724,54 +7757,88 @@
       <c r="U94" s="7"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="D95"/>
-      <c r="E95" s="25"/>
-      <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95"/>
-      <c r="I95"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95"/>
-      <c r="M95"/>
-      <c r="N95"/>
-      <c r="O95"/>
-      <c r="P95"/>
-      <c r="Q95"/>
-      <c r="R95"/>
-      <c r="S95"/>
-      <c r="T95"/>
-      <c r="U95"/>
+      <c r="A95" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F95" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N95" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O95" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P95" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q95" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R95" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="7"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B96" s="9"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
-      <c r="H96" s="10"/>
-      <c r="I96" s="10"/>
-      <c r="K96" s="9"/>
-      <c r="L96" s="10"/>
-      <c r="M96" s="10"/>
-      <c r="N96" s="10"/>
-      <c r="O96" s="10"/>
-      <c r="P96" s="10"/>
-      <c r="Q96" s="12"/>
-      <c r="R96" s="10"/>
-      <c r="S96" s="10"/>
-      <c r="T96" s="10"/>
-      <c r="U96" s="10"/>
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96" s="25"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
+      <c r="N96"/>
+      <c r="O96"/>
+      <c r="P96"/>
+      <c r="Q96"/>
+      <c r="R96"/>
+      <c r="S96"/>
+      <c r="T96"/>
+      <c r="U96"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
@@ -7793,17 +7860,17 @@
       <c r="U97" s="10"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B98" s="10"/>
+      <c r="A98" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
       <c r="I98" s="10"/>
-      <c r="K98" s="10"/>
+      <c r="K98" s="9"/>
       <c r="L98" s="10"/>
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
@@ -7817,7 +7884,7 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -7839,30 +7906,53 @@
       <c r="U99" s="10"/>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="K100" s="10"/>
+      <c r="L100" s="10"/>
+      <c r="M100" s="10"/>
+      <c r="N100" s="10"/>
+      <c r="O100" s="10"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="12"/>
+      <c r="R100" s="10"/>
+      <c r="S100" s="10"/>
+      <c r="T100" s="10"/>
+      <c r="U100" s="10"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A101" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-      <c r="K100" s="13"/>
-      <c r="L100" s="13"/>
-      <c r="M100" s="13"/>
-      <c r="N100" s="13"/>
-      <c r="O100" s="13"/>
-      <c r="P100" s="13"/>
-      <c r="R100" s="13"/>
-      <c r="S100" s="13"/>
-      <c r="T100" s="13"/>
-      <c r="U100" s="13"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="11" t="s">
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="13"/>
+      <c r="M101" s="13"/>
+      <c r="N101" s="13"/>
+      <c r="O101" s="13"/>
+      <c r="P101" s="13"/>
+      <c r="R101" s="13"/>
+      <c r="S101" s="13"/>
+      <c r="T101" s="13"/>
+      <c r="U101" s="13"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A102" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #460 : [ldd-request] Move the existing "wave" namespace
Issue #460 : [ldd-request] Move the existing "wave" namespace

Move the existing "wave" namespace from "Mission" to "Held for Future Use".

This update only affects the namespace registry. The config.properties files is not affected since the "wave" namespace entry needs to remain for backwards compatibility.

@c-suh  [namespace-registry] add new namespace "wave" #460

Resolves #460
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F984C-4CFF-451B-90D9-549AD784B9E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FDDD09-64F5-4336-99C7-2AC5FCC278E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="583">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -2317,9 +2317,9 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4357,146 +4357,146 @@
       </c>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="G35" s="5" t="s">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="H36" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K35" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q35" s="6">
-        <v>42118</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="S35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>217</v>
+      <c r="K36" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>42089</v>
+      </c>
+      <c r="R36" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>495</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I37" s="5" t="s">
+      <c r="H37" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>216</v>
       </c>
       <c r="J37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>221</v>
+      <c r="K37" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>180</v>
+        <v>110</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>181</v>
+        <v>112</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q37" s="6">
-        <v>42089</v>
+        <v>44329</v>
       </c>
       <c r="R37" s="16" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="S37" s="5" t="s">
         <v>33</v>
@@ -4506,30 +4506,30 @@
       </c>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>496</v>
+        <v>525</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>498</v>
+        <v>526</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>497</v>
+        <v>525</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>527</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>216</v>
@@ -4556,7 +4556,7 @@
         <v>44</v>
       </c>
       <c r="Q38" s="6">
-        <v>44329</v>
+        <v>44385</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>111</v>
@@ -4569,123 +4569,121 @@
       </c>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>527</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="G39" s="5" t="s">
+    <row r="39" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="G39" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="16" t="s">
-        <v>528</v>
-      </c>
-      <c r="I39" s="16" t="s">
+      <c r="H39" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="I39" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K39" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L39" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="M39" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N39" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="P39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>44385</v>
-      </c>
-      <c r="R39" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="S39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U39" s="7"/>
-    </row>
-    <row r="40" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>542</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>538</v>
+      <c r="K39" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="L39" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="M39" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="O39" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="P39" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q39" s="28">
+        <v>44426</v>
+      </c>
+      <c r="R39" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S39" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T39" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U39" s="29"/>
+    </row>
+    <row r="40" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>224</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>539</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>540</v>
-      </c>
-      <c r="I40" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="I40" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J40" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K40" s="19" t="s">
-        <v>541</v>
+      <c r="J40" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="27" t="s">
+        <v>226</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M40" s="19" t="s">
-        <v>179</v>
+        <v>35</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>149</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>534</v>
-      </c>
-      <c r="O40" s="19" t="s">
-        <v>535</v>
+        <v>42</v>
+      </c>
+      <c r="O40" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q40" s="28">
-        <v>44426</v>
+        <v>44193</v>
       </c>
       <c r="R40" s="19" t="s">
-        <v>188</v>
+        <v>524</v>
       </c>
       <c r="S40" s="27" t="s">
         <v>33</v>
@@ -4695,58 +4693,60 @@
       </c>
       <c r="U40" s="29"/>
     </row>
-    <row r="41" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>523</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>223</v>
+    <row r="41" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>568</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H41" s="27" t="s">
-        <v>225</v>
+        <v>550</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>544</v>
       </c>
       <c r="I41" s="27" t="s">
         <v>216</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K41" s="27" t="s">
-        <v>226</v>
+        <v>551</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>568</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" s="27" t="s">
-        <v>149</v>
+        <v>543</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>553</v>
       </c>
       <c r="N41" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O41" s="27" t="s">
-        <v>43</v>
+        <v>572</v>
+      </c>
+      <c r="O41" s="19" t="s">
+        <v>573</v>
       </c>
       <c r="P41" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q41" s="28">
-        <v>44193</v>
+        <v>44426</v>
       </c>
       <c r="R41" s="19" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="S41" s="27" t="s">
         <v>33</v>
@@ -4756,91 +4756,89 @@
       </c>
       <c r="U41" s="29"/>
     </row>
-    <row r="42" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>570</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>569</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>571</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>549</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>550</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="I42" s="27" t="s">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="I42" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="K42" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="L42" s="19" t="s">
-        <v>543</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>553</v>
-      </c>
-      <c r="N42" s="19" t="s">
-        <v>572</v>
-      </c>
-      <c r="O42" s="19" t="s">
-        <v>573</v>
-      </c>
-      <c r="P42" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="28">
-        <v>44426</v>
-      </c>
-      <c r="R42" s="19" t="s">
-        <v>547</v>
-      </c>
-      <c r="S42" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="29"/>
+      <c r="J42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N42" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>42119</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="7"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="16" t="s">
-        <v>231</v>
+      <c r="H43" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>216</v>
@@ -4849,28 +4847,28 @@
         <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N43" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="O43" s="16" t="s">
-        <v>194</v>
+        <v>101</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q43" s="6">
-        <v>42119</v>
+        <v>41837</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>196</v>
+        <v>239</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>33</v>
@@ -4886,13 +4884,13 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>234</v>
@@ -4941,91 +4939,93 @@
       </c>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="G45" s="5" t="s">
+    <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>565</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>566</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="G45" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="I45" s="5" t="s">
+      <c r="H45" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="I45" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N45" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O45" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P45" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q45" s="6">
-        <v>41837</v>
-      </c>
-      <c r="R45" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="7"/>
+      <c r="K45" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="L45" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="O45" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="P45" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q45" s="28">
+        <v>44608</v>
+      </c>
+      <c r="R45" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="S45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="29"/>
     </row>
     <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
-        <v>562</v>
+        <v>514</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>565</v>
+        <v>518</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>566</v>
+        <v>515</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>516</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="G46" s="27" t="s">
+        <v>514</v>
+      </c>
+      <c r="G46" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>567</v>
+        <v>519</v>
       </c>
       <c r="I46" s="27" t="s">
         <v>216</v>
@@ -5034,7 +5034,7 @@
         <v>25</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>567</v>
+        <v>517</v>
       </c>
       <c r="L46" s="19" t="s">
         <v>125</v>
@@ -5042,17 +5042,17 @@
       <c r="M46" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N46" s="19" t="s">
+      <c r="N46" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="O46" s="19" t="s">
+      <c r="O46" s="27" t="s">
         <v>194</v>
       </c>
       <c r="P46" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q46" s="28">
-        <v>44608</v>
+        <v>44333</v>
       </c>
       <c r="R46" s="19" t="s">
         <v>196</v>
@@ -5065,91 +5065,89 @@
       </c>
       <c r="U46" s="29"/>
     </row>
-    <row r="47" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>563</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>518</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>516</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G47" s="19" t="s">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="I47" s="27" t="s">
+        <v>520</v>
+      </c>
+      <c r="I47" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J47" s="27" t="s">
+      <c r="J47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K47" s="19" t="s">
-        <v>517</v>
-      </c>
-      <c r="L47" s="19" t="s">
+      <c r="K47" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="L47" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="M47" s="19" t="s">
+      <c r="M47" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="N47" s="27" t="s">
+      <c r="N47" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="O47" s="27" t="s">
+      <c r="O47" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P47" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="28">
-        <v>44333</v>
-      </c>
-      <c r="R47" s="19" t="s">
+      <c r="P47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>43935</v>
+      </c>
+      <c r="R47" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S47" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="29"/>
+      <c r="S47" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="7"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>244</v>
+        <v>249</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5158,28 +5156,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>246</v>
+        <v>110</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>43935</v>
+        <v>41600</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5191,26 +5189,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5219,7 +5217,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>109</v>
@@ -5237,10 +5235,10 @@
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>41600</v>
+        <v>42220</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>134</v>
+        <v>258</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5252,26 +5250,26 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="19" t="s">
-        <v>522</v>
+      <c r="H50" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5280,28 +5278,28 @@
         <v>25</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q50" s="6">
-        <v>42220</v>
+        <v>42158</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
       <c r="S50" s="5" t="s">
         <v>33</v>
@@ -5317,13 +5315,13 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>259</v>
@@ -5372,91 +5370,93 @@
       </c>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="G52" s="5" t="s">
+    <row r="52" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="G52" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="I52" s="5" t="s">
+      <c r="H52" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="I52" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J52" s="5" t="s">
+      <c r="J52" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="N52" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O52" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q52" s="6">
-        <v>42158</v>
-      </c>
-      <c r="R52" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="S52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U52" s="7"/>
-    </row>
-    <row r="53" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="L52" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="N52" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="O52" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="P52" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="28">
+        <v>43871</v>
+      </c>
+      <c r="R52" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="S52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U52" s="29"/>
+    </row>
+    <row r="53" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>561</v>
+        <v>582</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>555</v>
+        <v>581</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>556</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>557</v>
+        <v>575</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>576</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="G53" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>559</v>
+        <v>579</v>
       </c>
       <c r="I53" s="27" t="s">
         <v>216</v>
@@ -5465,7 +5465,7 @@
         <v>25</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="L53" s="27" t="s">
         <v>221</v>
@@ -5473,175 +5473,171 @@
       <c r="M53" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="N53" s="27" t="s">
+      <c r="N53" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="O53" s="19" t="s">
+        <v>578</v>
+      </c>
+      <c r="P53" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q53" s="28">
+        <v>44643</v>
+      </c>
+      <c r="R53" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" s="29"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="N54" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="O53" s="27" t="s">
+      <c r="O54" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="P53" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q53" s="28">
-        <v>43871</v>
-      </c>
-      <c r="R53" s="19" t="s">
-        <v>558</v>
-      </c>
-      <c r="S53" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T53" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U53" s="29"/>
-    </row>
-    <row r="54" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="19" t="s">
-        <v>574</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>582</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>575</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>576</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>574</v>
-      </c>
-      <c r="G54" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>579</v>
-      </c>
-      <c r="I54" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J54" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" s="19" t="s">
-        <v>580</v>
-      </c>
-      <c r="L54" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M54" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="N54" s="19" t="s">
-        <v>577</v>
-      </c>
-      <c r="O54" s="19" t="s">
-        <v>578</v>
-      </c>
-      <c r="P54" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q54" s="28">
-        <v>44643</v>
-      </c>
-      <c r="R54" s="19" t="s">
+      <c r="P54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>41771</v>
+      </c>
+      <c r="R54" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="S54" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T54" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U54" s="29"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U54" s="7"/>
+    </row>
+    <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>269</v>
+        <v>274</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>44</v>
+        <v>277</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>221</v>
+        <v>274</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>179</v>
+        <v>274</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q55" s="6">
-        <v>41771</v>
+        <v>43788</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="S55" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="U55" s="7"/>
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>274</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="D56" s="5"/>
       <c r="E56" s="8" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5662,7 +5658,7 @@
         <v>278</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>44</v>
@@ -5671,10 +5667,10 @@
         <v>43788</v>
       </c>
       <c r="R56" s="5" t="s">
-        <v>67</v>
+        <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5683,24 +5679,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5708,15 +5704,9 @@
       <c r="J57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K57" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="L57" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="M57" s="5" t="s">
-        <v>274</v>
-      </c>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
       <c r="N57" s="5" t="s">
         <v>278</v>
       </c>
@@ -5733,7 +5723,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5742,24 +5732,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5786,7 +5776,7 @@
         <v>288</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T58" s="5" t="s">
         <v>281</v>
@@ -5795,24 +5785,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5848,24 +5838,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5901,24 +5891,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5954,24 +5944,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -6007,24 +5997,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6060,24 +6050,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6113,24 +6103,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6166,24 +6156,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6219,24 +6209,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6272,24 +6262,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6325,135 +6315,137 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="D69" s="5"/>
+        <v>355</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="E69" s="8" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J69" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="L69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>44111</v>
+      </c>
+      <c r="R69" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U69" s="7"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q70" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="7"/>
+    </row>
+    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J71" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="O69" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R69" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="U69" s="7"/>
-    </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="L70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="O70" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>44111</v>
-      </c>
-      <c r="R70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U70" s="7"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="5"/>
+      <c r="K71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N71" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O71" s="5" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6461,33 +6453,37 @@
       <c r="Q71" s="6">
         <v>43788</v>
       </c>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
+      <c r="R71" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S71" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T71" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U71" s="7"/>
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>356</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6508,7 +6504,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6517,7 +6513,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6529,24 +6525,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6567,7 +6563,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6576,7 +6572,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6588,24 +6584,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6647,24 +6643,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="8" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6685,7 +6681,7 @@
         <v>359</v>
       </c>
       <c r="O75" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6694,7 +6690,7 @@
         <v>43788</v>
       </c>
       <c r="R75" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S75" s="5" t="s">
         <v>33</v>
@@ -6704,47 +6700,23 @@
       </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>379</v>
-      </c>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>383</v>
-      </c>
+      <c r="C76" s="5"/>
       <c r="D76" s="5"/>
-      <c r="E76" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L76" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M76" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
       <c r="O76" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>44</v>
@@ -6752,32 +6724,52 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="S76" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T76" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
       <c r="U76" s="7"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="5"/>
+    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N77" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="O77" s="5" t="s">
         <v>65</v>
       </c>
@@ -6787,33 +6779,37 @@
       <c r="Q77" s="6">
         <v>43788</v>
       </c>
-      <c r="R77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
+      <c r="R77" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S77" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T77" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U77" s="7"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>384</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="D78" s="5"/>
       <c r="E78" s="8" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6846,7 +6842,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6855,24 +6851,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6905,7 +6901,7 @@
         <v>361</v>
       </c>
       <c r="S79" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>281</v>
@@ -6914,24 +6910,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6973,24 +6969,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -7032,24 +7028,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7091,24 +7087,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7150,24 +7146,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7209,24 +7205,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7268,24 +7264,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7327,24 +7323,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7386,24 +7382,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7445,24 +7441,24 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>216</v>
@@ -7503,104 +7499,102 @@
       <c r="U89" s="7"/>
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P90" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q90" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R90" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S90" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T90" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="U90" s="7"/>
-    </row>
-    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+      <c r="A90" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B91" s="15"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
-      <c r="H91" s="10"/>
-      <c r="I91" s="10"/>
-      <c r="J91" s="10"/>
-      <c r="K91" s="10"/>
-      <c r="L91" s="10"/>
-      <c r="M91" s="10"/>
-      <c r="N91" s="10"/>
-      <c r="O91" s="10"/>
-      <c r="P91" s="10"/>
-      <c r="Q91" s="10"/>
-      <c r="R91" s="10"/>
-      <c r="S91" s="10"/>
-      <c r="T91" s="10"/>
-      <c r="U91" s="10"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>450</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K91" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="L91" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="M91" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N91" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O91" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P91" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q91" s="6">
+        <v>42507</v>
+      </c>
+      <c r="R91" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="S91" s="5"/>
+      <c r="T91" s="5"/>
+      <c r="U91" s="7"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7615,28 +7609,28 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>453</v>
+        <v>125</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>28</v>
+        <v>458</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>29</v>
+        <v>459</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q92" s="6">
-        <v>42507</v>
+        <v>41002</v>
       </c>
       <c r="R92" s="5" t="s">
-        <v>455</v>
+        <v>32</v>
       </c>
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
@@ -7644,20 +7638,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7672,19 +7666,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>126</v>
+        <v>464</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7701,20 +7695,20 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>23</v>
@@ -7729,19 +7723,19 @@
         <v>25</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="O94" s="5" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>44</v>
@@ -7756,28 +7750,30 @@
       <c r="T94" s="5"/>
       <c r="U94" s="7"/>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B95" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>492</v>
+      </c>
       <c r="C95" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="D95" s="21" t="s">
-        <v>468</v>
+        <v>205</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="F95" s="23" t="s">
-        <v>468</v>
+        <v>203</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="I95" s="5" t="s">
         <v>38</v>
@@ -7786,31 +7782,35 @@
         <v>25</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>470</v>
+        <v>90</v>
       </c>
       <c r="L95" s="5" t="s">
-        <v>468</v>
+        <v>91</v>
       </c>
       <c r="M95" s="5" t="s">
-        <v>471</v>
+        <v>92</v>
       </c>
       <c r="N95" s="5" t="s">
-        <v>472</v>
+        <v>93</v>
       </c>
       <c r="O95" s="5" t="s">
-        <v>473</v>
+        <v>94</v>
       </c>
       <c r="P95" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q95" s="6">
-        <v>41002</v>
+        <v>42118</v>
       </c>
       <c r="R95" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="S95" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T95" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U95" s="7"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Issue #460 : [ldd-request] Move the existing "wave" namespace (#464)
Issue #460 : [ldd-request] Move the existing "wave" namespace

Move the existing "wave" namespace from "Mission" to "Held for Future Use".

This update only affects the namespace registry. The config.properties files is not affected since the "wave" namespace entry needs to remain for backwards compatibility.

@c-suh  [namespace-registry] add new namespace "wave" #460

Resolves #460

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F984C-4CFF-451B-90D9-549AD784B9E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FDDD09-64F5-4336-99C7-2AC5FCC278E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="583">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -2317,9 +2317,9 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4357,146 +4357,146 @@
       </c>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="G35" s="5" t="s">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="H36" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K35" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q35" s="6">
-        <v>42118</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="S35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>217</v>
+      <c r="K36" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>42089</v>
+      </c>
+      <c r="R36" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>495</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I37" s="5" t="s">
+      <c r="H37" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>216</v>
       </c>
       <c r="J37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K37" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>221</v>
+      <c r="K37" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>180</v>
+        <v>110</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>181</v>
+        <v>112</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q37" s="6">
-        <v>42089</v>
+        <v>44329</v>
       </c>
       <c r="R37" s="16" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="S37" s="5" t="s">
         <v>33</v>
@@ -4506,30 +4506,30 @@
       </c>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>496</v>
+        <v>525</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>498</v>
+        <v>526</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>497</v>
+        <v>525</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>527</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>216</v>
@@ -4556,7 +4556,7 @@
         <v>44</v>
       </c>
       <c r="Q38" s="6">
-        <v>44329</v>
+        <v>44385</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>111</v>
@@ -4569,123 +4569,121 @@
       </c>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>527</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="G39" s="5" t="s">
+    <row r="39" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="G39" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="16" t="s">
-        <v>528</v>
-      </c>
-      <c r="I39" s="16" t="s">
+      <c r="H39" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="I39" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K39" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L39" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="M39" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N39" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="P39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>44385</v>
-      </c>
-      <c r="R39" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="S39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U39" s="7"/>
-    </row>
-    <row r="40" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>542</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>538</v>
+      <c r="K39" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="L39" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="M39" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="O39" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="P39" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q39" s="28">
+        <v>44426</v>
+      </c>
+      <c r="R39" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S39" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T39" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U39" s="29"/>
+    </row>
+    <row r="40" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>224</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>539</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>540</v>
-      </c>
-      <c r="I40" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="I40" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J40" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K40" s="19" t="s">
-        <v>541</v>
+      <c r="J40" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="27" t="s">
+        <v>226</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M40" s="19" t="s">
-        <v>179</v>
+        <v>35</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>149</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>534</v>
-      </c>
-      <c r="O40" s="19" t="s">
-        <v>535</v>
+        <v>42</v>
+      </c>
+      <c r="O40" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q40" s="28">
-        <v>44426</v>
+        <v>44193</v>
       </c>
       <c r="R40" s="19" t="s">
-        <v>188</v>
+        <v>524</v>
       </c>
       <c r="S40" s="27" t="s">
         <v>33</v>
@@ -4695,58 +4693,60 @@
       </c>
       <c r="U40" s="29"/>
     </row>
-    <row r="41" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>523</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>223</v>
+    <row r="41" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>568</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H41" s="27" t="s">
-        <v>225</v>
+        <v>550</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>544</v>
       </c>
       <c r="I41" s="27" t="s">
         <v>216</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K41" s="27" t="s">
-        <v>226</v>
+        <v>551</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>568</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" s="27" t="s">
-        <v>149</v>
+        <v>543</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>553</v>
       </c>
       <c r="N41" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O41" s="27" t="s">
-        <v>43</v>
+        <v>572</v>
+      </c>
+      <c r="O41" s="19" t="s">
+        <v>573</v>
       </c>
       <c r="P41" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q41" s="28">
-        <v>44193</v>
+        <v>44426</v>
       </c>
       <c r="R41" s="19" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="S41" s="27" t="s">
         <v>33</v>
@@ -4756,91 +4756,89 @@
       </c>
       <c r="U41" s="29"/>
     </row>
-    <row r="42" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>570</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>569</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>571</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>549</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>550</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="I42" s="27" t="s">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="I42" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="K42" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="L42" s="19" t="s">
-        <v>543</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>553</v>
-      </c>
-      <c r="N42" s="19" t="s">
-        <v>572</v>
-      </c>
-      <c r="O42" s="19" t="s">
-        <v>573</v>
-      </c>
-      <c r="P42" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="28">
-        <v>44426</v>
-      </c>
-      <c r="R42" s="19" t="s">
-        <v>547</v>
-      </c>
-      <c r="S42" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="29"/>
+      <c r="J42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N42" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>42119</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U42" s="7"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="16" t="s">
-        <v>231</v>
+      <c r="H43" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>216</v>
@@ -4849,28 +4847,28 @@
         <v>25</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N43" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="O43" s="16" t="s">
-        <v>194</v>
+        <v>101</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q43" s="6">
-        <v>42119</v>
+        <v>41837</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>196</v>
+        <v>239</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>33</v>
@@ -4886,13 +4884,13 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>234</v>
@@ -4941,91 +4939,93 @@
       </c>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="G45" s="5" t="s">
+    <row r="45" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>565</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>566</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="G45" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="I45" s="5" t="s">
+      <c r="H45" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="I45" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N45" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O45" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P45" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q45" s="6">
-        <v>41837</v>
-      </c>
-      <c r="R45" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U45" s="7"/>
+      <c r="K45" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="L45" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="O45" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="P45" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q45" s="28">
+        <v>44608</v>
+      </c>
+      <c r="R45" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="S45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T45" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="29"/>
     </row>
     <row r="46" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
-        <v>562</v>
+        <v>514</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>565</v>
+        <v>518</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>566</v>
+        <v>515</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>516</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="G46" s="27" t="s">
+        <v>514</v>
+      </c>
+      <c r="G46" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>567</v>
+        <v>519</v>
       </c>
       <c r="I46" s="27" t="s">
         <v>216</v>
@@ -5034,7 +5034,7 @@
         <v>25</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>567</v>
+        <v>517</v>
       </c>
       <c r="L46" s="19" t="s">
         <v>125</v>
@@ -5042,17 +5042,17 @@
       <c r="M46" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="N46" s="19" t="s">
+      <c r="N46" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="O46" s="19" t="s">
+      <c r="O46" s="27" t="s">
         <v>194</v>
       </c>
       <c r="P46" s="27" t="s">
         <v>44</v>
       </c>
       <c r="Q46" s="28">
-        <v>44608</v>
+        <v>44333</v>
       </c>
       <c r="R46" s="19" t="s">
         <v>196</v>
@@ -5065,91 +5065,89 @@
       </c>
       <c r="U46" s="29"/>
     </row>
-    <row r="47" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>563</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>518</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>516</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G47" s="19" t="s">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="I47" s="27" t="s">
+        <v>520</v>
+      </c>
+      <c r="I47" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J47" s="27" t="s">
+      <c r="J47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K47" s="19" t="s">
-        <v>517</v>
-      </c>
-      <c r="L47" s="19" t="s">
+      <c r="K47" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="L47" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="M47" s="19" t="s">
+      <c r="M47" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="N47" s="27" t="s">
+      <c r="N47" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="O47" s="27" t="s">
+      <c r="O47" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P47" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q47" s="28">
-        <v>44333</v>
-      </c>
-      <c r="R47" s="19" t="s">
+      <c r="P47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>43935</v>
+      </c>
+      <c r="R47" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S47" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="29"/>
+      <c r="S47" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="7"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>244</v>
+        <v>249</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>216</v>
@@ -5158,28 +5156,28 @@
         <v>25</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>246</v>
+        <v>110</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q48" s="6">
-        <v>43935</v>
+        <v>41600</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>33</v>
@@ -5191,26 +5189,26 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>216</v>
@@ -5219,7 +5217,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>109</v>
@@ -5237,10 +5235,10 @@
         <v>44</v>
       </c>
       <c r="Q49" s="6">
-        <v>41600</v>
+        <v>42220</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>134</v>
+        <v>258</v>
       </c>
       <c r="S49" s="5" t="s">
         <v>33</v>
@@ -5252,26 +5250,26 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="19" t="s">
-        <v>522</v>
+      <c r="H50" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>216</v>
@@ -5280,28 +5278,28 @@
         <v>25</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q50" s="6">
-        <v>42220</v>
+        <v>42158</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
       <c r="S50" s="5" t="s">
         <v>33</v>
@@ -5317,13 +5315,13 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>259</v>
@@ -5372,91 +5370,93 @@
       </c>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="G52" s="5" t="s">
+    <row r="52" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="G52" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="I52" s="5" t="s">
+      <c r="H52" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="I52" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J52" s="5" t="s">
+      <c r="J52" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="N52" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O52" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q52" s="6">
-        <v>42158</v>
-      </c>
-      <c r="R52" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="S52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U52" s="7"/>
-    </row>
-    <row r="53" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="L52" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="N52" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="O52" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="P52" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="28">
+        <v>43871</v>
+      </c>
+      <c r="R52" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="S52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T52" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U52" s="29"/>
+    </row>
+    <row r="53" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>561</v>
+        <v>582</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>555</v>
+        <v>581</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>556</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>557</v>
+        <v>575</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>576</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="G53" s="27" t="s">
         <v>23</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>559</v>
+        <v>579</v>
       </c>
       <c r="I53" s="27" t="s">
         <v>216</v>
@@ -5465,7 +5465,7 @@
         <v>25</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="L53" s="27" t="s">
         <v>221</v>
@@ -5473,175 +5473,171 @@
       <c r="M53" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="N53" s="27" t="s">
+      <c r="N53" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="O53" s="19" t="s">
+        <v>578</v>
+      </c>
+      <c r="P53" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q53" s="28">
+        <v>44643</v>
+      </c>
+      <c r="R53" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" s="29"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="N54" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="O53" s="27" t="s">
+      <c r="O54" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="P53" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q53" s="28">
-        <v>43871</v>
-      </c>
-      <c r="R53" s="19" t="s">
-        <v>558</v>
-      </c>
-      <c r="S53" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T53" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U53" s="29"/>
-    </row>
-    <row r="54" spans="1:21" s="17" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="19" t="s">
-        <v>574</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>582</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>575</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>576</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>574</v>
-      </c>
-      <c r="G54" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>579</v>
-      </c>
-      <c r="I54" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J54" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" s="19" t="s">
-        <v>580</v>
-      </c>
-      <c r="L54" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M54" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="N54" s="19" t="s">
-        <v>577</v>
-      </c>
-      <c r="O54" s="19" t="s">
-        <v>578</v>
-      </c>
-      <c r="P54" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q54" s="28">
-        <v>44643</v>
-      </c>
-      <c r="R54" s="19" t="s">
+      <c r="P54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>41771</v>
+      </c>
+      <c r="R54" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="S54" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T54" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U54" s="29"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U54" s="7"/>
+    </row>
+    <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>269</v>
+        <v>274</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>44</v>
+        <v>277</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>221</v>
+        <v>274</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>179</v>
+        <v>274</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q55" s="6">
-        <v>41771</v>
+        <v>43788</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="S55" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="U55" s="7"/>
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>274</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="D56" s="5"/>
       <c r="E56" s="8" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5662,7 +5658,7 @@
         <v>278</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>44</v>
@@ -5671,10 +5667,10 @@
         <v>43788</v>
       </c>
       <c r="R56" s="5" t="s">
-        <v>67</v>
+        <v>288</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5683,24 +5679,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5708,15 +5704,9 @@
       <c r="J57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K57" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="L57" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="M57" s="5" t="s">
-        <v>274</v>
-      </c>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
       <c r="N57" s="5" t="s">
         <v>278</v>
       </c>
@@ -5733,7 +5723,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5742,24 +5732,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5786,7 +5776,7 @@
         <v>288</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T58" s="5" t="s">
         <v>281</v>
@@ -5795,24 +5785,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5848,24 +5838,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5901,24 +5891,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5954,24 +5944,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -6007,24 +5997,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6060,24 +6050,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6113,24 +6103,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6166,24 +6156,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6219,24 +6209,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6272,24 +6262,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6325,135 +6315,137 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="D69" s="5"/>
+        <v>355</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="E69" s="8" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>276</v>
+        <v>23</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J69" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="L69" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>44111</v>
+      </c>
+      <c r="R69" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U69" s="7"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q70" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="7"/>
+    </row>
+    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J71" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="O69" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R69" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="U69" s="7"/>
-    </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="L70" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="O70" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="P70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>44111</v>
-      </c>
-      <c r="R70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U70" s="7"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="5"/>
+      <c r="K71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N71" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O71" s="5" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6461,33 +6453,37 @@
       <c r="Q71" s="6">
         <v>43788</v>
       </c>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
+      <c r="R71" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S71" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T71" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U71" s="7"/>
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>356</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="D72" s="5"/>
       <c r="E72" s="8" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6508,7 +6504,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6517,7 +6513,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6529,24 +6525,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6567,7 +6563,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6576,7 +6572,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6588,24 +6584,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6647,24 +6643,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="8" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6685,7 +6681,7 @@
         <v>359</v>
       </c>
       <c r="O75" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6694,7 +6690,7 @@
         <v>43788</v>
       </c>
       <c r="R75" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S75" s="5" t="s">
         <v>33</v>
@@ -6704,47 +6700,23 @@
       </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>379</v>
-      </c>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>383</v>
-      </c>
+      <c r="C76" s="5"/>
       <c r="D76" s="5"/>
-      <c r="E76" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L76" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M76" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
       <c r="O76" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>44</v>
@@ -6752,32 +6724,52 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="S76" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T76" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
       <c r="U76" s="7"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="5"/>
+    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M77" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N77" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="O77" s="5" t="s">
         <v>65</v>
       </c>
@@ -6787,33 +6779,37 @@
       <c r="Q77" s="6">
         <v>43788</v>
       </c>
-      <c r="R77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
+      <c r="R77" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S77" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T77" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U77" s="7"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>384</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="D78" s="5"/>
       <c r="E78" s="8" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6846,7 +6842,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6855,24 +6851,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6905,7 +6901,7 @@
         <v>361</v>
       </c>
       <c r="S79" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>281</v>
@@ -6914,24 +6910,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6973,24 +6969,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -7032,24 +7028,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7091,24 +7087,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7150,24 +7146,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7209,24 +7205,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7268,24 +7264,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7327,24 +7323,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7386,24 +7382,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7445,24 +7441,24 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>216</v>
@@ -7503,104 +7499,102 @@
       <c r="U89" s="7"/>
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P90" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q90" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R90" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S90" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T90" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="U90" s="7"/>
-    </row>
-    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+      <c r="A90" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B91" s="15"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
-      <c r="H91" s="10"/>
-      <c r="I91" s="10"/>
-      <c r="J91" s="10"/>
-      <c r="K91" s="10"/>
-      <c r="L91" s="10"/>
-      <c r="M91" s="10"/>
-      <c r="N91" s="10"/>
-      <c r="O91" s="10"/>
-      <c r="P91" s="10"/>
-      <c r="Q91" s="10"/>
-      <c r="R91" s="10"/>
-      <c r="S91" s="10"/>
-      <c r="T91" s="10"/>
-      <c r="U91" s="10"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>450</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K91" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="L91" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="M91" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N91" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O91" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P91" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q91" s="6">
+        <v>42507</v>
+      </c>
+      <c r="R91" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="S91" s="5"/>
+      <c r="T91" s="5"/>
+      <c r="U91" s="7"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7615,28 +7609,28 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>453</v>
+        <v>125</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>28</v>
+        <v>458</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>29</v>
+        <v>459</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q92" s="6">
-        <v>42507</v>
+        <v>41002</v>
       </c>
       <c r="R92" s="5" t="s">
-        <v>455</v>
+        <v>32</v>
       </c>
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
@@ -7644,20 +7638,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7672,19 +7666,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>126</v>
+        <v>464</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7701,20 +7695,20 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>23</v>
@@ -7729,19 +7723,19 @@
         <v>25</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="O94" s="5" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>44</v>
@@ -7756,28 +7750,30 @@
       <c r="T94" s="5"/>
       <c r="U94" s="7"/>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B95" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>492</v>
+      </c>
       <c r="C95" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="D95" s="21" t="s">
-        <v>468</v>
+        <v>205</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="F95" s="23" t="s">
-        <v>468</v>
+        <v>203</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="I95" s="5" t="s">
         <v>38</v>
@@ -7786,31 +7782,35 @@
         <v>25</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>470</v>
+        <v>90</v>
       </c>
       <c r="L95" s="5" t="s">
-        <v>468</v>
+        <v>91</v>
       </c>
       <c r="M95" s="5" t="s">
-        <v>471</v>
+        <v>92</v>
       </c>
       <c r="N95" s="5" t="s">
-        <v>472</v>
+        <v>93</v>
       </c>
       <c r="O95" s="5" t="s">
-        <v>473</v>
+        <v>94</v>
       </c>
       <c r="P95" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q95" s="6">
-        <v>41002</v>
+        <v>42118</v>
       </c>
       <c r="R95" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="S95" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T95" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U95" s="7"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Issue #253 : Namespace - add "vgr"
Issue #253 : [ldd-request] Create new LDD "vgr"

Local Data Dictionary Name: Voyager Mission Dictionary
Namespace ID Requested: vgr  VGR
Discipline or Mission LDD? Mission
Steward Organization Name: PDS RMS Node
LDD Steward Name: Matthew Tiscareno
LDD Steward Email: matt@seti.org
LDD Stewardship Team Members: Mitch Gordon, Mia Mace
LDD Description: This dictionary supports data from the Voyager missions
Rationale for creation of new LDD: This LDD is needed in order to support data providers preparing to deliver Voyager data

@c-suh  [namespace-registry] add new namespace "vgr" #253

Resolves #253
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FDDD09-64F5-4336-99C7-2AC5FCC278E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75405D70-7938-4A92-97E2-238137C195AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="593">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1774,6 +1774,36 @@
   </si>
   <si>
     <t>New Horizons Primary and Extended Missions</t>
+  </si>
+  <si>
+    <t>vgr</t>
+  </si>
+  <si>
+    <t>Voyager</t>
+  </si>
+  <si>
+    <t>Namespace for the Voyager dictionary.</t>
+  </si>
+  <si>
+    <t>mission/vgr</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/vgr/v1</t>
+  </si>
+  <si>
+    <t>VGR</t>
+  </si>
+  <si>
+    <t>Matthew Tiscareno</t>
+  </si>
+  <si>
+    <t>matt at seti.org</t>
+  </si>
+  <si>
+    <t>PDS4_VGR</t>
+  </si>
+  <si>
+    <t>M.  Tiscareno</t>
   </si>
 </sst>
 </file>
@@ -2314,12 +2344,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U102"/>
+  <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD95"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4078,7 +4108,7 @@
       <c r="K30" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="16" t="s">
         <v>168</v>
       </c>
       <c r="M30" s="5" t="s">
@@ -5557,87 +5587,91 @@
       </c>
       <c r="U54" s="7"/>
     </row>
-    <row r="55" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>274</v>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>583</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>277</v>
+        <v>23</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>591</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>274</v>
+        <v>25</v>
+      </c>
+      <c r="K55" s="16" t="s">
+        <v>588</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="O55" s="5" t="s">
-        <v>279</v>
+        <v>172</v>
+      </c>
+      <c r="N55" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="O55" s="16" t="s">
+        <v>590</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q55" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R55" s="5" t="s">
-        <v>67</v>
+        <v>44700</v>
+      </c>
+      <c r="R55" s="16" t="s">
+        <v>592</v>
       </c>
       <c r="S55" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="U55" s="7"/>
     </row>
     <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D56" s="5"/>
+        <v>280</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="E56" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>216</v>
@@ -5658,7 +5692,7 @@
         <v>278</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>44</v>
@@ -5667,10 +5701,10 @@
         <v>43788</v>
       </c>
       <c r="R56" s="5" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="S56" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T56" s="5" t="s">
         <v>281</v>
@@ -5679,24 +5713,24 @@
     </row>
     <row r="57" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>216</v>
@@ -5704,9 +5738,15 @@
       <c r="J57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
+      <c r="K57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N57" s="5" t="s">
         <v>278</v>
       </c>
@@ -5723,7 +5763,7 @@
         <v>288</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T57" s="5" t="s">
         <v>281</v>
@@ -5732,24 +5772,24 @@
     </row>
     <row r="58" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>216</v>
@@ -5776,7 +5816,7 @@
         <v>288</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T58" s="5" t="s">
         <v>281</v>
@@ -5785,24 +5825,24 @@
     </row>
     <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>216</v>
@@ -5838,24 +5878,24 @@
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>216</v>
@@ -5891,24 +5931,24 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>216</v>
@@ -5944,24 +5984,24 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>216</v>
@@ -5997,24 +6037,24 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>216</v>
@@ -6050,24 +6090,24 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>216</v>
@@ -6103,24 +6143,24 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>216</v>
@@ -6156,24 +6196,24 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>216</v>
@@ -6209,24 +6249,24 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>216</v>
@@ -6262,24 +6302,24 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
@@ -6315,137 +6355,135 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="D69" s="5"/>
       <c r="E69" s="8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>23</v>
+        <v>276</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J69" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R69" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U69" s="7"/>
+    </row>
+    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J70" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="K70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="L69" s="5" t="s">
+      <c r="L70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="M69" s="5" t="s">
+      <c r="M70" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="N69" s="5" t="s">
+      <c r="N70" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O69" s="5" t="s">
+      <c r="O70" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="P69" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="6">
+      <c r="P70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q70" s="6">
         <v>44111</v>
       </c>
-      <c r="R69" s="5" t="s">
+      <c r="R70" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U69" s="7"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P70" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>43788</v>
-      </c>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
+      <c r="S70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T70" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="U70" s="7"/>
     </row>
-    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>356</v>
-      </c>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="L71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="M71" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
       <c r="O71" s="5" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>44</v>
@@ -6453,37 +6491,33 @@
       <c r="Q71" s="6">
         <v>43788</v>
       </c>
-      <c r="R71" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S71" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T71" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
       <c r="U71" s="7"/>
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D72" s="5"/>
+        <v>360</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="E72" s="8" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>216</v>
@@ -6504,7 +6538,7 @@
         <v>359</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>44</v>
@@ -6513,7 +6547,7 @@
         <v>43788</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>33</v>
@@ -6525,24 +6559,24 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="8" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>216</v>
@@ -6563,7 +6597,7 @@
         <v>359</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>44</v>
@@ -6572,7 +6606,7 @@
         <v>43788</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>33</v>
@@ -6584,24 +6618,24 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>216</v>
@@ -6643,24 +6677,24 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>216</v>
@@ -6681,7 +6715,7 @@
         <v>359</v>
       </c>
       <c r="O75" s="5" t="s">
-        <v>366</v>
+        <v>65</v>
       </c>
       <c r="P75" s="5" t="s">
         <v>44</v>
@@ -6690,7 +6724,7 @@
         <v>43788</v>
       </c>
       <c r="R75" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="S75" s="5" t="s">
         <v>33</v>
@@ -6700,23 +6734,47 @@
       </c>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
+    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
+      <c r="E76" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="O76" s="5" t="s">
-        <v>65</v>
+        <v>366</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>44</v>
@@ -6724,52 +6782,32 @@
       <c r="Q76" s="6">
         <v>43788</v>
       </c>
-      <c r="R76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
+      <c r="R76" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T76" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="U76" s="7"/>
     </row>
-    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
-        <v>384</v>
-      </c>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A77" s="5"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="M77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N77" s="5" t="s">
-        <v>387</v>
-      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
       <c r="O77" s="5" t="s">
         <v>65</v>
       </c>
@@ -6779,37 +6817,33 @@
       <c r="Q77" s="6">
         <v>43788</v>
       </c>
-      <c r="R77" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="S77" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="T77" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
       <c r="U77" s="7"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D78" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="E78" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>216</v>
@@ -6842,7 +6876,7 @@
         <v>361</v>
       </c>
       <c r="S78" s="5" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>281</v>
@@ -6851,24 +6885,24 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>216</v>
@@ -6901,7 +6935,7 @@
         <v>361</v>
       </c>
       <c r="S79" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>281</v>
@@ -6910,24 +6944,24 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>216</v>
@@ -6969,24 +7003,24 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>216</v>
@@ -7028,24 +7062,24 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>216</v>
@@ -7087,24 +7121,24 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>216</v>
@@ -7146,24 +7180,24 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>216</v>
@@ -7205,24 +7239,24 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>216</v>
@@ -7264,24 +7298,24 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>216</v>
@@ -7323,24 +7357,24 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>216</v>
@@ -7382,24 +7416,24 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>216</v>
@@ -7441,24 +7475,24 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>216</v>
@@ -7499,102 +7533,104 @@
       <c r="U89" s="7"/>
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="O90" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P90" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q90" s="6">
+        <v>43788</v>
+      </c>
+      <c r="R90" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="S90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="U90" s="7"/>
+    </row>
+    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-      <c r="I90" s="10"/>
-      <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10"/>
-      <c r="O90" s="10"/>
-      <c r="P90" s="10"/>
-      <c r="Q90" s="10"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="10"/>
-      <c r="T90" s="10"/>
-      <c r="U90" s="10"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="F91" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="L91" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N91" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P91" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q91" s="6">
-        <v>42507</v>
-      </c>
-      <c r="R91" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="S91" s="5"/>
-      <c r="T91" s="5"/>
-      <c r="U91" s="7"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
+      <c r="U91" s="10"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>125</v>
+        <v>450</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>23</v>
@@ -7609,28 +7645,28 @@
         <v>25</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>458</v>
+        <v>28</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>459</v>
+        <v>29</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="Q92" s="6">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R92" s="5" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
@@ -7638,20 +7674,20 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>23</v>
@@ -7666,19 +7702,19 @@
         <v>25</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>461</v>
+        <v>125</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>464</v>
+        <v>126</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O93" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P93" s="5" t="s">
         <v>44</v>
@@ -7695,20 +7731,20 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>23</v>
@@ -7723,19 +7759,19 @@
         <v>25</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="O94" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>44</v>
@@ -7750,30 +7786,28 @@
       <c r="T94" s="5"/>
       <c r="U94" s="7"/>
     </row>
-    <row r="95" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>492</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="B95" s="5"/>
       <c r="C95" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>202</v>
+        <v>474</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>468</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>202</v>
+        <v>469</v>
+      </c>
+      <c r="F95" s="23" t="s">
+        <v>468</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>204</v>
+        <v>44</v>
       </c>
       <c r="I95" s="5" t="s">
         <v>38</v>
@@ -7782,86 +7816,122 @@
         <v>25</v>
       </c>
       <c r="K95" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="N95" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="O95" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P95" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q95" s="6">
+        <v>41002</v>
+      </c>
+      <c r="R95" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="7"/>
+    </row>
+    <row r="96" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K96" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L95" s="5" t="s">
+      <c r="L96" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M95" s="5" t="s">
+      <c r="M96" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="N95" s="5" t="s">
+      <c r="N96" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="O95" s="5" t="s">
+      <c r="O96" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="P95" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q95" s="6">
+      <c r="P96" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q96" s="6">
         <v>42118</v>
       </c>
-      <c r="R95" s="5" t="s">
+      <c r="R96" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S95" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T95" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U95" s="7"/>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-      <c r="D96"/>
-      <c r="E96" s="25"/>
-      <c r="F96"/>
-      <c r="G96"/>
-      <c r="H96"/>
-      <c r="I96"/>
-      <c r="J96"/>
-      <c r="K96"/>
-      <c r="L96"/>
-      <c r="M96"/>
-      <c r="N96"/>
-      <c r="O96"/>
-      <c r="P96"/>
-      <c r="Q96"/>
-      <c r="R96"/>
-      <c r="S96"/>
-      <c r="T96"/>
-      <c r="U96"/>
+      <c r="S96" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T96" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U96" s="7"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B97" s="9"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
-      <c r="H97" s="10"/>
-      <c r="I97" s="10"/>
-      <c r="K97" s="9"/>
-      <c r="L97" s="10"/>
-      <c r="M97" s="10"/>
-      <c r="N97" s="10"/>
-      <c r="O97" s="10"/>
-      <c r="P97" s="10"/>
-      <c r="Q97" s="12"/>
-      <c r="R97" s="10"/>
-      <c r="S97" s="10"/>
-      <c r="T97" s="10"/>
-      <c r="U97" s="10"/>
+      <c r="A97"/>
+      <c r="B97"/>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97" s="25"/>
+      <c r="F97"/>
+      <c r="G97"/>
+      <c r="H97"/>
+      <c r="I97"/>
+      <c r="J97"/>
+      <c r="K97"/>
+      <c r="L97"/>
+      <c r="M97"/>
+      <c r="N97"/>
+      <c r="O97"/>
+      <c r="P97"/>
+      <c r="Q97"/>
+      <c r="R97"/>
+      <c r="S97"/>
+      <c r="T97"/>
+      <c r="U97"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
@@ -7883,17 +7953,17 @@
       <c r="U98" s="10"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B99" s="10"/>
+      <c r="A99" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10"/>
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
       <c r="I99" s="10"/>
-      <c r="K99" s="10"/>
+      <c r="K99" s="9"/>
       <c r="L99" s="10"/>
       <c r="M99" s="10"/>
       <c r="N99" s="10"/>
@@ -7907,7 +7977,7 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
@@ -7929,30 +7999,53 @@
       <c r="U100" s="10"/>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="K101" s="10"/>
+      <c r="L101" s="10"/>
+      <c r="M101" s="10"/>
+      <c r="N101" s="10"/>
+      <c r="O101" s="10"/>
+      <c r="P101" s="10"/>
+      <c r="Q101" s="12"/>
+      <c r="R101" s="10"/>
+      <c r="S101" s="10"/>
+      <c r="T101" s="10"/>
+      <c r="U101" s="10"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-      <c r="K101" s="13"/>
-      <c r="L101" s="13"/>
-      <c r="M101" s="13"/>
-      <c r="N101" s="13"/>
-      <c r="O101" s="13"/>
-      <c r="P101" s="13"/>
-      <c r="R101" s="13"/>
-      <c r="S101" s="13"/>
-      <c r="T101" s="13"/>
-      <c r="U101" s="13"/>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="11" t="s">
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="13"/>
+      <c r="L102" s="13"/>
+      <c r="M102" s="13"/>
+      <c r="N102" s="13"/>
+      <c r="O102" s="13"/>
+      <c r="P102" s="13"/>
+      <c r="R102" s="13"/>
+      <c r="S102" s="13"/>
+      <c r="T102" s="13"/>
+      <c r="U102" s="13"/>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A103" s="11" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #490 : [namespace-registry] add new namespace "iras"
Issue #490 : [namespace-registry] add new namespace "iras"

Local Data Dictionary Name: Infrared Astronomical Satellite
Namespace ID Requested: iras
Discipline or Mission LDD? Mission
Steward Organization Name: SBN
LDD Steward Name: Kristina Lopez
LDD Steward Email: klopez@psi.edi
LDD Description: The mission dictionary for the IRAS mission that supports the migration of PDS3 keywords into the PDS4 standard

				Add the namespace "iras" to the Namespace Registry and the config.properties file.

@c-suh  [namespace-registry] add new namespace "iras" #490

Resolves #490
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F4A8E27-8E76-4371-859E-A79BADDC82BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6FFC768-4134-41FA-9CE5-9893F96FF326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6623" uniqueCount="639">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1918,6 +1918,30 @@
   </si>
   <si>
     <t xml:space="preserve">ExoMarsRSP </t>
+  </si>
+  <si>
+    <t>iras</t>
+  </si>
+  <si>
+    <t>mission/iras</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/iras/v1</t>
+  </si>
+  <si>
+    <t>K. Lopez</t>
+  </si>
+  <si>
+    <t>klope at psi.edi</t>
+  </si>
+  <si>
+    <t>PDS4_IRAS</t>
+  </si>
+  <si>
+    <t>Namespace for the Infrared Astronomical Satellite.</t>
+  </si>
+  <si>
+    <t>Infrared Astronomical Satellite</t>
   </si>
 </sst>
 </file>
@@ -2022,7 +2046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2087,6 +2111,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2405,12 +2432,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U106"/>
+  <dimension ref="A1:U107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4865,154 +4892,154 @@
     </row>
     <row r="42" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>568</v>
+        <v>638</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>567</v>
+        <v>637</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>569</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>547</v>
+        <v>632</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>633</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>548</v>
+        <v>21</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>542</v>
+        <v>636</v>
       </c>
       <c r="I42" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="O42" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="P42" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q42" s="18">
+        <v>44735</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="S42" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T42" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U42" s="19"/>
+    </row>
+    <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>542</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J43" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K42" s="17" t="s">
+      <c r="K43" s="17" t="s">
         <v>566</v>
       </c>
-      <c r="L42" s="17" t="s">
+      <c r="L43" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="M42" s="17" t="s">
+      <c r="M43" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="N42" s="17" t="s">
+      <c r="N43" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="O42" s="17" t="s">
+      <c r="O43" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="P42" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q42" s="18">
+      <c r="P43" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q43" s="18">
         <v>44426</v>
       </c>
-      <c r="R42" s="17" t="s">
+      <c r="R43" s="17" t="s">
         <v>545</v>
       </c>
-      <c r="S42" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T42" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U42" s="19"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>618</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="L43" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M43" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="N43" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="O43" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="P43" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q43" s="14">
-        <v>42119</v>
-      </c>
-      <c r="R43" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="S43" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T43" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U43" s="15"/>
+      <c r="S43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U43" s="19"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>235</v>
+        <v>618</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I44" s="13" t="s">
         <v>214</v>
@@ -5021,28 +5048,28 @@
         <v>23</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="O44" s="13" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="P44" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q44" s="14">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R44" s="13" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="S44" s="13" t="s">
         <v>31</v>
@@ -5060,13 +5087,13 @@
         <v>235</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>232</v>
@@ -5115,93 +5142,93 @@
       </c>
       <c r="U45" s="15"/>
     </row>
-    <row r="46" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>563</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>564</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="G46" s="17" t="s">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G46" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="I46" s="17" t="s">
+      <c r="H46" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="I46" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K46" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M46" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N46" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="O46" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q46" s="18">
-        <v>44608</v>
-      </c>
-      <c r="R46" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="S46" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T46" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U46" s="19"/>
+      <c r="K46" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N46" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="O46" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="P46" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q46" s="14">
+        <v>41837</v>
+      </c>
+      <c r="R46" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="S46" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T46" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U46" s="15"/>
     </row>
     <row r="47" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>516</v>
+        <v>563</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>513</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>514</v>
+        <v>560</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>564</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>517</v>
+        <v>565</v>
       </c>
       <c r="I47" s="17" t="s">
         <v>214</v>
@@ -5210,7 +5237,7 @@
         <v>23</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>515</v>
+        <v>565</v>
       </c>
       <c r="L47" s="17" t="s">
         <v>123</v>
@@ -5228,7 +5255,7 @@
         <v>42</v>
       </c>
       <c r="Q47" s="18">
-        <v>44333</v>
+        <v>44608</v>
       </c>
       <c r="R47" s="17" t="s">
         <v>194</v>
@@ -5241,93 +5268,93 @@
       </c>
       <c r="U47" s="19"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>620</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="G48" s="13" t="s">
+    <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="G48" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>518</v>
-      </c>
-      <c r="I48" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="I48" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="J48" s="13" t="s">
+      <c r="J48" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K48" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="L48" s="13" t="s">
+      <c r="K48" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="L48" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M48" s="13" t="s">
+      <c r="M48" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="N48" s="13" t="s">
+      <c r="N48" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="O48" s="13" t="s">
+      <c r="O48" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P48" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q48" s="14">
-        <v>43935</v>
-      </c>
-      <c r="R48" s="13" t="s">
+      <c r="P48" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q48" s="18">
+        <v>44333</v>
+      </c>
+      <c r="R48" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="S48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U48" s="15"/>
+      <c r="S48" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T48" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U48" s="19"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>242</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G49" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>214</v>
@@ -5336,28 +5363,28 @@
         <v>23</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="M49" s="13" t="s">
-        <v>108</v>
+        <v>244</v>
       </c>
       <c r="N49" s="13" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="P49" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q49" s="14">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R49" s="13" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="S49" s="13" t="s">
         <v>31</v>
@@ -5369,28 +5396,28 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>214</v>
@@ -5399,7 +5426,7 @@
         <v>23</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="L50" s="13" t="s">
         <v>107</v>
@@ -5417,10 +5444,10 @@
         <v>42</v>
       </c>
       <c r="Q50" s="14">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="S50" s="13" t="s">
         <v>31</v>
@@ -5432,28 +5459,28 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="13" t="s">
-        <v>260</v>
+      <c r="H51" s="17" t="s">
+        <v>520</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>214</v>
@@ -5462,28 +5489,28 @@
         <v>23</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="N51" s="13" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="P51" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q51" s="14">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>31</v>
@@ -5501,13 +5528,13 @@
         <v>619</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>257</v>
@@ -5556,93 +5583,93 @@
       </c>
       <c r="U52" s="15"/>
     </row>
-    <row r="53" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O53" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R53" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="S53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U53" s="15"/>
+    </row>
+    <row r="54" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B54" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>608</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E54" s="21" t="s">
         <v>609</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="17" t="s">
         <v>607</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>612</v>
-      </c>
-      <c r="I53" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="J53" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K53" s="17" t="s">
-        <v>613</v>
-      </c>
-      <c r="L53" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M53" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N53" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="O53" s="17" t="s">
-        <v>617</v>
-      </c>
-      <c r="P53" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q53" s="18">
-        <v>44713</v>
-      </c>
-      <c r="R53" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="S53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U53" s="19"/>
-    </row>
-    <row r="54" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>552</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>553</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>555</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
       <c r="I54" s="17" t="s">
         <v>214</v>
@@ -5651,28 +5678,28 @@
         <v>23</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="L54" s="17" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="M54" s="17" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N54" s="17" t="s">
-        <v>269</v>
+        <v>616</v>
       </c>
       <c r="O54" s="17" t="s">
-        <v>270</v>
+        <v>617</v>
       </c>
       <c r="P54" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q54" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R54" s="17" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="S54" s="17" t="s">
         <v>31</v>
@@ -5682,30 +5709,30 @@
       </c>
       <c r="U54" s="19"/>
     </row>
-    <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>214</v>
@@ -5714,7 +5741,7 @@
         <v>23</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="L55" s="17" t="s">
         <v>219</v>
@@ -5723,19 +5750,19 @@
         <v>177</v>
       </c>
       <c r="N55" s="17" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>576</v>
+        <v>270</v>
       </c>
       <c r="P55" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q55" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>186</v>
+        <v>556</v>
       </c>
       <c r="S55" s="17" t="s">
         <v>31</v>
@@ -5745,30 +5772,30 @@
       </c>
       <c r="U55" s="19"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>604</v>
+        <v>577</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>214</v>
@@ -5777,7 +5804,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="L56" s="17" t="s">
         <v>219</v>
@@ -5786,115 +5813,115 @@
         <v>177</v>
       </c>
       <c r="N56" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="O56" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="P56" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q56" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R56" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="S56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U56" s="19"/>
+    </row>
+    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="I57" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J57" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N57" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="O56" s="17" t="s">
+      <c r="O57" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="P56" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q56" s="18">
+      <c r="P57" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q57" s="18">
         <v>44713</v>
       </c>
-      <c r="R56" s="17" t="s">
+      <c r="R57" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="S56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U56" s="19"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F57" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I57" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J57" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K57" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="L57" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M57" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N57" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="O57" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="P57" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q57" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R57" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S57" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T57" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U57" s="15"/>
+      <c r="S57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U57" s="19"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>582</v>
+        <v>626</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>583</v>
+        <v>271</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>585</v>
+        <v>266</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>589</v>
+        <v>42</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>214</v>
@@ -5903,28 +5930,28 @@
         <v>23</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>586</v>
+        <v>268</v>
       </c>
       <c r="L58" s="13" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M58" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N58" s="13" t="s">
-        <v>587</v>
+        <v>269</v>
       </c>
       <c r="O58" s="13" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="P58" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q58" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R58" s="13" t="s">
-        <v>590</v>
+        <v>186</v>
       </c>
       <c r="S58" s="13" t="s">
         <v>31</v>
@@ -5934,91 +5961,93 @@
       </c>
       <c r="U58" s="15"/>
     </row>
-    <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>627</v>
+        <v>582</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>273</v>
+        <v>584</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>275</v>
+        <v>589</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>272</v>
+        <v>586</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>272</v>
+        <v>170</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>276</v>
+        <v>587</v>
       </c>
       <c r="O59" s="13" t="s">
-        <v>277</v>
+        <v>588</v>
       </c>
       <c r="P59" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q59" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R59" s="13" t="s">
-        <v>65</v>
+        <v>590</v>
       </c>
       <c r="S59" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T59" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="U59" s="15"/>
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D60" s="13"/>
+        <v>278</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="E60" s="20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>214</v>
@@ -6039,7 +6068,7 @@
         <v>276</v>
       </c>
       <c r="O60" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P60" s="13" t="s">
         <v>42</v>
@@ -6048,10 +6077,10 @@
         <v>43788</v>
       </c>
       <c r="R60" s="13" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="S60" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T60" s="13" t="s">
         <v>279</v>
@@ -6060,26 +6089,26 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="20" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>214</v>
@@ -6087,9 +6116,15 @@
       <c r="J61" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
+      <c r="K61" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L61" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="M61" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="N61" s="13" t="s">
         <v>276</v>
       </c>
@@ -6106,7 +6141,7 @@
         <v>286</v>
       </c>
       <c r="S61" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T61" s="13" t="s">
         <v>279</v>
@@ -6115,26 +6150,26 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="20" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>214</v>
@@ -6161,7 +6196,7 @@
         <v>286</v>
       </c>
       <c r="S62" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T62" s="13" t="s">
         <v>279</v>
@@ -6170,26 +6205,26 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>214</v>
@@ -6225,26 +6260,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>214</v>
@@ -6280,26 +6315,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>214</v>
@@ -6335,26 +6370,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>214</v>
@@ -6390,26 +6425,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>214</v>
@@ -6445,26 +6480,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>214</v>
@@ -6500,26 +6535,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>214</v>
@@ -6555,26 +6590,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>214</v>
@@ -6610,26 +6645,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>214</v>
@@ -6665,26 +6700,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>214</v>
@@ -6720,141 +6755,139 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>21</v>
+        <v>274</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J73" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="O73" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="P73" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q73" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R73" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="S73" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T73" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U73" s="15"/>
+    </row>
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J74" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K73" s="13" t="s">
+      <c r="K74" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="L73" s="13" t="s">
+      <c r="L74" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="M73" s="13" t="s">
+      <c r="M74" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="N73" s="13" t="s">
+      <c r="N74" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="O73" s="13" t="s">
+      <c r="O74" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="P73" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q73" s="14">
+      <c r="P74" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q74" s="14">
         <v>44111</v>
       </c>
-      <c r="R73" s="13" t="s">
+      <c r="R74" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="S73" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T73" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U73" s="15"/>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P74" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q74" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R74" s="13"/>
-      <c r="S74" s="13"/>
-      <c r="T74" s="13"/>
+      <c r="S74" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T74" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U74" s="15"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="F75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G75" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="I75" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J75" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="L75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="M75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="N75" s="13" t="s">
-        <v>357</v>
-      </c>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
       <c r="O75" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P75" s="13" t="s">
         <v>42</v>
@@ -6862,39 +6895,35 @@
       <c r="Q75" s="14">
         <v>43788</v>
       </c>
-      <c r="R75" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S75" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T75" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R75" s="13"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="13"/>
       <c r="U75" s="15"/>
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D76" s="13"/>
+        <v>358</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>354</v>
+      </c>
       <c r="E76" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>214</v>
@@ -6915,7 +6944,7 @@
         <v>357</v>
       </c>
       <c r="O76" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P76" s="13" t="s">
         <v>42</v>
@@ -6924,7 +6953,7 @@
         <v>43788</v>
       </c>
       <c r="R76" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S76" s="13" t="s">
         <v>31</v>
@@ -6936,26 +6965,26 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="20" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="I77" s="13" t="s">
         <v>214</v>
@@ -6976,7 +7005,7 @@
         <v>357</v>
       </c>
       <c r="O77" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>42</v>
@@ -6985,7 +7014,7 @@
         <v>43788</v>
       </c>
       <c r="R77" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="S77" s="13" t="s">
         <v>31</v>
@@ -6997,26 +7026,26 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>214</v>
@@ -7058,26 +7087,26 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>214</v>
@@ -7098,7 +7127,7 @@
         <v>357</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7107,7 +7136,7 @@
         <v>43788</v>
       </c>
       <c r="R79" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S79" s="13" t="s">
         <v>31</v>
@@ -7117,23 +7146,49 @@
       </c>
       <c r="U79" s="15"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+    <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A80" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
+      <c r="E80" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="I80" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J80" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K80" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="L80" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M80" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="N80" s="13" t="s">
+        <v>357</v>
+      </c>
       <c r="O80" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7141,54 +7196,32 @@
       <c r="Q80" s="14">
         <v>43788</v>
       </c>
-      <c r="R80" s="13"/>
-      <c r="S80" s="13"/>
-      <c r="T80" s="13"/>
+      <c r="R80" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="S80" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T80" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="U80" s="15"/>
     </row>
-    <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E81" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="G81" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H81" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J81" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="L81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="M81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="N81" s="13" t="s">
-        <v>385</v>
-      </c>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13"/>
       <c r="O81" s="13" t="s">
         <v>63</v>
       </c>
@@ -7198,39 +7231,35 @@
       <c r="Q81" s="14">
         <v>43788</v>
       </c>
-      <c r="R81" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S81" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="T81" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R81" s="13"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="13"/>
       <c r="U81" s="15"/>
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D82" s="13"/>
+        <v>386</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>382</v>
+      </c>
       <c r="E82" s="20" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>214</v>
@@ -7263,7 +7292,7 @@
         <v>359</v>
       </c>
       <c r="S82" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T82" s="13" t="s">
         <v>279</v>
@@ -7272,26 +7301,26 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>214</v>
@@ -7324,7 +7353,7 @@
         <v>359</v>
       </c>
       <c r="S83" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T83" s="13" t="s">
         <v>279</v>
@@ -7333,26 +7362,26 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="20" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>214</v>
@@ -7394,26 +7423,26 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="20" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>214</v>
@@ -7455,26 +7484,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>214</v>
@@ -7516,26 +7545,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>214</v>
@@ -7577,26 +7606,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>214</v>
@@ -7638,26 +7667,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>214</v>
@@ -7699,26 +7728,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>214</v>
@@ -7760,26 +7789,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>214</v>
@@ -7821,26 +7850,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>214</v>
@@ -7882,26 +7911,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>214</v>
@@ -7942,103 +7971,107 @@
       <c r="U93" s="15"/>
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D94" s="13"/>
+      <c r="E94" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F94" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G94" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J94" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K94" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="L94" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M94" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N94" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="O94" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P94" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q94" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R94" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="S94" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T94" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U94" s="15"/>
+    </row>
+    <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A95" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B94" s="12"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
-      <c r="J94" s="22"/>
-      <c r="K94" s="22"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="22"/>
-      <c r="O94" s="22"/>
-      <c r="P94" s="22"/>
-      <c r="Q94" s="22"/>
-      <c r="R94" s="22"/>
-      <c r="S94" s="22"/>
-      <c r="T94" s="22"/>
-      <c r="U94" s="22"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F95" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="G95" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H95" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I95" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J95" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K95" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="L95" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M95" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N95" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O95" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P95" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q95" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R95" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="S95" s="13"/>
-      <c r="T95" s="13"/>
-      <c r="U95" s="15"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="22"/>
+      <c r="K95" s="22"/>
+      <c r="L95" s="22"/>
+      <c r="M95" s="22"/>
+      <c r="N95" s="22"/>
+      <c r="O95" s="22"/>
+      <c r="P95" s="22"/>
+      <c r="Q95" s="22"/>
+      <c r="R95" s="22"/>
+      <c r="S95" s="22"/>
+      <c r="T95" s="22"/>
+      <c r="U95" s="22"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="B96" s="13"/>
       <c r="C96" s="13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="G96" s="13" t="s">
         <v>21</v>
@@ -8053,28 +8086,28 @@
         <v>23</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L96" s="13" t="s">
-        <v>123</v>
+        <v>451</v>
       </c>
       <c r="M96" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N96" s="13" t="s">
-        <v>456</v>
+        <v>26</v>
       </c>
       <c r="O96" s="13" t="s">
-        <v>457</v>
+        <v>27</v>
       </c>
       <c r="P96" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q96" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R96" s="13" t="s">
-        <v>30</v>
+        <v>453</v>
       </c>
       <c r="S96" s="13"/>
       <c r="T96" s="13"/>
@@ -8082,20 +8115,20 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="B97" s="13"/>
       <c r="C97" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="G97" s="13" t="s">
         <v>21</v>
@@ -8110,19 +8143,19 @@
         <v>23</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="M97" s="13" t="s">
-        <v>462</v>
+        <v>124</v>
       </c>
       <c r="N97" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O97" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P97" s="13" t="s">
         <v>42</v>
@@ -8139,20 +8172,20 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>21</v>
@@ -8167,19 +8200,19 @@
         <v>23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="N98" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="O98" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P98" s="13" t="s">
         <v>42</v>
@@ -8194,30 +8227,28 @@
       <c r="T98" s="13"/>
       <c r="U98" s="15"/>
     </row>
-    <row r="99" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B99" s="13" t="s">
-        <v>490</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="I99" s="13" t="s">
         <v>36</v>
@@ -8226,86 +8257,122 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="L99" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M99" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="N99" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="O99" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="P99" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q99" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R99" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="15"/>
+    </row>
+    <row r="100" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G100" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H100" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I100" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J100" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K100" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L99" s="13" t="s">
+      <c r="L100" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M99" s="13" t="s">
+      <c r="M100" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N99" s="13" t="s">
+      <c r="N100" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O99" s="13" t="s">
+      <c r="O100" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P99" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q99" s="14">
+      <c r="P100" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q100" s="14">
         <v>42118</v>
       </c>
-      <c r="R99" s="13" t="s">
+      <c r="R100" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S99" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T99" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U99" s="15"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100" s="10"/>
-      <c r="F100"/>
-      <c r="G100"/>
-      <c r="H100"/>
-      <c r="I100"/>
-      <c r="J100"/>
-      <c r="K100"/>
-      <c r="L100"/>
-      <c r="M100"/>
-      <c r="N100"/>
-      <c r="O100"/>
-      <c r="P100"/>
-      <c r="Q100"/>
-      <c r="R100"/>
-      <c r="S100"/>
-      <c r="T100"/>
-      <c r="U100"/>
+      <c r="S100" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T100" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U100" s="15"/>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="4"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="4"/>
-      <c r="S101" s="4"/>
-      <c r="T101" s="4"/>
-      <c r="U101" s="4"/>
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101" s="10"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="L101"/>
+      <c r="M101"/>
+      <c r="N101"/>
+      <c r="O101"/>
+      <c r="P101"/>
+      <c r="Q101"/>
+      <c r="R101"/>
+      <c r="S101"/>
+      <c r="T101"/>
+      <c r="U101"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="4"/>
@@ -8327,17 +8394,17 @@
       <c r="U102" s="4"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B103" s="4"/>
+      <c r="A103" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B103" s="3"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
-      <c r="K103" s="4"/>
+      <c r="K103" s="3"/>
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
@@ -8351,7 +8418,7 @@
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -8373,30 +8440,53 @@
       <c r="U104" s="4"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="4"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+      <c r="U105" s="4"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="H105" s="7"/>
-      <c r="I105" s="7"/>
-      <c r="J105" s="7"/>
-      <c r="K105" s="7"/>
-      <c r="L105" s="7"/>
-      <c r="M105" s="7"/>
-      <c r="N105" s="7"/>
-      <c r="O105" s="7"/>
-      <c r="P105" s="7"/>
-      <c r="R105" s="7"/>
-      <c r="S105" s="7"/>
-      <c r="T105" s="7"/>
-      <c r="U105" s="7"/>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="7"/>
+      <c r="M106" s="7"/>
+      <c r="N106" s="7"/>
+      <c r="O106" s="7"/>
+      <c r="P106" s="7"/>
+      <c r="R106" s="7"/>
+      <c r="S106" s="7"/>
+      <c r="T106" s="7"/>
+      <c r="U106" s="7"/>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #490 : [namespace-registry] add new namespace "iras" (#491)
Issue #490 : [namespace-registry] add new namespace "iras"

Local Data Dictionary Name: Infrared Astronomical Satellite
Namespace ID Requested: iras
Discipline or Mission LDD? Mission
Steward Organization Name: SBN
LDD Steward Name: Kristina Lopez
LDD Steward Email: klopez@psi.edi
LDD Description: The mission dictionary for the IRAS mission that supports the migration of PDS3 keywords into the PDS4 standard

				Add the namespace "iras" to the Namespace Registry and the config.properties file.

@c-suh  [namespace-registry] add new namespace "iras" #490

Resolves #490

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F4A8E27-8E76-4371-859E-A79BADDC82BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6FFC768-4134-41FA-9CE5-9893F96FF326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6623" uniqueCount="639">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1918,6 +1918,30 @@
   </si>
   <si>
     <t xml:space="preserve">ExoMarsRSP </t>
+  </si>
+  <si>
+    <t>iras</t>
+  </si>
+  <si>
+    <t>mission/iras</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/iras/v1</t>
+  </si>
+  <si>
+    <t>K. Lopez</t>
+  </si>
+  <si>
+    <t>klope at psi.edi</t>
+  </si>
+  <si>
+    <t>PDS4_IRAS</t>
+  </si>
+  <si>
+    <t>Namespace for the Infrared Astronomical Satellite.</t>
+  </si>
+  <si>
+    <t>Infrared Astronomical Satellite</t>
   </si>
 </sst>
 </file>
@@ -2022,7 +2046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2087,6 +2111,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2405,12 +2432,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U106"/>
+  <dimension ref="A1:U107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4865,154 +4892,154 @@
     </row>
     <row r="42" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>568</v>
+        <v>638</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>567</v>
+        <v>637</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>569</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>547</v>
+        <v>632</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>633</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>548</v>
+        <v>21</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>542</v>
+        <v>636</v>
       </c>
       <c r="I42" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="O42" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="P42" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q42" s="18">
+        <v>44735</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="S42" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T42" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U42" s="19"/>
+    </row>
+    <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>542</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J43" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K42" s="17" t="s">
+      <c r="K43" s="17" t="s">
         <v>566</v>
       </c>
-      <c r="L42" s="17" t="s">
+      <c r="L43" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="M42" s="17" t="s">
+      <c r="M43" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="N42" s="17" t="s">
+      <c r="N43" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="O42" s="17" t="s">
+      <c r="O43" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="P42" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q42" s="18">
+      <c r="P43" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q43" s="18">
         <v>44426</v>
       </c>
-      <c r="R42" s="17" t="s">
+      <c r="R43" s="17" t="s">
         <v>545</v>
       </c>
-      <c r="S42" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T42" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U42" s="19"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>618</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="L43" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M43" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="N43" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="O43" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="P43" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q43" s="14">
-        <v>42119</v>
-      </c>
-      <c r="R43" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="S43" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T43" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U43" s="15"/>
+      <c r="S43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U43" s="19"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>235</v>
+        <v>618</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I44" s="13" t="s">
         <v>214</v>
@@ -5021,28 +5048,28 @@
         <v>23</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="O44" s="13" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="P44" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q44" s="14">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R44" s="13" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="S44" s="13" t="s">
         <v>31</v>
@@ -5060,13 +5087,13 @@
         <v>235</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>232</v>
@@ -5115,93 +5142,93 @@
       </c>
       <c r="U45" s="15"/>
     </row>
-    <row r="46" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>563</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>564</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="G46" s="17" t="s">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G46" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="I46" s="17" t="s">
+      <c r="H46" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="I46" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K46" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M46" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N46" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="O46" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q46" s="18">
-        <v>44608</v>
-      </c>
-      <c r="R46" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="S46" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T46" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U46" s="19"/>
+      <c r="K46" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N46" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="O46" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="P46" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q46" s="14">
+        <v>41837</v>
+      </c>
+      <c r="R46" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="S46" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T46" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U46" s="15"/>
     </row>
     <row r="47" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>516</v>
+        <v>563</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>513</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>514</v>
+        <v>560</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>564</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>517</v>
+        <v>565</v>
       </c>
       <c r="I47" s="17" t="s">
         <v>214</v>
@@ -5210,7 +5237,7 @@
         <v>23</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>515</v>
+        <v>565</v>
       </c>
       <c r="L47" s="17" t="s">
         <v>123</v>
@@ -5228,7 +5255,7 @@
         <v>42</v>
       </c>
       <c r="Q47" s="18">
-        <v>44333</v>
+        <v>44608</v>
       </c>
       <c r="R47" s="17" t="s">
         <v>194</v>
@@ -5241,93 +5268,93 @@
       </c>
       <c r="U47" s="19"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>620</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="G48" s="13" t="s">
+    <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="G48" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>518</v>
-      </c>
-      <c r="I48" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="I48" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="J48" s="13" t="s">
+      <c r="J48" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K48" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="L48" s="13" t="s">
+      <c r="K48" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="L48" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M48" s="13" t="s">
+      <c r="M48" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="N48" s="13" t="s">
+      <c r="N48" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="O48" s="13" t="s">
+      <c r="O48" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P48" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q48" s="14">
-        <v>43935</v>
-      </c>
-      <c r="R48" s="13" t="s">
+      <c r="P48" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q48" s="18">
+        <v>44333</v>
+      </c>
+      <c r="R48" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="S48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U48" s="15"/>
+      <c r="S48" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T48" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U48" s="19"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>242</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G49" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>214</v>
@@ -5336,28 +5363,28 @@
         <v>23</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="M49" s="13" t="s">
-        <v>108</v>
+        <v>244</v>
       </c>
       <c r="N49" s="13" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="P49" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q49" s="14">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R49" s="13" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="S49" s="13" t="s">
         <v>31</v>
@@ -5369,28 +5396,28 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>214</v>
@@ -5399,7 +5426,7 @@
         <v>23</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="L50" s="13" t="s">
         <v>107</v>
@@ -5417,10 +5444,10 @@
         <v>42</v>
       </c>
       <c r="Q50" s="14">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="S50" s="13" t="s">
         <v>31</v>
@@ -5432,28 +5459,28 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="13" t="s">
-        <v>260</v>
+      <c r="H51" s="17" t="s">
+        <v>520</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>214</v>
@@ -5462,28 +5489,28 @@
         <v>23</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="N51" s="13" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="P51" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q51" s="14">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>31</v>
@@ -5501,13 +5528,13 @@
         <v>619</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>257</v>
@@ -5556,93 +5583,93 @@
       </c>
       <c r="U52" s="15"/>
     </row>
-    <row r="53" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O53" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R53" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="S53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U53" s="15"/>
+    </row>
+    <row r="54" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B54" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>608</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E54" s="21" t="s">
         <v>609</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="17" t="s">
         <v>607</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>612</v>
-      </c>
-      <c r="I53" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="J53" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K53" s="17" t="s">
-        <v>613</v>
-      </c>
-      <c r="L53" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M53" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N53" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="O53" s="17" t="s">
-        <v>617</v>
-      </c>
-      <c r="P53" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q53" s="18">
-        <v>44713</v>
-      </c>
-      <c r="R53" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="S53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U53" s="19"/>
-    </row>
-    <row r="54" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>552</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>553</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>555</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
       <c r="I54" s="17" t="s">
         <v>214</v>
@@ -5651,28 +5678,28 @@
         <v>23</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="L54" s="17" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="M54" s="17" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N54" s="17" t="s">
-        <v>269</v>
+        <v>616</v>
       </c>
       <c r="O54" s="17" t="s">
-        <v>270</v>
+        <v>617</v>
       </c>
       <c r="P54" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q54" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R54" s="17" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="S54" s="17" t="s">
         <v>31</v>
@@ -5682,30 +5709,30 @@
       </c>
       <c r="U54" s="19"/>
     </row>
-    <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>214</v>
@@ -5714,7 +5741,7 @@
         <v>23</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="L55" s="17" t="s">
         <v>219</v>
@@ -5723,19 +5750,19 @@
         <v>177</v>
       </c>
       <c r="N55" s="17" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>576</v>
+        <v>270</v>
       </c>
       <c r="P55" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q55" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>186</v>
+        <v>556</v>
       </c>
       <c r="S55" s="17" t="s">
         <v>31</v>
@@ -5745,30 +5772,30 @@
       </c>
       <c r="U55" s="19"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>604</v>
+        <v>577</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>214</v>
@@ -5777,7 +5804,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="L56" s="17" t="s">
         <v>219</v>
@@ -5786,115 +5813,115 @@
         <v>177</v>
       </c>
       <c r="N56" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="O56" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="P56" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q56" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R56" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="S56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U56" s="19"/>
+    </row>
+    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="I57" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J57" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N57" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="O56" s="17" t="s">
+      <c r="O57" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="P56" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q56" s="18">
+      <c r="P57" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q57" s="18">
         <v>44713</v>
       </c>
-      <c r="R56" s="17" t="s">
+      <c r="R57" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="S56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U56" s="19"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F57" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I57" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J57" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K57" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="L57" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M57" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N57" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="O57" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="P57" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q57" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R57" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S57" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T57" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U57" s="15"/>
+      <c r="S57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U57" s="19"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>582</v>
+        <v>626</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>583</v>
+        <v>271</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>585</v>
+        <v>266</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>589</v>
+        <v>42</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>214</v>
@@ -5903,28 +5930,28 @@
         <v>23</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>586</v>
+        <v>268</v>
       </c>
       <c r="L58" s="13" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M58" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N58" s="13" t="s">
-        <v>587</v>
+        <v>269</v>
       </c>
       <c r="O58" s="13" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="P58" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q58" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R58" s="13" t="s">
-        <v>590</v>
+        <v>186</v>
       </c>
       <c r="S58" s="13" t="s">
         <v>31</v>
@@ -5934,91 +5961,93 @@
       </c>
       <c r="U58" s="15"/>
     </row>
-    <row r="59" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>627</v>
+        <v>582</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>273</v>
+        <v>584</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>275</v>
+        <v>589</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>272</v>
+        <v>586</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>272</v>
+        <v>170</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>276</v>
+        <v>587</v>
       </c>
       <c r="O59" s="13" t="s">
-        <v>277</v>
+        <v>588</v>
       </c>
       <c r="P59" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q59" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R59" s="13" t="s">
-        <v>65</v>
+        <v>590</v>
       </c>
       <c r="S59" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T59" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="U59" s="15"/>
     </row>
     <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D60" s="13"/>
+        <v>278</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="E60" s="20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>214</v>
@@ -6039,7 +6068,7 @@
         <v>276</v>
       </c>
       <c r="O60" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P60" s="13" t="s">
         <v>42</v>
@@ -6048,10 +6077,10 @@
         <v>43788</v>
       </c>
       <c r="R60" s="13" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="S60" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T60" s="13" t="s">
         <v>279</v>
@@ -6060,26 +6089,26 @@
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="20" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>214</v>
@@ -6087,9 +6116,15 @@
       <c r="J61" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
+      <c r="K61" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L61" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="M61" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="N61" s="13" t="s">
         <v>276</v>
       </c>
@@ -6106,7 +6141,7 @@
         <v>286</v>
       </c>
       <c r="S61" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T61" s="13" t="s">
         <v>279</v>
@@ -6115,26 +6150,26 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="20" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>214</v>
@@ -6161,7 +6196,7 @@
         <v>286</v>
       </c>
       <c r="S62" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T62" s="13" t="s">
         <v>279</v>
@@ -6170,26 +6205,26 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>214</v>
@@ -6225,26 +6260,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>214</v>
@@ -6280,26 +6315,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>214</v>
@@ -6335,26 +6370,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>214</v>
@@ -6390,26 +6425,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>214</v>
@@ -6445,26 +6480,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>214</v>
@@ -6500,26 +6535,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>214</v>
@@ -6555,26 +6590,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>214</v>
@@ -6610,26 +6645,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>214</v>
@@ -6665,26 +6700,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>214</v>
@@ -6720,141 +6755,139 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>21</v>
+        <v>274</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J73" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="O73" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="P73" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q73" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R73" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="S73" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T73" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U73" s="15"/>
+    </row>
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J74" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K73" s="13" t="s">
+      <c r="K74" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="L73" s="13" t="s">
+      <c r="L74" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="M73" s="13" t="s">
+      <c r="M74" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="N73" s="13" t="s">
+      <c r="N74" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="O73" s="13" t="s">
+      <c r="O74" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="P73" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q73" s="14">
+      <c r="P74" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q74" s="14">
         <v>44111</v>
       </c>
-      <c r="R73" s="13" t="s">
+      <c r="R74" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="S73" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T73" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U73" s="15"/>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P74" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q74" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R74" s="13"/>
-      <c r="S74" s="13"/>
-      <c r="T74" s="13"/>
+      <c r="S74" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T74" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U74" s="15"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="F75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G75" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="I75" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J75" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="L75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="M75" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="N75" s="13" t="s">
-        <v>357</v>
-      </c>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
       <c r="O75" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P75" s="13" t="s">
         <v>42</v>
@@ -6862,39 +6895,35 @@
       <c r="Q75" s="14">
         <v>43788</v>
       </c>
-      <c r="R75" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S75" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T75" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R75" s="13"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="13"/>
       <c r="U75" s="15"/>
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D76" s="13"/>
+        <v>358</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>354</v>
+      </c>
       <c r="E76" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>214</v>
@@ -6915,7 +6944,7 @@
         <v>357</v>
       </c>
       <c r="O76" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P76" s="13" t="s">
         <v>42</v>
@@ -6924,7 +6953,7 @@
         <v>43788</v>
       </c>
       <c r="R76" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S76" s="13" t="s">
         <v>31</v>
@@ -6936,26 +6965,26 @@
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="20" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="I77" s="13" t="s">
         <v>214</v>
@@ -6976,7 +7005,7 @@
         <v>357</v>
       </c>
       <c r="O77" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>42</v>
@@ -6985,7 +7014,7 @@
         <v>43788</v>
       </c>
       <c r="R77" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="S77" s="13" t="s">
         <v>31</v>
@@ -6997,26 +7026,26 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>214</v>
@@ -7058,26 +7087,26 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>214</v>
@@ -7098,7 +7127,7 @@
         <v>357</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7107,7 +7136,7 @@
         <v>43788</v>
       </c>
       <c r="R79" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S79" s="13" t="s">
         <v>31</v>
@@ -7117,23 +7146,49 @@
       </c>
       <c r="U79" s="15"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+    <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A80" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
+      <c r="E80" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="I80" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J80" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K80" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="L80" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M80" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="N80" s="13" t="s">
+        <v>357</v>
+      </c>
       <c r="O80" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7141,54 +7196,32 @@
       <c r="Q80" s="14">
         <v>43788</v>
       </c>
-      <c r="R80" s="13"/>
-      <c r="S80" s="13"/>
-      <c r="T80" s="13"/>
+      <c r="R80" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="S80" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T80" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="U80" s="15"/>
     </row>
-    <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E81" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="G81" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H81" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J81" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="L81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="M81" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="N81" s="13" t="s">
-        <v>385</v>
-      </c>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13"/>
       <c r="O81" s="13" t="s">
         <v>63</v>
       </c>
@@ -7198,39 +7231,35 @@
       <c r="Q81" s="14">
         <v>43788</v>
       </c>
-      <c r="R81" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S81" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="T81" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R81" s="13"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="13"/>
       <c r="U81" s="15"/>
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D82" s="13"/>
+        <v>386</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>382</v>
+      </c>
       <c r="E82" s="20" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>214</v>
@@ -7263,7 +7292,7 @@
         <v>359</v>
       </c>
       <c r="S82" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T82" s="13" t="s">
         <v>279</v>
@@ -7272,26 +7301,26 @@
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>214</v>
@@ -7324,7 +7353,7 @@
         <v>359</v>
       </c>
       <c r="S83" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T83" s="13" t="s">
         <v>279</v>
@@ -7333,26 +7362,26 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="20" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>214</v>
@@ -7394,26 +7423,26 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="20" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>214</v>
@@ -7455,26 +7484,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>214</v>
@@ -7516,26 +7545,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>214</v>
@@ -7577,26 +7606,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>214</v>
@@ -7638,26 +7667,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>214</v>
@@ -7699,26 +7728,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>214</v>
@@ -7760,26 +7789,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>214</v>
@@ -7821,26 +7850,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>214</v>
@@ -7882,26 +7911,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>214</v>
@@ -7942,103 +7971,107 @@
       <c r="U93" s="15"/>
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D94" s="13"/>
+      <c r="E94" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F94" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G94" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J94" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K94" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="L94" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M94" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N94" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="O94" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P94" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q94" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R94" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="S94" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T94" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U94" s="15"/>
+    </row>
+    <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A95" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B94" s="12"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
-      <c r="J94" s="22"/>
-      <c r="K94" s="22"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="22"/>
-      <c r="O94" s="22"/>
-      <c r="P94" s="22"/>
-      <c r="Q94" s="22"/>
-      <c r="R94" s="22"/>
-      <c r="S94" s="22"/>
-      <c r="T94" s="22"/>
-      <c r="U94" s="22"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F95" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="G95" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H95" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I95" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J95" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K95" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="L95" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M95" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N95" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O95" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P95" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q95" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R95" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="S95" s="13"/>
-      <c r="T95" s="13"/>
-      <c r="U95" s="15"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="22"/>
+      <c r="K95" s="22"/>
+      <c r="L95" s="22"/>
+      <c r="M95" s="22"/>
+      <c r="N95" s="22"/>
+      <c r="O95" s="22"/>
+      <c r="P95" s="22"/>
+      <c r="Q95" s="22"/>
+      <c r="R95" s="22"/>
+      <c r="S95" s="22"/>
+      <c r="T95" s="22"/>
+      <c r="U95" s="22"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="B96" s="13"/>
       <c r="C96" s="13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="G96" s="13" t="s">
         <v>21</v>
@@ -8053,28 +8086,28 @@
         <v>23</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L96" s="13" t="s">
-        <v>123</v>
+        <v>451</v>
       </c>
       <c r="M96" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N96" s="13" t="s">
-        <v>456</v>
+        <v>26</v>
       </c>
       <c r="O96" s="13" t="s">
-        <v>457</v>
+        <v>27</v>
       </c>
       <c r="P96" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q96" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R96" s="13" t="s">
-        <v>30</v>
+        <v>453</v>
       </c>
       <c r="S96" s="13"/>
       <c r="T96" s="13"/>
@@ -8082,20 +8115,20 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="B97" s="13"/>
       <c r="C97" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="G97" s="13" t="s">
         <v>21</v>
@@ -8110,19 +8143,19 @@
         <v>23</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L97" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="M97" s="13" t="s">
-        <v>462</v>
+        <v>124</v>
       </c>
       <c r="N97" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O97" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P97" s="13" t="s">
         <v>42</v>
@@ -8139,20 +8172,20 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>21</v>
@@ -8167,19 +8200,19 @@
         <v>23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="N98" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="O98" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P98" s="13" t="s">
         <v>42</v>
@@ -8194,30 +8227,28 @@
       <c r="T98" s="13"/>
       <c r="U98" s="15"/>
     </row>
-    <row r="99" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B99" s="13" t="s">
-        <v>490</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="I99" s="13" t="s">
         <v>36</v>
@@ -8226,86 +8257,122 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="L99" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M99" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="N99" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="O99" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="P99" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q99" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R99" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="15"/>
+    </row>
+    <row r="100" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G100" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H100" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I100" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J100" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K100" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L99" s="13" t="s">
+      <c r="L100" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M99" s="13" t="s">
+      <c r="M100" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N99" s="13" t="s">
+      <c r="N100" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O99" s="13" t="s">
+      <c r="O100" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P99" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q99" s="14">
+      <c r="P100" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q100" s="14">
         <v>42118</v>
       </c>
-      <c r="R99" s="13" t="s">
+      <c r="R100" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S99" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T99" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U99" s="15"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100" s="10"/>
-      <c r="F100"/>
-      <c r="G100"/>
-      <c r="H100"/>
-      <c r="I100"/>
-      <c r="J100"/>
-      <c r="K100"/>
-      <c r="L100"/>
-      <c r="M100"/>
-      <c r="N100"/>
-      <c r="O100"/>
-      <c r="P100"/>
-      <c r="Q100"/>
-      <c r="R100"/>
-      <c r="S100"/>
-      <c r="T100"/>
-      <c r="U100"/>
+      <c r="S100" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T100" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U100" s="15"/>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="4"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="4"/>
-      <c r="S101" s="4"/>
-      <c r="T101" s="4"/>
-      <c r="U101" s="4"/>
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101" s="10"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="L101"/>
+      <c r="M101"/>
+      <c r="N101"/>
+      <c r="O101"/>
+      <c r="P101"/>
+      <c r="Q101"/>
+      <c r="R101"/>
+      <c r="S101"/>
+      <c r="T101"/>
+      <c r="U101"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="4"/>
@@ -8327,17 +8394,17 @@
       <c r="U102" s="4"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B103" s="4"/>
+      <c r="A103" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B103" s="3"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
-      <c r="K103" s="4"/>
+      <c r="K103" s="3"/>
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
@@ -8351,7 +8418,7 @@
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -8373,30 +8440,53 @@
       <c r="U104" s="4"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="4"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+      <c r="U105" s="4"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="H105" s="7"/>
-      <c r="I105" s="7"/>
-      <c r="J105" s="7"/>
-      <c r="K105" s="7"/>
-      <c r="L105" s="7"/>
-      <c r="M105" s="7"/>
-      <c r="N105" s="7"/>
-      <c r="O105" s="7"/>
-      <c r="P105" s="7"/>
-      <c r="R105" s="7"/>
-      <c r="S105" s="7"/>
-      <c r="T105" s="7"/>
-      <c r="U105" s="7"/>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="7"/>
+      <c r="M106" s="7"/>
+      <c r="N106" s="7"/>
+      <c r="O106" s="7"/>
+      <c r="P106" s="7"/>
+      <c r="R106" s="7"/>
+      <c r="S106" s="7"/>
+      <c r="T106" s="7"/>
+      <c r="U106" s="7"/>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #495 : [namespace-registry] add new namespace "apollo"
Issue #495 : [namespace-registry] add new namespace "apollo"

Add the namespace "apollo" to the Namespace Registry and the config.properties file.

@c-suh  [namespace-registry] add new namespace "apollo" #495

Resolves #495
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6FFC768-4134-41FA-9CE5-9893F96FF326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBA4DBA-16D7-4F59-B5DD-C6986DB38C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6623" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4577" uniqueCount="649">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1942,6 +1942,36 @@
   </si>
   <si>
     <t>Infrared Astronomical Satellite</t>
+  </si>
+  <si>
+    <t>apollo</t>
+  </si>
+  <si>
+    <t>mission/apollo</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/apollo/v1</t>
+  </si>
+  <si>
+    <t>APOLLO</t>
+  </si>
+  <si>
+    <t>J. Ward</t>
+  </si>
+  <si>
+    <t>Jennifer Ward</t>
+  </si>
+  <si>
+    <t>jgward at wustl.edu</t>
+  </si>
+  <si>
+    <t>The Apollo Mission Dictionary (apollo) contains classes, attributes and rules specific to the Apollo missions and their instruments.</t>
+  </si>
+  <si>
+    <t>Apollo</t>
+  </si>
+  <si>
+    <t>Balloon Observation Platform for Planetary Science</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2114,6 +2144,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2432,12 +2465,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U107"/>
+  <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4514,91 +4547,93 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>641</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="O36" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="P36" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q36" s="18">
+        <v>44791</v>
+      </c>
+      <c r="R36" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="S36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U36" s="19"/>
+    </row>
+    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
+      <c r="B37" s="13" t="s">
+        <v>648</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E37" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>215</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M36" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N36" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="O36" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="P36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q36" s="14">
-        <v>42089</v>
-      </c>
-      <c r="R36" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U36" s="15"/>
-    </row>
-    <row r="37" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
-        <v>493</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>494</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>496</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>493</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>493</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>527</v>
+        <v>218</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>214</v>
@@ -4607,28 +4642,28 @@
         <v>23</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
       <c r="O37" s="13" t="s">
-        <v>110</v>
+        <v>179</v>
       </c>
       <c r="P37" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q37" s="14">
-        <v>44329</v>
+        <v>42089</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>109</v>
+        <v>186</v>
       </c>
       <c r="S37" s="13" t="s">
         <v>31</v>
@@ -4638,30 +4673,30 @@
       </c>
       <c r="U37" s="15"/>
     </row>
-    <row r="38" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>523</v>
+        <v>493</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>523</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>525</v>
+        <v>493</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>495</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>523</v>
+        <v>493</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>214</v>
@@ -4688,7 +4723,7 @@
         <v>42</v>
       </c>
       <c r="Q38" s="14">
-        <v>44385</v>
+        <v>44329</v>
       </c>
       <c r="R38" s="13" t="s">
         <v>109</v>
@@ -4701,93 +4736,93 @@
       </c>
       <c r="U38" s="15"/>
     </row>
-    <row r="39" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>540</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="G39" s="17" t="s">
+    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>538</v>
-      </c>
-      <c r="I39" s="17" t="s">
+      <c r="H39" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="I39" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="J39" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="17" t="s">
-        <v>539</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>532</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>533</v>
-      </c>
-      <c r="P39" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q39" s="18">
-        <v>44426</v>
-      </c>
-      <c r="R39" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="S39" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T39" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U39" s="19"/>
+      <c r="K39" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="N39" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="O39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="P39" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>44385</v>
+      </c>
+      <c r="R39" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="S39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U39" s="15"/>
     </row>
     <row r="40" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>591</v>
+        <v>536</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>595</v>
+        <v>536</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>596</v>
+        <v>540</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>592</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>593</v>
+        <v>536</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>537</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>591</v>
+        <v>536</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>594</v>
+        <v>538</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>214</v>
@@ -4796,28 +4831,28 @@
         <v>23</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>169</v>
+        <v>539</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="N40" s="17" t="s">
-        <v>587</v>
+        <v>532</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>588</v>
+        <v>533</v>
       </c>
       <c r="P40" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q40" s="18">
-        <v>44707</v>
+        <v>44426</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>597</v>
+        <v>186</v>
       </c>
       <c r="S40" s="17" t="s">
         <v>31</v>
@@ -4827,60 +4862,60 @@
       </c>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>221</v>
+        <v>591</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>625</v>
+        <v>595</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>225</v>
+        <v>596</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>521</v>
+        <v>592</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>593</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>221</v>
+        <v>591</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>223</v>
+        <v>594</v>
       </c>
       <c r="I41" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J41" s="17" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>224</v>
+        <v>169</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>40</v>
+        <v>587</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>41</v>
+        <v>588</v>
       </c>
       <c r="P41" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q41" s="18">
-        <v>44193</v>
+        <v>44707</v>
       </c>
       <c r="R41" s="17" t="s">
-        <v>522</v>
+        <v>597</v>
       </c>
       <c r="S41" s="17" t="s">
         <v>31</v>
@@ -4890,60 +4925,60 @@
       </c>
       <c r="U41" s="19"/>
     </row>
-    <row r="42" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>631</v>
+        <v>221</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>637</v>
+        <v>225</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>632</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>633</v>
+        <v>222</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>521</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>631</v>
+        <v>221</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>636</v>
+        <v>223</v>
       </c>
       <c r="I42" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J42" s="17" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>539</v>
+        <v>224</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>219</v>
+        <v>33</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="N42" s="17" t="s">
-        <v>616</v>
+        <v>40</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>635</v>
+        <v>41</v>
       </c>
       <c r="P42" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q42" s="18">
-        <v>44735</v>
+        <v>44193</v>
       </c>
       <c r="R42" s="17" t="s">
-        <v>634</v>
+        <v>522</v>
       </c>
       <c r="S42" s="17" t="s">
         <v>31</v>
@@ -4955,154 +4990,154 @@
     </row>
     <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>568</v>
+        <v>638</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>567</v>
+        <v>637</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>569</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>547</v>
+        <v>632</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>633</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>548</v>
+        <v>21</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>542</v>
+        <v>636</v>
       </c>
       <c r="I43" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J43" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="O43" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="P43" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q43" s="18">
+        <v>44735</v>
+      </c>
+      <c r="R43" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="S43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U43" s="19"/>
+    </row>
+    <row r="44" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>542</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J44" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K44" s="17" t="s">
         <v>566</v>
       </c>
-      <c r="L43" s="17" t="s">
+      <c r="L44" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="M43" s="17" t="s">
+      <c r="M44" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="N43" s="17" t="s">
+      <c r="N44" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="O43" s="17" t="s">
+      <c r="O44" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="P43" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q43" s="18">
+      <c r="P44" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q44" s="18">
         <v>44426</v>
       </c>
-      <c r="R43" s="17" t="s">
+      <c r="R44" s="17" t="s">
         <v>545</v>
       </c>
-      <c r="S43" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T43" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U43" s="19"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>618</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M44" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="N44" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="O44" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="P44" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q44" s="14">
-        <v>42119</v>
-      </c>
-      <c r="R44" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="S44" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T44" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U44" s="15"/>
+      <c r="S44" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T44" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U44" s="19"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>235</v>
+        <v>618</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I45" s="13" t="s">
         <v>214</v>
@@ -5111,28 +5146,28 @@
         <v>23</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="O45" s="13" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="P45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q45" s="14">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R45" s="13" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="S45" s="13" t="s">
         <v>31</v>
@@ -5150,13 +5185,13 @@
         <v>235</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>232</v>
@@ -5205,93 +5240,93 @@
       </c>
       <c r="U46" s="15"/>
     </row>
-    <row r="47" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>563</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>564</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="G47" s="17" t="s">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="I47" s="17" t="s">
+      <c r="H47" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="I47" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K47" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="L47" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M47" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N47" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="O47" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="P47" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q47" s="18">
-        <v>44608</v>
-      </c>
-      <c r="R47" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="S47" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T47" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U47" s="19"/>
+      <c r="K47" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M47" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N47" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="O47" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="P47" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q47" s="14">
+        <v>41837</v>
+      </c>
+      <c r="R47" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="S47" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U47" s="15"/>
     </row>
     <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>516</v>
+        <v>563</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>513</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>514</v>
+        <v>560</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>564</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>517</v>
+        <v>565</v>
       </c>
       <c r="I48" s="17" t="s">
         <v>214</v>
@@ -5300,7 +5335,7 @@
         <v>23</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>515</v>
+        <v>565</v>
       </c>
       <c r="L48" s="17" t="s">
         <v>123</v>
@@ -5318,7 +5353,7 @@
         <v>42</v>
       </c>
       <c r="Q48" s="18">
-        <v>44333</v>
+        <v>44608</v>
       </c>
       <c r="R48" s="17" t="s">
         <v>194</v>
@@ -5331,93 +5366,93 @@
       </c>
       <c r="U48" s="19"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>620</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="F49" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="G49" s="13" t="s">
+    <row r="49" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="G49" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>518</v>
-      </c>
-      <c r="I49" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="I49" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="J49" s="13" t="s">
+      <c r="J49" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K49" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="L49" s="13" t="s">
+      <c r="K49" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="L49" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M49" s="13" t="s">
+      <c r="M49" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="N49" s="13" t="s">
+      <c r="N49" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="O49" s="13" t="s">
+      <c r="O49" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P49" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q49" s="14">
-        <v>43935</v>
-      </c>
-      <c r="R49" s="13" t="s">
+      <c r="P49" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" s="18">
+        <v>44333</v>
+      </c>
+      <c r="R49" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="S49" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T49" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U49" s="15"/>
+      <c r="S49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U49" s="19"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>242</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>214</v>
@@ -5426,28 +5461,28 @@
         <v>23</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="M50" s="13" t="s">
-        <v>108</v>
+        <v>244</v>
       </c>
       <c r="N50" s="13" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="O50" s="13" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="P50" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q50" s="14">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="S50" s="13" t="s">
         <v>31</v>
@@ -5459,28 +5494,28 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>214</v>
@@ -5489,7 +5524,7 @@
         <v>23</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="L51" s="13" t="s">
         <v>107</v>
@@ -5507,10 +5542,10 @@
         <v>42</v>
       </c>
       <c r="Q51" s="14">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>31</v>
@@ -5522,28 +5557,28 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H52" s="13" t="s">
-        <v>260</v>
+      <c r="H52" s="17" t="s">
+        <v>520</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>214</v>
@@ -5552,28 +5587,28 @@
         <v>23</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="M52" s="13" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="N52" s="13" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="O52" s="13" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="P52" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q52" s="14">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R52" s="13" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="S52" s="13" t="s">
         <v>31</v>
@@ -5591,13 +5626,13 @@
         <v>619</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F53" s="13" t="s">
         <v>257</v>
@@ -5646,93 +5681,93 @@
       </c>
       <c r="U53" s="15"/>
     </row>
-    <row r="54" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M54" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N54" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O54" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P54" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q54" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R54" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="S54" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T54" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U54" s="15"/>
+    </row>
+    <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B55" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C55" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D55" s="17" t="s">
         <v>608</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E55" s="21" t="s">
         <v>609</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F55" s="17" t="s">
         <v>607</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>612</v>
-      </c>
-      <c r="I54" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="17" t="s">
-        <v>613</v>
-      </c>
-      <c r="L54" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M54" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N54" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="O54" s="17" t="s">
-        <v>617</v>
-      </c>
-      <c r="P54" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q54" s="18">
-        <v>44713</v>
-      </c>
-      <c r="R54" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="S54" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T54" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U54" s="19"/>
-    </row>
-    <row r="55" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>552</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>553</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>555</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>214</v>
@@ -5741,28 +5776,28 @@
         <v>23</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="L55" s="17" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="M55" s="17" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N55" s="17" t="s">
-        <v>269</v>
+        <v>616</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>270</v>
+        <v>617</v>
       </c>
       <c r="P55" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q55" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="S55" s="17" t="s">
         <v>31</v>
@@ -5772,30 +5807,30 @@
       </c>
       <c r="U55" s="19"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>214</v>
@@ -5804,7 +5839,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="L56" s="17" t="s">
         <v>219</v>
@@ -5813,19 +5848,19 @@
         <v>177</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>576</v>
+        <v>270</v>
       </c>
       <c r="P56" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q56" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>186</v>
+        <v>556</v>
       </c>
       <c r="S56" s="17" t="s">
         <v>31</v>
@@ -5835,30 +5870,30 @@
       </c>
       <c r="U56" s="19"/>
     </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>604</v>
+        <v>577</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>214</v>
@@ -5867,7 +5902,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>219</v>
@@ -5876,115 +5911,115 @@
         <v>177</v>
       </c>
       <c r="N57" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="O57" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="P57" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q57" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R57" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="S57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U57" s="19"/>
+    </row>
+    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J58" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K58" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N58" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="O57" s="17" t="s">
+      <c r="O58" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="P57" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q57" s="18">
+      <c r="P58" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58" s="18">
         <v>44713</v>
       </c>
-      <c r="R57" s="17" t="s">
+      <c r="R58" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="S57" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T57" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U57" s="19"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J58" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K58" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="L58" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M58" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N58" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="O58" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="P58" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q58" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R58" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S58" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T58" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U58" s="15"/>
+      <c r="S58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U58" s="19"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>582</v>
+        <v>626</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>583</v>
+        <v>271</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>585</v>
+        <v>266</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="G59" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>589</v>
+        <v>42</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>214</v>
@@ -5993,28 +6028,28 @@
         <v>23</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>586</v>
+        <v>268</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>587</v>
+        <v>269</v>
       </c>
       <c r="O59" s="13" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="P59" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q59" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R59" s="13" t="s">
-        <v>590</v>
+        <v>186</v>
       </c>
       <c r="S59" s="13" t="s">
         <v>31</v>
@@ -6024,91 +6059,93 @@
       </c>
       <c r="U59" s="15"/>
     </row>
-    <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>627</v>
+        <v>582</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>273</v>
+        <v>584</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>275</v>
+        <v>589</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K60" s="13" t="s">
-        <v>272</v>
+        <v>586</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="M60" s="13" t="s">
-        <v>272</v>
+        <v>170</v>
       </c>
       <c r="N60" s="13" t="s">
-        <v>276</v>
+        <v>587</v>
       </c>
       <c r="O60" s="13" t="s">
-        <v>277</v>
+        <v>588</v>
       </c>
       <c r="P60" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q60" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R60" s="13" t="s">
-        <v>65</v>
+        <v>590</v>
       </c>
       <c r="S60" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T60" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="U60" s="15"/>
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D61" s="13"/>
+        <v>278</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="E61" s="20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>214</v>
@@ -6129,7 +6166,7 @@
         <v>276</v>
       </c>
       <c r="O61" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P61" s="13" t="s">
         <v>42</v>
@@ -6138,10 +6175,10 @@
         <v>43788</v>
       </c>
       <c r="R61" s="13" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="S61" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T61" s="13" t="s">
         <v>279</v>
@@ -6150,26 +6187,26 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="20" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>214</v>
@@ -6177,9 +6214,15 @@
       <c r="J62" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
+      <c r="K62" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L62" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="M62" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="N62" s="13" t="s">
         <v>276</v>
       </c>
@@ -6196,7 +6239,7 @@
         <v>286</v>
       </c>
       <c r="S62" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T62" s="13" t="s">
         <v>279</v>
@@ -6205,26 +6248,26 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>214</v>
@@ -6251,7 +6294,7 @@
         <v>286</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T63" s="13" t="s">
         <v>279</v>
@@ -6260,26 +6303,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>214</v>
@@ -6315,26 +6358,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>214</v>
@@ -6370,26 +6413,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>214</v>
@@ -6425,26 +6468,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>214</v>
@@ -6480,26 +6523,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>214</v>
@@ -6535,26 +6578,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>214</v>
@@ -6590,26 +6633,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>214</v>
@@ -6645,26 +6688,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>214</v>
@@ -6700,26 +6743,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>214</v>
@@ -6755,26 +6798,26 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>214</v>
@@ -6810,141 +6853,139 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="D74" s="13" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>21</v>
+        <v>274</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J74" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="O74" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="P74" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q74" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R74" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="S74" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T74" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U74" s="15"/>
+    </row>
+    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E75" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G75" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J75" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K74" s="13" t="s">
+      <c r="K75" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="L74" s="13" t="s">
+      <c r="L75" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="M74" s="13" t="s">
+      <c r="M75" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="N74" s="13" t="s">
+      <c r="N75" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="O74" s="13" t="s">
+      <c r="O75" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="P74" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q74" s="14">
+      <c r="P75" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q75" s="14">
         <v>44111</v>
       </c>
-      <c r="R74" s="13" t="s">
+      <c r="R75" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="S74" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T74" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U74" s="15"/>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q75" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R75" s="13"/>
-      <c r="S75" s="13"/>
-      <c r="T75" s="13"/>
+      <c r="S75" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T75" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U75" s="15"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B76" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="F76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G76" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H76" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="I76" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J76" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="L76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="M76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="N76" s="13" t="s">
-        <v>357</v>
-      </c>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
       <c r="O76" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P76" s="13" t="s">
         <v>42</v>
@@ -6952,39 +6993,35 @@
       <c r="Q76" s="14">
         <v>43788</v>
       </c>
-      <c r="R76" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S76" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T76" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R76" s="13"/>
+      <c r="S76" s="13"/>
+      <c r="T76" s="13"/>
       <c r="U76" s="15"/>
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D77" s="13"/>
+        <v>358</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>354</v>
+      </c>
       <c r="E77" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I77" s="13" t="s">
         <v>214</v>
@@ -7005,7 +7042,7 @@
         <v>357</v>
       </c>
       <c r="O77" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>42</v>
@@ -7014,7 +7051,7 @@
         <v>43788</v>
       </c>
       <c r="R77" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S77" s="13" t="s">
         <v>31</v>
@@ -7026,26 +7063,26 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="20" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>214</v>
@@ -7066,7 +7103,7 @@
         <v>357</v>
       </c>
       <c r="O78" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P78" s="13" t="s">
         <v>42</v>
@@ -7075,7 +7112,7 @@
         <v>43788</v>
       </c>
       <c r="R78" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="S78" s="13" t="s">
         <v>31</v>
@@ -7087,26 +7124,26 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>214</v>
@@ -7148,26 +7185,26 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>214</v>
@@ -7188,7 +7225,7 @@
         <v>357</v>
       </c>
       <c r="O80" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7197,7 +7234,7 @@
         <v>43788</v>
       </c>
       <c r="R80" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S80" s="13" t="s">
         <v>31</v>
@@ -7207,23 +7244,49 @@
       </c>
       <c r="U80" s="15"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+    <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
+      <c r="E81" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K81" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="L81" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M81" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="N81" s="13" t="s">
+        <v>357</v>
+      </c>
       <c r="O81" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P81" s="13" t="s">
         <v>42</v>
@@ -7231,54 +7294,32 @@
       <c r="Q81" s="14">
         <v>43788</v>
       </c>
-      <c r="R81" s="13"/>
-      <c r="S81" s="13"/>
-      <c r="T81" s="13"/>
+      <c r="R81" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="S81" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T81" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="U81" s="15"/>
     </row>
-    <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B82" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C82" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="D82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E82" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="F82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="G82" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H82" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J82" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="L82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="M82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="N82" s="13" t="s">
-        <v>385</v>
-      </c>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13"/>
       <c r="O82" s="13" t="s">
         <v>63</v>
       </c>
@@ -7288,39 +7329,35 @@
       <c r="Q82" s="14">
         <v>43788</v>
       </c>
-      <c r="R82" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S82" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="T82" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R82" s="13"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="13"/>
       <c r="U82" s="15"/>
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D83" s="13"/>
+        <v>386</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>382</v>
+      </c>
       <c r="E83" s="20" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>214</v>
@@ -7353,7 +7390,7 @@
         <v>359</v>
       </c>
       <c r="S83" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T83" s="13" t="s">
         <v>279</v>
@@ -7362,26 +7399,26 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>214</v>
@@ -7414,7 +7451,7 @@
         <v>359</v>
       </c>
       <c r="S84" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T84" s="13" t="s">
         <v>279</v>
@@ -7423,26 +7460,26 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="20" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>214</v>
@@ -7484,26 +7521,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>214</v>
@@ -7545,26 +7582,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>214</v>
@@ -7606,26 +7643,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>214</v>
@@ -7667,26 +7704,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>214</v>
@@ -7728,26 +7765,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>214</v>
@@ -7789,26 +7826,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>214</v>
@@ -7850,26 +7887,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>214</v>
@@ -7911,26 +7948,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>214</v>
@@ -7972,26 +8009,26 @@
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>214</v>
@@ -8032,103 +8069,107 @@
       <c r="U94" s="15"/>
     </row>
     <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D95" s="13"/>
+      <c r="E95" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F95" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I95" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J95" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K95" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="L95" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M95" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N95" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="O95" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P95" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q95" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R95" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="S95" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T95" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U95" s="15"/>
+    </row>
+    <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A96" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B95" s="12"/>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="22"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
-      <c r="J95" s="22"/>
-      <c r="K95" s="22"/>
-      <c r="L95" s="22"/>
-      <c r="M95" s="22"/>
-      <c r="N95" s="22"/>
-      <c r="O95" s="22"/>
-      <c r="P95" s="22"/>
-      <c r="Q95" s="22"/>
-      <c r="R95" s="22"/>
-      <c r="S95" s="22"/>
-      <c r="T95" s="22"/>
-      <c r="U95" s="22"/>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I96" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J96" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K96" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="L96" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M96" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N96" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O96" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P96" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q96" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R96" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="S96" s="13"/>
-      <c r="T96" s="13"/>
-      <c r="U96" s="15"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="22"/>
+      <c r="J96" s="22"/>
+      <c r="K96" s="22"/>
+      <c r="L96" s="22"/>
+      <c r="M96" s="22"/>
+      <c r="N96" s="22"/>
+      <c r="O96" s="22"/>
+      <c r="P96" s="22"/>
+      <c r="Q96" s="22"/>
+      <c r="R96" s="22"/>
+      <c r="S96" s="22"/>
+      <c r="T96" s="22"/>
+      <c r="U96" s="22"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="B97" s="13"/>
       <c r="C97" s="13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="G97" s="13" t="s">
         <v>21</v>
@@ -8143,28 +8184,28 @@
         <v>23</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L97" s="13" t="s">
-        <v>123</v>
+        <v>451</v>
       </c>
       <c r="M97" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N97" s="13" t="s">
-        <v>456</v>
+        <v>26</v>
       </c>
       <c r="O97" s="13" t="s">
-        <v>457</v>
+        <v>27</v>
       </c>
       <c r="P97" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q97" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R97" s="13" t="s">
-        <v>30</v>
+        <v>453</v>
       </c>
       <c r="S97" s="13"/>
       <c r="T97" s="13"/>
@@ -8172,20 +8213,20 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>21</v>
@@ -8200,19 +8241,19 @@
         <v>23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>462</v>
+        <v>124</v>
       </c>
       <c r="N98" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O98" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P98" s="13" t="s">
         <v>42</v>
@@ -8229,20 +8270,20 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
@@ -8257,19 +8298,19 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="N99" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="O99" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P99" s="13" t="s">
         <v>42</v>
@@ -8284,30 +8325,28 @@
       <c r="T99" s="13"/>
       <c r="U99" s="15"/>
     </row>
-    <row r="100" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B100" s="13" t="s">
-        <v>490</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="I100" s="13" t="s">
         <v>36</v>
@@ -8316,86 +8355,122 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="L100" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M100" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="N100" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="O100" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="P100" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q100" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R100" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="15"/>
+    </row>
+    <row r="101" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G101" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I101" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J101" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K101" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L100" s="13" t="s">
+      <c r="L101" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M100" s="13" t="s">
+      <c r="M101" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N100" s="13" t="s">
+      <c r="N101" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O100" s="13" t="s">
+      <c r="O101" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P100" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q100" s="14">
+      <c r="P101" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q101" s="14">
         <v>42118</v>
       </c>
-      <c r="R100" s="13" t="s">
+      <c r="R101" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S100" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T100" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U100" s="15"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-      <c r="D101"/>
-      <c r="E101" s="10"/>
-      <c r="F101"/>
-      <c r="G101"/>
-      <c r="H101"/>
-      <c r="I101"/>
-      <c r="J101"/>
-      <c r="K101"/>
-      <c r="L101"/>
-      <c r="M101"/>
-      <c r="N101"/>
-      <c r="O101"/>
-      <c r="P101"/>
-      <c r="Q101"/>
-      <c r="R101"/>
-      <c r="S101"/>
-      <c r="T101"/>
-      <c r="U101"/>
+      <c r="S101" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T101" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U101" s="15"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="4"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="4"/>
-      <c r="S102" s="4"/>
-      <c r="T102" s="4"/>
-      <c r="U102" s="4"/>
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102" s="10"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="L102"/>
+      <c r="M102"/>
+      <c r="N102"/>
+      <c r="O102"/>
+      <c r="P102"/>
+      <c r="Q102"/>
+      <c r="R102"/>
+      <c r="S102"/>
+      <c r="T102"/>
+      <c r="U102"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="4"/>
@@ -8417,17 +8492,17 @@
       <c r="U103" s="4"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B104" s="4"/>
+      <c r="A104" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B104" s="3"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
-      <c r="K104" s="4"/>
+      <c r="K104" s="3"/>
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
@@ -8441,7 +8516,7 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -8463,30 +8538,53 @@
       <c r="U105" s="4"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="4"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+      <c r="U106" s="4"/>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A107" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
-      <c r="J106" s="7"/>
-      <c r="K106" s="7"/>
-      <c r="L106" s="7"/>
-      <c r="M106" s="7"/>
-      <c r="N106" s="7"/>
-      <c r="O106" s="7"/>
-      <c r="P106" s="7"/>
-      <c r="R106" s="7"/>
-      <c r="S106" s="7"/>
-      <c r="T106" s="7"/>
-      <c r="U106" s="7"/>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="7"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="7"/>
+      <c r="P107" s="7"/>
+      <c r="R107" s="7"/>
+      <c r="S107" s="7"/>
+      <c r="T107" s="7"/>
+      <c r="U107" s="7"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #495 : [namespace-registry] add new namespace "apollo" (#496)
Issue #495 : [namespace-registry] add new namespace "apollo"

Add the namespace "apollo" to the Namespace Registry and the config.properties file.

@c-suh  [namespace-registry] add new namespace "apollo" #495

Resolves #495

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6FFC768-4134-41FA-9CE5-9893F96FF326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBA4DBA-16D7-4F59-B5DD-C6986DB38C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6623" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4577" uniqueCount="649">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1942,6 +1942,36 @@
   </si>
   <si>
     <t>Infrared Astronomical Satellite</t>
+  </si>
+  <si>
+    <t>apollo</t>
+  </si>
+  <si>
+    <t>mission/apollo</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/apollo/v1</t>
+  </si>
+  <si>
+    <t>APOLLO</t>
+  </si>
+  <si>
+    <t>J. Ward</t>
+  </si>
+  <si>
+    <t>Jennifer Ward</t>
+  </si>
+  <si>
+    <t>jgward at wustl.edu</t>
+  </si>
+  <si>
+    <t>The Apollo Mission Dictionary (apollo) contains classes, attributes and rules specific to the Apollo missions and their instruments.</t>
+  </si>
+  <si>
+    <t>Apollo</t>
+  </si>
+  <si>
+    <t>Balloon Observation Platform for Planetary Science</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2114,6 +2144,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2432,12 +2465,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U107"/>
+  <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4514,91 +4547,93 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>641</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="O36" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="P36" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q36" s="18">
+        <v>44791</v>
+      </c>
+      <c r="R36" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="S36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U36" s="19"/>
+    </row>
+    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
+      <c r="B37" s="13" t="s">
+        <v>648</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E37" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>215</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M36" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N36" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="O36" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="P36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q36" s="14">
-        <v>42089</v>
-      </c>
-      <c r="R36" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U36" s="15"/>
-    </row>
-    <row r="37" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
-        <v>493</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>494</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>496</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>493</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>493</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>527</v>
+        <v>218</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>214</v>
@@ -4607,28 +4642,28 @@
         <v>23</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
       <c r="O37" s="13" t="s">
-        <v>110</v>
+        <v>179</v>
       </c>
       <c r="P37" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q37" s="14">
-        <v>44329</v>
+        <v>42089</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>109</v>
+        <v>186</v>
       </c>
       <c r="S37" s="13" t="s">
         <v>31</v>
@@ -4638,30 +4673,30 @@
       </c>
       <c r="U37" s="15"/>
     </row>
-    <row r="38" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>523</v>
+        <v>493</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>523</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>525</v>
+        <v>493</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>495</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>523</v>
+        <v>493</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>214</v>
@@ -4688,7 +4723,7 @@
         <v>42</v>
       </c>
       <c r="Q38" s="14">
-        <v>44385</v>
+        <v>44329</v>
       </c>
       <c r="R38" s="13" t="s">
         <v>109</v>
@@ -4701,93 +4736,93 @@
       </c>
       <c r="U38" s="15"/>
     </row>
-    <row r="39" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>540</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="G39" s="17" t="s">
+    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>538</v>
-      </c>
-      <c r="I39" s="17" t="s">
+      <c r="H39" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="I39" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="J39" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="17" t="s">
-        <v>539</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>532</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>533</v>
-      </c>
-      <c r="P39" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q39" s="18">
-        <v>44426</v>
-      </c>
-      <c r="R39" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="S39" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T39" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U39" s="19"/>
+      <c r="K39" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="N39" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="O39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="P39" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>44385</v>
+      </c>
+      <c r="R39" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="S39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U39" s="15"/>
     </row>
     <row r="40" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>591</v>
+        <v>536</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>595</v>
+        <v>536</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>596</v>
+        <v>540</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>592</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>593</v>
+        <v>536</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>537</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>591</v>
+        <v>536</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>594</v>
+        <v>538</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>214</v>
@@ -4796,28 +4831,28 @@
         <v>23</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>169</v>
+        <v>539</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="N40" s="17" t="s">
-        <v>587</v>
+        <v>532</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>588</v>
+        <v>533</v>
       </c>
       <c r="P40" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q40" s="18">
-        <v>44707</v>
+        <v>44426</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>597</v>
+        <v>186</v>
       </c>
       <c r="S40" s="17" t="s">
         <v>31</v>
@@ -4827,60 +4862,60 @@
       </c>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>221</v>
+        <v>591</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>625</v>
+        <v>595</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>225</v>
+        <v>596</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>521</v>
+        <v>592</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>593</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>221</v>
+        <v>591</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>223</v>
+        <v>594</v>
       </c>
       <c r="I41" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J41" s="17" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>224</v>
+        <v>169</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>40</v>
+        <v>587</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>41</v>
+        <v>588</v>
       </c>
       <c r="P41" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q41" s="18">
-        <v>44193</v>
+        <v>44707</v>
       </c>
       <c r="R41" s="17" t="s">
-        <v>522</v>
+        <v>597</v>
       </c>
       <c r="S41" s="17" t="s">
         <v>31</v>
@@ -4890,60 +4925,60 @@
       </c>
       <c r="U41" s="19"/>
     </row>
-    <row r="42" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>631</v>
+        <v>221</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>637</v>
+        <v>225</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>632</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>633</v>
+        <v>222</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>521</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>631</v>
+        <v>221</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>636</v>
+        <v>223</v>
       </c>
       <c r="I42" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J42" s="17" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>539</v>
+        <v>224</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>219</v>
+        <v>33</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="N42" s="17" t="s">
-        <v>616</v>
+        <v>40</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>635</v>
+        <v>41</v>
       </c>
       <c r="P42" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q42" s="18">
-        <v>44735</v>
+        <v>44193</v>
       </c>
       <c r="R42" s="17" t="s">
-        <v>634</v>
+        <v>522</v>
       </c>
       <c r="S42" s="17" t="s">
         <v>31</v>
@@ -4955,154 +4990,154 @@
     </row>
     <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>568</v>
+        <v>638</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>567</v>
+        <v>637</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>569</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>547</v>
+        <v>632</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>633</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>566</v>
+        <v>631</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>548</v>
+        <v>21</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>542</v>
+        <v>636</v>
       </c>
       <c r="I43" s="17" t="s">
         <v>214</v>
       </c>
       <c r="J43" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="O43" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="P43" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q43" s="18">
+        <v>44735</v>
+      </c>
+      <c r="R43" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="S43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T43" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U43" s="19"/>
+    </row>
+    <row r="44" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>542</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J44" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K44" s="17" t="s">
         <v>566</v>
       </c>
-      <c r="L43" s="17" t="s">
+      <c r="L44" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="M43" s="17" t="s">
+      <c r="M44" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="N43" s="17" t="s">
+      <c r="N44" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="O43" s="17" t="s">
+      <c r="O44" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="P43" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q43" s="18">
+      <c r="P44" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q44" s="18">
         <v>44426</v>
       </c>
-      <c r="R43" s="17" t="s">
+      <c r="R44" s="17" t="s">
         <v>545</v>
       </c>
-      <c r="S43" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T43" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U43" s="19"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>618</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M44" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="N44" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="O44" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="P44" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q44" s="14">
-        <v>42119</v>
-      </c>
-      <c r="R44" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="S44" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T44" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U44" s="15"/>
+      <c r="S44" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T44" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U44" s="19"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>235</v>
+        <v>618</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I45" s="13" t="s">
         <v>214</v>
@@ -5111,28 +5146,28 @@
         <v>23</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="O45" s="13" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="P45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q45" s="14">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="R45" s="13" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="S45" s="13" t="s">
         <v>31</v>
@@ -5150,13 +5185,13 @@
         <v>235</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>232</v>
@@ -5205,93 +5240,93 @@
       </c>
       <c r="U46" s="15"/>
     </row>
-    <row r="47" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>563</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>564</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>560</v>
-      </c>
-      <c r="G47" s="17" t="s">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="I47" s="17" t="s">
+      <c r="H47" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="I47" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K47" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="L47" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M47" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N47" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="O47" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="P47" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q47" s="18">
-        <v>44608</v>
-      </c>
-      <c r="R47" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="S47" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T47" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U47" s="19"/>
+      <c r="K47" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M47" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N47" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="O47" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="P47" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q47" s="14">
+        <v>41837</v>
+      </c>
+      <c r="R47" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="S47" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U47" s="15"/>
     </row>
     <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>516</v>
+        <v>563</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>513</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>514</v>
+        <v>560</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>564</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>517</v>
+        <v>565</v>
       </c>
       <c r="I48" s="17" t="s">
         <v>214</v>
@@ -5300,7 +5335,7 @@
         <v>23</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>515</v>
+        <v>565</v>
       </c>
       <c r="L48" s="17" t="s">
         <v>123</v>
@@ -5318,7 +5353,7 @@
         <v>42</v>
       </c>
       <c r="Q48" s="18">
-        <v>44333</v>
+        <v>44608</v>
       </c>
       <c r="R48" s="17" t="s">
         <v>194</v>
@@ -5331,93 +5366,93 @@
       </c>
       <c r="U48" s="19"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>620</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="F49" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="G49" s="13" t="s">
+    <row r="49" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="G49" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>518</v>
-      </c>
-      <c r="I49" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="I49" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="J49" s="13" t="s">
+      <c r="J49" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K49" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="L49" s="13" t="s">
+      <c r="K49" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="L49" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M49" s="13" t="s">
+      <c r="M49" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="N49" s="13" t="s">
+      <c r="N49" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="O49" s="13" t="s">
+      <c r="O49" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P49" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q49" s="14">
-        <v>43935</v>
-      </c>
-      <c r="R49" s="13" t="s">
+      <c r="P49" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" s="18">
+        <v>44333</v>
+      </c>
+      <c r="R49" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="S49" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T49" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U49" s="15"/>
+      <c r="S49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U49" s="19"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>242</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>214</v>
@@ -5426,28 +5461,28 @@
         <v>23</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="M50" s="13" t="s">
-        <v>108</v>
+        <v>244</v>
       </c>
       <c r="N50" s="13" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="O50" s="13" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="P50" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q50" s="14">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="S50" s="13" t="s">
         <v>31</v>
@@ -5459,28 +5494,28 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>214</v>
@@ -5489,7 +5524,7 @@
         <v>23</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="L51" s="13" t="s">
         <v>107</v>
@@ -5507,10 +5542,10 @@
         <v>42</v>
       </c>
       <c r="Q51" s="14">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>31</v>
@@ -5522,28 +5557,28 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H52" s="13" t="s">
-        <v>260</v>
+      <c r="H52" s="17" t="s">
+        <v>520</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>214</v>
@@ -5552,28 +5587,28 @@
         <v>23</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="M52" s="13" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="N52" s="13" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="O52" s="13" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="P52" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q52" s="14">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="R52" s="13" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="S52" s="13" t="s">
         <v>31</v>
@@ -5591,13 +5626,13 @@
         <v>619</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F53" s="13" t="s">
         <v>257</v>
@@ -5646,93 +5681,93 @@
       </c>
       <c r="U53" s="15"/>
     </row>
-    <row r="54" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M54" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N54" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O54" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P54" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q54" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R54" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="S54" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T54" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U54" s="15"/>
+    </row>
+    <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B55" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C55" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D55" s="17" t="s">
         <v>608</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E55" s="21" t="s">
         <v>609</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F55" s="17" t="s">
         <v>607</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>612</v>
-      </c>
-      <c r="I54" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="17" t="s">
-        <v>613</v>
-      </c>
-      <c r="L54" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M54" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="N54" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="O54" s="17" t="s">
-        <v>617</v>
-      </c>
-      <c r="P54" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q54" s="18">
-        <v>44713</v>
-      </c>
-      <c r="R54" s="17" t="s">
-        <v>616</v>
-      </c>
-      <c r="S54" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T54" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U54" s="19"/>
-    </row>
-    <row r="55" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>552</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>553</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>555</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>214</v>
@@ -5741,28 +5776,28 @@
         <v>23</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="L55" s="17" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="M55" s="17" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N55" s="17" t="s">
-        <v>269</v>
+        <v>616</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>270</v>
+        <v>617</v>
       </c>
       <c r="P55" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q55" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="S55" s="17" t="s">
         <v>31</v>
@@ -5772,30 +5807,30 @@
       </c>
       <c r="U55" s="19"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>214</v>
@@ -5804,7 +5839,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="L56" s="17" t="s">
         <v>219</v>
@@ -5813,19 +5848,19 @@
         <v>177</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>576</v>
+        <v>270</v>
       </c>
       <c r="P56" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q56" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>186</v>
+        <v>556</v>
       </c>
       <c r="S56" s="17" t="s">
         <v>31</v>
@@ -5835,30 +5870,30 @@
       </c>
       <c r="U56" s="19"/>
     </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>604</v>
+        <v>577</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>214</v>
@@ -5867,7 +5902,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>219</v>
@@ -5876,115 +5911,115 @@
         <v>177</v>
       </c>
       <c r="N57" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="O57" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="P57" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q57" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R57" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="S57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U57" s="19"/>
+    </row>
+    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J58" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K58" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N58" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="O57" s="17" t="s">
+      <c r="O58" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="P57" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q57" s="18">
+      <c r="P58" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58" s="18">
         <v>44713</v>
       </c>
-      <c r="R57" s="17" t="s">
+      <c r="R58" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="S57" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T57" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U57" s="19"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J58" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K58" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="L58" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M58" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N58" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="O58" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="P58" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q58" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R58" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S58" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T58" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U58" s="15"/>
+      <c r="S58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U58" s="19"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>582</v>
+        <v>626</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>583</v>
+        <v>271</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>585</v>
+        <v>266</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="G59" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>589</v>
+        <v>42</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>214</v>
@@ -5993,28 +6028,28 @@
         <v>23</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>586</v>
+        <v>268</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>587</v>
+        <v>269</v>
       </c>
       <c r="O59" s="13" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="P59" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q59" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R59" s="13" t="s">
-        <v>590</v>
+        <v>186</v>
       </c>
       <c r="S59" s="13" t="s">
         <v>31</v>
@@ -6024,91 +6059,93 @@
       </c>
       <c r="U59" s="15"/>
     </row>
-    <row r="60" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>627</v>
+        <v>582</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>273</v>
+        <v>584</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>275</v>
+        <v>589</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K60" s="13" t="s">
-        <v>272</v>
+        <v>586</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="M60" s="13" t="s">
-        <v>272</v>
+        <v>170</v>
       </c>
       <c r="N60" s="13" t="s">
-        <v>276</v>
+        <v>587</v>
       </c>
       <c r="O60" s="13" t="s">
-        <v>277</v>
+        <v>588</v>
       </c>
       <c r="P60" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q60" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R60" s="13" t="s">
-        <v>65</v>
+        <v>590</v>
       </c>
       <c r="S60" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T60" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="U60" s="15"/>
     </row>
     <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D61" s="13"/>
+        <v>278</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="E61" s="20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>214</v>
@@ -6129,7 +6166,7 @@
         <v>276</v>
       </c>
       <c r="O61" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P61" s="13" t="s">
         <v>42</v>
@@ -6138,10 +6175,10 @@
         <v>43788</v>
       </c>
       <c r="R61" s="13" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="S61" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T61" s="13" t="s">
         <v>279</v>
@@ -6150,26 +6187,26 @@
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="20" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>214</v>
@@ -6177,9 +6214,15 @@
       <c r="J62" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
+      <c r="K62" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L62" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="M62" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="N62" s="13" t="s">
         <v>276</v>
       </c>
@@ -6196,7 +6239,7 @@
         <v>286</v>
       </c>
       <c r="S62" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T62" s="13" t="s">
         <v>279</v>
@@ -6205,26 +6248,26 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>214</v>
@@ -6251,7 +6294,7 @@
         <v>286</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T63" s="13" t="s">
         <v>279</v>
@@ -6260,26 +6303,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>214</v>
@@ -6315,26 +6358,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>214</v>
@@ -6370,26 +6413,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>214</v>
@@ -6425,26 +6468,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>214</v>
@@ -6480,26 +6523,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>214</v>
@@ -6535,26 +6578,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>214</v>
@@ -6590,26 +6633,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>214</v>
@@ -6645,26 +6688,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>214</v>
@@ -6700,26 +6743,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>214</v>
@@ -6755,26 +6798,26 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>214</v>
@@ -6810,141 +6853,139 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="D74" s="13" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>21</v>
+        <v>274</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J74" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="O74" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="P74" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q74" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R74" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="S74" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T74" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U74" s="15"/>
+    </row>
+    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E75" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G75" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J75" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K74" s="13" t="s">
+      <c r="K75" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="L74" s="13" t="s">
+      <c r="L75" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="M74" s="13" t="s">
+      <c r="M75" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="N74" s="13" t="s">
+      <c r="N75" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="O74" s="13" t="s">
+      <c r="O75" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="P74" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q74" s="14">
+      <c r="P75" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q75" s="14">
         <v>44111</v>
       </c>
-      <c r="R74" s="13" t="s">
+      <c r="R75" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="S74" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T74" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U74" s="15"/>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q75" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R75" s="13"/>
-      <c r="S75" s="13"/>
-      <c r="T75" s="13"/>
+      <c r="S75" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T75" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U75" s="15"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B76" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="F76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G76" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H76" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="I76" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J76" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="L76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="M76" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="N76" s="13" t="s">
-        <v>357</v>
-      </c>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
       <c r="O76" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P76" s="13" t="s">
         <v>42</v>
@@ -6952,39 +6993,35 @@
       <c r="Q76" s="14">
         <v>43788</v>
       </c>
-      <c r="R76" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S76" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T76" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R76" s="13"/>
+      <c r="S76" s="13"/>
+      <c r="T76" s="13"/>
       <c r="U76" s="15"/>
     </row>
     <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D77" s="13"/>
+        <v>358</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>354</v>
+      </c>
       <c r="E77" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I77" s="13" t="s">
         <v>214</v>
@@ -7005,7 +7042,7 @@
         <v>357</v>
       </c>
       <c r="O77" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>42</v>
@@ -7014,7 +7051,7 @@
         <v>43788</v>
       </c>
       <c r="R77" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S77" s="13" t="s">
         <v>31</v>
@@ -7026,26 +7063,26 @@
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="20" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>214</v>
@@ -7066,7 +7103,7 @@
         <v>357</v>
       </c>
       <c r="O78" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P78" s="13" t="s">
         <v>42</v>
@@ -7075,7 +7112,7 @@
         <v>43788</v>
       </c>
       <c r="R78" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="S78" s="13" t="s">
         <v>31</v>
@@ -7087,26 +7124,26 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>214</v>
@@ -7148,26 +7185,26 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>214</v>
@@ -7188,7 +7225,7 @@
         <v>357</v>
       </c>
       <c r="O80" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7197,7 +7234,7 @@
         <v>43788</v>
       </c>
       <c r="R80" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S80" s="13" t="s">
         <v>31</v>
@@ -7207,23 +7244,49 @@
       </c>
       <c r="U80" s="15"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+    <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
+      <c r="E81" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K81" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="L81" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M81" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="N81" s="13" t="s">
+        <v>357</v>
+      </c>
       <c r="O81" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P81" s="13" t="s">
         <v>42</v>
@@ -7231,54 +7294,32 @@
       <c r="Q81" s="14">
         <v>43788</v>
       </c>
-      <c r="R81" s="13"/>
-      <c r="S81" s="13"/>
-      <c r="T81" s="13"/>
+      <c r="R81" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="S81" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T81" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="U81" s="15"/>
     </row>
-    <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B82" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C82" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="D82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E82" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="F82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="G82" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H82" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J82" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="L82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="M82" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="N82" s="13" t="s">
-        <v>385</v>
-      </c>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13"/>
       <c r="O82" s="13" t="s">
         <v>63</v>
       </c>
@@ -7288,39 +7329,35 @@
       <c r="Q82" s="14">
         <v>43788</v>
       </c>
-      <c r="R82" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S82" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="T82" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R82" s="13"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="13"/>
       <c r="U82" s="15"/>
     </row>
     <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D83" s="13"/>
+        <v>386</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>382</v>
+      </c>
       <c r="E83" s="20" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>214</v>
@@ -7353,7 +7390,7 @@
         <v>359</v>
       </c>
       <c r="S83" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T83" s="13" t="s">
         <v>279</v>
@@ -7362,26 +7399,26 @@
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>214</v>
@@ -7414,7 +7451,7 @@
         <v>359</v>
       </c>
       <c r="S84" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T84" s="13" t="s">
         <v>279</v>
@@ -7423,26 +7460,26 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="20" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>214</v>
@@ -7484,26 +7521,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>214</v>
@@ -7545,26 +7582,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>214</v>
@@ -7606,26 +7643,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>214</v>
@@ -7667,26 +7704,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>214</v>
@@ -7728,26 +7765,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>214</v>
@@ -7789,26 +7826,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>214</v>
@@ -7850,26 +7887,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>214</v>
@@ -7911,26 +7948,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>214</v>
@@ -7972,26 +8009,26 @@
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>214</v>
@@ -8032,103 +8069,107 @@
       <c r="U94" s="15"/>
     </row>
     <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D95" s="13"/>
+      <c r="E95" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F95" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I95" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J95" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K95" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="L95" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M95" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N95" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="O95" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P95" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q95" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R95" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="S95" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T95" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U95" s="15"/>
+    </row>
+    <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A96" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B95" s="12"/>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="22"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
-      <c r="J95" s="22"/>
-      <c r="K95" s="22"/>
-      <c r="L95" s="22"/>
-      <c r="M95" s="22"/>
-      <c r="N95" s="22"/>
-      <c r="O95" s="22"/>
-      <c r="P95" s="22"/>
-      <c r="Q95" s="22"/>
-      <c r="R95" s="22"/>
-      <c r="S95" s="22"/>
-      <c r="T95" s="22"/>
-      <c r="U95" s="22"/>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I96" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J96" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K96" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="L96" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M96" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N96" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O96" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P96" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q96" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R96" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="S96" s="13"/>
-      <c r="T96" s="13"/>
-      <c r="U96" s="15"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="22"/>
+      <c r="J96" s="22"/>
+      <c r="K96" s="22"/>
+      <c r="L96" s="22"/>
+      <c r="M96" s="22"/>
+      <c r="N96" s="22"/>
+      <c r="O96" s="22"/>
+      <c r="P96" s="22"/>
+      <c r="Q96" s="22"/>
+      <c r="R96" s="22"/>
+      <c r="S96" s="22"/>
+      <c r="T96" s="22"/>
+      <c r="U96" s="22"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="B97" s="13"/>
       <c r="C97" s="13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="G97" s="13" t="s">
         <v>21</v>
@@ -8143,28 +8184,28 @@
         <v>23</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L97" s="13" t="s">
-        <v>123</v>
+        <v>451</v>
       </c>
       <c r="M97" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N97" s="13" t="s">
-        <v>456</v>
+        <v>26</v>
       </c>
       <c r="O97" s="13" t="s">
-        <v>457</v>
+        <v>27</v>
       </c>
       <c r="P97" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q97" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R97" s="13" t="s">
-        <v>30</v>
+        <v>453</v>
       </c>
       <c r="S97" s="13"/>
       <c r="T97" s="13"/>
@@ -8172,20 +8213,20 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>21</v>
@@ -8200,19 +8241,19 @@
         <v>23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>462</v>
+        <v>124</v>
       </c>
       <c r="N98" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O98" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P98" s="13" t="s">
         <v>42</v>
@@ -8229,20 +8270,20 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
@@ -8257,19 +8298,19 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="N99" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="O99" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P99" s="13" t="s">
         <v>42</v>
@@ -8284,30 +8325,28 @@
       <c r="T99" s="13"/>
       <c r="U99" s="15"/>
     </row>
-    <row r="100" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B100" s="13" t="s">
-        <v>490</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="I100" s="13" t="s">
         <v>36</v>
@@ -8316,86 +8355,122 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="L100" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M100" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="N100" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="O100" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="P100" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q100" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R100" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="15"/>
+    </row>
+    <row r="101" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G101" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I101" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J101" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K101" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L100" s="13" t="s">
+      <c r="L101" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M100" s="13" t="s">
+      <c r="M101" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N100" s="13" t="s">
+      <c r="N101" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O100" s="13" t="s">
+      <c r="O101" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P100" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q100" s="14">
+      <c r="P101" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q101" s="14">
         <v>42118</v>
       </c>
-      <c r="R100" s="13" t="s">
+      <c r="R101" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S100" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T100" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U100" s="15"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-      <c r="D101"/>
-      <c r="E101" s="10"/>
-      <c r="F101"/>
-      <c r="G101"/>
-      <c r="H101"/>
-      <c r="I101"/>
-      <c r="J101"/>
-      <c r="K101"/>
-      <c r="L101"/>
-      <c r="M101"/>
-      <c r="N101"/>
-      <c r="O101"/>
-      <c r="P101"/>
-      <c r="Q101"/>
-      <c r="R101"/>
-      <c r="S101"/>
-      <c r="T101"/>
-      <c r="U101"/>
+      <c r="S101" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T101" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U101" s="15"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="4"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="4"/>
-      <c r="S102" s="4"/>
-      <c r="T102" s="4"/>
-      <c r="U102" s="4"/>
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102" s="10"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="L102"/>
+      <c r="M102"/>
+      <c r="N102"/>
+      <c r="O102"/>
+      <c r="P102"/>
+      <c r="Q102"/>
+      <c r="R102"/>
+      <c r="S102"/>
+      <c r="T102"/>
+      <c r="U102"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="4"/>
@@ -8417,17 +8492,17 @@
       <c r="U103" s="4"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B104" s="4"/>
+      <c r="A104" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B104" s="3"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
-      <c r="K104" s="4"/>
+      <c r="K104" s="3"/>
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
@@ -8441,7 +8516,7 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -8463,30 +8538,53 @@
       <c r="U105" s="4"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="4"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+      <c r="U106" s="4"/>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A107" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
-      <c r="J106" s="7"/>
-      <c r="K106" s="7"/>
-      <c r="L106" s="7"/>
-      <c r="M106" s="7"/>
-      <c r="N106" s="7"/>
-      <c r="O106" s="7"/>
-      <c r="P106" s="7"/>
-      <c r="R106" s="7"/>
-      <c r="S106" s="7"/>
-      <c r="T106" s="7"/>
-      <c r="U106" s="7"/>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="7"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="7"/>
+      <c r="P107" s="7"/>
+      <c r="R107" s="7"/>
+      <c r="S107" s="7"/>
+      <c r="T107" s="7"/>
+      <c r="U107" s="7"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #505 : [namespace-registry] add new namespace "mro"
Issue #505 : [namespace-registry] add new namespace "mro"

Add the namespace "mro" to the Namespace Registry and the config.properties file.

The Mars Reconnaissance Orbiter Mission Dictionary (mro) contains classes, attributes and rules specific to the MRO mission and its instruments.

@c-suh  [namespace-registry] add new namespace "mro" #505

Resolves #505
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBA4DBA-16D7-4F59-B5DD-C6986DB38C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B91EE98-EC10-424B-B3AA-5D0CDC94DABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4577" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6710" uniqueCount="655">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1972,6 +1972,24 @@
   </si>
   <si>
     <t>Balloon Observation Platform for Planetary Science</t>
+  </si>
+  <si>
+    <t>mro</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mro/v1</t>
+  </si>
+  <si>
+    <t>MRO</t>
+  </si>
+  <si>
+    <t>PDS4_MRO</t>
+  </si>
+  <si>
+    <t>Mars Reconnaissance Orbiter</t>
+  </si>
+  <si>
+    <t>Namespace for the Mars Reconnaissance Orbiter.</t>
   </si>
 </sst>
 </file>
@@ -2465,12 +2483,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U108"/>
+  <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5746,28 +5764,28 @@
     </row>
     <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>607</v>
+        <v>649</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>610</v>
+        <v>653</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>611</v>
+        <v>654</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>608</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>609</v>
+        <v>649</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>650</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>607</v>
+        <v>649</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>612</v>
+        <v>652</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>214</v>
@@ -5776,7 +5794,7 @@
         <v>23</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>613</v>
+        <v>651</v>
       </c>
       <c r="L55" s="17" t="s">
         <v>123</v>
@@ -5785,19 +5803,19 @@
         <v>244</v>
       </c>
       <c r="N55" s="17" t="s">
-        <v>616</v>
+        <v>644</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>617</v>
+        <v>645</v>
       </c>
       <c r="P55" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q55" s="18">
-        <v>44713</v>
+        <v>44833</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>616</v>
+        <v>643</v>
       </c>
       <c r="S55" s="17" t="s">
         <v>31</v>
@@ -5807,30 +5825,30 @@
       </c>
       <c r="U55" s="19"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>552</v>
+        <v>607</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>559</v>
+        <v>610</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>553</v>
+        <v>611</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>554</v>
+        <v>608</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>555</v>
+        <v>609</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>552</v>
+        <v>607</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>214</v>
@@ -5839,28 +5857,28 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="L56" s="17" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="M56" s="17" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>269</v>
+        <v>616</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>270</v>
+        <v>617</v>
       </c>
       <c r="P56" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q56" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="S56" s="17" t="s">
         <v>31</v>
@@ -5870,30 +5888,30 @@
       </c>
       <c r="U56" s="19"/>
     </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>214</v>
@@ -5902,7 +5920,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>219</v>
@@ -5911,19 +5929,19 @@
         <v>177</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>576</v>
+        <v>270</v>
       </c>
       <c r="P57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q57" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>186</v>
+        <v>556</v>
       </c>
       <c r="S57" s="17" t="s">
         <v>31</v>
@@ -5933,30 +5951,30 @@
       </c>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>604</v>
+        <v>577</v>
       </c>
       <c r="I58" s="17" t="s">
         <v>214</v>
@@ -5965,7 +5983,7 @@
         <v>23</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="L58" s="17" t="s">
         <v>219</v>
@@ -5974,115 +5992,115 @@
         <v>177</v>
       </c>
       <c r="N58" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="O58" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="P58" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R58" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="S58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U58" s="19"/>
+    </row>
+    <row r="59" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J59" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K59" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N59" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="O58" s="17" t="s">
+      <c r="O59" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="P58" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q58" s="18">
+      <c r="P59" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q59" s="18">
         <v>44713</v>
       </c>
-      <c r="R58" s="17" t="s">
+      <c r="R59" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="S58" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T58" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U58" s="19"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I59" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J59" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K59" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="L59" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M59" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N59" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="O59" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="P59" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q59" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R59" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S59" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T59" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U59" s="15"/>
+      <c r="S59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U59" s="19"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>582</v>
+        <v>626</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>583</v>
+        <v>271</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="E60" s="21" t="s">
-        <v>585</v>
+        <v>266</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>589</v>
+        <v>42</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>214</v>
@@ -6091,28 +6109,28 @@
         <v>23</v>
       </c>
       <c r="K60" s="13" t="s">
-        <v>586</v>
+        <v>268</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M60" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N60" s="13" t="s">
-        <v>587</v>
+        <v>269</v>
       </c>
       <c r="O60" s="13" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="P60" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q60" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R60" s="13" t="s">
-        <v>590</v>
+        <v>186</v>
       </c>
       <c r="S60" s="13" t="s">
         <v>31</v>
@@ -6122,91 +6140,93 @@
       </c>
       <c r="U60" s="15"/>
     </row>
-    <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>627</v>
+        <v>582</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>273</v>
+        <v>584</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>275</v>
+        <v>589</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>272</v>
+        <v>586</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>272</v>
+        <v>170</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>276</v>
+        <v>587</v>
       </c>
       <c r="O61" s="13" t="s">
-        <v>277</v>
+        <v>588</v>
       </c>
       <c r="P61" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q61" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R61" s="13" t="s">
-        <v>65</v>
+        <v>590</v>
       </c>
       <c r="S61" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T61" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="U61" s="15"/>
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D62" s="13"/>
+        <v>278</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="E62" s="20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>214</v>
@@ -6227,7 +6247,7 @@
         <v>276</v>
       </c>
       <c r="O62" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P62" s="13" t="s">
         <v>42</v>
@@ -6236,10 +6256,10 @@
         <v>43788</v>
       </c>
       <c r="R62" s="13" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="S62" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T62" s="13" t="s">
         <v>279</v>
@@ -6248,26 +6268,26 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>214</v>
@@ -6275,9 +6295,15 @@
       <c r="J63" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
+      <c r="K63" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L63" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="M63" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="N63" s="13" t="s">
         <v>276</v>
       </c>
@@ -6294,7 +6320,7 @@
         <v>286</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T63" s="13" t="s">
         <v>279</v>
@@ -6303,26 +6329,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>214</v>
@@ -6349,7 +6375,7 @@
         <v>286</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T64" s="13" t="s">
         <v>279</v>
@@ -6358,26 +6384,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>214</v>
@@ -6413,26 +6439,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>214</v>
@@ -6468,26 +6494,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>214</v>
@@ -6523,26 +6549,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>214</v>
@@ -6578,26 +6604,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>214</v>
@@ -6633,26 +6659,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>214</v>
@@ -6688,26 +6714,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>214</v>
@@ -6743,26 +6769,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>214</v>
@@ -6798,26 +6824,26 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>214</v>
@@ -6853,26 +6879,26 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>214</v>
@@ -6908,141 +6934,139 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="D75" s="13"/>
       <c r="E75" s="20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>21</v>
+        <v>274</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I75" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J75" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="O75" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="P75" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q75" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R75" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="S75" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T75" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U75" s="15"/>
+    </row>
+    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I76" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J76" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K75" s="13" t="s">
+      <c r="K76" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="L75" s="13" t="s">
+      <c r="L76" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="M75" s="13" t="s">
+      <c r="M76" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="N75" s="13" t="s">
+      <c r="N76" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="O75" s="13" t="s">
+      <c r="O76" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="P75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q75" s="14">
+      <c r="P76" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q76" s="14">
         <v>44111</v>
       </c>
-      <c r="R75" s="13" t="s">
+      <c r="R76" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="S75" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T75" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U75" s="15"/>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P76" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q76" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R76" s="13"/>
-      <c r="S76" s="13"/>
-      <c r="T76" s="13"/>
+      <c r="S76" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T76" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U76" s="15"/>
     </row>
-    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E77" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="F77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G77" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H77" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="I77" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J77" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="L77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="M77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="N77" s="13" t="s">
-        <v>357</v>
-      </c>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
       <c r="O77" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>42</v>
@@ -7050,39 +7074,35 @@
       <c r="Q77" s="14">
         <v>43788</v>
       </c>
-      <c r="R77" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S77" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T77" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
       <c r="U77" s="15"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D78" s="13"/>
+        <v>358</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>354</v>
+      </c>
       <c r="E78" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>214</v>
@@ -7103,7 +7123,7 @@
         <v>357</v>
       </c>
       <c r="O78" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P78" s="13" t="s">
         <v>42</v>
@@ -7112,7 +7132,7 @@
         <v>43788</v>
       </c>
       <c r="R78" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S78" s="13" t="s">
         <v>31</v>
@@ -7124,26 +7144,26 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="20" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>214</v>
@@ -7164,7 +7184,7 @@
         <v>357</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7173,7 +7193,7 @@
         <v>43788</v>
       </c>
       <c r="R79" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="S79" s="13" t="s">
         <v>31</v>
@@ -7185,26 +7205,26 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>214</v>
@@ -7246,26 +7266,26 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>214</v>
@@ -7286,7 +7306,7 @@
         <v>357</v>
       </c>
       <c r="O81" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P81" s="13" t="s">
         <v>42</v>
@@ -7295,7 +7315,7 @@
         <v>43788</v>
       </c>
       <c r="R81" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S81" s="13" t="s">
         <v>31</v>
@@ -7305,23 +7325,49 @@
       </c>
       <c r="U81" s="15"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+    <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
+      <c r="E82" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="L82" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M82" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="N82" s="13" t="s">
+        <v>357</v>
+      </c>
       <c r="O82" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P82" s="13" t="s">
         <v>42</v>
@@ -7329,54 +7375,32 @@
       <c r="Q82" s="14">
         <v>43788</v>
       </c>
-      <c r="R82" s="13"/>
-      <c r="S82" s="13"/>
-      <c r="T82" s="13"/>
+      <c r="R82" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="S82" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T82" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="U82" s="15"/>
     </row>
-    <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E83" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="F83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H83" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I83" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J83" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="L83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="M83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="N83" s="13" t="s">
-        <v>385</v>
-      </c>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
       <c r="O83" s="13" t="s">
         <v>63</v>
       </c>
@@ -7386,39 +7410,35 @@
       <c r="Q83" s="14">
         <v>43788</v>
       </c>
-      <c r="R83" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S83" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="T83" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R83" s="13"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="13"/>
       <c r="U83" s="15"/>
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D84" s="13"/>
+        <v>386</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>382</v>
+      </c>
       <c r="E84" s="20" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>214</v>
@@ -7451,7 +7471,7 @@
         <v>359</v>
       </c>
       <c r="S84" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T84" s="13" t="s">
         <v>279</v>
@@ -7460,26 +7480,26 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>214</v>
@@ -7512,7 +7532,7 @@
         <v>359</v>
       </c>
       <c r="S85" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T85" s="13" t="s">
         <v>279</v>
@@ -7521,26 +7541,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>214</v>
@@ -7582,26 +7602,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>214</v>
@@ -7643,26 +7663,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>214</v>
@@ -7704,26 +7724,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>214</v>
@@ -7765,26 +7785,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>214</v>
@@ -7826,26 +7846,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>214</v>
@@ -7887,26 +7907,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>214</v>
@@ -7948,26 +7968,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>214</v>
@@ -8009,26 +8029,26 @@
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>214</v>
@@ -8070,26 +8090,26 @@
     </row>
     <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G95" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I95" s="13" t="s">
         <v>214</v>
@@ -8130,103 +8150,107 @@
       <c r="U95" s="15"/>
     </row>
     <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D96" s="13"/>
+      <c r="E96" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G96" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I96" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J96" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K96" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="L96" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M96" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N96" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="O96" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P96" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q96" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R96" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="S96" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T96" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U96" s="15"/>
+    </row>
+    <row r="97" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="22"/>
-      <c r="I96" s="22"/>
-      <c r="J96" s="22"/>
-      <c r="K96" s="22"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="22"/>
-      <c r="N96" s="22"/>
-      <c r="O96" s="22"/>
-      <c r="P96" s="22"/>
-      <c r="Q96" s="22"/>
-      <c r="R96" s="22"/>
-      <c r="S96" s="22"/>
-      <c r="T96" s="22"/>
-      <c r="U96" s="22"/>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D97" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="E97" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F97" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="G97" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I97" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J97" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K97" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="L97" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M97" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N97" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O97" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P97" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q97" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R97" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="S97" s="13"/>
-      <c r="T97" s="13"/>
-      <c r="U97" s="15"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="22"/>
+      <c r="L97" s="22"/>
+      <c r="M97" s="22"/>
+      <c r="N97" s="22"/>
+      <c r="O97" s="22"/>
+      <c r="P97" s="22"/>
+      <c r="Q97" s="22"/>
+      <c r="R97" s="22"/>
+      <c r="S97" s="22"/>
+      <c r="T97" s="22"/>
+      <c r="U97" s="22"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>21</v>
@@ -8241,28 +8265,28 @@
         <v>23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>123</v>
+        <v>451</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N98" s="13" t="s">
-        <v>456</v>
+        <v>26</v>
       </c>
       <c r="O98" s="13" t="s">
-        <v>457</v>
+        <v>27</v>
       </c>
       <c r="P98" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q98" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R98" s="13" t="s">
-        <v>30</v>
+        <v>453</v>
       </c>
       <c r="S98" s="13"/>
       <c r="T98" s="13"/>
@@ -8270,20 +8294,20 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
@@ -8298,19 +8322,19 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>462</v>
+        <v>124</v>
       </c>
       <c r="N99" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O99" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P99" s="13" t="s">
         <v>42</v>
@@ -8327,20 +8351,20 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
@@ -8355,19 +8379,19 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="M100" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="N100" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="O100" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P100" s="13" t="s">
         <v>42</v>
@@ -8382,30 +8406,28 @@
       <c r="T100" s="13"/>
       <c r="U100" s="15"/>
     </row>
-    <row r="101" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>490</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="G101" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="I101" s="13" t="s">
         <v>36</v>
@@ -8414,86 +8436,122 @@
         <v>23</v>
       </c>
       <c r="K101" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="L101" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M101" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="N101" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="O101" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="P101" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q101" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R101" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S101" s="13"/>
+      <c r="T101" s="13"/>
+      <c r="U101" s="15"/>
+    </row>
+    <row r="102" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I102" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L101" s="13" t="s">
+      <c r="L102" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M101" s="13" t="s">
+      <c r="M102" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N101" s="13" t="s">
+      <c r="N102" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O101" s="13" t="s">
+      <c r="O102" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P101" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q101" s="14">
+      <c r="P102" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q102" s="14">
         <v>42118</v>
       </c>
-      <c r="R101" s="13" t="s">
+      <c r="R102" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S101" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T101" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U101" s="15"/>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102" s="10"/>
-      <c r="F102"/>
-      <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
-      <c r="J102"/>
-      <c r="K102"/>
-      <c r="L102"/>
-      <c r="M102"/>
-      <c r="N102"/>
-      <c r="O102"/>
-      <c r="P102"/>
-      <c r="Q102"/>
-      <c r="R102"/>
-      <c r="S102"/>
-      <c r="T102"/>
-      <c r="U102"/>
+      <c r="S102" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T102" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U102" s="15"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="K103" s="3"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="4"/>
-      <c r="S103" s="4"/>
-      <c r="T103" s="4"/>
-      <c r="U103" s="4"/>
+      <c r="A103"/>
+      <c r="B103"/>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103" s="10"/>
+      <c r="F103"/>
+      <c r="G103"/>
+      <c r="H103"/>
+      <c r="I103"/>
+      <c r="J103"/>
+      <c r="K103"/>
+      <c r="L103"/>
+      <c r="M103"/>
+      <c r="N103"/>
+      <c r="O103"/>
+      <c r="P103"/>
+      <c r="Q103"/>
+      <c r="R103"/>
+      <c r="S103"/>
+      <c r="T103"/>
+      <c r="U103"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
@@ -8515,17 +8573,17 @@
       <c r="U104" s="4"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B105" s="4"/>
+      <c r="A105" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B105" s="3"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
-      <c r="K105" s="4"/>
+      <c r="K105" s="3"/>
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
@@ -8539,7 +8597,7 @@
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -8561,30 +8619,53 @@
       <c r="U106" s="4"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="7"/>
-      <c r="J107" s="7"/>
-      <c r="K107" s="7"/>
-      <c r="L107" s="7"/>
-      <c r="M107" s="7"/>
-      <c r="N107" s="7"/>
-      <c r="O107" s="7"/>
-      <c r="P107" s="7"/>
-      <c r="R107" s="7"/>
-      <c r="S107" s="7"/>
-      <c r="T107" s="7"/>
-      <c r="U107" s="7"/>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="7"/>
+      <c r="N108" s="7"/>
+      <c r="O108" s="7"/>
+      <c r="P108" s="7"/>
+      <c r="R108" s="7"/>
+      <c r="S108" s="7"/>
+      <c r="T108" s="7"/>
+      <c r="U108" s="7"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #505 : [namespace-registry] add new namespace "mro" (#508)
Issue #505 : [namespace-registry] add new namespace "mro"

Add the namespace "mro" to the Namespace Registry and the config.properties file.

The Mars Reconnaissance Orbiter Mission Dictionary (mro) contains classes, attributes and rules specific to the MRO mission and its instruments.

@c-suh  [namespace-registry] add new namespace "mro" #505

Resolves #505

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBA4DBA-16D7-4F59-B5DD-C6986DB38C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B91EE98-EC10-424B-B3AA-5D0CDC94DABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4577" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6710" uniqueCount="655">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1972,6 +1972,24 @@
   </si>
   <si>
     <t>Balloon Observation Platform for Planetary Science</t>
+  </si>
+  <si>
+    <t>mro</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mro/v1</t>
+  </si>
+  <si>
+    <t>MRO</t>
+  </si>
+  <si>
+    <t>PDS4_MRO</t>
+  </si>
+  <si>
+    <t>Mars Reconnaissance Orbiter</t>
+  </si>
+  <si>
+    <t>Namespace for the Mars Reconnaissance Orbiter.</t>
   </si>
 </sst>
 </file>
@@ -2465,12 +2483,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U108"/>
+  <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5746,28 +5764,28 @@
     </row>
     <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>607</v>
+        <v>649</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>610</v>
+        <v>653</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>611</v>
+        <v>654</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>608</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>609</v>
+        <v>649</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>650</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>607</v>
+        <v>649</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>612</v>
+        <v>652</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>214</v>
@@ -5776,7 +5794,7 @@
         <v>23</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>613</v>
+        <v>651</v>
       </c>
       <c r="L55" s="17" t="s">
         <v>123</v>
@@ -5785,19 +5803,19 @@
         <v>244</v>
       </c>
       <c r="N55" s="17" t="s">
-        <v>616</v>
+        <v>644</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>617</v>
+        <v>645</v>
       </c>
       <c r="P55" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q55" s="18">
-        <v>44713</v>
+        <v>44833</v>
       </c>
       <c r="R55" s="17" t="s">
-        <v>616</v>
+        <v>643</v>
       </c>
       <c r="S55" s="17" t="s">
         <v>31</v>
@@ -5807,30 +5825,30 @@
       </c>
       <c r="U55" s="19"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>552</v>
+        <v>607</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>559</v>
+        <v>610</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>553</v>
+        <v>611</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>554</v>
+        <v>608</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>555</v>
+        <v>609</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>552</v>
+        <v>607</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>214</v>
@@ -5839,28 +5857,28 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="L56" s="17" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="M56" s="17" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>269</v>
+        <v>616</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>270</v>
+        <v>617</v>
       </c>
       <c r="P56" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q56" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="S56" s="17" t="s">
         <v>31</v>
@@ -5870,30 +5888,30 @@
       </c>
       <c r="U56" s="19"/>
     </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>214</v>
@@ -5902,7 +5920,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>219</v>
@@ -5911,19 +5929,19 @@
         <v>177</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>576</v>
+        <v>270</v>
       </c>
       <c r="P57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q57" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>186</v>
+        <v>556</v>
       </c>
       <c r="S57" s="17" t="s">
         <v>31</v>
@@ -5933,30 +5951,30 @@
       </c>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>604</v>
+        <v>577</v>
       </c>
       <c r="I58" s="17" t="s">
         <v>214</v>
@@ -5965,7 +5983,7 @@
         <v>23</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="L58" s="17" t="s">
         <v>219</v>
@@ -5974,115 +5992,115 @@
         <v>177</v>
       </c>
       <c r="N58" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="O58" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="P58" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R58" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="S58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U58" s="19"/>
+    </row>
+    <row r="59" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J59" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K59" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N59" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="O58" s="17" t="s">
+      <c r="O59" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="P58" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q58" s="18">
+      <c r="P59" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q59" s="18">
         <v>44713</v>
       </c>
-      <c r="R58" s="17" t="s">
+      <c r="R59" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="S58" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T58" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U58" s="19"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I59" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J59" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K59" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="L59" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="M59" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N59" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="O59" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="P59" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q59" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R59" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="S59" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T59" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U59" s="15"/>
+      <c r="S59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U59" s="19"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>582</v>
+        <v>626</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>583</v>
+        <v>271</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="E60" s="21" t="s">
-        <v>585</v>
+        <v>266</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>581</v>
+        <v>265</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>589</v>
+        <v>42</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>214</v>
@@ -6091,28 +6109,28 @@
         <v>23</v>
       </c>
       <c r="K60" s="13" t="s">
-        <v>586</v>
+        <v>268</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="M60" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N60" s="13" t="s">
-        <v>587</v>
+        <v>269</v>
       </c>
       <c r="O60" s="13" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="P60" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q60" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R60" s="13" t="s">
-        <v>590</v>
+        <v>186</v>
       </c>
       <c r="S60" s="13" t="s">
         <v>31</v>
@@ -6122,91 +6140,93 @@
       </c>
       <c r="U60" s="15"/>
     </row>
-    <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>627</v>
+        <v>582</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>273</v>
+        <v>584</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>585</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>272</v>
+        <v>581</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>275</v>
+        <v>589</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>272</v>
+        <v>586</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>272</v>
+        <v>166</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>272</v>
+        <v>170</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>276</v>
+        <v>587</v>
       </c>
       <c r="O61" s="13" t="s">
-        <v>277</v>
+        <v>588</v>
       </c>
       <c r="P61" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q61" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R61" s="13" t="s">
-        <v>65</v>
+        <v>590</v>
       </c>
       <c r="S61" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T61" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="U61" s="15"/>
     </row>
     <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D62" s="13"/>
+        <v>278</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="E62" s="20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>214</v>
@@ -6227,7 +6247,7 @@
         <v>276</v>
       </c>
       <c r="O62" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P62" s="13" t="s">
         <v>42</v>
@@ -6236,10 +6256,10 @@
         <v>43788</v>
       </c>
       <c r="R62" s="13" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="S62" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T62" s="13" t="s">
         <v>279</v>
@@ -6248,26 +6268,26 @@
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="20" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>214</v>
@@ -6275,9 +6295,15 @@
       <c r="J63" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
+      <c r="K63" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L63" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="M63" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="N63" s="13" t="s">
         <v>276</v>
       </c>
@@ -6294,7 +6320,7 @@
         <v>286</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T63" s="13" t="s">
         <v>279</v>
@@ -6303,26 +6329,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>214</v>
@@ -6349,7 +6375,7 @@
         <v>286</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T64" s="13" t="s">
         <v>279</v>
@@ -6358,26 +6384,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>214</v>
@@ -6413,26 +6439,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>214</v>
@@ -6468,26 +6494,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>214</v>
@@ -6523,26 +6549,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>214</v>
@@ -6578,26 +6604,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>214</v>
@@ -6633,26 +6659,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>214</v>
@@ -6688,26 +6714,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>214</v>
@@ -6743,26 +6769,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>214</v>
@@ -6798,26 +6824,26 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>214</v>
@@ -6853,26 +6879,26 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>214</v>
@@ -6908,141 +6934,139 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="D75" s="13"/>
       <c r="E75" s="20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>21</v>
+        <v>274</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I75" s="13" t="s">
         <v>214</v>
       </c>
       <c r="J75" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="O75" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="P75" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q75" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R75" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="S75" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T75" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U75" s="15"/>
+    </row>
+    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I76" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J76" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K75" s="13" t="s">
+      <c r="K76" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="L75" s="13" t="s">
+      <c r="L76" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="M75" s="13" t="s">
+      <c r="M76" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="N75" s="13" t="s">
+      <c r="N76" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="O75" s="13" t="s">
+      <c r="O76" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="P75" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q75" s="14">
+      <c r="P76" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q76" s="14">
         <v>44111</v>
       </c>
-      <c r="R75" s="13" t="s">
+      <c r="R76" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="S75" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T75" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U75" s="15"/>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P76" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q76" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R76" s="13"/>
-      <c r="S76" s="13"/>
-      <c r="T76" s="13"/>
+      <c r="S76" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T76" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U76" s="15"/>
     </row>
-    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E77" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="F77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G77" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H77" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="I77" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J77" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="L77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="M77" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="N77" s="13" t="s">
-        <v>357</v>
-      </c>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
       <c r="O77" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>42</v>
@@ -7050,39 +7074,35 @@
       <c r="Q77" s="14">
         <v>43788</v>
       </c>
-      <c r="R77" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S77" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T77" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
       <c r="U77" s="15"/>
     </row>
     <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D78" s="13"/>
+        <v>358</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>354</v>
+      </c>
       <c r="E78" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>214</v>
@@ -7103,7 +7123,7 @@
         <v>357</v>
       </c>
       <c r="O78" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P78" s="13" t="s">
         <v>42</v>
@@ -7112,7 +7132,7 @@
         <v>43788</v>
       </c>
       <c r="R78" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S78" s="13" t="s">
         <v>31</v>
@@ -7124,26 +7144,26 @@
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="20" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>214</v>
@@ -7164,7 +7184,7 @@
         <v>357</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7173,7 +7193,7 @@
         <v>43788</v>
       </c>
       <c r="R79" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="S79" s="13" t="s">
         <v>31</v>
@@ -7185,26 +7205,26 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>214</v>
@@ -7246,26 +7266,26 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>629</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>214</v>
@@ -7286,7 +7306,7 @@
         <v>357</v>
       </c>
       <c r="O81" s="13" t="s">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="P81" s="13" t="s">
         <v>42</v>
@@ -7295,7 +7315,7 @@
         <v>43788</v>
       </c>
       <c r="R81" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="S81" s="13" t="s">
         <v>31</v>
@@ -7305,23 +7325,49 @@
       </c>
       <c r="U81" s="15"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+    <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
+      <c r="E82" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="L82" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M82" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="N82" s="13" t="s">
+        <v>357</v>
+      </c>
       <c r="O82" s="13" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="P82" s="13" t="s">
         <v>42</v>
@@ -7329,54 +7375,32 @@
       <c r="Q82" s="14">
         <v>43788</v>
       </c>
-      <c r="R82" s="13"/>
-      <c r="S82" s="13"/>
-      <c r="T82" s="13"/>
+      <c r="R82" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="S82" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T82" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="U82" s="15"/>
     </row>
-    <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E83" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="F83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H83" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I83" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="J83" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="L83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="M83" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="N83" s="13" t="s">
-        <v>385</v>
-      </c>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
       <c r="O83" s="13" t="s">
         <v>63</v>
       </c>
@@ -7386,39 +7410,35 @@
       <c r="Q83" s="14">
         <v>43788</v>
       </c>
-      <c r="R83" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="S83" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="T83" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="R83" s="13"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="13"/>
       <c r="U83" s="15"/>
     </row>
     <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D84" s="13"/>
+        <v>386</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>382</v>
+      </c>
       <c r="E84" s="20" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>214</v>
@@ -7451,7 +7471,7 @@
         <v>359</v>
       </c>
       <c r="S84" s="13" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="T84" s="13" t="s">
         <v>279</v>
@@ -7460,26 +7480,26 @@
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>214</v>
@@ -7512,7 +7532,7 @@
         <v>359</v>
       </c>
       <c r="S85" s="13" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="T85" s="13" t="s">
         <v>279</v>
@@ -7521,26 +7541,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>214</v>
@@ -7582,26 +7602,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>214</v>
@@ -7643,26 +7663,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>214</v>
@@ -7704,26 +7724,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>214</v>
@@ -7765,26 +7785,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>214</v>
@@ -7826,26 +7846,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>214</v>
@@ -7887,26 +7907,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>214</v>
@@ -7948,26 +7968,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>214</v>
@@ -8009,26 +8029,26 @@
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>214</v>
@@ -8070,26 +8090,26 @@
     </row>
     <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>630</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G95" s="13" t="s">
         <v>274</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I95" s="13" t="s">
         <v>214</v>
@@ -8130,103 +8150,107 @@
       <c r="U95" s="15"/>
     </row>
     <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D96" s="13"/>
+      <c r="E96" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G96" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I96" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J96" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K96" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="L96" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M96" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N96" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="O96" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P96" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q96" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R96" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="S96" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="T96" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="U96" s="15"/>
+    </row>
+    <row r="97" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="22"/>
-      <c r="I96" s="22"/>
-      <c r="J96" s="22"/>
-      <c r="K96" s="22"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="22"/>
-      <c r="N96" s="22"/>
-      <c r="O96" s="22"/>
-      <c r="P96" s="22"/>
-      <c r="Q96" s="22"/>
-      <c r="R96" s="22"/>
-      <c r="S96" s="22"/>
-      <c r="T96" s="22"/>
-      <c r="U96" s="22"/>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D97" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="E97" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F97" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="G97" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I97" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J97" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K97" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="L97" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M97" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N97" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O97" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P97" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q97" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R97" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="S97" s="13"/>
-      <c r="T97" s="13"/>
-      <c r="U97" s="15"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="22"/>
+      <c r="L97" s="22"/>
+      <c r="M97" s="22"/>
+      <c r="N97" s="22"/>
+      <c r="O97" s="22"/>
+      <c r="P97" s="22"/>
+      <c r="Q97" s="22"/>
+      <c r="R97" s="22"/>
+      <c r="S97" s="22"/>
+      <c r="T97" s="22"/>
+      <c r="U97" s="22"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>123</v>
+        <v>448</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>21</v>
@@ -8241,28 +8265,28 @@
         <v>23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>123</v>
+        <v>451</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N98" s="13" t="s">
-        <v>456</v>
+        <v>26</v>
       </c>
       <c r="O98" s="13" t="s">
-        <v>457</v>
+        <v>27</v>
       </c>
       <c r="P98" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q98" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R98" s="13" t="s">
-        <v>30</v>
+        <v>453</v>
       </c>
       <c r="S98" s="13"/>
       <c r="T98" s="13"/>
@@ -8270,20 +8294,20 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
@@ -8298,19 +8322,19 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>459</v>
+        <v>123</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>462</v>
+        <v>124</v>
       </c>
       <c r="N99" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O99" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P99" s="13" t="s">
         <v>42</v>
@@ -8327,20 +8351,20 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
@@ -8355,19 +8379,19 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="M100" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="N100" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="O100" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P100" s="13" t="s">
         <v>42</v>
@@ -8382,30 +8406,28 @@
       <c r="T100" s="13"/>
       <c r="U100" s="15"/>
     </row>
-    <row r="101" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>490</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
-        <v>203</v>
+        <v>472</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>200</v>
+        <v>466</v>
       </c>
       <c r="G101" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="I101" s="13" t="s">
         <v>36</v>
@@ -8414,86 +8436,122 @@
         <v>23</v>
       </c>
       <c r="K101" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="L101" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M101" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="N101" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="O101" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="P101" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q101" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R101" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S101" s="13"/>
+      <c r="T101" s="13"/>
+      <c r="U101" s="15"/>
+    </row>
+    <row r="102" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I102" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L101" s="13" t="s">
+      <c r="L102" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M101" s="13" t="s">
+      <c r="M102" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N101" s="13" t="s">
+      <c r="N102" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O101" s="13" t="s">
+      <c r="O102" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P101" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q101" s="14">
+      <c r="P102" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q102" s="14">
         <v>42118</v>
       </c>
-      <c r="R101" s="13" t="s">
+      <c r="R102" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S101" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T101" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U101" s="15"/>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102" s="10"/>
-      <c r="F102"/>
-      <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
-      <c r="J102"/>
-      <c r="K102"/>
-      <c r="L102"/>
-      <c r="M102"/>
-      <c r="N102"/>
-      <c r="O102"/>
-      <c r="P102"/>
-      <c r="Q102"/>
-      <c r="R102"/>
-      <c r="S102"/>
-      <c r="T102"/>
-      <c r="U102"/>
+      <c r="S102" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T102" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U102" s="15"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="K103" s="3"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="4"/>
-      <c r="S103" s="4"/>
-      <c r="T103" s="4"/>
-      <c r="U103" s="4"/>
+      <c r="A103"/>
+      <c r="B103"/>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103" s="10"/>
+      <c r="F103"/>
+      <c r="G103"/>
+      <c r="H103"/>
+      <c r="I103"/>
+      <c r="J103"/>
+      <c r="K103"/>
+      <c r="L103"/>
+      <c r="M103"/>
+      <c r="N103"/>
+      <c r="O103"/>
+      <c r="P103"/>
+      <c r="Q103"/>
+      <c r="R103"/>
+      <c r="S103"/>
+      <c r="T103"/>
+      <c r="U103"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
@@ -8515,17 +8573,17 @@
       <c r="U104" s="4"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B105" s="4"/>
+      <c r="A105" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B105" s="3"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
-      <c r="K105" s="4"/>
+      <c r="K105" s="3"/>
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
@@ -8539,7 +8597,7 @@
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -8561,30 +8619,53 @@
       <c r="U106" s="4"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="7"/>
-      <c r="J107" s="7"/>
-      <c r="K107" s="7"/>
-      <c r="L107" s="7"/>
-      <c r="M107" s="7"/>
-      <c r="N107" s="7"/>
-      <c r="O107" s="7"/>
-      <c r="P107" s="7"/>
-      <c r="R107" s="7"/>
-      <c r="S107" s="7"/>
-      <c r="T107" s="7"/>
-      <c r="U107" s="7"/>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="7"/>
+      <c r="N108" s="7"/>
+      <c r="O108" s="7"/>
+      <c r="P108" s="7"/>
+      <c r="R108" s="7"/>
+      <c r="S108" s="7"/>
+      <c r="T108" s="7"/>
+      <c r="U108" s="7"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #563 : [namespace-registry] add new namespace "sb"
Issue #563 : [namespace-registry] add new namespace "sb"

Add the namespace "sb" to the Namespace Registry and the config.properties file.

This dictionary will provide classes to support the documentation, support, discovery, and reuse of data from, by, and for small bodies research.

This is a redo of 552. Instead of "sbn" the namespace id should be "sb".

@c-suh  [namespace-registry] add new namespace "sb" #563

Resolves #563
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6DEF08-9C28-4A30-806F-FCA01C7D51F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92BEB4D4-0E44-4F04-B3F1-256CB4DD27CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6001" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="660">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1993,6 +1993,18 @@
   </si>
   <si>
     <t>PDS4_SBN</t>
+  </si>
+  <si>
+    <t>Namespace for the Small Bodies node's dictionary.</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/sb/v1</t>
+  </si>
+  <si>
+    <t>PDS4_SB</t>
   </si>
 </sst>
 </file>
@@ -2097,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2167,6 +2179,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2486,10 +2501,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U109"/>
+  <dimension ref="A1:U110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
@@ -4295,7 +4310,7 @@
     </row>
     <row r="31" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>174</v>
+        <v>657</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>653</v>
@@ -4304,19 +4319,19 @@
         <v>654</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>175</v>
+        <v>657</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>658</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>174</v>
+        <v>657</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="I31" s="17" t="s">
         <v>36</v>
@@ -4328,7 +4343,7 @@
         <v>176</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="M31" s="17" t="s">
         <v>177</v>
@@ -4343,7 +4358,7 @@
         <v>42</v>
       </c>
       <c r="Q31" s="18">
-        <v>41002</v>
+        <v>44943</v>
       </c>
       <c r="R31" s="17" t="s">
         <v>30</v>
@@ -8468,118 +8483,152 @@
       <c r="T101" s="13"/>
       <c r="U101" s="15"/>
     </row>
-    <row r="102" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A102" s="13" t="s">
+    <row r="102" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B102" s="17"/>
+      <c r="C102" s="13" t="s">
+        <v>656</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G102" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="I102" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J102" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M102" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="P102" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q102" s="18">
+        <v>41002</v>
+      </c>
+      <c r="R102" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S102" s="17"/>
+      <c r="T102" s="17"/>
+      <c r="U102" s="19"/>
+    </row>
+    <row r="103" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B103" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C103" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D103" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E102" s="13" t="s">
+      <c r="E103" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F102" s="13" t="s">
+      <c r="F103" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="G102" s="13" t="s">
+      <c r="G103" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H102" s="13" t="s">
+      <c r="H103" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I102" s="13" t="s">
+      <c r="I103" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J102" s="13" t="s">
+      <c r="J103" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K102" s="13" t="s">
+      <c r="K103" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L102" s="13" t="s">
+      <c r="L103" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M102" s="13" t="s">
+      <c r="M103" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N102" s="13" t="s">
+      <c r="N103" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O102" s="13" t="s">
+      <c r="O103" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P102" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q102" s="14">
+      <c r="P103" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q103" s="14">
         <v>42118</v>
       </c>
-      <c r="R102" s="13" t="s">
+      <c r="R103" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S102" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T102" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U102" s="15"/>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103" s="10"/>
-      <c r="F103"/>
-      <c r="G103"/>
-      <c r="H103"/>
-      <c r="I103"/>
-      <c r="J103"/>
-      <c r="K103"/>
-      <c r="L103"/>
-      <c r="M103"/>
-      <c r="N103"/>
-      <c r="O103"/>
-      <c r="P103"/>
-      <c r="Q103"/>
-      <c r="R103"/>
-      <c r="S103"/>
-      <c r="T103"/>
-      <c r="U103"/>
+      <c r="S103" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T103" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U103" s="15"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="4"/>
-      <c r="S104" s="4"/>
-      <c r="T104" s="4"/>
-      <c r="U104" s="4"/>
+      <c r="A104"/>
+      <c r="B104"/>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104" s="10"/>
+      <c r="F104"/>
+      <c r="G104"/>
+      <c r="H104"/>
+      <c r="I104"/>
+      <c r="J104"/>
+      <c r="K104"/>
+      <c r="L104"/>
+      <c r="M104"/>
+      <c r="N104"/>
+      <c r="O104"/>
+      <c r="P104"/>
+      <c r="Q104"/>
+      <c r="R104"/>
+      <c r="S104"/>
+      <c r="T104"/>
+      <c r="U104"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="4"/>
@@ -8601,17 +8650,17 @@
       <c r="U105" s="4"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="B106" s="4"/>
+      <c r="A106" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B106" s="3"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
-      <c r="K106" s="4"/>
+      <c r="K106" s="3"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
@@ -8625,7 +8674,7 @@
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -8647,30 +8696,53 @@
       <c r="U107" s="4"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="4"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+      <c r="U108" s="4"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A109" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="7"/>
-      <c r="J108" s="7"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="7"/>
-      <c r="M108" s="7"/>
-      <c r="N108" s="7"/>
-      <c r="O108" s="7"/>
-      <c r="P108" s="7"/>
-      <c r="R108" s="7"/>
-      <c r="S108" s="7"/>
-      <c r="T108" s="7"/>
-      <c r="U108" s="7"/>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="7"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="7"/>
+      <c r="P109" s="7"/>
+      <c r="R109" s="7"/>
+      <c r="S109" s="7"/>
+      <c r="T109" s="7"/>
+      <c r="U109" s="7"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #563 : [namespace-registry] add new namespace "sb" (#564)
Issue #563 : [namespace-registry] add new namespace "sb"

Add the namespace "sb" to the Namespace Registry and the config.properties file.

This dictionary will provide classes to support the documentation, support, discovery, and reuse of data from, by, and for small bodies research.

This is a redo of 552. Instead of "sbn" the namespace id should be "sb".

@c-suh  [namespace-registry] add new namespace "sb" #563

Resolves #563

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6DEF08-9C28-4A30-806F-FCA01C7D51F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92BEB4D4-0E44-4F04-B3F1-256CB4DD27CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6001" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="660">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -1993,6 +1993,18 @@
   </si>
   <si>
     <t>PDS4_SBN</t>
+  </si>
+  <si>
+    <t>Namespace for the Small Bodies node's dictionary.</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/sb/v1</t>
+  </si>
+  <si>
+    <t>PDS4_SB</t>
   </si>
 </sst>
 </file>
@@ -2097,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2167,6 +2179,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2486,10 +2501,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U109"/>
+  <dimension ref="A1:U110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
@@ -4295,7 +4310,7 @@
     </row>
     <row r="31" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>174</v>
+        <v>657</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>653</v>
@@ -4304,19 +4319,19 @@
         <v>654</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>175</v>
+        <v>657</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>658</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>174</v>
+        <v>657</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="I31" s="17" t="s">
         <v>36</v>
@@ -4328,7 +4343,7 @@
         <v>176</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="M31" s="17" t="s">
         <v>177</v>
@@ -4343,7 +4358,7 @@
         <v>42</v>
       </c>
       <c r="Q31" s="18">
-        <v>41002</v>
+        <v>44943</v>
       </c>
       <c r="R31" s="17" t="s">
         <v>30</v>
@@ -8468,118 +8483,152 @@
       <c r="T101" s="13"/>
       <c r="U101" s="15"/>
     </row>
-    <row r="102" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A102" s="13" t="s">
+    <row r="102" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B102" s="17"/>
+      <c r="C102" s="13" t="s">
+        <v>656</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G102" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="I102" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J102" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L102" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M102" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="P102" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q102" s="18">
+        <v>41002</v>
+      </c>
+      <c r="R102" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S102" s="17"/>
+      <c r="T102" s="17"/>
+      <c r="U102" s="19"/>
+    </row>
+    <row r="103" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B103" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C103" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D103" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E102" s="13" t="s">
+      <c r="E103" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F102" s="13" t="s">
+      <c r="F103" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="G102" s="13" t="s">
+      <c r="G103" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H102" s="13" t="s">
+      <c r="H103" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I102" s="13" t="s">
+      <c r="I103" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J102" s="13" t="s">
+      <c r="J103" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K102" s="13" t="s">
+      <c r="K103" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L102" s="13" t="s">
+      <c r="L103" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M102" s="13" t="s">
+      <c r="M103" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N102" s="13" t="s">
+      <c r="N103" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O102" s="13" t="s">
+      <c r="O103" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P102" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q102" s="14">
+      <c r="P103" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q103" s="14">
         <v>42118</v>
       </c>
-      <c r="R102" s="13" t="s">
+      <c r="R103" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S102" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T102" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U102" s="15"/>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103" s="10"/>
-      <c r="F103"/>
-      <c r="G103"/>
-      <c r="H103"/>
-      <c r="I103"/>
-      <c r="J103"/>
-      <c r="K103"/>
-      <c r="L103"/>
-      <c r="M103"/>
-      <c r="N103"/>
-      <c r="O103"/>
-      <c r="P103"/>
-      <c r="Q103"/>
-      <c r="R103"/>
-      <c r="S103"/>
-      <c r="T103"/>
-      <c r="U103"/>
+      <c r="S103" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T103" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U103" s="15"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="4"/>
-      <c r="S104" s="4"/>
-      <c r="T104" s="4"/>
-      <c r="U104" s="4"/>
+      <c r="A104"/>
+      <c r="B104"/>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104" s="10"/>
+      <c r="F104"/>
+      <c r="G104"/>
+      <c r="H104"/>
+      <c r="I104"/>
+      <c r="J104"/>
+      <c r="K104"/>
+      <c r="L104"/>
+      <c r="M104"/>
+      <c r="N104"/>
+      <c r="O104"/>
+      <c r="P104"/>
+      <c r="Q104"/>
+      <c r="R104"/>
+      <c r="S104"/>
+      <c r="T104"/>
+      <c r="U104"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="4"/>
@@ -8601,17 +8650,17 @@
       <c r="U105" s="4"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="B106" s="4"/>
+      <c r="A106" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B106" s="3"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
-      <c r="K106" s="4"/>
+      <c r="K106" s="3"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
@@ -8625,7 +8674,7 @@
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -8647,30 +8696,53 @@
       <c r="U107" s="4"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="4"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+      <c r="U108" s="4"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A109" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="7"/>
-      <c r="J108" s="7"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="7"/>
-      <c r="M108" s="7"/>
-      <c r="N108" s="7"/>
-      <c r="O108" s="7"/>
-      <c r="P108" s="7"/>
-      <c r="R108" s="7"/>
-      <c r="S108" s="7"/>
-      <c r="T108" s="7"/>
-      <c r="U108" s="7"/>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="7"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="7"/>
+      <c r="P109" s="7"/>
+      <c r="R109" s="7"/>
+      <c r="S109" s="7"/>
+      <c r="T109" s="7"/>
+      <c r="U109" s="7"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #566 : add new namespace "msl"
Issue #566 : add new namespace "msl"

Add the namespace "msl" to the Namespace Registry and the config.properties file.

The Mars Science Laboratory Mission Dictionary (msl) contains classes, attributes and rules specific to the MSL mission and its instruments.

@c-suh  [namespace-registry] add new namespace "msl" #566

Resolves #566
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92BEB4D4-0E44-4F04-B3F1-256CB4DD27CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2399724B-D8D0-4B77-9005-02F32E811604}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="668">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -2005,6 +2005,30 @@
   </si>
   <si>
     <t>PDS4_SB</t>
+  </si>
+  <si>
+    <t>msl</t>
+  </si>
+  <si>
+    <t>mission/msl</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/msl/v1</t>
+  </si>
+  <si>
+    <t>2023--1-25</t>
+  </si>
+  <si>
+    <t>MSL</t>
+  </si>
+  <si>
+    <t>PDS4_MSL</t>
+  </si>
+  <si>
+    <t>Mars Science Laboratory</t>
+  </si>
+  <si>
+    <t>Namespace for the Mars Science Laboratory dictionary.</t>
   </si>
 </sst>
 </file>
@@ -2109,7 +2133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2183,6 +2207,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2501,12 +2528,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U110"/>
+  <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5656,68 +5683,68 @@
       </c>
       <c r="U52" s="15"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>617</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="G53" s="13" t="s">
+    <row r="53" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>666</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="G53" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H53" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="I53" s="13" t="s">
+      <c r="H53" s="17" t="s">
+        <v>665</v>
+      </c>
+      <c r="I53" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="J53" s="13" t="s">
+      <c r="J53" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K53" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="L53" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M53" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="N53" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="O53" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="P53" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q53" s="14">
-        <v>42158</v>
-      </c>
-      <c r="R53" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="S53" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U53" s="15"/>
+      <c r="K53" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="L53" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M53" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="N53" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="O53" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="P53" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" s="26" t="s">
+        <v>663</v>
+      </c>
+      <c r="R53" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S53" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U53" s="19"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
@@ -5727,13 +5754,13 @@
         <v>617</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>256</v>
@@ -5782,93 +5809,93 @@
       </c>
       <c r="U54" s="15"/>
     </row>
-    <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>651</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>652</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>648</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="G55" s="17" t="s">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="G55" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H55" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="I55" s="17" t="s">
+      <c r="H55" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="I55" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="J55" s="17" t="s">
+      <c r="J55" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K55" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="L55" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M55" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N55" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="O55" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="P55" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q55" s="18">
-        <v>44833</v>
-      </c>
-      <c r="R55" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="S55" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T55" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U55" s="19"/>
+      <c r="K55" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M55" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N55" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O55" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P55" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q55" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R55" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="S55" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T55" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U55" s="15"/>
     </row>
     <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>605</v>
+        <v>647</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>608</v>
+        <v>651</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>609</v>
+        <v>652</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>606</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>607</v>
+        <v>647</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>648</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>605</v>
+        <v>647</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>213</v>
@@ -5877,7 +5904,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="L56" s="17" t="s">
         <v>123</v>
@@ -5886,19 +5913,19 @@
         <v>243</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>614</v>
+        <v>642</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>615</v>
+        <v>643</v>
       </c>
       <c r="P56" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q56" s="18">
-        <v>44713</v>
+        <v>44833</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>614</v>
+        <v>641</v>
       </c>
       <c r="S56" s="17" t="s">
         <v>31</v>
@@ -5908,30 +5935,30 @@
       </c>
       <c r="U56" s="19"/>
     </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>557</v>
+        <v>608</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>551</v>
+        <v>609</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>552</v>
+        <v>606</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>553</v>
+        <v>607</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>555</v>
+        <v>610</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>213</v>
@@ -5940,28 +5967,28 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>556</v>
+        <v>611</v>
       </c>
       <c r="L57" s="17" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="M57" s="17" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>268</v>
+        <v>614</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>269</v>
+        <v>615</v>
       </c>
       <c r="P57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q57" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="S57" s="17" t="s">
         <v>31</v>
@@ -5971,30 +5998,30 @@
       </c>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>571</v>
+        <v>552</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="I58" s="17" t="s">
         <v>213</v>
@@ -6003,7 +6030,7 @@
         <v>23</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="L58" s="17" t="s">
         <v>218</v>
@@ -6012,19 +6039,19 @@
         <v>177</v>
       </c>
       <c r="N58" s="17" t="s">
-        <v>573</v>
+        <v>268</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>574</v>
+        <v>269</v>
       </c>
       <c r="P58" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q58" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>185</v>
+        <v>554</v>
       </c>
       <c r="S58" s="17" t="s">
         <v>31</v>
@@ -6034,30 +6061,30 @@
       </c>
       <c r="U58" s="19"/>
     </row>
-    <row r="59" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>601</v>
+        <v>577</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>597</v>
+        <v>571</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="G59" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>602</v>
+        <v>575</v>
       </c>
       <c r="I59" s="17" t="s">
         <v>213</v>
@@ -6066,7 +6093,7 @@
         <v>23</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="L59" s="17" t="s">
         <v>218</v>
@@ -6075,115 +6102,115 @@
         <v>177</v>
       </c>
       <c r="N59" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="O59" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="P59" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q59" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R59" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="S59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U59" s="19"/>
+    </row>
+    <row r="60" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="I60" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K60" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N60" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="O59" s="17" t="s">
+      <c r="O60" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="P59" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q59" s="18">
+      <c r="P60" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q60" s="18">
         <v>44713</v>
       </c>
-      <c r="R59" s="17" t="s">
+      <c r="R60" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="S59" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T59" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U59" s="19"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>624</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I60" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J60" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K60" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="L60" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="M60" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N60" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="O60" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="P60" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q60" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R60" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="S60" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T60" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U60" s="15"/>
+      <c r="S60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U60" s="19"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>579</v>
+        <v>264</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>580</v>
+        <v>624</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>581</v>
+        <v>270</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>582</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>583</v>
+        <v>265</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>579</v>
+        <v>264</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>587</v>
+        <v>42</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>213</v>
@@ -6192,28 +6219,28 @@
         <v>23</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>584</v>
+        <v>267</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>585</v>
+        <v>268</v>
       </c>
       <c r="O61" s="13" t="s">
-        <v>586</v>
+        <v>269</v>
       </c>
       <c r="P61" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q61" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R61" s="13" t="s">
-        <v>588</v>
+        <v>185</v>
       </c>
       <c r="S61" s="13" t="s">
         <v>31</v>
@@ -6223,91 +6250,93 @@
       </c>
       <c r="U61" s="15"/>
     </row>
-    <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>271</v>
+        <v>579</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>625</v>
+        <v>580</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>277</v>
+        <v>581</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>272</v>
+        <v>582</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>583</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>271</v>
+        <v>579</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>273</v>
+        <v>21</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>274</v>
+        <v>587</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K62" s="13" t="s">
-        <v>271</v>
+        <v>584</v>
       </c>
       <c r="L62" s="13" t="s">
-        <v>271</v>
+        <v>166</v>
       </c>
       <c r="M62" s="13" t="s">
-        <v>271</v>
+        <v>170</v>
       </c>
       <c r="N62" s="13" t="s">
-        <v>275</v>
+        <v>585</v>
       </c>
       <c r="O62" s="13" t="s">
-        <v>276</v>
+        <v>586</v>
       </c>
       <c r="P62" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q62" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R62" s="13" t="s">
-        <v>65</v>
+        <v>588</v>
       </c>
       <c r="S62" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T62" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="U62" s="15"/>
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D63" s="13"/>
+        <v>277</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="E63" s="20" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>213</v>
@@ -6328,7 +6357,7 @@
         <v>275</v>
       </c>
       <c r="O63" s="13" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="P63" s="13" t="s">
         <v>42</v>
@@ -6337,10 +6366,10 @@
         <v>43788</v>
       </c>
       <c r="R63" s="13" t="s">
-        <v>285</v>
+        <v>65</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T63" s="13" t="s">
         <v>278</v>
@@ -6349,26 +6378,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>213</v>
@@ -6376,9 +6405,15 @@
       <c r="J64" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
+      <c r="K64" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="L64" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="M64" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="N64" s="13" t="s">
         <v>275</v>
       </c>
@@ -6395,7 +6430,7 @@
         <v>285</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="T64" s="13" t="s">
         <v>278</v>
@@ -6404,26 +6439,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>213</v>
@@ -6450,7 +6485,7 @@
         <v>285</v>
       </c>
       <c r="S65" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T65" s="13" t="s">
         <v>278</v>
@@ -6459,26 +6494,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>213</v>
@@ -6514,26 +6549,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>213</v>
@@ -6569,26 +6604,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>213</v>
@@ -6624,26 +6659,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>213</v>
@@ -6679,26 +6714,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>213</v>
@@ -6734,26 +6769,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>213</v>
@@ -6789,26 +6824,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>213</v>
@@ -6844,26 +6879,26 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>213</v>
@@ -6899,26 +6934,26 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>213</v>
@@ -6954,26 +6989,26 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="20" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I75" s="13" t="s">
         <v>213</v>
@@ -7009,141 +7044,139 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>347</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="D76" s="13"/>
       <c r="E76" s="20" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>21</v>
+        <v>273</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J76" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="O76" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="P76" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q76" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R76" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="S76" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="T76" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="U76" s="15"/>
+    </row>
+    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="E77" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="I77" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J77" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K76" s="13" t="s">
+      <c r="K77" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="L76" s="13" t="s">
+      <c r="L77" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="M76" s="13" t="s">
+      <c r="M77" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="N76" s="13" t="s">
+      <c r="N77" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="O76" s="13" t="s">
+      <c r="O77" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="P76" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q76" s="14">
+      <c r="P77" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q77" s="14">
         <v>44111</v>
       </c>
-      <c r="R76" s="13" t="s">
+      <c r="R77" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="S76" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T76" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U76" s="15"/>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P77" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q77" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R77" s="13"/>
-      <c r="S77" s="13"/>
-      <c r="T77" s="13"/>
+      <c r="S77" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T77" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U77" s="15"/>
     </row>
-    <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>627</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E78" s="20" t="s">
-        <v>354</v>
-      </c>
-      <c r="F78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="I78" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J78" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="L78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="M78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="N78" s="13" t="s">
-        <v>356</v>
-      </c>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
       <c r="O78" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P78" s="13" t="s">
         <v>42</v>
@@ -7151,39 +7184,35 @@
       <c r="Q78" s="14">
         <v>43788</v>
       </c>
-      <c r="R78" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="S78" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T78" s="13" t="s">
-        <v>278</v>
-      </c>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="13"/>
       <c r="U78" s="15"/>
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="D79" s="13"/>
+        <v>357</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>353</v>
+      </c>
       <c r="E79" s="20" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>213</v>
@@ -7204,7 +7233,7 @@
         <v>356</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7213,7 +7242,7 @@
         <v>43788</v>
       </c>
       <c r="R79" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S79" s="13" t="s">
         <v>31</v>
@@ -7225,26 +7254,26 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="20" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>213</v>
@@ -7265,7 +7294,7 @@
         <v>356</v>
       </c>
       <c r="O80" s="13" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7274,7 +7303,7 @@
         <v>43788</v>
       </c>
       <c r="R80" s="13" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="S80" s="13" t="s">
         <v>31</v>
@@ -7286,26 +7315,26 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="20" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>213</v>
@@ -7347,26 +7376,26 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="20" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>213</v>
@@ -7387,7 +7416,7 @@
         <v>356</v>
       </c>
       <c r="O82" s="13" t="s">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="P82" s="13" t="s">
         <v>42</v>
@@ -7396,7 +7425,7 @@
         <v>43788</v>
       </c>
       <c r="R82" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S82" s="13" t="s">
         <v>31</v>
@@ -7406,23 +7435,49 @@
       </c>
       <c r="U82" s="15"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+    <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>627</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>380</v>
+      </c>
       <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
+      <c r="E83" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J83" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K83" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="L83" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="M83" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="N83" s="13" t="s">
+        <v>356</v>
+      </c>
       <c r="O83" s="13" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="P83" s="13" t="s">
         <v>42</v>
@@ -7430,54 +7485,32 @@
       <c r="Q83" s="14">
         <v>43788</v>
       </c>
-      <c r="R83" s="13"/>
-      <c r="S83" s="13"/>
-      <c r="T83" s="13"/>
+      <c r="R83" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="S83" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T83" s="13" t="s">
+        <v>278</v>
+      </c>
       <c r="U83" s="15"/>
     </row>
-    <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>628</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="D84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="F84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H84" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="I84" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J84" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="L84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="M84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="N84" s="13" t="s">
-        <v>384</v>
-      </c>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13"/>
       <c r="O84" s="13" t="s">
         <v>63</v>
       </c>
@@ -7487,39 +7520,35 @@
       <c r="Q84" s="14">
         <v>43788</v>
       </c>
-      <c r="R84" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="S84" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="T84" s="13" t="s">
-        <v>278</v>
-      </c>
+      <c r="R84" s="13"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="13"/>
       <c r="U84" s="15"/>
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="D85" s="13"/>
+        <v>385</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="E85" s="20" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>213</v>
@@ -7552,7 +7581,7 @@
         <v>358</v>
       </c>
       <c r="S85" s="13" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="T85" s="13" t="s">
         <v>278</v>
@@ -7561,26 +7590,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>213</v>
@@ -7613,7 +7642,7 @@
         <v>358</v>
       </c>
       <c r="S86" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T86" s="13" t="s">
         <v>278</v>
@@ -7622,26 +7651,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>213</v>
@@ -7683,26 +7712,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>213</v>
@@ -7744,26 +7773,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>213</v>
@@ -7805,26 +7834,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>213</v>
@@ -7866,26 +7895,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>213</v>
@@ -7927,26 +7956,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>213</v>
@@ -7988,26 +8017,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>213</v>
@@ -8049,26 +8078,26 @@
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>213</v>
@@ -8110,26 +8139,26 @@
     </row>
     <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="20" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G95" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="I95" s="13" t="s">
         <v>213</v>
@@ -8171,26 +8200,26 @@
     </row>
     <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="20" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="G96" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="I96" s="13" t="s">
         <v>213</v>
@@ -8231,103 +8260,107 @@
       <c r="U96" s="15"/>
     </row>
     <row r="97" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="D97" s="13"/>
+      <c r="E97" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="G97" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="I97" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J97" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K97" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="L97" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="M97" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="N97" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="O97" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P97" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q97" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R97" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="S97" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="T97" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="U97" s="15"/>
+    </row>
+    <row r="98" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="22"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="22"/>
-      <c r="I97" s="22"/>
-      <c r="J97" s="22"/>
-      <c r="K97" s="22"/>
-      <c r="L97" s="22"/>
-      <c r="M97" s="22"/>
-      <c r="N97" s="22"/>
-      <c r="O97" s="22"/>
-      <c r="P97" s="22"/>
-      <c r="Q97" s="22"/>
-      <c r="R97" s="22"/>
-      <c r="S97" s="22"/>
-      <c r="T97" s="22"/>
-      <c r="U97" s="22"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="D98" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="E98" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="F98" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="G98" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I98" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J98" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K98" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="L98" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="M98" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N98" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O98" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P98" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q98" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R98" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="S98" s="13"/>
-      <c r="T98" s="13"/>
-      <c r="U98" s="15"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
+      <c r="K98" s="22"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="22"/>
+      <c r="N98" s="22"/>
+      <c r="O98" s="22"/>
+      <c r="P98" s="22"/>
+      <c r="Q98" s="22"/>
+      <c r="R98" s="22"/>
+      <c r="S98" s="22"/>
+      <c r="T98" s="22"/>
+      <c r="U98" s="22"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
@@ -8342,28 +8375,28 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>123</v>
+        <v>450</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N99" s="13" t="s">
-        <v>455</v>
+        <v>26</v>
       </c>
       <c r="O99" s="13" t="s">
-        <v>456</v>
+        <v>27</v>
       </c>
       <c r="P99" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q99" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R99" s="13" t="s">
-        <v>30</v>
+        <v>452</v>
       </c>
       <c r="S99" s="13"/>
       <c r="T99" s="13"/>
@@ -8371,20 +8404,20 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
@@ -8399,19 +8432,19 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="M100" s="13" t="s">
-        <v>461</v>
+        <v>124</v>
       </c>
       <c r="N100" s="13" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O100" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="P100" s="13" t="s">
         <v>42</v>
@@ -8428,20 +8461,20 @@
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="G101" s="13" t="s">
         <v>21</v>
@@ -8456,19 +8489,19 @@
         <v>23</v>
       </c>
       <c r="K101" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="L101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="M101" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="N101" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="O101" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="P101" s="13" t="s">
         <v>42</v>
@@ -8483,175 +8516,209 @@
       <c r="T101" s="13"/>
       <c r="U101" s="15"/>
     </row>
-    <row r="102" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="17" t="s">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I102" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="L102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="M102" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="N102" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="O102" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="P102" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q102" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R102" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S102" s="13"/>
+      <c r="T102" s="13"/>
+      <c r="U102" s="15"/>
+    </row>
+    <row r="103" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B102" s="17"/>
-      <c r="C102" s="13" t="s">
+      <c r="B103" s="17"/>
+      <c r="C103" s="13" t="s">
         <v>656</v>
       </c>
-      <c r="D102" s="17" t="s">
+      <c r="D103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E102" s="17" t="s">
+      <c r="E103" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="F102" s="17" t="s">
+      <c r="F103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G102" s="17" t="s">
+      <c r="G103" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H102" s="17" t="s">
+      <c r="H103" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="I102" s="17" t="s">
+      <c r="I103" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J102" s="17" t="s">
+      <c r="J103" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K102" s="17" t="s">
+      <c r="K103" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="L102" s="17" t="s">
+      <c r="L103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M102" s="17" t="s">
+      <c r="M103" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="N102" s="17" t="s">
+      <c r="N103" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="O102" s="17" t="s">
+      <c r="O103" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P102" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q102" s="18">
+      <c r="P103" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q103" s="18">
         <v>41002</v>
       </c>
-      <c r="R102" s="17" t="s">
+      <c r="R103" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S102" s="17"/>
-      <c r="T102" s="17"/>
-      <c r="U102" s="19"/>
-    </row>
-    <row r="103" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
+      <c r="S103" s="17"/>
+      <c r="T103" s="17"/>
+      <c r="U103" s="19"/>
+    </row>
+    <row r="104" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B104" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C104" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D103" s="13" t="s">
+      <c r="D104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E103" s="13" t="s">
+      <c r="E104" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F103" s="13" t="s">
+      <c r="F104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="G103" s="13" t="s">
+      <c r="G104" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H103" s="13" t="s">
+      <c r="H104" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I103" s="13" t="s">
+      <c r="I104" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J103" s="13" t="s">
+      <c r="J104" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K103" s="13" t="s">
+      <c r="K104" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L103" s="13" t="s">
+      <c r="L104" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M103" s="13" t="s">
+      <c r="M104" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N103" s="13" t="s">
+      <c r="N104" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O103" s="13" t="s">
+      <c r="O104" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P103" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q103" s="14">
+      <c r="P104" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q104" s="14">
         <v>42118</v>
       </c>
-      <c r="R103" s="13" t="s">
+      <c r="R104" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S103" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T103" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U103" s="15"/>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104" s="10"/>
-      <c r="F104"/>
-      <c r="G104"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="L104"/>
-      <c r="M104"/>
-      <c r="N104"/>
-      <c r="O104"/>
-      <c r="P104"/>
-      <c r="Q104"/>
-      <c r="R104"/>
-      <c r="S104"/>
-      <c r="T104"/>
-      <c r="U104"/>
+      <c r="S104" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T104" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U104" s="15"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
-      <c r="Q105" s="6"/>
-      <c r="R105" s="4"/>
-      <c r="S105" s="4"/>
-      <c r="T105" s="4"/>
-      <c r="U105" s="4"/>
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105" s="10"/>
+      <c r="F105"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+      <c r="P105"/>
+      <c r="Q105"/>
+      <c r="R105"/>
+      <c r="S105"/>
+      <c r="T105"/>
+      <c r="U105"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="4"/>
@@ -8673,17 +8740,17 @@
       <c r="U106" s="4"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="B107" s="4"/>
+      <c r="A107" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B107" s="3"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
-      <c r="K107" s="4"/>
+      <c r="K107" s="3"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
@@ -8697,7 +8764,7 @@
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -8719,30 +8786,53 @@
       <c r="U108" s="4"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="6"/>
+      <c r="R109" s="4"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+      <c r="U109" s="4"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A110" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
-      <c r="F109" s="7"/>
-      <c r="G109" s="7"/>
-      <c r="H109" s="7"/>
-      <c r="I109" s="7"/>
-      <c r="J109" s="7"/>
-      <c r="K109" s="7"/>
-      <c r="L109" s="7"/>
-      <c r="M109" s="7"/>
-      <c r="N109" s="7"/>
-      <c r="O109" s="7"/>
-      <c r="P109" s="7"/>
-      <c r="R109" s="7"/>
-      <c r="S109" s="7"/>
-      <c r="T109" s="7"/>
-      <c r="U109" s="7"/>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="7"/>
+      <c r="N110" s="7"/>
+      <c r="O110" s="7"/>
+      <c r="P110" s="7"/>
+      <c r="R110" s="7"/>
+      <c r="S110" s="7"/>
+      <c r="T110" s="7"/>
+      <c r="U110" s="7"/>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue #566 : add new namespace "msl" (#567)
Issue #566 : add new namespace "msl"

Add the namespace "msl" to the Namespace Registry and the config.properties file.

The Mars Science Laboratory Mission Dictionary (msl) contains classes, attributes and rules specific to the MSL mission and its instruments.

@c-suh  [namespace-registry] add new namespace "msl" #566

Resolves #566

Co-authored-by: John Hughes <jsh416@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92BEB4D4-0E44-4F04-B3F1-256CB4DD27CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2399724B-D8D0-4B77-9005-02F32E811604}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="668">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -2005,6 +2005,30 @@
   </si>
   <si>
     <t>PDS4_SB</t>
+  </si>
+  <si>
+    <t>msl</t>
+  </si>
+  <si>
+    <t>mission/msl</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/mission/msl/v1</t>
+  </si>
+  <si>
+    <t>2023--1-25</t>
+  </si>
+  <si>
+    <t>MSL</t>
+  </si>
+  <si>
+    <t>PDS4_MSL</t>
+  </si>
+  <si>
+    <t>Mars Science Laboratory</t>
+  </si>
+  <si>
+    <t>Namespace for the Mars Science Laboratory dictionary.</t>
   </si>
 </sst>
 </file>
@@ -2109,7 +2133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2183,6 +2207,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2501,12 +2528,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U110"/>
+  <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5656,68 +5683,68 @@
       </c>
       <c r="U52" s="15"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>617</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="G53" s="13" t="s">
+    <row r="53" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>666</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="G53" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H53" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="I53" s="13" t="s">
+      <c r="H53" s="17" t="s">
+        <v>665</v>
+      </c>
+      <c r="I53" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="J53" s="13" t="s">
+      <c r="J53" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K53" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="L53" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M53" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="N53" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="O53" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="P53" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q53" s="14">
-        <v>42158</v>
-      </c>
-      <c r="R53" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="S53" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U53" s="15"/>
+      <c r="K53" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="L53" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M53" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="N53" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="O53" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="P53" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" s="26" t="s">
+        <v>663</v>
+      </c>
+      <c r="R53" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S53" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U53" s="19"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
@@ -5727,13 +5754,13 @@
         <v>617</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>256</v>
@@ -5782,93 +5809,93 @@
       </c>
       <c r="U54" s="15"/>
     </row>
-    <row r="55" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>651</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>652</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>648</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="G55" s="17" t="s">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="G55" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H55" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="I55" s="17" t="s">
+      <c r="H55" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="I55" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="J55" s="17" t="s">
+      <c r="J55" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K55" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="L55" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M55" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N55" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="O55" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="P55" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q55" s="18">
-        <v>44833</v>
-      </c>
-      <c r="R55" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="S55" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T55" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U55" s="19"/>
+      <c r="K55" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M55" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N55" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O55" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P55" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q55" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R55" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="S55" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T55" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U55" s="15"/>
     </row>
     <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>605</v>
+        <v>647</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>608</v>
+        <v>651</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>609</v>
+        <v>652</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>606</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>607</v>
+        <v>647</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>648</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>605</v>
+        <v>647</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>213</v>
@@ -5877,7 +5904,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="L56" s="17" t="s">
         <v>123</v>
@@ -5886,19 +5913,19 @@
         <v>243</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>614</v>
+        <v>642</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>615</v>
+        <v>643</v>
       </c>
       <c r="P56" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q56" s="18">
-        <v>44713</v>
+        <v>44833</v>
       </c>
       <c r="R56" s="17" t="s">
-        <v>614</v>
+        <v>641</v>
       </c>
       <c r="S56" s="17" t="s">
         <v>31</v>
@@ -5908,30 +5935,30 @@
       </c>
       <c r="U56" s="19"/>
     </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>557</v>
+        <v>608</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>551</v>
+        <v>609</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>552</v>
+        <v>606</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>553</v>
+        <v>607</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>555</v>
+        <v>610</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>213</v>
@@ -5940,28 +5967,28 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>556</v>
+        <v>611</v>
       </c>
       <c r="L57" s="17" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="M57" s="17" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>268</v>
+        <v>614</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>269</v>
+        <v>615</v>
       </c>
       <c r="P57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q57" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="S57" s="17" t="s">
         <v>31</v>
@@ -5971,30 +5998,30 @@
       </c>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>571</v>
+        <v>552</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="I58" s="17" t="s">
         <v>213</v>
@@ -6003,7 +6030,7 @@
         <v>23</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="L58" s="17" t="s">
         <v>218</v>
@@ -6012,19 +6039,19 @@
         <v>177</v>
       </c>
       <c r="N58" s="17" t="s">
-        <v>573</v>
+        <v>268</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>574</v>
+        <v>269</v>
       </c>
       <c r="P58" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q58" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>185</v>
+        <v>554</v>
       </c>
       <c r="S58" s="17" t="s">
         <v>31</v>
@@ -6034,30 +6061,30 @@
       </c>
       <c r="U58" s="19"/>
     </row>
-    <row r="59" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>601</v>
+        <v>577</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>597</v>
+        <v>571</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="G59" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>602</v>
+        <v>575</v>
       </c>
       <c r="I59" s="17" t="s">
         <v>213</v>
@@ -6066,7 +6093,7 @@
         <v>23</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="L59" s="17" t="s">
         <v>218</v>
@@ -6075,115 +6102,115 @@
         <v>177</v>
       </c>
       <c r="N59" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="O59" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="P59" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q59" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R59" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="S59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U59" s="19"/>
+    </row>
+    <row r="60" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="I60" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K60" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N60" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="O59" s="17" t="s">
+      <c r="O60" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="P59" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q59" s="18">
+      <c r="P60" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q60" s="18">
         <v>44713</v>
       </c>
-      <c r="R59" s="17" t="s">
+      <c r="R60" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="S59" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T59" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U59" s="19"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>624</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I60" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J60" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K60" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="L60" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="M60" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N60" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="O60" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="P60" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q60" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R60" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="S60" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T60" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U60" s="15"/>
+      <c r="S60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U60" s="19"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>579</v>
+        <v>264</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>580</v>
+        <v>624</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>581</v>
+        <v>270</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>582</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>583</v>
+        <v>265</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>579</v>
+        <v>264</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>587</v>
+        <v>42</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>213</v>
@@ -6192,28 +6219,28 @@
         <v>23</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>584</v>
+        <v>267</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>585</v>
+        <v>268</v>
       </c>
       <c r="O61" s="13" t="s">
-        <v>586</v>
+        <v>269</v>
       </c>
       <c r="P61" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q61" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R61" s="13" t="s">
-        <v>588</v>
+        <v>185</v>
       </c>
       <c r="S61" s="13" t="s">
         <v>31</v>
@@ -6223,91 +6250,93 @@
       </c>
       <c r="U61" s="15"/>
     </row>
-    <row r="62" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>271</v>
+        <v>579</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>625</v>
+        <v>580</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>277</v>
+        <v>581</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>272</v>
+        <v>582</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>583</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>271</v>
+        <v>579</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>273</v>
+        <v>21</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>274</v>
+        <v>587</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K62" s="13" t="s">
-        <v>271</v>
+        <v>584</v>
       </c>
       <c r="L62" s="13" t="s">
-        <v>271</v>
+        <v>166</v>
       </c>
       <c r="M62" s="13" t="s">
-        <v>271</v>
+        <v>170</v>
       </c>
       <c r="N62" s="13" t="s">
-        <v>275</v>
+        <v>585</v>
       </c>
       <c r="O62" s="13" t="s">
-        <v>276</v>
+        <v>586</v>
       </c>
       <c r="P62" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q62" s="14">
-        <v>43788</v>
+        <v>44700</v>
       </c>
       <c r="R62" s="13" t="s">
-        <v>65</v>
+        <v>588</v>
       </c>
       <c r="S62" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T62" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="U62" s="15"/>
     </row>
     <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D63" s="13"/>
+        <v>277</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="E63" s="20" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>213</v>
@@ -6328,7 +6357,7 @@
         <v>275</v>
       </c>
       <c r="O63" s="13" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="P63" s="13" t="s">
         <v>42</v>
@@ -6337,10 +6366,10 @@
         <v>43788</v>
       </c>
       <c r="R63" s="13" t="s">
-        <v>285</v>
+        <v>65</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T63" s="13" t="s">
         <v>278</v>
@@ -6349,26 +6378,26 @@
     </row>
     <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="20" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>213</v>
@@ -6376,9 +6405,15 @@
       <c r="J64" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
+      <c r="K64" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="L64" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="M64" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="N64" s="13" t="s">
         <v>275</v>
       </c>
@@ -6395,7 +6430,7 @@
         <v>285</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="T64" s="13" t="s">
         <v>278</v>
@@ -6404,26 +6439,26 @@
     </row>
     <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>213</v>
@@ -6450,7 +6485,7 @@
         <v>285</v>
       </c>
       <c r="S65" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T65" s="13" t="s">
         <v>278</v>
@@ -6459,26 +6494,26 @@
     </row>
     <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>213</v>
@@ -6514,26 +6549,26 @@
     </row>
     <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>213</v>
@@ -6569,26 +6604,26 @@
     </row>
     <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>213</v>
@@ -6624,26 +6659,26 @@
     </row>
     <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>213</v>
@@ -6679,26 +6714,26 @@
     </row>
     <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>213</v>
@@ -6734,26 +6769,26 @@
     </row>
     <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>213</v>
@@ -6789,26 +6824,26 @@
     </row>
     <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>213</v>
@@ -6844,26 +6879,26 @@
     </row>
     <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>213</v>
@@ -6899,26 +6934,26 @@
     </row>
     <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>213</v>
@@ -6954,26 +6989,26 @@
     </row>
     <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="20" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I75" s="13" t="s">
         <v>213</v>
@@ -7009,141 +7044,139 @@
     </row>
     <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>347</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="D76" s="13"/>
       <c r="E76" s="20" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>21</v>
+        <v>273</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J76" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="O76" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="P76" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q76" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R76" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="S76" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="T76" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="U76" s="15"/>
+    </row>
+    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="E77" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="I77" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J77" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K76" s="13" t="s">
+      <c r="K77" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="L76" s="13" t="s">
+      <c r="L77" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="M76" s="13" t="s">
+      <c r="M77" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="N76" s="13" t="s">
+      <c r="N77" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="O76" s="13" t="s">
+      <c r="O77" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="P76" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q76" s="14">
+      <c r="P77" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q77" s="14">
         <v>44111</v>
       </c>
-      <c r="R76" s="13" t="s">
+      <c r="R77" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="S76" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T76" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U76" s="15"/>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P77" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q77" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R77" s="13"/>
-      <c r="S77" s="13"/>
-      <c r="T77" s="13"/>
+      <c r="S77" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T77" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U77" s="15"/>
     </row>
-    <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>627</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E78" s="20" t="s">
-        <v>354</v>
-      </c>
-      <c r="F78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="I78" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J78" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="L78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="M78" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="N78" s="13" t="s">
-        <v>356</v>
-      </c>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
       <c r="O78" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P78" s="13" t="s">
         <v>42</v>
@@ -7151,39 +7184,35 @@
       <c r="Q78" s="14">
         <v>43788</v>
       </c>
-      <c r="R78" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="S78" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T78" s="13" t="s">
-        <v>278</v>
-      </c>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="13"/>
       <c r="U78" s="15"/>
     </row>
     <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="D79" s="13"/>
+        <v>357</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>353</v>
+      </c>
       <c r="E79" s="20" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>213</v>
@@ -7204,7 +7233,7 @@
         <v>356</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7213,7 +7242,7 @@
         <v>43788</v>
       </c>
       <c r="R79" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S79" s="13" t="s">
         <v>31</v>
@@ -7225,26 +7254,26 @@
     </row>
     <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="20" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>213</v>
@@ -7265,7 +7294,7 @@
         <v>356</v>
       </c>
       <c r="O80" s="13" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7274,7 +7303,7 @@
         <v>43788</v>
       </c>
       <c r="R80" s="13" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="S80" s="13" t="s">
         <v>31</v>
@@ -7286,26 +7315,26 @@
     </row>
     <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="20" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>213</v>
@@ -7347,26 +7376,26 @@
     </row>
     <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="20" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>213</v>
@@ -7387,7 +7416,7 @@
         <v>356</v>
       </c>
       <c r="O82" s="13" t="s">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="P82" s="13" t="s">
         <v>42</v>
@@ -7396,7 +7425,7 @@
         <v>43788</v>
       </c>
       <c r="R82" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S82" s="13" t="s">
         <v>31</v>
@@ -7406,23 +7435,49 @@
       </c>
       <c r="U82" s="15"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+    <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>627</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>380</v>
+      </c>
       <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
+      <c r="E83" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J83" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K83" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="L83" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="M83" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="N83" s="13" t="s">
+        <v>356</v>
+      </c>
       <c r="O83" s="13" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="P83" s="13" t="s">
         <v>42</v>
@@ -7430,54 +7485,32 @@
       <c r="Q83" s="14">
         <v>43788</v>
       </c>
-      <c r="R83" s="13"/>
-      <c r="S83" s="13"/>
-      <c r="T83" s="13"/>
+      <c r="R83" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="S83" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T83" s="13" t="s">
+        <v>278</v>
+      </c>
       <c r="U83" s="15"/>
     </row>
-    <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>628</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="D84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="F84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H84" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="I84" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J84" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="L84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="M84" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="N84" s="13" t="s">
-        <v>384</v>
-      </c>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13"/>
       <c r="O84" s="13" t="s">
         <v>63</v>
       </c>
@@ -7487,39 +7520,35 @@
       <c r="Q84" s="14">
         <v>43788</v>
       </c>
-      <c r="R84" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="S84" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="T84" s="13" t="s">
-        <v>278</v>
-      </c>
+      <c r="R84" s="13"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="13"/>
       <c r="U84" s="15"/>
     </row>
     <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="D85" s="13"/>
+        <v>385</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="E85" s="20" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>213</v>
@@ -7552,7 +7581,7 @@
         <v>358</v>
       </c>
       <c r="S85" s="13" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="T85" s="13" t="s">
         <v>278</v>
@@ -7561,26 +7590,26 @@
     </row>
     <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="20" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>213</v>
@@ -7613,7 +7642,7 @@
         <v>358</v>
       </c>
       <c r="S86" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T86" s="13" t="s">
         <v>278</v>
@@ -7622,26 +7651,26 @@
     </row>
     <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>213</v>
@@ -7683,26 +7712,26 @@
     </row>
     <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>213</v>
@@ -7744,26 +7773,26 @@
     </row>
     <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>213</v>
@@ -7805,26 +7834,26 @@
     </row>
     <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>213</v>
@@ -7866,26 +7895,26 @@
     </row>
     <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>213</v>
@@ -7927,26 +7956,26 @@
     </row>
     <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>213</v>
@@ -7988,26 +8017,26 @@
     </row>
     <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>213</v>
@@ -8049,26 +8078,26 @@
     </row>
     <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>213</v>
@@ -8110,26 +8139,26 @@
     </row>
     <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="20" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G95" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="I95" s="13" t="s">
         <v>213</v>
@@ -8171,26 +8200,26 @@
     </row>
     <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="20" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="G96" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="I96" s="13" t="s">
         <v>213</v>
@@ -8231,103 +8260,107 @@
       <c r="U96" s="15"/>
     </row>
     <row r="97" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="D97" s="13"/>
+      <c r="E97" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="G97" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="I97" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J97" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K97" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="L97" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="M97" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="N97" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="O97" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P97" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q97" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R97" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="S97" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="T97" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="U97" s="15"/>
+    </row>
+    <row r="98" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="22"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="22"/>
-      <c r="I97" s="22"/>
-      <c r="J97" s="22"/>
-      <c r="K97" s="22"/>
-      <c r="L97" s="22"/>
-      <c r="M97" s="22"/>
-      <c r="N97" s="22"/>
-      <c r="O97" s="22"/>
-      <c r="P97" s="22"/>
-      <c r="Q97" s="22"/>
-      <c r="R97" s="22"/>
-      <c r="S97" s="22"/>
-      <c r="T97" s="22"/>
-      <c r="U97" s="22"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="D98" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="E98" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="F98" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="G98" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I98" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J98" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K98" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="L98" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="M98" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N98" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O98" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P98" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q98" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R98" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="S98" s="13"/>
-      <c r="T98" s="13"/>
-      <c r="U98" s="15"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
+      <c r="K98" s="22"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="22"/>
+      <c r="N98" s="22"/>
+      <c r="O98" s="22"/>
+      <c r="P98" s="22"/>
+      <c r="Q98" s="22"/>
+      <c r="R98" s="22"/>
+      <c r="S98" s="22"/>
+      <c r="T98" s="22"/>
+      <c r="U98" s="22"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>21</v>
@@ -8342,28 +8375,28 @@
         <v>23</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>123</v>
+        <v>450</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N99" s="13" t="s">
-        <v>455</v>
+        <v>26</v>
       </c>
       <c r="O99" s="13" t="s">
-        <v>456</v>
+        <v>27</v>
       </c>
       <c r="P99" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q99" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R99" s="13" t="s">
-        <v>30</v>
+        <v>452</v>
       </c>
       <c r="S99" s="13"/>
       <c r="T99" s="13"/>
@@ -8371,20 +8404,20 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
@@ -8399,19 +8432,19 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="M100" s="13" t="s">
-        <v>461</v>
+        <v>124</v>
       </c>
       <c r="N100" s="13" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O100" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="P100" s="13" t="s">
         <v>42</v>
@@ -8428,20 +8461,20 @@
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="G101" s="13" t="s">
         <v>21</v>
@@ -8456,19 +8489,19 @@
         <v>23</v>
       </c>
       <c r="K101" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="L101" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="M101" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="N101" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="O101" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="P101" s="13" t="s">
         <v>42</v>
@@ -8483,175 +8516,209 @@
       <c r="T101" s="13"/>
       <c r="U101" s="15"/>
     </row>
-    <row r="102" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="17" t="s">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I102" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="L102" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="M102" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="N102" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="O102" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="P102" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q102" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R102" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S102" s="13"/>
+      <c r="T102" s="13"/>
+      <c r="U102" s="15"/>
+    </row>
+    <row r="103" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B102" s="17"/>
-      <c r="C102" s="13" t="s">
+      <c r="B103" s="17"/>
+      <c r="C103" s="13" t="s">
         <v>656</v>
       </c>
-      <c r="D102" s="17" t="s">
+      <c r="D103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E102" s="17" t="s">
+      <c r="E103" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="F102" s="17" t="s">
+      <c r="F103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G102" s="17" t="s">
+      <c r="G103" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H102" s="17" t="s">
+      <c r="H103" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="I102" s="17" t="s">
+      <c r="I103" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J102" s="17" t="s">
+      <c r="J103" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K102" s="17" t="s">
+      <c r="K103" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="L102" s="17" t="s">
+      <c r="L103" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M102" s="17" t="s">
+      <c r="M103" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="N102" s="17" t="s">
+      <c r="N103" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="O102" s="17" t="s">
+      <c r="O103" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P102" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q102" s="18">
+      <c r="P103" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q103" s="18">
         <v>41002</v>
       </c>
-      <c r="R102" s="17" t="s">
+      <c r="R103" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S102" s="17"/>
-      <c r="T102" s="17"/>
-      <c r="U102" s="19"/>
-    </row>
-    <row r="103" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
+      <c r="S103" s="17"/>
+      <c r="T103" s="17"/>
+      <c r="U103" s="19"/>
+    </row>
+    <row r="104" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B104" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C104" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D103" s="13" t="s">
+      <c r="D104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E103" s="13" t="s">
+      <c r="E104" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F103" s="13" t="s">
+      <c r="F104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="G103" s="13" t="s">
+      <c r="G104" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H103" s="13" t="s">
+      <c r="H104" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I103" s="13" t="s">
+      <c r="I104" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J103" s="13" t="s">
+      <c r="J104" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K103" s="13" t="s">
+      <c r="K104" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L103" s="13" t="s">
+      <c r="L104" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M103" s="13" t="s">
+      <c r="M104" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N103" s="13" t="s">
+      <c r="N104" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O103" s="13" t="s">
+      <c r="O104" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P103" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q103" s="14">
+      <c r="P104" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q104" s="14">
         <v>42118</v>
       </c>
-      <c r="R103" s="13" t="s">
+      <c r="R104" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S103" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T103" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U103" s="15"/>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104" s="10"/>
-      <c r="F104"/>
-      <c r="G104"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="L104"/>
-      <c r="M104"/>
-      <c r="N104"/>
-      <c r="O104"/>
-      <c r="P104"/>
-      <c r="Q104"/>
-      <c r="R104"/>
-      <c r="S104"/>
-      <c r="T104"/>
-      <c r="U104"/>
+      <c r="S104" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T104" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U104" s="15"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
-      <c r="Q105" s="6"/>
-      <c r="R105" s="4"/>
-      <c r="S105" s="4"/>
-      <c r="T105" s="4"/>
-      <c r="U105" s="4"/>
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105" s="10"/>
+      <c r="F105"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+      <c r="P105"/>
+      <c r="Q105"/>
+      <c r="R105"/>
+      <c r="S105"/>
+      <c r="T105"/>
+      <c r="U105"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="4"/>
@@ -8673,17 +8740,17 @@
       <c r="U106" s="4"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="B107" s="4"/>
+      <c r="A107" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B107" s="3"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
-      <c r="K107" s="4"/>
+      <c r="K107" s="3"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
@@ -8697,7 +8764,7 @@
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -8719,30 +8786,53 @@
       <c r="U108" s="4"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="6"/>
+      <c r="R109" s="4"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+      <c r="U109" s="4"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A110" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
-      <c r="F109" s="7"/>
-      <c r="G109" s="7"/>
-      <c r="H109" s="7"/>
-      <c r="I109" s="7"/>
-      <c r="J109" s="7"/>
-      <c r="K109" s="7"/>
-      <c r="L109" s="7"/>
-      <c r="M109" s="7"/>
-      <c r="N109" s="7"/>
-      <c r="O109" s="7"/>
-      <c r="P109" s="7"/>
-      <c r="R109" s="7"/>
-      <c r="S109" s="7"/>
-      <c r="T109" s="7"/>
-      <c r="U109" s="7"/>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="7"/>
+      <c r="N110" s="7"/>
+      <c r="O110" s="7"/>
+      <c r="P110" s="7"/>
+      <c r="R110" s="7"/>
+      <c r="S110" s="7"/>
+      <c r="T110" s="7"/>
+      <c r="U110" s="7"/>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the namespace "lucy" to the Namespace Registry and the config.properties file.
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jshughes\git\pds4-information-model\docs\namespace-registry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2399724B-D8D0-4B77-9005-02F32E811604}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF2CB9B-E968-4E61-8438-0BC778A188FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="676">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -2029,6 +2029,30 @@
   </si>
   <si>
     <t>Namespace for the Mars Science Laboratory dictionary.</t>
+  </si>
+  <si>
+    <t>lucy</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/lucy/v1</t>
+  </si>
+  <si>
+    <t>LUCY</t>
+  </si>
+  <si>
+    <t>msk at astro.umd.edu</t>
+  </si>
+  <si>
+    <t>Michael Kelley</t>
+  </si>
+  <si>
+    <t>M. Kelley</t>
+  </si>
+  <si>
+    <t>Namespace for the Lucy Mission Dictionary.</t>
+  </si>
+  <si>
+    <t>Lucy Mission</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2210,6 +2234,9 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2528,15 +2555,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="14.296875" style="5" customWidth="1"/>
     <col min="2" max="2" width="23.796875" style="5" customWidth="1"/>
@@ -2561,7 +2588,7 @@
     <col min="21" max="21" width="13.69921875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -2651,7 +2678,7 @@
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
@@ -2714,7 +2741,7 @@
       </c>
       <c r="U3" s="15"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
@@ -2739,7 +2766,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
     </row>
-    <row r="5" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -2802,7 +2829,7 @@
       </c>
       <c r="U5" s="15"/>
     </row>
-    <row r="6" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
@@ -2865,7 +2892,7 @@
       </c>
       <c r="U6" s="15"/>
     </row>
-    <row r="7" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A7" s="17" t="s">
         <v>539</v>
       </c>
@@ -2924,7 +2951,7 @@
       <c r="T7" s="17"/>
       <c r="U7" s="19"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2989,7 +3016,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A9" s="13" t="s">
         <v>66</v>
       </c>
@@ -3052,7 +3079,7 @@
       </c>
       <c r="U9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A10" s="13" t="s">
         <v>75</v>
       </c>
@@ -3115,7 +3142,7 @@
       </c>
       <c r="U10" s="15"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -3140,7 +3167,7 @@
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
     </row>
-    <row r="12" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A12" s="13" t="s">
         <v>85</v>
       </c>
@@ -3203,7 +3230,7 @@
       </c>
       <c r="U12" s="15"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A13" s="13" t="s">
         <v>95</v>
       </c>
@@ -3266,7 +3293,7 @@
       </c>
       <c r="U13" s="15"/>
     </row>
-    <row r="14" spans="1:21" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="124.8" x14ac:dyDescent="0.6">
       <c r="A14" s="13" t="s">
         <v>103</v>
       </c>
@@ -3329,7 +3356,7 @@
       </c>
       <c r="U14" s="15"/>
     </row>
-    <row r="15" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="13" t="s">
         <v>495</v>
       </c>
@@ -3392,7 +3419,7 @@
       </c>
       <c r="U15" s="15"/>
     </row>
-    <row r="16" spans="1:21" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A16" s="13" t="s">
         <v>113</v>
       </c>
@@ -3455,7 +3482,7 @@
       </c>
       <c r="U16" s="15"/>
     </row>
-    <row r="17" spans="1:21" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A17" s="17" t="s">
         <v>526</v>
       </c>
@@ -3518,7 +3545,7 @@
       </c>
       <c r="U17" s="19"/>
     </row>
-    <row r="18" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A18" s="13" t="s">
         <v>119</v>
       </c>
@@ -3581,7 +3608,7 @@
       </c>
       <c r="U18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A19" s="13" t="s">
         <v>107</v>
       </c>
@@ -3644,7 +3671,7 @@
       </c>
       <c r="U19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A20" s="13" t="s">
         <v>133</v>
       </c>
@@ -3707,7 +3734,7 @@
       </c>
       <c r="U20" s="15"/>
     </row>
-    <row r="21" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A21" s="17" t="s">
         <v>501</v>
       </c>
@@ -3770,7 +3797,7 @@
       </c>
       <c r="U21" s="19"/>
     </row>
-    <row r="22" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A22" s="13" t="s">
         <v>208</v>
       </c>
@@ -3833,7 +3860,7 @@
       </c>
       <c r="U22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A23" s="13" t="s">
         <v>139</v>
       </c>
@@ -3896,7 +3923,7 @@
       </c>
       <c r="U23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="78" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="78" x14ac:dyDescent="0.6">
       <c r="A24" s="13" t="s">
         <v>203</v>
       </c>
@@ -3959,7 +3986,7 @@
       </c>
       <c r="U24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A25" s="13" t="s">
         <v>144</v>
       </c>
@@ -4022,7 +4049,7 @@
       </c>
       <c r="U25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A26" s="13" t="s">
         <v>151</v>
       </c>
@@ -4085,7 +4112,7 @@
       </c>
       <c r="U26" s="15"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A27" s="13" t="s">
         <v>19</v>
       </c>
@@ -4148,7 +4175,7 @@
       </c>
       <c r="U27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A28" s="13" t="s">
         <v>89</v>
       </c>
@@ -4209,7 +4236,7 @@
       </c>
       <c r="U28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A29" s="13" t="s">
         <v>161</v>
       </c>
@@ -4272,7 +4299,7 @@
       </c>
       <c r="U29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A30" s="13" t="s">
         <v>166</v>
       </c>
@@ -4335,7 +4362,7 @@
       </c>
       <c r="U30" s="15"/>
     </row>
-    <row r="31" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A31" s="17" t="s">
         <v>657</v>
       </c>
@@ -4398,7 +4425,7 @@
       </c>
       <c r="U31" s="19"/>
     </row>
-    <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A32" s="13" t="s">
         <v>180</v>
       </c>
@@ -4461,7 +4488,7 @@
       </c>
       <c r="U32" s="15"/>
     </row>
-    <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A33" s="13" t="s">
         <v>186</v>
       </c>
@@ -4524,7 +4551,7 @@
       </c>
       <c r="U33" s="15"/>
     </row>
-    <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A34" s="13" t="s">
         <v>194</v>
       </c>
@@ -4587,7 +4614,7 @@
       </c>
       <c r="U34" s="15"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A35" s="12" t="s">
         <v>213</v>
       </c>
@@ -4612,7 +4639,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A36" s="17" t="s">
         <v>637</v>
       </c>
@@ -4675,7 +4702,7 @@
       </c>
       <c r="U36" s="19"/>
     </row>
-    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A37" s="13" t="s">
         <v>214</v>
       </c>
@@ -4738,7 +4765,7 @@
       </c>
       <c r="U37" s="15"/>
     </row>
-    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A38" s="13" t="s">
         <v>491</v>
       </c>
@@ -4801,7 +4828,7 @@
       </c>
       <c r="U38" s="15"/>
     </row>
-    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A39" s="13" t="s">
         <v>521</v>
       </c>
@@ -4864,7 +4891,7 @@
       </c>
       <c r="U39" s="15"/>
     </row>
-    <row r="40" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A40" s="17" t="s">
         <v>534</v>
       </c>
@@ -4927,7 +4954,7 @@
       </c>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A41" s="17" t="s">
         <v>589</v>
       </c>
@@ -4990,7 +5017,7 @@
       </c>
       <c r="U41" s="19"/>
     </row>
-    <row r="42" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A42" s="17" t="s">
         <v>220</v>
       </c>
@@ -5053,7 +5080,7 @@
       </c>
       <c r="U42" s="19"/>
     </row>
-    <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A43" s="17" t="s">
         <v>629</v>
       </c>
@@ -5116,7 +5143,7 @@
       </c>
       <c r="U43" s="19"/>
     </row>
-    <row r="44" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A44" s="17" t="s">
         <v>564</v>
       </c>
@@ -5179,7 +5206,7 @@
       </c>
       <c r="U44" s="19"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A45" s="13" t="s">
         <v>225</v>
       </c>
@@ -5242,7 +5269,7 @@
       </c>
       <c r="U45" s="15"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A46" s="13" t="s">
         <v>231</v>
       </c>
@@ -5305,7 +5332,7 @@
       </c>
       <c r="U46" s="15"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A47" s="13" t="s">
         <v>231</v>
       </c>
@@ -5368,7 +5395,7 @@
       </c>
       <c r="U47" s="15"/>
     </row>
-    <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A48" s="17" t="s">
         <v>558</v>
       </c>
@@ -5431,30 +5458,30 @@
       </c>
       <c r="U48" s="19"/>
     </row>
-    <row r="49" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A49" s="17" t="s">
-        <v>510</v>
+        <v>668</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>559</v>
+        <v>675</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>514</v>
+        <v>674</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>512</v>
+        <v>668</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>669</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>510</v>
+        <v>668</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>515</v>
+        <v>670</v>
       </c>
       <c r="I49" s="17" t="s">
         <v>213</v>
@@ -5463,124 +5490,124 @@
         <v>23</v>
       </c>
       <c r="K49" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="M49" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N49" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="O49" s="17" t="s">
+        <v>671</v>
+      </c>
+      <c r="P49" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" s="18">
+        <v>44957</v>
+      </c>
+      <c r="R49" s="17" t="s">
+        <v>673</v>
+      </c>
+      <c r="S49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U49" s="19"/>
+    </row>
+    <row r="50" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A50" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="17" t="s">
         <v>513</v>
       </c>
-      <c r="L49" s="17" t="s">
+      <c r="L50" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M49" s="17" t="s">
+      <c r="M50" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="N49" s="17" t="s">
+      <c r="N50" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="O49" s="17" t="s">
+      <c r="O50" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="P49" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q49" s="18">
+      <c r="P50" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q50" s="18">
         <v>44333</v>
       </c>
-      <c r="R49" s="17" t="s">
+      <c r="R50" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="S49" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T49" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U49" s="19"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
+      <c r="S50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U50" s="19"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A51" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="13" t="s">
         <v>618</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D51" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E51" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F51" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>516</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J50" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K50" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M50" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="N50" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="O50" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="P50" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q50" s="14">
-        <v>43935</v>
-      </c>
-      <c r="R50" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="S50" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T50" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U50" s="15"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>619</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>245</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>213</v>
@@ -5589,28 +5616,28 @@
         <v>23</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>108</v>
+        <v>243</v>
       </c>
       <c r="N51" s="13" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="P51" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q51" s="14">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>31</v>
@@ -5620,30 +5647,30 @@
       </c>
       <c r="U51" s="15"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A52" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>213</v>
@@ -5652,7 +5679,7 @@
         <v>23</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="L52" s="13" t="s">
         <v>107</v>
@@ -5670,146 +5697,146 @@
         <v>42</v>
       </c>
       <c r="Q52" s="14">
+        <v>41600</v>
+      </c>
+      <c r="R52" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="S52" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T52" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U52" s="15"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A53" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>620</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="17" t="s">
+        <v>518</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="N53" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="O53" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="P53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" s="14">
         <v>42220</v>
       </c>
-      <c r="R52" s="13" t="s">
+      <c r="R53" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="S52" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T52" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U52" s="15"/>
-    </row>
-    <row r="53" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
+      <c r="S53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U53" s="15"/>
+    </row>
+    <row r="54" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A54" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B54" s="17" t="s">
         <v>666</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>661</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E54" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="G54" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="H54" s="17" t="s">
         <v>665</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I54" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="J53" s="17" t="s">
+      <c r="J54" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="K54" s="17" t="s">
         <v>664</v>
       </c>
-      <c r="L53" s="17" t="s">
+      <c r="L54" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M53" s="17" t="s">
+      <c r="M54" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="N53" s="17" t="s">
+      <c r="N54" s="17" t="s">
         <v>642</v>
       </c>
-      <c r="O53" s="17" t="s">
+      <c r="O54" s="17" t="s">
         <v>643</v>
       </c>
-      <c r="P53" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q53" s="26" t="s">
+      <c r="P54" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q54" s="26" t="s">
         <v>663</v>
       </c>
-      <c r="R53" s="17" t="s">
+      <c r="R54" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U53" s="19"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>617</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="I54" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="L54" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M54" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="N54" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="O54" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="P54" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q54" s="14">
-        <v>42158</v>
-      </c>
-      <c r="R54" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="S54" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T54" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U54" s="15"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S54" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T54" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U54" s="19"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A55" s="13" t="s">
         <v>256</v>
       </c>
@@ -5817,13 +5844,13 @@
         <v>617</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>256</v>
@@ -5872,93 +5899,93 @@
       </c>
       <c r="U55" s="15"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="17" t="s">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M56" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N56" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O56" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P56" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q56" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R56" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="S56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U56" s="15"/>
+    </row>
+    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A57" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B57" s="17" t="s">
         <v>651</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C57" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D57" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="E56" s="24" t="s">
+      <c r="E57" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F57" s="17" t="s">
         <v>647</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K56" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="L56" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M56" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N56" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="O56" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="P56" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q56" s="18">
-        <v>44833</v>
-      </c>
-      <c r="R56" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="S56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U56" s="19"/>
-    </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="17" t="s">
-        <v>605</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>608</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>606</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>607</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>605</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>213</v>
@@ -5967,7 +5994,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>123</v>
@@ -5976,19 +6003,19 @@
         <v>243</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>614</v>
+        <v>642</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>615</v>
+        <v>643</v>
       </c>
       <c r="P57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q57" s="18">
-        <v>44713</v>
+        <v>44833</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>614</v>
+        <v>641</v>
       </c>
       <c r="S57" s="17" t="s">
         <v>31</v>
@@ -5998,30 +6025,30 @@
       </c>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A58" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>557</v>
+        <v>608</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>551</v>
+        <v>609</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>552</v>
+        <v>606</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>553</v>
+        <v>607</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>555</v>
+        <v>610</v>
       </c>
       <c r="I58" s="17" t="s">
         <v>213</v>
@@ -6030,28 +6057,28 @@
         <v>23</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>556</v>
+        <v>611</v>
       </c>
       <c r="L58" s="17" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="M58" s="17" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="N58" s="17" t="s">
-        <v>268</v>
+        <v>614</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>269</v>
+        <v>615</v>
       </c>
       <c r="P58" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q58" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="S58" s="17" t="s">
         <v>31</v>
@@ -6061,30 +6088,30 @@
       </c>
       <c r="U58" s="19"/>
     </row>
-    <row r="59" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A59" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>571</v>
+        <v>552</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="G59" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="I59" s="17" t="s">
         <v>213</v>
@@ -6093,7 +6120,7 @@
         <v>23</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="L59" s="17" t="s">
         <v>218</v>
@@ -6102,19 +6129,19 @@
         <v>177</v>
       </c>
       <c r="N59" s="17" t="s">
-        <v>573</v>
+        <v>268</v>
       </c>
       <c r="O59" s="17" t="s">
-        <v>574</v>
+        <v>269</v>
       </c>
       <c r="P59" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q59" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R59" s="17" t="s">
-        <v>185</v>
+        <v>554</v>
       </c>
       <c r="S59" s="17" t="s">
         <v>31</v>
@@ -6124,30 +6151,30 @@
       </c>
       <c r="U59" s="19"/>
     </row>
-    <row r="60" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A60" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>601</v>
+        <v>577</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>597</v>
+        <v>571</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="G60" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>602</v>
+        <v>575</v>
       </c>
       <c r="I60" s="17" t="s">
         <v>213</v>
@@ -6156,7 +6183,7 @@
         <v>23</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="L60" s="17" t="s">
         <v>218</v>
@@ -6165,115 +6192,115 @@
         <v>177</v>
       </c>
       <c r="N60" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="O60" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="P60" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q60" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R60" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="S60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U60" s="19"/>
+    </row>
+    <row r="61" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A61" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N61" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="O60" s="17" t="s">
+      <c r="O61" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="P60" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q60" s="18">
+      <c r="P61" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q61" s="18">
         <v>44713</v>
       </c>
-      <c r="R60" s="17" t="s">
+      <c r="R61" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="S60" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T60" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U60" s="19"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
+      <c r="S61" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T61" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U61" s="19"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A62" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B62" s="13" t="s">
         <v>624</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C62" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D62" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E62" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F62" s="13" t="s">
         <v>264</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I61" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J61" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K61" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="L61" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="M61" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="N61" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="O61" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="P61" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q61" s="14">
-        <v>41771</v>
-      </c>
-      <c r="R61" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="S61" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T61" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U61" s="15"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
-        <v>579</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>581</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>582</v>
-      </c>
-      <c r="E62" s="21" t="s">
-        <v>583</v>
-      </c>
-      <c r="F62" s="13" t="s">
-        <v>579</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>587</v>
+        <v>42</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>213</v>
@@ -6282,28 +6309,28 @@
         <v>23</v>
       </c>
       <c r="K62" s="13" t="s">
-        <v>584</v>
+        <v>267</v>
       </c>
       <c r="L62" s="13" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="M62" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="N62" s="13" t="s">
-        <v>585</v>
+        <v>268</v>
       </c>
       <c r="O62" s="13" t="s">
-        <v>586</v>
+        <v>269</v>
       </c>
       <c r="P62" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q62" s="14">
-        <v>44700</v>
+        <v>41771</v>
       </c>
       <c r="R62" s="13" t="s">
-        <v>588</v>
+        <v>185</v>
       </c>
       <c r="S62" s="13" t="s">
         <v>31</v>
@@ -6313,91 +6340,93 @@
       </c>
       <c r="U62" s="15"/>
     </row>
-    <row r="63" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A63" s="13" t="s">
-        <v>271</v>
+        <v>579</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>625</v>
+        <v>580</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>277</v>
+        <v>581</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>272</v>
+        <v>582</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>583</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>271</v>
+        <v>579</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>273</v>
+        <v>21</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>274</v>
+        <v>587</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K63" s="13" t="s">
+        <v>584</v>
+      </c>
+      <c r="L63" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="M63" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="N63" s="13" t="s">
+        <v>585</v>
+      </c>
+      <c r="O63" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="P63" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q63" s="14">
+        <v>44700</v>
+      </c>
+      <c r="R63" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="S63" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T63" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U63" s="15"/>
+    </row>
+    <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A64" s="13" t="s">
         <v>271</v>
-      </c>
-      <c r="L63" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="M63" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="N63" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="O63" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="P63" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q63" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R63" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="S63" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T63" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="U63" s="15"/>
-    </row>
-    <row r="64" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
-        <v>279</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D64" s="13"/>
+        <v>277</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="E64" s="20" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>213</v>
@@ -6418,7 +6447,7 @@
         <v>275</v>
       </c>
       <c r="O64" s="13" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="P64" s="13" t="s">
         <v>42</v>
@@ -6427,38 +6456,38 @@
         <v>43788</v>
       </c>
       <c r="R64" s="13" t="s">
-        <v>285</v>
+        <v>65</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T64" s="13" t="s">
         <v>278</v>
       </c>
       <c r="U64" s="15"/>
     </row>
-    <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A65" s="13" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="20" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>213</v>
@@ -6466,9 +6495,15 @@
       <c r="J65" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
+      <c r="K65" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="L65" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="M65" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="N65" s="13" t="s">
         <v>275</v>
       </c>
@@ -6485,35 +6520,35 @@
         <v>285</v>
       </c>
       <c r="S65" s="13" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="T65" s="13" t="s">
         <v>278</v>
       </c>
       <c r="U65" s="15"/>
     </row>
-    <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A66" s="13" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>213</v>
@@ -6540,35 +6575,35 @@
         <v>285</v>
       </c>
       <c r="S66" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T66" s="13" t="s">
         <v>278</v>
       </c>
       <c r="U66" s="15"/>
     </row>
-    <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A67" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="20" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>213</v>
@@ -6602,28 +6637,28 @@
       </c>
       <c r="U67" s="15"/>
     </row>
-    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A68" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="20" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>213</v>
@@ -6657,28 +6692,28 @@
       </c>
       <c r="U68" s="15"/>
     </row>
-    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A69" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="20" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>213</v>
@@ -6712,28 +6747,28 @@
       </c>
       <c r="U69" s="15"/>
     </row>
-    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A70" s="13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="20" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>213</v>
@@ -6767,28 +6802,28 @@
       </c>
       <c r="U70" s="15"/>
     </row>
-    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A71" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="20" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>213</v>
@@ -6822,28 +6857,28 @@
       </c>
       <c r="U71" s="15"/>
     </row>
-    <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A72" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="20" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>213</v>
@@ -6877,28 +6912,28 @@
       </c>
       <c r="U72" s="15"/>
     </row>
-    <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A73" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="20" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>213</v>
@@ -6932,28 +6967,28 @@
       </c>
       <c r="U73" s="15"/>
     </row>
-    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A74" s="13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="20" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>213</v>
@@ -6987,28 +7022,28 @@
       </c>
       <c r="U74" s="15"/>
     </row>
-    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A75" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="20" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I75" s="13" t="s">
         <v>213</v>
@@ -7042,28 +7077,28 @@
       </c>
       <c r="U75" s="15"/>
     </row>
-    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A76" s="13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>625</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="20" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>213</v>
@@ -7097,143 +7132,141 @@
       </c>
       <c r="U76" s="15"/>
     </row>
-    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A77" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="D77" s="13" t="s">
-        <v>347</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="D77" s="13"/>
       <c r="E77" s="20" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>21</v>
+        <v>273</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I77" s="13" t="s">
         <v>213</v>
       </c>
       <c r="J77" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="O77" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="P77" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q77" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R77" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="S77" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="T77" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="U77" s="15"/>
+    </row>
+    <row r="78" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A78" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="I78" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J78" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K77" s="13" t="s">
+      <c r="K78" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="L77" s="13" t="s">
+      <c r="L78" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="M77" s="13" t="s">
+      <c r="M78" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="N77" s="13" t="s">
+      <c r="N78" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="O77" s="13" t="s">
+      <c r="O78" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="P77" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q77" s="14">
+      <c r="P78" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q78" s="14">
         <v>44111</v>
       </c>
-      <c r="R77" s="13" t="s">
+      <c r="R78" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="S77" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T77" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U77" s="15"/>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P78" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q78" s="14">
-        <v>43788</v>
-      </c>
-      <c r="R78" s="13"/>
-      <c r="S78" s="13"/>
-      <c r="T78" s="13"/>
+      <c r="S78" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T78" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="U78" s="15"/>
     </row>
-    <row r="79" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>627</v>
-      </c>
-      <c r="C79" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="D79" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E79" s="20" t="s">
-        <v>354</v>
-      </c>
-      <c r="F79" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="G79" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H79" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="I79" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J79" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K79" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="L79" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="M79" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="N79" s="13" t="s">
-        <v>356</v>
-      </c>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13"/>
       <c r="O79" s="13" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="P79" s="13" t="s">
         <v>42</v>
@@ -7241,39 +7274,35 @@
       <c r="Q79" s="14">
         <v>43788</v>
       </c>
-      <c r="R79" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="S79" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T79" s="13" t="s">
-        <v>278</v>
-      </c>
+      <c r="R79" s="13"/>
+      <c r="S79" s="13"/>
+      <c r="T79" s="13"/>
       <c r="U79" s="15"/>
     </row>
-    <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A80" s="13" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="D80" s="13"/>
+        <v>357</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>353</v>
+      </c>
       <c r="E80" s="20" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>213</v>
@@ -7294,7 +7323,7 @@
         <v>356</v>
       </c>
       <c r="O80" s="13" t="s">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>42</v>
@@ -7303,7 +7332,7 @@
         <v>43788</v>
       </c>
       <c r="R80" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S80" s="13" t="s">
         <v>31</v>
@@ -7313,28 +7342,28 @@
       </c>
       <c r="U80" s="15"/>
     </row>
-    <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A81" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="20" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>213</v>
@@ -7355,7 +7384,7 @@
         <v>356</v>
       </c>
       <c r="O81" s="13" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="P81" s="13" t="s">
         <v>42</v>
@@ -7364,7 +7393,7 @@
         <v>43788</v>
       </c>
       <c r="R81" s="13" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="S81" s="13" t="s">
         <v>31</v>
@@ -7374,28 +7403,28 @@
       </c>
       <c r="U81" s="15"/>
     </row>
-    <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A82" s="13" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="20" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>213</v>
@@ -7435,28 +7464,28 @@
       </c>
       <c r="U82" s="15"/>
     </row>
-    <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A83" s="13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>627</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="20" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>213</v>
@@ -7477,7 +7506,7 @@
         <v>356</v>
       </c>
       <c r="O83" s="13" t="s">
-        <v>363</v>
+        <v>63</v>
       </c>
       <c r="P83" s="13" t="s">
         <v>42</v>
@@ -7486,7 +7515,7 @@
         <v>43788</v>
       </c>
       <c r="R83" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S83" s="13" t="s">
         <v>31</v>
@@ -7496,23 +7525,49 @@
       </c>
       <c r="U83" s="15"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+    <row r="84" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A84" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>627</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>380</v>
+      </c>
       <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
+      <c r="E84" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J84" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K84" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="L84" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="M84" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="N84" s="13" t="s">
+        <v>356</v>
+      </c>
       <c r="O84" s="13" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="P84" s="13" t="s">
         <v>42</v>
@@ -7520,54 +7575,32 @@
       <c r="Q84" s="14">
         <v>43788</v>
       </c>
-      <c r="R84" s="13"/>
-      <c r="S84" s="13"/>
-      <c r="T84" s="13"/>
+      <c r="R84" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="S84" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T84" s="13" t="s">
+        <v>278</v>
+      </c>
       <c r="U84" s="15"/>
     </row>
-    <row r="85" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="B85" s="13" t="s">
-        <v>628</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="D85" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="E85" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="F85" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="G85" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H85" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="I85" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J85" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K85" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="L85" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="M85" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="N85" s="13" t="s">
-        <v>384</v>
-      </c>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13"/>
       <c r="O85" s="13" t="s">
         <v>63</v>
       </c>
@@ -7577,39 +7610,35 @@
       <c r="Q85" s="14">
         <v>43788</v>
       </c>
-      <c r="R85" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="S85" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="T85" s="13" t="s">
-        <v>278</v>
-      </c>
+      <c r="R85" s="13"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="13"/>
       <c r="U85" s="15"/>
     </row>
-    <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A86" s="13" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="D86" s="13"/>
+        <v>385</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>381</v>
+      </c>
       <c r="E86" s="20" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>213</v>
@@ -7642,35 +7671,35 @@
         <v>358</v>
       </c>
       <c r="S86" s="13" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="T86" s="13" t="s">
         <v>278</v>
       </c>
       <c r="U86" s="15"/>
     </row>
-    <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A87" s="13" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="20" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>213</v>
@@ -7703,35 +7732,35 @@
         <v>358</v>
       </c>
       <c r="S87" s="13" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="T87" s="13" t="s">
         <v>278</v>
       </c>
       <c r="U87" s="15"/>
     </row>
-    <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A88" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="20" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>213</v>
@@ -7771,28 +7800,28 @@
       </c>
       <c r="U88" s="15"/>
     </row>
-    <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A89" s="13" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="20" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>213</v>
@@ -7832,28 +7861,28 @@
       </c>
       <c r="U89" s="15"/>
     </row>
-    <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A90" s="13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="20" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>213</v>
@@ -7893,28 +7922,28 @@
       </c>
       <c r="U90" s="15"/>
     </row>
-    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A91" s="13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="20" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>213</v>
@@ -7954,28 +7983,28 @@
       </c>
       <c r="U91" s="15"/>
     </row>
-    <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A92" s="13" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="20" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>213</v>
@@ -8015,28 +8044,28 @@
       </c>
       <c r="U92" s="15"/>
     </row>
-    <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A93" s="13" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="20" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>213</v>
@@ -8076,28 +8105,28 @@
       </c>
       <c r="U93" s="15"/>
     </row>
-    <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A94" s="13" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="20" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>213</v>
@@ -8137,28 +8166,28 @@
       </c>
       <c r="U94" s="15"/>
     </row>
-    <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A95" s="13" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="20" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G95" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I95" s="13" t="s">
         <v>213</v>
@@ -8198,28 +8227,28 @@
       </c>
       <c r="U95" s="15"/>
     </row>
-    <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A96" s="13" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="20" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G96" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="I96" s="13" t="s">
         <v>213</v>
@@ -8259,28 +8288,28 @@
       </c>
       <c r="U96" s="15"/>
     </row>
-    <row r="97" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A97" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B97" s="13" t="s">
         <v>628</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D97" s="13"/>
       <c r="E97" s="20" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="G97" s="13" t="s">
         <v>273</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="I97" s="13" t="s">
         <v>213</v>
@@ -8320,104 +8349,108 @@
       </c>
       <c r="U97" s="15"/>
     </row>
-    <row r="98" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A98" s="12" t="s">
+    <row r="98" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A98" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="D98" s="13"/>
+      <c r="E98" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="F98" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="G98" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="I98" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J98" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K98" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="L98" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="M98" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="N98" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="O98" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P98" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q98" s="14">
+        <v>43788</v>
+      </c>
+      <c r="R98" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="S98" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="T98" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="U98" s="15"/>
+    </row>
+    <row r="99" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A99" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="22"/>
-      <c r="D98" s="22"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="22"/>
-      <c r="G98" s="22"/>
-      <c r="H98" s="22"/>
-      <c r="I98" s="22"/>
-      <c r="J98" s="22"/>
-      <c r="K98" s="22"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="22"/>
-      <c r="N98" s="22"/>
-      <c r="O98" s="22"/>
-      <c r="P98" s="22"/>
-      <c r="Q98" s="22"/>
-      <c r="R98" s="22"/>
-      <c r="S98" s="22"/>
-      <c r="T98" s="22"/>
-      <c r="U98" s="22"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="13" t="s">
+      <c r="B99" s="12"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
+      <c r="K99" s="22"/>
+      <c r="L99" s="22"/>
+      <c r="M99" s="22"/>
+      <c r="N99" s="22"/>
+      <c r="O99" s="22"/>
+      <c r="P99" s="22"/>
+      <c r="Q99" s="22"/>
+      <c r="R99" s="22"/>
+      <c r="S99" s="22"/>
+      <c r="T99" s="22"/>
+      <c r="U99" s="22"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A100" s="13" t="s">
         <v>447</v>
-      </c>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="D99" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="E99" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="F99" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="G99" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H99" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I99" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J99" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K99" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="L99" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="M99" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N99" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O99" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P99" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q99" s="14">
-        <v>42507</v>
-      </c>
-      <c r="R99" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="S99" s="13"/>
-      <c r="T99" s="13"/>
-      <c r="U99" s="15"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A100" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>123</v>
+        <v>447</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>21</v>
@@ -8432,49 +8465,49 @@
         <v>23</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>123</v>
+        <v>450</v>
       </c>
       <c r="M100" s="13" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="N100" s="13" t="s">
-        <v>455</v>
+        <v>26</v>
       </c>
       <c r="O100" s="13" t="s">
-        <v>456</v>
+        <v>27</v>
       </c>
       <c r="P100" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q100" s="14">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="R100" s="13" t="s">
-        <v>30</v>
+        <v>452</v>
       </c>
       <c r="S100" s="13"/>
       <c r="T100" s="13"/>
       <c r="U100" s="15"/>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A101" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="G101" s="13" t="s">
         <v>21</v>
@@ -8489,19 +8522,19 @@
         <v>23</v>
       </c>
       <c r="K101" s="13" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="L101" s="13" t="s">
-        <v>458</v>
+        <v>123</v>
       </c>
       <c r="M101" s="13" t="s">
-        <v>461</v>
+        <v>124</v>
       </c>
       <c r="N101" s="13" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O101" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="P101" s="13" t="s">
         <v>42</v>
@@ -8516,22 +8549,22 @@
       <c r="T101" s="13"/>
       <c r="U101" s="15"/>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A102" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="B102" s="13"/>
       <c r="C102" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="G102" s="13" t="s">
         <v>21</v>
@@ -8546,19 +8579,19 @@
         <v>23</v>
       </c>
       <c r="K102" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="L102" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="M102" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="N102" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="O102" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="P102" s="13" t="s">
         <v>42</v>
@@ -8573,175 +8606,209 @@
       <c r="T102" s="13"/>
       <c r="U102" s="15"/>
     </row>
-    <row r="103" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="17" t="s">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A103" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="G103" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I103" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J103" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K103" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="L103" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="M103" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="N103" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="O103" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="P103" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q103" s="14">
+        <v>41002</v>
+      </c>
+      <c r="R103" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S103" s="13"/>
+      <c r="T103" s="13"/>
+      <c r="U103" s="15"/>
+    </row>
+    <row r="104" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A104" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B103" s="17"/>
-      <c r="C103" s="13" t="s">
+      <c r="B104" s="17"/>
+      <c r="C104" s="13" t="s">
         <v>656</v>
       </c>
-      <c r="D103" s="17" t="s">
+      <c r="D104" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E103" s="17" t="s">
+      <c r="E104" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="F103" s="17" t="s">
+      <c r="F104" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G103" s="17" t="s">
+      <c r="G104" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H103" s="17" t="s">
+      <c r="H104" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="I103" s="17" t="s">
+      <c r="I104" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J103" s="17" t="s">
+      <c r="J104" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K103" s="17" t="s">
+      <c r="K104" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="L103" s="17" t="s">
+      <c r="L104" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M103" s="17" t="s">
+      <c r="M104" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="N103" s="17" t="s">
+      <c r="N104" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="O103" s="17" t="s">
+      <c r="O104" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P103" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q103" s="18">
+      <c r="P104" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q104" s="18">
         <v>41002</v>
       </c>
-      <c r="R103" s="17" t="s">
+      <c r="R104" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S103" s="17"/>
-      <c r="T103" s="17"/>
-      <c r="U103" s="19"/>
-    </row>
-    <row r="104" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A104" s="13" t="s">
+      <c r="S104" s="17"/>
+      <c r="T104" s="17"/>
+      <c r="U104" s="19"/>
+    </row>
+    <row r="105" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A105" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B104" s="13" t="s">
+      <c r="B105" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="C105" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D104" s="13" t="s">
+      <c r="D105" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E104" s="13" t="s">
+      <c r="E105" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F104" s="13" t="s">
+      <c r="F105" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="G104" s="13" t="s">
+      <c r="G105" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H104" s="13" t="s">
+      <c r="H105" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I104" s="13" t="s">
+      <c r="I105" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J104" s="13" t="s">
+      <c r="J105" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K104" s="13" t="s">
+      <c r="K105" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L104" s="13" t="s">
+      <c r="L105" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="M104" s="13" t="s">
+      <c r="M105" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N104" s="13" t="s">
+      <c r="N105" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O104" s="13" t="s">
+      <c r="O105" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P104" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q104" s="14">
+      <c r="P105" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q105" s="14">
         <v>42118</v>
       </c>
-      <c r="R104" s="13" t="s">
+      <c r="R105" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S104" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T104" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U104" s="15"/>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-      <c r="D105"/>
-      <c r="E105" s="10"/>
-      <c r="F105"/>
-      <c r="G105"/>
-      <c r="H105"/>
-      <c r="I105"/>
-      <c r="J105"/>
-      <c r="K105"/>
-      <c r="L105"/>
-      <c r="M105"/>
-      <c r="N105"/>
-      <c r="O105"/>
-      <c r="P105"/>
-      <c r="Q105"/>
-      <c r="R105"/>
-      <c r="S105"/>
-      <c r="T105"/>
-      <c r="U105"/>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+      <c r="S105" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T105" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U105" s="15"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A106"/>
+      <c r="B106"/>
+      <c r="C106"/>
+      <c r="D106"/>
+      <c r="E106" s="10"/>
+      <c r="F106"/>
+      <c r="G106"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="L106"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+      <c r="P106"/>
+      <c r="Q106"/>
+      <c r="R106"/>
+      <c r="S106"/>
+      <c r="T106"/>
+      <c r="U106"/>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A107" s="3" t="s">
         <v>472</v>
-      </c>
-      <c r="B106" s="3"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
-      <c r="K106" s="3"/>
-      <c r="L106" s="4"/>
-      <c r="M106" s="4"/>
-      <c r="N106" s="4"/>
-      <c r="O106" s="4"/>
-      <c r="P106" s="4"/>
-      <c r="Q106" s="6"/>
-      <c r="R106" s="4"/>
-      <c r="S106" s="4"/>
-      <c r="T106" s="4"/>
-      <c r="U106" s="4"/>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
-        <v>473</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="4"/>
@@ -8762,18 +8829,18 @@
       <c r="T107" s="4"/>
       <c r="U107" s="4"/>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="B108" s="4"/>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A108" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B108" s="3"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
-      <c r="K108" s="4"/>
+      <c r="K108" s="3"/>
       <c r="L108" s="4"/>
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
@@ -8785,9 +8852,9 @@
       <c r="T108" s="4"/>
       <c r="U108" s="4"/>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A109" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -8808,31 +8875,54 @@
       <c r="T109" s="4"/>
       <c r="U109" s="4"/>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="7" t="s">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A110" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="6"/>
+      <c r="R110" s="4"/>
+      <c r="S110" s="4"/>
+      <c r="T110" s="4"/>
+      <c r="U110" s="4"/>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A111" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
-      <c r="I110" s="7"/>
-      <c r="J110" s="7"/>
-      <c r="K110" s="7"/>
-      <c r="L110" s="7"/>
-      <c r="M110" s="7"/>
-      <c r="N110" s="7"/>
-      <c r="O110" s="7"/>
-      <c r="P110" s="7"/>
-      <c r="R110" s="7"/>
-      <c r="S110" s="7"/>
-      <c r="T110" s="7"/>
-      <c r="U110" s="7"/>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A111" s="5" t="s">
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="7"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="7"/>
+      <c r="P111" s="7"/>
+      <c r="R111" s="7"/>
+      <c r="S111" s="7"/>
+      <c r="T111" s="7"/>
+      <c r="U111" s="7"/>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A112" s="5" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the namespace "lucy" to the Namespace Registry and the (#576)
config.properties file.
</commit_message>
<xml_diff>
--- a/docs/namespace-registry/pds-namespace-registry.xlsx
+++ b/docs/namespace-registry/pds-namespace-registry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\8888_Namespaces\NameSpaceRegistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jshughes\git\pds4-information-model\docs\namespace-registry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2399724B-D8D0-4B77-9005-02F32E811604}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF2CB9B-E968-4E61-8438-0BC778A188FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{FAC3036B-2C0F-0A46-BDED-22E3426EC150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="676">
   <si>
     <t>Namespace Id (1)</t>
   </si>
@@ -2029,6 +2029,30 @@
   </si>
   <si>
     <t>Namespace for the Mars Science Laboratory dictionary.</t>
+  </si>
+  <si>
+    <t>lucy</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/lucy/v1</t>
+  </si>
+  <si>
+    <t>LUCY</t>
+  </si>
+  <si>
+    <t>msk at astro.umd.edu</t>
+  </si>
+  <si>
+    <t>Michael Kelley</t>
+  </si>
+  <si>
+    <t>M. Kelley</t>
+  </si>
+  <si>
+    <t>Namespace for the Lucy Mission Dictionary.</t>
+  </si>
+  <si>
+    <t>Lucy Mission</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2210,6 +2234,9 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2528,15 +2555,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="14.296875" style="5" customWidth="1"/>
     <col min="2" max="2" width="23.796875" style="5" customWidth="1"/>
@@ -2561,7 +2588,7 @@
     <col min="21" max="21" width="13.69921875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -2651,7 +2678,7 @@
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
@@ -2714,7 +2741,7 @@
       </c>
       <c r="U3" s="15"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
@@ -2739,7 +2766,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
     </row>
-    <row r="5" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -2802,7 +2829,7 @@
       </c>
       <c r="U5" s="15"/>
     </row>
-    <row r="6" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
@@ -2865,7 +2892,7 @@
       </c>
       <c r="U6" s="15"/>
     </row>
-    <row r="7" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A7" s="17" t="s">
         <v>539</v>
       </c>
@@ -2924,7 +2951,7 @@
       <c r="T7" s="17"/>
       <c r="U7" s="19"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2989,7 +3016,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A9" s="13" t="s">
         <v>66</v>
       </c>
@@ -3052,7 +3079,7 @@
       </c>
       <c r="U9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A10" s="13" t="s">
         <v>75</v>
       </c>
@@ -3115,7 +3142,7 @@
       </c>
       <c r="U10" s="15"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -3140,7 +3167,7 @@
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
     </row>
-    <row r="12" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A12" s="13" t="s">
         <v>85</v>
       </c>
@@ -3203,7 +3230,7 @@
       </c>
       <c r="U12" s="15"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A13" s="13" t="s">
         <v>95</v>
       </c>
@@ -3266,7 +3293,7 @@
       </c>
       <c r="U13" s="15"/>
     </row>
-    <row r="14" spans="1:21" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="124.8" x14ac:dyDescent="0.6">
       <c r="A14" s="13" t="s">
         <v>103</v>
       </c>
@@ -3329,7 +3356,7 @@
       </c>
       <c r="U14" s="15"/>
     </row>
-    <row r="15" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="13" t="s">
         <v>495</v>
       </c>
@@ -3392,7 +3419,7 @@
       </c>
       <c r="U15" s="15"/>
     </row>
-    <row r="16" spans="1:21" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A16" s="13" t="s">
         <v>113</v>
       </c>
@@ -3455,7 +3482,7 @@
       </c>
       <c r="U16" s="15"/>
     </row>
-    <row r="17" spans="1:21" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A17" s="17" t="s">
         <v>526</v>
       </c>
@@ -3518,7 +3545,7 @@
       </c>
       <c r="U17" s="19"/>
     </row>
-    <row r="18" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A18" s="13" t="s">
         <v>119</v>
       </c>
@@ -3581,7 +3608,7 @@
       </c>
       <c r="U18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A19" s="13" t="s">
         <v>107</v>
       </c>
@@ -3644,7 +3671,7 @@
       </c>
       <c r="U19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A20" s="13" t="s">
         <v>133</v>
       </c>
@@ -3707,7 +3734,7 @@
       </c>
       <c r="U20" s="15"/>
     </row>
-    <row r="21" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A21" s="17" t="s">
         <v>501</v>
       </c>
@@ -3770,7 +3797,7 @@
       </c>
       <c r="U21" s="19"/>
     </row>
-    <row r="22" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A22" s="13" t="s">
         <v>208</v>
       </c>
@@ -3833,7 +3860,7 @@
       </c>
       <c r="U22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A23" s="13" t="s">
         <v>139</v>
       </c>
@@ -3896,7 +3923,7 @@
       </c>
       <c r="U23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="78" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="78" x14ac:dyDescent="0.6">
       <c r="A24" s="13" t="s">
         <v>203</v>
       </c>
@@ -3959,7 +3986,7 @@
       </c>
       <c r="U24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A25" s="13" t="s">
         <v>144</v>
       </c>
@@ -4022,7 +4049,7 @@
       </c>
       <c r="U25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A26" s="13" t="s">
         <v>151</v>
       </c>
@@ -4085,7 +4112,7 @@
       </c>
       <c r="U26" s="15"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A27" s="13" t="s">
         <v>19</v>
       </c>
@@ -4148,7 +4175,7 @@
       </c>
       <c r="U27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A28" s="13" t="s">
         <v>89</v>
       </c>
@@ -4209,7 +4236,7 @@
       </c>
       <c r="U28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A29" s="13" t="s">
         <v>161</v>
       </c>
@@ -4272,7 +4299,7 @@
       </c>
       <c r="U29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A30" s="13" t="s">
         <v>166</v>
       </c>
@@ -4335,7 +4362,7 @@
       </c>
       <c r="U30" s="15"/>
     </row>
-    <row r="31" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A31" s="17" t="s">
         <v>657</v>
       </c>
@@ -4398,7 +4425,7 @@
       </c>
       <c r="U31" s="19"/>
     </row>
-    <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A32" s="13" t="s">
         <v>180</v>
       </c>
@@ -4461,7 +4488,7 @@
       </c>
       <c r="U32" s="15"/>
     </row>
-    <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A33" s="13" t="s">
         <v>186</v>
       </c>
@@ -4524,7 +4551,7 @@
       </c>
       <c r="U33" s="15"/>
     </row>
-    <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A34" s="13" t="s">
         <v>194</v>
       </c>
@@ -4587,7 +4614,7 @@
       </c>
       <c r="U34" s="15"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A35" s="12" t="s">
         <v>213</v>
       </c>
@@ -4612,7 +4639,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A36" s="17" t="s">
         <v>637</v>
       </c>
@@ -4675,7 +4702,7 @@
       </c>
       <c r="U36" s="19"/>
     </row>
-    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A37" s="13" t="s">
         <v>214</v>
       </c>
@@ -4738,7 +4765,7 @@
       </c>
       <c r="U37" s="15"/>
     </row>
-    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A38" s="13" t="s">
         <v>491</v>
       </c>
@@ -4801,7 +4828,7 @@
       </c>
       <c r="U38" s="15"/>
     </row>
-    <row r="39" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A39" s="13" t="s">
         <v>521</v>
       </c>
@@ -4864,7 +4891,7 @@
       </c>
       <c r="U39" s="15"/>
     </row>
-    <row r="40" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A40" s="17" t="s">
         <v>534</v>
       </c>
@@ -4927,7 +4954,7 @@
       </c>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A41" s="17" t="s">
         <v>589</v>
       </c>
@@ -4990,7 +5017,7 @@
       </c>
       <c r="U41" s="19"/>
     </row>
-    <row r="42" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A42" s="17" t="s">
         <v>220</v>
       </c>
@@ -5053,7 +5080,7 @@
       </c>
       <c r="U42" s="19"/>
     </row>
-    <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A43" s="17" t="s">
         <v>629</v>
       </c>
@@ -5116,7 +5143,7 @@
       </c>
       <c r="U43" s="19"/>
     </row>
-    <row r="44" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A44" s="17" t="s">
         <v>564</v>
       </c>
@@ -5179,7 +5206,7 @@
       </c>
       <c r="U44" s="19"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A45" s="13" t="s">
         <v>225</v>
       </c>
@@ -5242,7 +5269,7 @@
       </c>
       <c r="U45" s="15"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A46" s="13" t="s">
         <v>231</v>
       </c>
@@ -5305,7 +5332,7 @@
       </c>
       <c r="U46" s="15"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A47" s="13" t="s">
         <v>231</v>
       </c>
@@ -5368,7 +5395,7 @@
       </c>
       <c r="U47" s="15"/>
     </row>
-    <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A48" s="17" t="s">
         <v>558</v>
       </c>
@@ -5431,30 +5458,30 @@
       </c>
       <c r="U48" s="19"/>
     </row>
-    <row r="49" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A49" s="17" t="s">
-        <v>510</v>
+        <v>668</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>559</v>
+        <v>675</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>514</v>
+        <v>674</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>512</v>
+        <v>668</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>669</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>510</v>
+        <v>668</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>515</v>
+        <v>670</v>
       </c>
       <c r="I49" s="17" t="s">
         <v>213</v>
@@ -5463,124 +5490,124 @@
         <v>23</v>
       </c>
       <c r="K49" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="M49" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N49" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="O49" s="17" t="s">
+        <v>671</v>
+      </c>
+      <c r="P49" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" s="18">
+        <v>44957</v>
+      </c>
+      <c r="R49" s="17" t="s">
+        <v>673</v>
+      </c>
+      <c r="S49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U49" s="19"/>
+    </row>
+    <row r="50" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A50" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="17" t="s">
         <v>513</v>
       </c>
-      <c r="L49" s="17" t="s">
+      <c r="L50" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M49" s="17" t="s">
+      <c r="M50" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="N49" s="17" t="s">
+      <c r="N50" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="O49" s="17" t="s">
+      <c r="O50" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="P49" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q49" s="18">
+      <c r="P50" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q50" s="18">
         <v>44333</v>
       </c>
-      <c r="R49" s="17" t="s">
+      <c r="R50" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="S49" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T49" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U49" s="19"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
+      <c r="S50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U50" s="19"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A51" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="13" t="s">
         <v>618</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D51" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E51" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F51" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>516</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J50" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K50" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M50" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="N50" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="O50" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="P50" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q50" s="14">
-        <v>43935</v>
-      </c>
-      <c r="R50" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="S50" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T50" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U50" s="15"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>619</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>245</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>213</v>
@@ -5589,28 +5616,28 @@
         <v>23</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>108</v>
+        <v>243</v>
       </c>
       <c r="N51" s="13" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="P51" s="13" t="s">
         <v>42</v>
       </c>
       <c r="Q51" s="14">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>31</v>
@@ -5620,30 +5647,30 @@
       </c>
       <c r="U51" s="15"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A52" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>213</v>
@@ -5652,7 +5679,7 @@
         <v>23</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="L52" s="13" t="s">
         <v>107</v>
@@ -5670,146 +5697,146 @@
         <v>42</v>
       </c>
       <c r="Q52" s="14">
+        <v>41600</v>
+      </c>
+      <c r="R52" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="S52" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T52" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U52" s="15"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A53" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>620</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="17" t="s">
+        <v>518</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="N53" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="O53" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="P53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" s="14">
         <v>42220</v>
       </c>
-      <c r="R52" s="13" t="s">
+      <c r="R53" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="S52" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T52" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U52" s="15"/>
-    </row>
-    <row r="53" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
+      <c r="S53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U53" s="15"/>
+    </row>
+    <row r="54" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A54" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B54" s="17" t="s">
         <v>666</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>661</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E54" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="G54" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="H54" s="17" t="s">
         <v>665</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I54" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="J53" s="17" t="s">
+      <c r="J54" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="K54" s="17" t="s">
         <v>664</v>
       </c>
-      <c r="L53" s="17" t="s">
+      <c r="L54" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M53" s="17" t="s">
+      <c r="M54" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="N53" s="17" t="s">
+      <c r="N54" s="17" t="s">
         <v>642</v>
       </c>
-      <c r="O53" s="17" t="s">
+      <c r="O54" s="17" t="s">
         <v>643</v>
       </c>
-      <c r="P53" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q53" s="26" t="s">
+      <c r="P54" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q54" s="26" t="s">
         <v>663</v>
       </c>
-      <c r="R53" s="17" t="s">
+      <c r="R54" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U53" s="19"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>617</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="I54" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="L54" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M54" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="N54" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="O54" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="P54" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q54" s="14">
-        <v>42158</v>
-      </c>
-      <c r="R54" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="S54" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T54" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U54" s="15"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S54" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T54" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U54" s="19"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.6">
       <c r="A55" s="13" t="s">
         <v>256</v>
       </c>
@@ -5817,13 +5844,13 @@
         <v>617</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>256</v>
@@ -5872,93 +5899,93 @@
       </c>
       <c r="U55" s="15"/>
     </row>
-    <row r="56" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="17" t="s">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.6">
+      <c r="A56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M56" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N56" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O56" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="P56" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q56" s="14">
+        <v>42158</v>
+      </c>
+      <c r="R56" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="S56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U56" s="15"/>
+    </row>
+    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A57" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B57" s="17" t="s">
         <v>651</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C57" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D57" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="E56" s="24" t="s">
+      <c r="E57" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F57" s="17" t="s">
         <v>647</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K56" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="L56" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="M56" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N56" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="O56" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="P56" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q56" s="18">
-        <v>44833</v>
-      </c>
-      <c r="R56" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="S56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="U56" s="19"/>
-    </row>
-    <row r="57" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="17" t="s">
-        <v>605</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>608</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>606</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>607</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>605</v>
       </c>
       <c r="G57" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>213</v>
@@ -5967,7 +5994,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>123</v>
@@ -5976,19 +6003,19 @@
         <v>243</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>614</v>
+        <v>642</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>615</v>
+        <v>643</v>
       </c>
       <c r="P57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q57" s="18">
-        <v>44713</v>
+        <v>44833</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>614</v>
+        <v>641</v>
       </c>
       <c r="S57" s="17" t="s">
         <v>31</v>
@@ -5998,30 +6025,30 @@
       </c>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A58" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>557</v>
+        <v>608</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>551</v>
+        <v>609</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>552</v>
+        <v>606</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>553</v>
+        <v>607</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>555</v>
+        <v>610</v>
       </c>
       <c r="I58" s="17" t="s">
         <v>213</v>
@@ -6030,28 +6057,28 @@
         <v>23</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>556</v>
+        <v>611</v>
       </c>
       <c r="L58" s="17" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="M58" s="17" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="N58" s="17" t="s">
-        <v>268</v>
+        <v>614</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>269</v>
+        <v>615</v>
       </c>
       <c r="P58" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q58" s="18">
-        <v>43871</v>
+        <v>44713</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="S58" s="17" t="s">
         <v>31</v>
@@ -6061,30 +6088,30 @@
       </c>
       <c r="U58" s="19"/>
     </row>
-    <row r="59" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A59" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>571</v>
+        <v>552</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="G59" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="I59" s="17" t="s">
         <v>213</v>
@@ -6093,7 +6120,7 @@
         <v>23</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="L59" s="17" t="s">
         <v>218</v>
@@ -6102,19 +6129,19 @@
         <v>177</v>
       </c>
       <c r="N59" s="17" t="s">
-        <v>573</v>
+        <v>268</v>
       </c>
       <c r="O59" s="17" t="s">
-        <v>574</v>
+        <v>269</v>
       </c>
       <c r="P59" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q59" s="18">
-        <v>44643</v>
+        <v>43871</v>
       </c>
       <c r="R59" s="17" t="s">
-        <v>185</v>
+        <v>554</v>
       </c>
       <c r="S59" s="17" t="s">
         <v>31</v>
@@ -6124,30 +6151,30 @@
       </c>
       <c r="U59" s="19"/>
     </row>
-    <row r="60" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A60" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>601</v>
+        <v>577</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>597</v>
+        <v>571</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
       <c r="G60" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>602</v>
+        <v>575</v>
       </c>
       <c r="I60" s="17" t="s">
         <v>213</v>
@@ -6156,7 +6183,7 @@
         <v>23</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="L60" s="17" t="s">
         <v>218</v>
@@ -6165,115 +6192,115 @@
         <v>177</v>
       </c>
       <c r="N60" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="O60" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="P60" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q60" s="18">
+        <v>44643</v>
+      </c>
+      <c r="R60" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="S60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="U60" s="19"/>
+    </row>
+    <row r="61" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A61" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="N61" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="O60" s="17" t=